<commit_message>
Reading List.xlsx: added books for August 2023.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Projects\Project - Continuous Education\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Repositories\jupnb-nwreadinglistmanager\nwreadinglistmanager\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4169" uniqueCount="890">
   <si>
     <t>Format</t>
   </si>
@@ -2675,6 +2675,42 @@
   </si>
   <si>
     <t>CommentLenght</t>
+  </si>
+  <si>
+    <t>Python Tricks: A Buffet of Awesome Python Features</t>
+  </si>
+  <si>
+    <t>2023-08-16</t>
+  </si>
+  <si>
+    <t>Useful. An ok book for beginners.</t>
+  </si>
+  <si>
+    <t>Fluent Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useless. The book could be three times less pages and still provide the same amout of actionable knowledge. The author indulges into adding pages and pages of unrelevant information (mailing list discussions, implementation details, ...) that the reader who's looking into starting solving problems using Python does't need. </t>
+  </si>
+  <si>
+    <t>How To Become Fluent in Data Science</t>
+  </si>
+  <si>
+    <t>2023-08-17</t>
+  </si>
+  <si>
+    <t>Sharp Sight</t>
+  </si>
+  <si>
+    <t>Useless. Full of assumptions and arrogance.</t>
+  </si>
+  <si>
+    <t>Pandas Workout (MEAP)</t>
+  </si>
+  <si>
+    <t>2023-08-31</t>
+  </si>
+  <si>
+    <t>Useful. An enough readable "getting started" book.</t>
   </si>
 </sst>
 </file>
@@ -2814,7 +2850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2941,37 +2977,34 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3289,16 +3322,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46">
+      <c r="A1" s="54">
         <v>2016</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -4815,16 +4848,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46">
+      <c r="A1" s="54">
         <v>2017</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -5771,16 +5804,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46">
+      <c r="A1" s="54">
         <v>2018</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -6727,16 +6760,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46">
+      <c r="A1" s="54">
         <v>2019</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -7683,16 +7716,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46">
+      <c r="A1" s="54">
         <v>2020</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -8639,16 +8672,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46">
+      <c r="A1" s="54">
         <v>2021</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -9595,16 +9628,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46">
+      <c r="A1" s="54">
         <v>2022</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -10541,9 +10574,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:S255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A246" sqref="A246"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -11668,7 +11701,7 @@
       <c r="O18" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P18" s="56" t="s">
+      <c r="P18" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q18" s="9" t="s">
@@ -11916,7 +11949,7 @@
       <c r="O22" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P22" s="56" t="s">
+      <c r="P22" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q22" s="9" t="s">
@@ -12660,7 +12693,7 @@
       <c r="O34" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P34" s="56" t="s">
+      <c r="P34" s="47" t="s">
         <v>688</v>
       </c>
       <c r="Q34" s="9" t="s">
@@ -13342,7 +13375,7 @@
       <c r="O45" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P45" s="56" t="s">
+      <c r="P45" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q45" s="9" t="s">
@@ -13404,7 +13437,7 @@
       <c r="O46" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P46" s="56" t="s">
+      <c r="P46" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q46" s="9" t="s">
@@ -13528,7 +13561,7 @@
       <c r="O48" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P48" s="56" t="s">
+      <c r="P48" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q48" s="9" t="s">
@@ -13838,7 +13871,7 @@
       <c r="O53" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P53" s="56" t="s">
+      <c r="P53" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q53" s="9" t="s">
@@ -14210,7 +14243,7 @@
       <c r="O59" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P59" s="56" t="s">
+      <c r="P59" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q59" s="9" t="s">
@@ -14334,7 +14367,7 @@
       <c r="O61" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P61" s="56" t="s">
+      <c r="P61" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q61" s="9" t="s">
@@ -14396,7 +14429,7 @@
       <c r="O62" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P62" s="56" t="s">
+      <c r="P62" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q62" s="9" t="s">
@@ -15388,7 +15421,7 @@
       <c r="O78" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P78" s="56" t="s">
+      <c r="P78" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q78" s="9" t="s">
@@ -15760,7 +15793,7 @@
       <c r="O84" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P84" s="56" t="s">
+      <c r="P84" s="47" t="s">
         <v>742</v>
       </c>
       <c r="Q84" s="9" t="s">
@@ -17868,7 +17901,7 @@
       <c r="O118" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P118" s="56" t="s">
+      <c r="P118" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q118" s="9" t="s">
@@ -17930,7 +17963,7 @@
       <c r="O119" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P119" s="56" t="s">
+      <c r="P119" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q119" s="9" t="s">
@@ -18115,7 +18148,7 @@
       <c r="O122" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P122" s="56" t="s">
+      <c r="P122" s="47" t="s">
         <v>773</v>
       </c>
       <c r="Q122" s="9" t="s">
@@ -18177,7 +18210,7 @@
       <c r="O123" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P123" s="56" t="s">
+      <c r="P123" s="47" t="s">
         <v>774</v>
       </c>
       <c r="Q123" s="9" t="s">
@@ -24253,7 +24286,7 @@
       <c r="O221" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P221" s="56" t="s">
+      <c r="P221" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q221" s="9" t="s">
@@ -24563,7 +24596,7 @@
       <c r="O226" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P226" s="56" t="s">
+      <c r="P226" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q226" s="9" t="s">
@@ -24873,7 +24906,7 @@
       <c r="O231" s="18" t="s">
         <v>679</v>
       </c>
-      <c r="P231" s="56" t="s">
+      <c r="P231" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q231" s="9" t="s">
@@ -24910,11 +24943,11 @@
         <v>664</v>
       </c>
       <c r="H232" s="9">
-        <f t="shared" ref="H232:H243" si="30">YEAR(G232)</f>
+        <f t="shared" ref="H232:H247" si="30">YEAR(G232)</f>
         <v>2021</v>
       </c>
       <c r="I232" s="9">
-        <f t="shared" ref="I232:I243" si="31">MONTH(G232)</f>
+        <f t="shared" ref="I232:I247" si="31">MONTH(G232)</f>
         <v>3</v>
       </c>
       <c r="J232" s="9" t="s">
@@ -24945,7 +24978,7 @@
         <v>158</v>
       </c>
       <c r="S232" s="17">
-        <f t="shared" ref="S232:S243" si="32">LEN(P232)</f>
+        <f t="shared" ref="S232:S247" si="32">LEN(P232)</f>
         <v>54</v>
       </c>
     </row>
@@ -25632,256 +25665,420 @@
       </c>
     </row>
     <row r="244" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A244" s="13"/>
-      <c r="B244" s="14"/>
-      <c r="C244" s="9"/>
-      <c r="D244" s="9"/>
-      <c r="E244" s="9"/>
-      <c r="F244" s="14"/>
-      <c r="G244" s="9"/>
-      <c r="H244" s="9"/>
-      <c r="I244" s="9"/>
-      <c r="J244" s="9"/>
-      <c r="K244" s="9"/>
-      <c r="L244" s="9"/>
-      <c r="M244" s="14"/>
-      <c r="N244" s="43"/>
-      <c r="O244" s="9"/>
-      <c r="P244" s="28"/>
-      <c r="Q244" s="9"/>
-      <c r="R244" s="9"/>
-      <c r="S244" s="17"/>
+      <c r="A244" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="B244" s="14">
+        <v>2019</v>
+      </c>
+      <c r="C244" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D244" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E244" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="F244" s="14">
+        <v>175</v>
+      </c>
+      <c r="G244" s="9" t="s">
+        <v>879</v>
+      </c>
+      <c r="H244" s="9">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I244" s="9">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="J244" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K244" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L244" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="M244" s="14">
+        <v>3</v>
+      </c>
+      <c r="N244" s="43">
+        <v>29.9</v>
+      </c>
+      <c r="O244" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="P244" s="28" t="s">
+        <v>880</v>
+      </c>
+      <c r="Q244" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="R244" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S244" s="17">
+        <f t="shared" si="32"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="245" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A245" s="13"/>
-      <c r="B245" s="14"/>
-      <c r="C245" s="9"/>
-      <c r="D245" s="9"/>
-      <c r="E245" s="9"/>
-      <c r="F245" s="14"/>
-      <c r="G245" s="9"/>
-      <c r="H245" s="9"/>
-      <c r="I245" s="9"/>
-      <c r="J245" s="9"/>
-      <c r="K245" s="9"/>
-      <c r="L245" s="9"/>
-      <c r="M245" s="14"/>
-      <c r="N245" s="43"/>
-      <c r="O245" s="9"/>
-      <c r="P245" s="28"/>
-      <c r="Q245" s="9"/>
-      <c r="R245" s="9"/>
-      <c r="S245" s="17"/>
+      <c r="A245" s="13" t="s">
+        <v>881</v>
+      </c>
+      <c r="B245" s="14">
+        <v>2015</v>
+      </c>
+      <c r="C245" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D245" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E245" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="F245" s="14">
+        <v>766</v>
+      </c>
+      <c r="G245" s="9" t="s">
+        <v>879</v>
+      </c>
+      <c r="H245" s="9">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I245" s="9">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="J245" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K245" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L245" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="M245" s="14">
+        <v>1</v>
+      </c>
+      <c r="N245" s="43">
+        <v>49.99</v>
+      </c>
+      <c r="O245" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="P245" s="16" t="s">
+        <v>882</v>
+      </c>
+      <c r="Q245" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="R245" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S245" s="17">
+        <f t="shared" si="32"/>
+        <v>325</v>
+      </c>
     </row>
     <row r="246" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A246" s="13"/>
-      <c r="B246" s="14"/>
-      <c r="C246" s="9"/>
-      <c r="D246" s="9"/>
-      <c r="E246" s="9"/>
-      <c r="F246" s="14"/>
-      <c r="G246" s="9"/>
-      <c r="H246" s="9"/>
-      <c r="I246" s="9"/>
-      <c r="J246" s="9"/>
-      <c r="K246" s="9"/>
-      <c r="L246" s="9"/>
-      <c r="M246" s="14"/>
-      <c r="N246" s="43"/>
-      <c r="O246" s="9"/>
-      <c r="P246" s="28"/>
-      <c r="Q246" s="9"/>
-      <c r="R246" s="9"/>
-      <c r="S246" s="17"/>
+      <c r="A246" s="13" t="s">
+        <v>883</v>
+      </c>
+      <c r="B246" s="14">
+        <v>2023</v>
+      </c>
+      <c r="C246" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D246" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E246" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="F246" s="14">
+        <v>42</v>
+      </c>
+      <c r="G246" s="9" t="s">
+        <v>884</v>
+      </c>
+      <c r="H246" s="9">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I246" s="9">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="J246" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K246" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L246" s="9" t="s">
+        <v>885</v>
+      </c>
+      <c r="M246" s="14">
+        <v>1</v>
+      </c>
+      <c r="N246" s="43">
+        <v>0</v>
+      </c>
+      <c r="O246" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="P246" s="28" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q246" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="R246" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S246" s="17">
+        <f t="shared" si="32"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="247" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A247" s="13"/>
-      <c r="B247" s="13"/>
-      <c r="C247" s="13"/>
-      <c r="D247" s="13"/>
-      <c r="E247" s="13"/>
-      <c r="F247" s="55"/>
-      <c r="G247" s="13"/>
-      <c r="H247" s="13"/>
-      <c r="I247" s="13"/>
-      <c r="J247" s="13"/>
-      <c r="K247" s="13"/>
-      <c r="L247" s="13"/>
-      <c r="M247" s="55"/>
-      <c r="N247" s="13"/>
-      <c r="O247" s="13"/>
-      <c r="P247" s="28"/>
-      <c r="Q247" s="13"/>
-      <c r="R247" s="13"/>
-      <c r="S247" s="49"/>
+      <c r="A247" s="13" t="s">
+        <v>887</v>
+      </c>
+      <c r="B247" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C247" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D247" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E247" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="F247" s="14">
+        <v>187</v>
+      </c>
+      <c r="G247" s="9" t="s">
+        <v>888</v>
+      </c>
+      <c r="H247" s="9">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I247" s="9">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="J247" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K247" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L247" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="M247" s="14">
+        <v>2</v>
+      </c>
+      <c r="N247" s="43">
+        <v>49.99</v>
+      </c>
+      <c r="O247" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="P247" s="13" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q247" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="R247" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S247" s="17">
+        <f t="shared" si="32"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="248" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A248" s="48"/>
+      <c r="A248" s="46"/>
       <c r="B248" s="48"/>
       <c r="C248" s="48"/>
       <c r="D248" s="48"/>
       <c r="E248" s="48"/>
-      <c r="F248" s="50"/>
+      <c r="F248" s="49"/>
       <c r="G248" s="48"/>
-      <c r="H248" s="51"/>
-      <c r="I248" s="51"/>
-      <c r="J248" s="52"/>
+      <c r="H248" s="50"/>
+      <c r="I248" s="50"/>
+      <c r="J248" s="51"/>
       <c r="K248" s="48"/>
-      <c r="L248" s="52"/>
-      <c r="M248" s="53"/>
-      <c r="N248" s="54"/>
-      <c r="O248" s="54"/>
-      <c r="P248" s="28"/>
-      <c r="Q248" s="13"/>
-      <c r="R248" s="13"/>
-      <c r="S248" s="49"/>
+      <c r="L248" s="51"/>
+      <c r="M248" s="52"/>
+      <c r="N248" s="53"/>
+      <c r="O248" s="53"/>
+      <c r="P248" s="9"/>
+      <c r="Q248" s="9"/>
+      <c r="R248" s="9"/>
+      <c r="S248" s="17"/>
     </row>
     <row r="249" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A249" s="13"/>
-      <c r="B249" s="13"/>
-      <c r="C249" s="13"/>
-      <c r="D249" s="13"/>
-      <c r="E249" s="13"/>
-      <c r="F249" s="55"/>
-      <c r="G249" s="13"/>
-      <c r="H249" s="13"/>
-      <c r="I249" s="13"/>
-      <c r="J249" s="13"/>
-      <c r="K249" s="13"/>
-      <c r="L249" s="13"/>
-      <c r="M249" s="55"/>
-      <c r="N249" s="13"/>
-      <c r="O249" s="13"/>
-      <c r="P249" s="28"/>
-      <c r="Q249" s="13"/>
-      <c r="R249" s="13"/>
-      <c r="S249" s="49"/>
+      <c r="B249" s="9"/>
+      <c r="C249" s="9"/>
+      <c r="D249" s="9"/>
+      <c r="E249" s="9"/>
+      <c r="F249" s="14"/>
+      <c r="G249" s="9"/>
+      <c r="H249" s="9"/>
+      <c r="I249" s="9"/>
+      <c r="J249" s="9"/>
+      <c r="K249" s="9"/>
+      <c r="L249" s="9"/>
+      <c r="M249" s="14"/>
+      <c r="N249" s="9"/>
+      <c r="O249" s="9"/>
+      <c r="P249" s="9"/>
+      <c r="Q249" s="9"/>
+      <c r="R249" s="9"/>
+      <c r="S249" s="17"/>
     </row>
     <row r="250" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A250" s="13"/>
-      <c r="B250" s="13"/>
-      <c r="C250" s="13"/>
-      <c r="D250" s="13"/>
-      <c r="E250" s="13"/>
-      <c r="F250" s="55"/>
-      <c r="G250" s="13"/>
-      <c r="H250" s="13"/>
-      <c r="I250" s="13"/>
-      <c r="J250" s="13"/>
-      <c r="K250" s="13"/>
-      <c r="L250" s="13"/>
-      <c r="M250" s="55"/>
-      <c r="N250" s="13"/>
-      <c r="O250" s="13"/>
-      <c r="P250" s="28"/>
-      <c r="Q250" s="13"/>
-      <c r="R250" s="13"/>
-      <c r="S250" s="49"/>
+      <c r="B250" s="9"/>
+      <c r="C250" s="9"/>
+      <c r="D250" s="9"/>
+      <c r="E250" s="9"/>
+      <c r="F250" s="14"/>
+      <c r="G250" s="9"/>
+      <c r="H250" s="9"/>
+      <c r="I250" s="9"/>
+      <c r="J250" s="9"/>
+      <c r="K250" s="9"/>
+      <c r="L250" s="9"/>
+      <c r="M250" s="14"/>
+      <c r="N250" s="9"/>
+      <c r="O250" s="9"/>
+      <c r="P250" s="9"/>
+      <c r="Q250" s="9"/>
+      <c r="R250" s="9"/>
+      <c r="S250" s="17"/>
     </row>
     <row r="251" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A251" s="13"/>
-      <c r="B251" s="13"/>
-      <c r="C251" s="13"/>
-      <c r="D251" s="13"/>
-      <c r="E251" s="13"/>
-      <c r="F251" s="55"/>
-      <c r="G251" s="13"/>
-      <c r="H251" s="13"/>
-      <c r="I251" s="13"/>
-      <c r="J251" s="13"/>
-      <c r="K251" s="13"/>
-      <c r="L251" s="13"/>
-      <c r="M251" s="55"/>
-      <c r="N251" s="13"/>
-      <c r="O251" s="13"/>
-      <c r="P251" s="28"/>
-      <c r="Q251" s="13"/>
-      <c r="R251" s="13"/>
-      <c r="S251" s="49"/>
+      <c r="B251" s="9"/>
+      <c r="C251" s="9"/>
+      <c r="D251" s="9"/>
+      <c r="E251" s="9"/>
+      <c r="F251" s="14"/>
+      <c r="G251" s="9"/>
+      <c r="H251" s="9"/>
+      <c r="I251" s="9"/>
+      <c r="J251" s="9"/>
+      <c r="K251" s="9"/>
+      <c r="L251" s="9"/>
+      <c r="M251" s="14"/>
+      <c r="N251" s="9"/>
+      <c r="O251" s="9"/>
+      <c r="P251" s="9"/>
+      <c r="Q251" s="9"/>
+      <c r="R251" s="9"/>
+      <c r="S251" s="17"/>
     </row>
     <row r="252" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A252" s="13"/>
-      <c r="B252" s="13"/>
-      <c r="C252" s="13"/>
-      <c r="D252" s="13"/>
-      <c r="E252" s="13"/>
-      <c r="F252" s="55"/>
-      <c r="G252" s="13"/>
-      <c r="H252" s="13"/>
-      <c r="I252" s="13"/>
-      <c r="J252" s="13"/>
-      <c r="K252" s="13"/>
-      <c r="L252" s="13"/>
-      <c r="M252" s="55"/>
-      <c r="N252" s="13"/>
-      <c r="O252" s="13"/>
-      <c r="P252" s="28"/>
-      <c r="Q252" s="13"/>
-      <c r="R252" s="13"/>
-      <c r="S252" s="49"/>
+      <c r="B252" s="9"/>
+      <c r="C252" s="9"/>
+      <c r="D252" s="9"/>
+      <c r="E252" s="9"/>
+      <c r="F252" s="14"/>
+      <c r="G252" s="9"/>
+      <c r="H252" s="9"/>
+      <c r="I252" s="9"/>
+      <c r="J252" s="9"/>
+      <c r="K252" s="9"/>
+      <c r="L252" s="9"/>
+      <c r="M252" s="14"/>
+      <c r="N252" s="9"/>
+      <c r="O252" s="9"/>
+      <c r="P252" s="9"/>
+      <c r="Q252" s="9"/>
+      <c r="R252" s="9"/>
+      <c r="S252" s="17"/>
     </row>
     <row r="253" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A253" s="13"/>
-      <c r="B253" s="13"/>
-      <c r="C253" s="13"/>
-      <c r="D253" s="13"/>
-      <c r="E253" s="13"/>
-      <c r="F253" s="55"/>
-      <c r="G253" s="13"/>
-      <c r="H253" s="13"/>
-      <c r="I253" s="13"/>
-      <c r="J253" s="13"/>
-      <c r="K253" s="13"/>
-      <c r="L253" s="13"/>
-      <c r="M253" s="55"/>
-      <c r="N253" s="13"/>
-      <c r="O253" s="13"/>
-      <c r="P253" s="28"/>
-      <c r="Q253" s="13"/>
-      <c r="R253" s="13"/>
-      <c r="S253" s="49"/>
+      <c r="B253" s="9"/>
+      <c r="C253" s="9"/>
+      <c r="D253" s="9"/>
+      <c r="E253" s="9"/>
+      <c r="F253" s="14"/>
+      <c r="G253" s="9"/>
+      <c r="H253" s="9"/>
+      <c r="I253" s="9"/>
+      <c r="J253" s="9"/>
+      <c r="K253" s="9"/>
+      <c r="L253" s="9"/>
+      <c r="M253" s="14"/>
+      <c r="N253" s="9"/>
+      <c r="O253" s="9"/>
+      <c r="P253" s="9"/>
+      <c r="Q253" s="9"/>
+      <c r="R253" s="9"/>
+      <c r="S253" s="17"/>
     </row>
     <row r="254" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A254" s="13"/>
-      <c r="B254" s="13"/>
-      <c r="C254" s="13"/>
-      <c r="D254" s="13"/>
-      <c r="E254" s="13"/>
-      <c r="F254" s="55"/>
-      <c r="G254" s="13"/>
-      <c r="H254" s="13"/>
-      <c r="I254" s="13"/>
-      <c r="J254" s="13"/>
-      <c r="K254" s="13"/>
-      <c r="L254" s="13"/>
-      <c r="M254" s="55"/>
-      <c r="N254" s="13"/>
-      <c r="O254" s="13"/>
-      <c r="P254" s="28"/>
-      <c r="Q254" s="13"/>
-      <c r="R254" s="13"/>
-      <c r="S254" s="49"/>
+      <c r="B254" s="9"/>
+      <c r="C254" s="9"/>
+      <c r="D254" s="9"/>
+      <c r="E254" s="9"/>
+      <c r="F254" s="14"/>
+      <c r="G254" s="9"/>
+      <c r="H254" s="9"/>
+      <c r="I254" s="9"/>
+      <c r="J254" s="9"/>
+      <c r="K254" s="9"/>
+      <c r="L254" s="9"/>
+      <c r="M254" s="14"/>
+      <c r="N254" s="9"/>
+      <c r="O254" s="9"/>
+      <c r="P254" s="9"/>
+      <c r="Q254" s="9"/>
+      <c r="R254" s="9"/>
+      <c r="S254" s="17"/>
     </row>
     <row r="255" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A255" s="13"/>
-      <c r="B255" s="13"/>
-      <c r="C255" s="13"/>
-      <c r="D255" s="13"/>
-      <c r="E255" s="13"/>
-      <c r="F255" s="55"/>
-      <c r="G255" s="13"/>
-      <c r="H255" s="13"/>
-      <c r="I255" s="13"/>
-      <c r="J255" s="13"/>
-      <c r="K255" s="13"/>
-      <c r="L255" s="13"/>
-      <c r="M255" s="55"/>
-      <c r="N255" s="13"/>
-      <c r="O255" s="13"/>
-      <c r="P255" s="28"/>
-      <c r="Q255" s="13"/>
-      <c r="R255" s="13"/>
-      <c r="S255" s="49"/>
+      <c r="B255" s="9"/>
+      <c r="C255" s="9"/>
+      <c r="D255" s="9"/>
+      <c r="E255" s="9"/>
+      <c r="F255" s="14"/>
+      <c r="G255" s="9"/>
+      <c r="H255" s="9"/>
+      <c r="I255" s="9"/>
+      <c r="J255" s="9"/>
+      <c r="K255" s="9"/>
+      <c r="L255" s="9"/>
+      <c r="M255" s="14"/>
+      <c r="N255" s="9"/>
+      <c r="O255" s="9"/>
+      <c r="P255" s="9"/>
+      <c r="Q255" s="9"/>
+      <c r="R255" s="9"/>
+      <c r="S255" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Books updated to: 2023-09-13
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4169" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4277" uniqueCount="917">
   <si>
     <t>Format</t>
   </si>
@@ -2708,6 +2708,90 @@
   </si>
   <si>
     <t>Electronics, IoT</t>
+  </si>
+  <si>
+    <t>Pandas in 7 Days</t>
+  </si>
+  <si>
+    <t>2023-09-04</t>
+  </si>
+  <si>
+    <t>BPB Publications</t>
+  </si>
+  <si>
+    <t>Useful. A decent "Getting Started" book about Pandas, but nothing extraordinary. My copy lacks of bold fonts, which makes it a bit hard to read.</t>
+  </si>
+  <si>
+    <t>Effective Pandas: Patterns for Data Manipulation</t>
+  </si>
+  <si>
+    <t>2023-09-07</t>
+  </si>
+  <si>
+    <t>Useful. The book indeed contains information that other books about Pandas don't - for ex. about performances -, but the author advocates for big blocks of chained methods which it's a quite debatable way to write maintanable code.</t>
+  </si>
+  <si>
+    <t>Clean Architecture in Python</t>
+  </si>
+  <si>
+    <t>2023-09-08</t>
+  </si>
+  <si>
+    <t>Useful. Good overview for whom knows nothing about the topic and quite language-agnostic as well. But it advocates too much for the TDD methodology, which makes the book less objective.</t>
+  </si>
+  <si>
+    <t>Machine Learning Yearning (Draft)</t>
+  </si>
+  <si>
+    <t>2023-09-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useful. A lightweight introduction to neural networks and image classification. </t>
+  </si>
+  <si>
+    <t>Open Source Projects: Beyond Code</t>
+  </si>
+  <si>
+    <t>Useful. A good introduction for beginners, but nothing new for advanced users.</t>
+  </si>
+  <si>
+    <t>Useful Python</t>
+  </si>
+  <si>
+    <t>2023-09-12</t>
+  </si>
+  <si>
+    <t>SitePoint</t>
+  </si>
+  <si>
+    <t>Useful. Fifty pages of basic Python knowledge for beginners.</t>
+  </si>
+  <si>
+    <t>Be Data Analytical</t>
+  </si>
+  <si>
+    <t>KoganPage</t>
+  </si>
+  <si>
+    <t>Useful. A decent introduction for beginners, but it could have been shorter without impacting the content, because it's a but repetitive.</t>
+  </si>
+  <si>
+    <t>Creating Software with Modern Diagramming Techniques</t>
+  </si>
+  <si>
+    <t>2023-09-13</t>
+  </si>
+  <si>
+    <t>The Pragmatic Bookshelf</t>
+  </si>
+  <si>
+    <t>Useful. A comprehensive "Getting Started" book for Mermaid beginners, but nothing new for advanced users.</t>
+  </si>
+  <si>
+    <t>Python for Excel</t>
+  </si>
+  <si>
+    <t>Useful. It contains knowledge I didn't find in other books about Python and it's well written.</t>
   </si>
 </sst>
 </file>
@@ -2847,7 +2931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2974,33 +3058,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3319,16 +3385,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54">
+      <c r="A1" s="47">
         <v>2016</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -4845,16 +4911,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54">
+      <c r="A1" s="47">
         <v>2017</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -5801,16 +5867,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54">
+      <c r="A1" s="47">
         <v>2018</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -6757,16 +6823,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54">
+      <c r="A1" s="47">
         <v>2019</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -7713,16 +7779,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54">
+      <c r="A1" s="47">
         <v>2020</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -8669,16 +8735,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54">
+      <c r="A1" s="47">
         <v>2021</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -9625,16 +9691,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54">
+      <c r="A1" s="47">
         <v>2022</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -10569,11 +10635,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:S255"/>
+  <dimension ref="A1:S263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G256" sqref="G256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -11698,7 +11764,7 @@
       <c r="O18" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P18" s="47" t="s">
+      <c r="P18" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q18" s="9" t="s">
@@ -11946,7 +12012,7 @@
       <c r="O22" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P22" s="47" t="s">
+      <c r="P22" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q22" s="9" t="s">
@@ -12690,7 +12756,7 @@
       <c r="O34" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P34" s="47" t="s">
+      <c r="P34" s="46" t="s">
         <v>682</v>
       </c>
       <c r="Q34" s="9" t="s">
@@ -13372,7 +13438,7 @@
       <c r="O45" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P45" s="47" t="s">
+      <c r="P45" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q45" s="9" t="s">
@@ -13434,7 +13500,7 @@
       <c r="O46" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P46" s="47" t="s">
+      <c r="P46" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q46" s="9" t="s">
@@ -13558,7 +13624,7 @@
       <c r="O48" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P48" s="47" t="s">
+      <c r="P48" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q48" s="9" t="s">
@@ -13868,7 +13934,7 @@
       <c r="O53" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P53" s="47" t="s">
+      <c r="P53" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q53" s="9" t="s">
@@ -14240,7 +14306,7 @@
       <c r="O59" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P59" s="47" t="s">
+      <c r="P59" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q59" s="9" t="s">
@@ -14364,7 +14430,7 @@
       <c r="O61" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P61" s="47" t="s">
+      <c r="P61" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q61" s="9" t="s">
@@ -14426,7 +14492,7 @@
       <c r="O62" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P62" s="47" t="s">
+      <c r="P62" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q62" s="9" t="s">
@@ -15418,7 +15484,7 @@
       <c r="O78" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P78" s="47" t="s">
+      <c r="P78" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q78" s="9" t="s">
@@ -15790,7 +15856,7 @@
       <c r="O84" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P84" s="47" t="s">
+      <c r="P84" s="46" t="s">
         <v>736</v>
       </c>
       <c r="Q84" s="9" t="s">
@@ -17898,7 +17964,7 @@
       <c r="O118" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P118" s="47" t="s">
+      <c r="P118" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q118" s="9" t="s">
@@ -17960,7 +18026,7 @@
       <c r="O119" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P119" s="47" t="s">
+      <c r="P119" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q119" s="9" t="s">
@@ -18145,7 +18211,7 @@
       <c r="O122" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P122" s="47" t="s">
+      <c r="P122" s="46" t="s">
         <v>767</v>
       </c>
       <c r="Q122" s="9" t="s">
@@ -18207,7 +18273,7 @@
       <c r="O123" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P123" s="47" t="s">
+      <c r="P123" s="46" t="s">
         <v>768</v>
       </c>
       <c r="Q123" s="9" t="s">
@@ -24283,7 +24349,7 @@
       <c r="O221" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P221" s="47" t="s">
+      <c r="P221" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q221" s="9" t="s">
@@ -24593,7 +24659,7 @@
       <c r="O226" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P226" s="47" t="s">
+      <c r="P226" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q226" s="9" t="s">
@@ -24903,7 +24969,7 @@
       <c r="O231" s="18" t="s">
         <v>673</v>
       </c>
-      <c r="P231" s="47" t="s">
+      <c r="P231" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Q231" s="9" t="s">
@@ -24940,11 +25006,11 @@
         <v>659</v>
       </c>
       <c r="H232" s="9">
-        <f t="shared" ref="H232:H247" si="30">YEAR(G232)</f>
+        <f t="shared" ref="H232:H256" si="30">YEAR(G232)</f>
         <v>2021</v>
       </c>
       <c r="I232" s="9">
-        <f t="shared" ref="I232:I247" si="31">MONTH(G232)</f>
+        <f t="shared" ref="I232:I256" si="31">MONTH(G232)</f>
         <v>3</v>
       </c>
       <c r="J232" s="9" t="s">
@@ -24975,7 +25041,7 @@
         <v>158</v>
       </c>
       <c r="S232" s="17">
-        <f t="shared" ref="S232:S247" si="32">LEN(P232)</f>
+        <f t="shared" ref="S232:S256" si="32">LEN(P232)</f>
         <v>54</v>
       </c>
     </row>
@@ -25910,172 +25976,709 @@
       </c>
     </row>
     <row r="248" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A248" s="46"/>
-      <c r="B248" s="48"/>
-      <c r="C248" s="48"/>
-      <c r="D248" s="48"/>
-      <c r="E248" s="48"/>
-      <c r="F248" s="49"/>
-      <c r="G248" s="48"/>
-      <c r="H248" s="50"/>
-      <c r="I248" s="50"/>
-      <c r="J248" s="51"/>
-      <c r="K248" s="48"/>
-      <c r="L248" s="51"/>
-      <c r="M248" s="52"/>
-      <c r="N248" s="53"/>
-      <c r="O248" s="53"/>
-      <c r="P248" s="9"/>
-      <c r="Q248" s="9"/>
-      <c r="R248" s="9"/>
-      <c r="S248" s="17"/>
+      <c r="A248" s="13" t="s">
+        <v>889</v>
+      </c>
+      <c r="B248" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C248" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D248" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E248" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F248" s="14">
+        <v>280</v>
+      </c>
+      <c r="G248" s="9" t="s">
+        <v>890</v>
+      </c>
+      <c r="H248" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I248" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J248" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K248" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L248" s="11" t="s">
+        <v>891</v>
+      </c>
+      <c r="M248" s="8">
+        <v>2</v>
+      </c>
+      <c r="N248" s="43">
+        <v>29.95</v>
+      </c>
+      <c r="O248" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P248" s="16" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q248" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="R248" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S248" s="17">
+        <f t="shared" si="32"/>
+        <v>144</v>
+      </c>
     </row>
     <row r="249" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A249" s="13"/>
-      <c r="B249" s="9"/>
-      <c r="C249" s="9"/>
-      <c r="D249" s="9"/>
-      <c r="E249" s="9"/>
-      <c r="F249" s="14"/>
-      <c r="G249" s="9"/>
-      <c r="H249" s="9"/>
-      <c r="I249" s="9"/>
-      <c r="J249" s="9"/>
-      <c r="K249" s="9"/>
-      <c r="L249" s="9"/>
-      <c r="M249" s="14"/>
-      <c r="N249" s="9"/>
-      <c r="O249" s="9"/>
-      <c r="P249" s="9"/>
-      <c r="Q249" s="9"/>
-      <c r="R249" s="9"/>
-      <c r="S249" s="17"/>
+      <c r="A249" s="13" t="s">
+        <v>893</v>
+      </c>
+      <c r="B249" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C249" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D249" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E249" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F249" s="14">
+        <v>391</v>
+      </c>
+      <c r="G249" s="9" t="s">
+        <v>894</v>
+      </c>
+      <c r="H249" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I249" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J249" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K249" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L249" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="M249" s="14">
+        <v>3</v>
+      </c>
+      <c r="N249" s="43">
+        <v>39</v>
+      </c>
+      <c r="O249" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P249" s="16" t="s">
+        <v>895</v>
+      </c>
+      <c r="Q249" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="R249" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S249" s="17">
+        <f t="shared" si="32"/>
+        <v>231</v>
+      </c>
     </row>
     <row r="250" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A250" s="13"/>
-      <c r="B250" s="9"/>
-      <c r="C250" s="9"/>
-      <c r="D250" s="9"/>
-      <c r="E250" s="9"/>
-      <c r="F250" s="14"/>
-      <c r="G250" s="9"/>
-      <c r="H250" s="9"/>
-      <c r="I250" s="9"/>
-      <c r="J250" s="9"/>
-      <c r="K250" s="9"/>
-      <c r="L250" s="9"/>
-      <c r="M250" s="14"/>
-      <c r="N250" s="9"/>
-      <c r="O250" s="9"/>
-      <c r="P250" s="9"/>
-      <c r="Q250" s="9"/>
-      <c r="R250" s="9"/>
-      <c r="S250" s="17"/>
+      <c r="A250" s="13" t="s">
+        <v>896</v>
+      </c>
+      <c r="B250" s="17">
+        <v>2020</v>
+      </c>
+      <c r="C250" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D250" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E250" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F250" s="14">
+        <v>177</v>
+      </c>
+      <c r="G250" s="9" t="s">
+        <v>897</v>
+      </c>
+      <c r="H250" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I250" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J250" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K250" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L250" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="M250" s="14">
+        <v>2</v>
+      </c>
+      <c r="N250" s="43">
+        <v>0</v>
+      </c>
+      <c r="O250" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P250" s="16" t="s">
+        <v>898</v>
+      </c>
+      <c r="Q250" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="R250" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S250" s="17">
+        <f t="shared" si="32"/>
+        <v>185</v>
+      </c>
     </row>
     <row r="251" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A251" s="13"/>
-      <c r="B251" s="9"/>
-      <c r="C251" s="9"/>
-      <c r="D251" s="9"/>
-      <c r="E251" s="9"/>
-      <c r="F251" s="14"/>
-      <c r="G251" s="9"/>
-      <c r="H251" s="9"/>
-      <c r="I251" s="9"/>
-      <c r="J251" s="9"/>
-      <c r="K251" s="9"/>
-      <c r="L251" s="9"/>
-      <c r="M251" s="14"/>
-      <c r="N251" s="9"/>
-      <c r="O251" s="9"/>
-      <c r="P251" s="9"/>
-      <c r="Q251" s="9"/>
-      <c r="R251" s="9"/>
-      <c r="S251" s="17"/>
+      <c r="A251" s="13" t="s">
+        <v>899</v>
+      </c>
+      <c r="B251" s="17">
+        <v>2018</v>
+      </c>
+      <c r="C251" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D251" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E251" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F251" s="14">
+        <v>105</v>
+      </c>
+      <c r="G251" s="9" t="s">
+        <v>900</v>
+      </c>
+      <c r="H251" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I251" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J251" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K251" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L251" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="M251" s="14">
+        <v>2</v>
+      </c>
+      <c r="N251" s="43">
+        <v>0</v>
+      </c>
+      <c r="O251" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P251" s="49" t="s">
+        <v>901</v>
+      </c>
+      <c r="Q251" s="9" t="s">
+        <v>887</v>
+      </c>
+      <c r="R251" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S251" s="17">
+        <f t="shared" si="32"/>
+        <v>80</v>
+      </c>
     </row>
     <row r="252" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A252" s="13"/>
-      <c r="B252" s="9"/>
-      <c r="C252" s="9"/>
-      <c r="D252" s="9"/>
-      <c r="E252" s="9"/>
-      <c r="F252" s="14"/>
-      <c r="G252" s="9"/>
-      <c r="H252" s="9"/>
-      <c r="I252" s="9"/>
-      <c r="J252" s="9"/>
-      <c r="K252" s="9"/>
-      <c r="L252" s="9"/>
-      <c r="M252" s="14"/>
-      <c r="N252" s="9"/>
-      <c r="O252" s="9"/>
-      <c r="P252" s="9"/>
-      <c r="Q252" s="9"/>
-      <c r="R252" s="9"/>
-      <c r="S252" s="17"/>
+      <c r="A252" s="13" t="s">
+        <v>902</v>
+      </c>
+      <c r="B252" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C252" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D252" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E252" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F252" s="14">
+        <v>240</v>
+      </c>
+      <c r="G252" s="9" t="s">
+        <v>900</v>
+      </c>
+      <c r="H252" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I252" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J252" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K252" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L252" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="M252" s="14">
+        <v>3</v>
+      </c>
+      <c r="N252" s="43">
+        <v>39.99</v>
+      </c>
+      <c r="O252" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P252" s="13" t="s">
+        <v>903</v>
+      </c>
+      <c r="Q252" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="R252" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S252" s="17">
+        <f t="shared" si="32"/>
+        <v>78</v>
+      </c>
     </row>
     <row r="253" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A253" s="13"/>
-      <c r="B253" s="9"/>
-      <c r="C253" s="9"/>
-      <c r="D253" s="9"/>
-      <c r="E253" s="9"/>
-      <c r="F253" s="14"/>
-      <c r="G253" s="9"/>
-      <c r="H253" s="9"/>
-      <c r="I253" s="9"/>
-      <c r="J253" s="9"/>
-      <c r="K253" s="9"/>
-      <c r="L253" s="9"/>
-      <c r="M253" s="14"/>
-      <c r="N253" s="9"/>
-      <c r="O253" s="9"/>
-      <c r="P253" s="9"/>
-      <c r="Q253" s="9"/>
-      <c r="R253" s="9"/>
-      <c r="S253" s="17"/>
+      <c r="A253" s="13" t="s">
+        <v>904</v>
+      </c>
+      <c r="B253" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C253" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D253" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E253" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F253" s="14">
+        <v>51</v>
+      </c>
+      <c r="G253" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="H253" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I253" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J253" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K253" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L253" s="9" t="s">
+        <v>906</v>
+      </c>
+      <c r="M253" s="14">
+        <v>2</v>
+      </c>
+      <c r="N253" s="43">
+        <v>0</v>
+      </c>
+      <c r="O253" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P253" s="13" t="s">
+        <v>907</v>
+      </c>
+      <c r="Q253" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="R253" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S253" s="17">
+        <f t="shared" si="32"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="254" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A254" s="13"/>
-      <c r="B254" s="9"/>
-      <c r="C254" s="9"/>
-      <c r="D254" s="9"/>
-      <c r="E254" s="9"/>
-      <c r="F254" s="14"/>
-      <c r="G254" s="9"/>
-      <c r="H254" s="9"/>
-      <c r="I254" s="9"/>
-      <c r="J254" s="9"/>
-      <c r="K254" s="9"/>
-      <c r="L254" s="9"/>
-      <c r="M254" s="14"/>
-      <c r="N254" s="9"/>
-      <c r="O254" s="9"/>
-      <c r="P254" s="9"/>
-      <c r="Q254" s="9"/>
-      <c r="R254" s="9"/>
-      <c r="S254" s="17"/>
+      <c r="A254" s="13" t="s">
+        <v>908</v>
+      </c>
+      <c r="B254" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C254" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D254" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E254" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F254" s="14">
+        <v>184</v>
+      </c>
+      <c r="G254" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="H254" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I254" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J254" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K254" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L254" s="9" t="s">
+        <v>909</v>
+      </c>
+      <c r="M254" s="14">
+        <v>2</v>
+      </c>
+      <c r="N254" s="43">
+        <v>29.99</v>
+      </c>
+      <c r="O254" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P254" s="16" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q254" s="9" t="s">
+        <v>887</v>
+      </c>
+      <c r="R254" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S254" s="17">
+        <f t="shared" si="32"/>
+        <v>137</v>
+      </c>
     </row>
     <row r="255" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A255" s="13"/>
-      <c r="B255" s="9"/>
-      <c r="C255" s="9"/>
-      <c r="D255" s="9"/>
-      <c r="E255" s="9"/>
-      <c r="F255" s="14"/>
-      <c r="G255" s="9"/>
-      <c r="H255" s="9"/>
-      <c r="I255" s="9"/>
-      <c r="J255" s="9"/>
-      <c r="K255" s="9"/>
-      <c r="L255" s="9"/>
-      <c r="M255" s="14"/>
-      <c r="N255" s="9"/>
-      <c r="O255" s="9"/>
-      <c r="P255" s="9"/>
-      <c r="Q255" s="9"/>
-      <c r="R255" s="9"/>
-      <c r="S255" s="17"/>
+      <c r="A255" s="13" t="s">
+        <v>911</v>
+      </c>
+      <c r="B255" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C255" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D255" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E255" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F255" s="14">
+        <v>203</v>
+      </c>
+      <c r="G255" s="9" t="s">
+        <v>912</v>
+      </c>
+      <c r="H255" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I255" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J255" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K255" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L255" s="9" t="s">
+        <v>913</v>
+      </c>
+      <c r="M255" s="14">
+        <v>2</v>
+      </c>
+      <c r="N255" s="43">
+        <v>29.49</v>
+      </c>
+      <c r="O255" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P255" s="9" t="s">
+        <v>914</v>
+      </c>
+      <c r="Q255" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="R255" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S255" s="17">
+        <f t="shared" si="32"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="256" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A256" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="B256" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C256" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D256" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E256" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="F256" s="17">
+        <v>338</v>
+      </c>
+      <c r="G256" s="9" t="s">
+        <v>912</v>
+      </c>
+      <c r="H256" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I256" s="17">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="J256" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K256" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L256" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="M256" s="17">
+        <v>3</v>
+      </c>
+      <c r="N256" s="43">
+        <v>36.49</v>
+      </c>
+      <c r="O256" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="P256" s="13" t="s">
+        <v>916</v>
+      </c>
+      <c r="Q256" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="R256" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S256" s="17">
+        <f t="shared" si="32"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="257" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A257" s="9"/>
+      <c r="B257" s="9"/>
+      <c r="C257" s="9"/>
+      <c r="D257" s="9"/>
+      <c r="E257" s="9"/>
+      <c r="F257" s="9"/>
+      <c r="G257" s="9"/>
+      <c r="H257" s="9"/>
+      <c r="I257" s="9"/>
+      <c r="J257" s="9"/>
+      <c r="K257" s="9"/>
+      <c r="L257" s="9"/>
+      <c r="M257" s="9"/>
+      <c r="N257" s="9"/>
+      <c r="O257" s="9"/>
+      <c r="P257" s="9"/>
+      <c r="Q257" s="9"/>
+      <c r="R257" s="9"/>
+      <c r="S257" s="17"/>
+    </row>
+    <row r="258" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A258" s="9"/>
+      <c r="B258" s="9"/>
+      <c r="C258" s="9"/>
+      <c r="D258" s="9"/>
+      <c r="E258" s="9"/>
+      <c r="F258" s="9"/>
+      <c r="G258" s="9"/>
+      <c r="H258" s="9"/>
+      <c r="I258" s="9"/>
+      <c r="J258" s="9"/>
+      <c r="K258" s="9"/>
+      <c r="L258" s="9"/>
+      <c r="M258" s="9"/>
+      <c r="N258" s="9"/>
+      <c r="O258" s="9"/>
+      <c r="P258" s="9"/>
+      <c r="Q258" s="9"/>
+      <c r="R258" s="9"/>
+      <c r="S258" s="17"/>
+    </row>
+    <row r="259" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A259" s="9"/>
+      <c r="B259" s="9"/>
+      <c r="C259" s="9"/>
+      <c r="D259" s="9"/>
+      <c r="E259" s="9"/>
+      <c r="F259" s="9"/>
+      <c r="G259" s="9"/>
+      <c r="H259" s="9"/>
+      <c r="I259" s="9"/>
+      <c r="J259" s="9"/>
+      <c r="K259" s="9"/>
+      <c r="L259" s="9"/>
+      <c r="M259" s="9"/>
+      <c r="N259" s="9"/>
+      <c r="O259" s="9"/>
+      <c r="P259" s="9"/>
+      <c r="Q259" s="9"/>
+      <c r="R259" s="9"/>
+      <c r="S259" s="17"/>
+    </row>
+    <row r="260" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A260" s="9"/>
+      <c r="B260" s="9"/>
+      <c r="C260" s="9"/>
+      <c r="D260" s="9"/>
+      <c r="E260" s="9"/>
+      <c r="F260" s="9"/>
+      <c r="G260" s="9"/>
+      <c r="H260" s="9"/>
+      <c r="I260" s="9"/>
+      <c r="J260" s="9"/>
+      <c r="K260" s="9"/>
+      <c r="L260" s="9"/>
+      <c r="M260" s="9"/>
+      <c r="N260" s="9"/>
+      <c r="O260" s="9"/>
+      <c r="P260" s="9"/>
+      <c r="Q260" s="9"/>
+      <c r="R260" s="9"/>
+      <c r="S260" s="17"/>
+    </row>
+    <row r="261" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A261" s="9"/>
+      <c r="B261" s="9"/>
+      <c r="C261" s="9"/>
+      <c r="D261" s="9"/>
+      <c r="E261" s="9"/>
+      <c r="F261" s="9"/>
+      <c r="G261" s="9"/>
+      <c r="H261" s="9"/>
+      <c r="I261" s="9"/>
+      <c r="J261" s="9"/>
+      <c r="K261" s="9"/>
+      <c r="L261" s="9"/>
+      <c r="M261" s="9"/>
+      <c r="N261" s="9"/>
+      <c r="O261" s="9"/>
+      <c r="P261" s="9"/>
+      <c r="Q261" s="9"/>
+      <c r="R261" s="9"/>
+      <c r="S261" s="17"/>
+    </row>
+    <row r="262" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A262" s="9"/>
+      <c r="B262" s="9"/>
+      <c r="C262" s="9"/>
+      <c r="D262" s="9"/>
+      <c r="E262" s="9"/>
+      <c r="F262" s="9"/>
+      <c r="G262" s="9"/>
+      <c r="H262" s="9"/>
+      <c r="I262" s="9"/>
+      <c r="J262" s="9"/>
+      <c r="K262" s="9"/>
+      <c r="L262" s="9"/>
+      <c r="M262" s="9"/>
+      <c r="N262" s="9"/>
+      <c r="O262" s="9"/>
+      <c r="P262" s="9"/>
+      <c r="Q262" s="9"/>
+      <c r="R262" s="9"/>
+      <c r="S262" s="17"/>
+    </row>
+    <row r="263" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A263" s="9"/>
+      <c r="B263" s="9"/>
+      <c r="C263" s="9"/>
+      <c r="D263" s="9"/>
+      <c r="E263" s="9"/>
+      <c r="F263" s="9"/>
+      <c r="G263" s="9"/>
+      <c r="H263" s="9"/>
+      <c r="I263" s="9"/>
+      <c r="J263" s="9"/>
+      <c r="K263" s="9"/>
+      <c r="L263" s="9"/>
+      <c r="M263" s="9"/>
+      <c r="N263" s="9"/>
+      <c r="O263" s="9"/>
+      <c r="P263" s="9"/>
+      <c r="Q263" s="9"/>
+      <c r="R263" s="9"/>
+      <c r="S263" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#1 Reading List*: * => 'Data Analysis, Data Science, ML'
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Articles!$A$1:$Q$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Books!$A$1:$S$247</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Books!$A$1:$S$256</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Others!$A$1:$Q$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -2704,9 +2704,6 @@
     <t>Entrepreneurship, Learning</t>
   </si>
   <si>
-    <t>Data Science, ML</t>
-  </si>
-  <si>
     <t>Electronics, IoT</t>
   </si>
   <si>
@@ -2792,6 +2789,9 @@
   </si>
   <si>
     <t>Useful. It contains knowledge I didn't find in other books about Python and it's well written.</t>
+  </si>
+  <si>
+    <t>Data Analysis, Data Science, ML</t>
   </si>
 </sst>
 </file>
@@ -3059,14 +3059,14 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3385,16 +3385,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="48">
         <v>2016</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -4911,16 +4911,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="48">
         <v>2017</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -5867,16 +5867,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="48">
         <v>2018</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -6823,16 +6823,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="48">
         <v>2019</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -7779,16 +7779,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="48">
         <v>2020</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -8735,16 +8735,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="48">
         <v>2021</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -9691,16 +9691,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47">
+      <c r="A1" s="48">
         <v>2022</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -10637,9 +10637,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:S263"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G256" sqref="G256"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q261" sqref="Q261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -11706,7 +11706,7 @@
         <v>696</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R17" s="9" t="s">
         <v>159</v>
@@ -11768,7 +11768,7 @@
         <v>60</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R18" s="9" t="s">
         <v>159</v>
@@ -11954,7 +11954,7 @@
         <v>704</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R21" s="9" t="s">
         <v>159</v>
@@ -12326,7 +12326,7 @@
         <v>707</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R27" s="9" t="s">
         <v>159</v>
@@ -12388,7 +12388,7 @@
         <v>708</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R28" s="9" t="s">
         <v>159</v>
@@ -12450,7 +12450,7 @@
         <v>677</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R29" s="9" t="s">
         <v>159</v>
@@ -13442,7 +13442,7 @@
         <v>60</v>
       </c>
       <c r="Q45" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="R45" s="9" t="s">
         <v>159</v>
@@ -13504,7 +13504,7 @@
         <v>60</v>
       </c>
       <c r="Q46" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="R46" s="9" t="s">
         <v>159</v>
@@ -13566,7 +13566,7 @@
         <v>684</v>
       </c>
       <c r="Q47" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="R47" s="9" t="s">
         <v>159</v>
@@ -14310,7 +14310,7 @@
         <v>60</v>
       </c>
       <c r="Q59" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R59" s="9" t="s">
         <v>159</v>
@@ -14620,7 +14620,7 @@
         <v>720</v>
       </c>
       <c r="Q64" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R64" s="9" t="s">
         <v>159</v>
@@ -16232,7 +16232,7 @@
         <v>742</v>
       </c>
       <c r="Q90" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R90" s="9" t="s">
         <v>159</v>
@@ -16914,7 +16914,7 @@
         <v>749</v>
       </c>
       <c r="Q101" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="R101" s="9" t="s">
         <v>159</v>
@@ -17038,7 +17038,7 @@
         <v>751</v>
       </c>
       <c r="Q103" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R103" s="9" t="s">
         <v>159</v>
@@ -17100,7 +17100,7 @@
         <v>752</v>
       </c>
       <c r="Q104" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R104" s="9" t="s">
         <v>159</v>
@@ -17224,7 +17224,7 @@
         <v>754</v>
       </c>
       <c r="Q106" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R106" s="9" t="s">
         <v>159</v>
@@ -17286,7 +17286,7 @@
         <v>755</v>
       </c>
       <c r="Q107" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R107" s="9" t="s">
         <v>159</v>
@@ -18215,7 +18215,7 @@
         <v>767</v>
       </c>
       <c r="Q122" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R122" s="9" t="s">
         <v>159</v>
@@ -18525,7 +18525,7 @@
         <v>772</v>
       </c>
       <c r="Q127" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R127" s="9" t="s">
         <v>159</v>
@@ -18587,7 +18587,7 @@
         <v>773</v>
       </c>
       <c r="Q128" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R128" s="9" t="s">
         <v>159</v>
@@ -18835,7 +18835,7 @@
         <v>777</v>
       </c>
       <c r="Q132" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R132" s="9" t="s">
         <v>159</v>
@@ -19269,7 +19269,7 @@
         <v>784</v>
       </c>
       <c r="Q139" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R139" s="9" t="s">
         <v>159</v>
@@ -19331,7 +19331,7 @@
         <v>785</v>
       </c>
       <c r="Q140" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R140" s="9" t="s">
         <v>159</v>
@@ -19703,7 +19703,7 @@
         <v>789</v>
       </c>
       <c r="Q146" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R146" s="9" t="s">
         <v>159</v>
@@ -19765,7 +19765,7 @@
         <v>683</v>
       </c>
       <c r="Q147" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R147" s="9" t="s">
         <v>159</v>
@@ -20323,7 +20323,7 @@
         <v>796</v>
       </c>
       <c r="Q156" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R156" s="9" t="s">
         <v>158</v>
@@ -21315,7 +21315,7 @@
         <v>809</v>
       </c>
       <c r="Q172" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R172" s="9" t="s">
         <v>158</v>
@@ -22183,7 +22183,7 @@
         <v>816</v>
       </c>
       <c r="Q186" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R186" s="9" t="s">
         <v>158</v>
@@ -22245,7 +22245,7 @@
         <v>817</v>
       </c>
       <c r="Q187" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R187" s="9" t="s">
         <v>158</v>
@@ -22369,7 +22369,7 @@
         <v>683</v>
       </c>
       <c r="Q189" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R189" s="9" t="s">
         <v>159</v>
@@ -23733,7 +23733,7 @@
         <v>831</v>
       </c>
       <c r="Q211" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R211" s="9" t="s">
         <v>159</v>
@@ -23795,7 +23795,7 @@
         <v>832</v>
       </c>
       <c r="Q212" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R212" s="9" t="s">
         <v>159</v>
@@ -25159,7 +25159,7 @@
         <v>847</v>
       </c>
       <c r="Q234" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R234" s="9" t="s">
         <v>159</v>
@@ -25283,7 +25283,7 @@
         <v>869</v>
       </c>
       <c r="Q236" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R236" s="9" t="s">
         <v>159</v>
@@ -25407,7 +25407,7 @@
         <v>857</v>
       </c>
       <c r="Q238" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R238" s="9" t="s">
         <v>159</v>
@@ -25531,7 +25531,7 @@
         <v>58</v>
       </c>
       <c r="Q240" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R240" s="9" t="s">
         <v>159</v>
@@ -25903,7 +25903,7 @@
         <v>879</v>
       </c>
       <c r="Q246" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R246" s="9" t="s">
         <v>159</v>
@@ -25977,7 +25977,7 @@
     </row>
     <row r="248" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A248" s="13" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B248" s="17">
         <v>2023</v>
@@ -25995,7 +25995,7 @@
         <v>280</v>
       </c>
       <c r="G248" s="9" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="H248" s="17">
         <f t="shared" si="30"/>
@@ -26012,7 +26012,7 @@
         <v>159</v>
       </c>
       <c r="L248" s="11" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="M248" s="8">
         <v>2</v>
@@ -26024,7 +26024,7 @@
         <v>673</v>
       </c>
       <c r="P248" s="16" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="Q248" s="9" t="s">
         <v>575</v>
@@ -26039,7 +26039,7 @@
     </row>
     <row r="249" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A249" s="13" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B249" s="17">
         <v>2021</v>
@@ -26057,7 +26057,7 @@
         <v>391</v>
       </c>
       <c r="G249" s="9" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H249" s="17">
         <f t="shared" si="30"/>
@@ -26086,7 +26086,7 @@
         <v>673</v>
       </c>
       <c r="P249" s="16" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="Q249" s="9" t="s">
         <v>575</v>
@@ -26101,7 +26101,7 @@
     </row>
     <row r="250" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B250" s="17">
         <v>2020</v>
@@ -26119,7 +26119,7 @@
         <v>177</v>
       </c>
       <c r="G250" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H250" s="17">
         <f t="shared" si="30"/>
@@ -26148,7 +26148,7 @@
         <v>673</v>
       </c>
       <c r="P250" s="16" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="Q250" s="9" t="s">
         <v>575</v>
@@ -26163,7 +26163,7 @@
     </row>
     <row r="251" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B251" s="17">
         <v>2018</v>
@@ -26181,7 +26181,7 @@
         <v>105</v>
       </c>
       <c r="G251" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H251" s="17">
         <f t="shared" si="30"/>
@@ -26209,11 +26209,11 @@
       <c r="O251" s="9" t="s">
         <v>673</v>
       </c>
-      <c r="P251" s="49" t="s">
-        <v>901</v>
+      <c r="P251" s="47" t="s">
+        <v>900</v>
       </c>
       <c r="Q251" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R251" s="9" t="s">
         <v>159</v>
@@ -26225,7 +26225,7 @@
     </row>
     <row r="252" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B252" s="17">
         <v>2023</v>
@@ -26243,7 +26243,7 @@
         <v>240</v>
       </c>
       <c r="G252" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H252" s="17">
         <f t="shared" si="30"/>
@@ -26272,7 +26272,7 @@
         <v>673</v>
       </c>
       <c r="P252" s="13" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q252" s="9" t="s">
         <v>475</v>
@@ -26287,7 +26287,7 @@
     </row>
     <row r="253" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A253" s="13" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B253" s="17">
         <v>2023</v>
@@ -26305,7 +26305,7 @@
         <v>51</v>
       </c>
       <c r="G253" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H253" s="17">
         <f t="shared" si="30"/>
@@ -26322,7 +26322,7 @@
         <v>159</v>
       </c>
       <c r="L253" s="9" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="M253" s="14">
         <v>2</v>
@@ -26334,7 +26334,7 @@
         <v>673</v>
       </c>
       <c r="P253" s="13" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="Q253" s="9" t="s">
         <v>575</v>
@@ -26349,7 +26349,7 @@
     </row>
     <row r="254" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A254" s="13" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B254" s="17">
         <v>2023</v>
@@ -26367,7 +26367,7 @@
         <v>184</v>
       </c>
       <c r="G254" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H254" s="17">
         <f t="shared" si="30"/>
@@ -26384,7 +26384,7 @@
         <v>159</v>
       </c>
       <c r="L254" s="9" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="M254" s="14">
         <v>2</v>
@@ -26396,10 +26396,10 @@
         <v>673</v>
       </c>
       <c r="P254" s="16" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="Q254" s="9" t="s">
-        <v>887</v>
+        <v>916</v>
       </c>
       <c r="R254" s="9" t="s">
         <v>159</v>
@@ -26411,7 +26411,7 @@
     </row>
     <row r="255" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A255" s="13" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B255" s="17">
         <v>2023</v>
@@ -26429,7 +26429,7 @@
         <v>203</v>
       </c>
       <c r="G255" s="9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H255" s="17">
         <f t="shared" si="30"/>
@@ -26446,7 +26446,7 @@
         <v>159</v>
       </c>
       <c r="L255" s="9" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="M255" s="14">
         <v>2</v>
@@ -26458,7 +26458,7 @@
         <v>673</v>
       </c>
       <c r="P255" s="9" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q255" s="9" t="s">
         <v>475</v>
@@ -26473,7 +26473,7 @@
     </row>
     <row r="256" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A256" s="13" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B256" s="17">
         <v>2021</v>
@@ -26491,7 +26491,7 @@
         <v>338</v>
       </c>
       <c r="G256" s="9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H256" s="17">
         <f t="shared" si="30"/>
@@ -26520,7 +26520,7 @@
         <v>673</v>
       </c>
       <c r="P256" s="13" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Q256" s="9" t="s">
         <v>575</v>

</xml_diff>

<commit_message>
#4 Reading List.xlsx: added KBSize field.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4277" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4278" uniqueCount="909">
   <si>
     <t>Format</t>
   </si>
@@ -2765,6 +2765,9 @@
   </si>
   <si>
     <t>Red Gate Books</t>
+  </si>
+  <si>
+    <t>KBSize</t>
   </si>
 </sst>
 </file>
@@ -10608,11 +10611,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:S263"/>
+  <dimension ref="A1:T263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -10638,7 +10641,7 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -10696,8 +10699,11 @@
       <c r="S1" s="6" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" s="6" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -10758,8 +10764,11 @@
         <f t="shared" ref="S2:S30" si="2">LEN(P2)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" s="14">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -10820,8 +10829,11 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3" s="14">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -10882,8 +10894,11 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4" s="14">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>604</v>
       </c>
@@ -10944,8 +10959,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5" s="14"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>13</v>
       </c>
@@ -11006,8 +11022,9 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6" s="14"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
@@ -11068,8 +11085,9 @@
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7" s="14"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -11130,8 +11148,9 @@
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" s="14"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
@@ -11192,8 +11211,9 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9" s="14"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -11254,8 +11274,9 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" s="14"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>22</v>
       </c>
@@ -11316,8 +11337,9 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11" s="14"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
@@ -11378,8 +11400,9 @@
         <f t="shared" si="2"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12" s="14"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>62</v>
       </c>
@@ -11440,8 +11463,9 @@
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13" s="14"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>63</v>
       </c>
@@ -11502,8 +11526,9 @@
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14" s="14"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>70</v>
       </c>
@@ -11564,8 +11589,9 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" s="14"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>73</v>
       </c>
@@ -11626,8 +11652,9 @@
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>75</v>
       </c>
@@ -11688,8 +11715,9 @@
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17" s="14"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>83</v>
       </c>
@@ -11750,8 +11778,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>84</v>
       </c>
@@ -11812,8 +11841,9 @@
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19" s="14"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>91</v>
       </c>
@@ -11874,8 +11904,9 @@
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T20" s="14"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>99</v>
       </c>
@@ -11936,8 +11967,9 @@
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T21" s="14"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>102</v>
       </c>
@@ -11998,8 +12030,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T22" s="14"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>103</v>
       </c>
@@ -12060,8 +12093,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T23" s="14"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>105</v>
       </c>
@@ -12122,8 +12156,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T24" s="14"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>107</v>
       </c>
@@ -12184,8 +12219,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T25" s="14"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>109</v>
       </c>
@@ -12246,8 +12282,9 @@
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T26" s="14"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>111</v>
       </c>
@@ -12308,8 +12345,9 @@
         <f t="shared" si="2"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T27" s="14"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>117</v>
       </c>
@@ -12370,8 +12408,9 @@
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T28" s="14"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>119</v>
       </c>
@@ -12432,8 +12471,9 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T29" s="14"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>121</v>
       </c>
@@ -12494,8 +12534,9 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T30" s="14"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>123</v>
       </c>
@@ -12556,8 +12597,9 @@
         <f t="shared" ref="S31:S80" si="5">LEN(P31)</f>
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T31" s="14"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>125</v>
       </c>
@@ -12618,8 +12660,9 @@
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T32" s="14"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>127</v>
       </c>
@@ -12680,8 +12723,9 @@
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T33" s="14"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>128</v>
       </c>
@@ -12742,8 +12786,9 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T34" s="14"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>130</v>
       </c>
@@ -12804,8 +12849,9 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T35" s="14"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
         <v>132</v>
       </c>
@@ -12866,8 +12912,9 @@
         <f t="shared" si="5"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T36" s="14"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>133</v>
       </c>
@@ -12928,8 +12975,9 @@
         <f t="shared" si="5"/>
         <v>121</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T37" s="14"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>135</v>
       </c>
@@ -12990,8 +13038,9 @@
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T38" s="14"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>139</v>
       </c>
@@ -13052,8 +13101,9 @@
         <f t="shared" si="5"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T39" s="14"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>141</v>
       </c>
@@ -13114,8 +13164,9 @@
         <f t="shared" si="5"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T40" s="14"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>142</v>
       </c>
@@ -13176,8 +13227,9 @@
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T41" s="14"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>143</v>
       </c>
@@ -13238,8 +13290,9 @@
         <f t="shared" si="5"/>
         <v>116</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T42" s="14"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>145</v>
       </c>
@@ -13300,8 +13353,9 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T43" s="14"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>146</v>
       </c>
@@ -13362,8 +13416,9 @@
         <f t="shared" si="5"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T44" s="14"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>151</v>
       </c>
@@ -13424,8 +13479,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T45" s="14"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>153</v>
       </c>
@@ -13486,8 +13542,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T46" s="14"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>154</v>
       </c>
@@ -13548,8 +13605,9 @@
         <f t="shared" si="5"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T47" s="14"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>155</v>
       </c>
@@ -13610,8 +13668,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T48" s="14"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>156</v>
       </c>
@@ -13672,8 +13731,9 @@
         <f t="shared" si="5"/>
         <v>174</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T49" s="14"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>160</v>
       </c>
@@ -13734,8 +13794,9 @@
         <f t="shared" si="5"/>
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T50" s="14"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
         <v>380</v>
       </c>
@@ -13796,8 +13857,9 @@
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T51" s="14"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
         <v>161</v>
       </c>
@@ -13858,8 +13920,9 @@
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T52" s="14"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>163</v>
       </c>
@@ -13920,8 +13983,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T53" s="14"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>164</v>
       </c>
@@ -13982,8 +14046,9 @@
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T54" s="14"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>166</v>
       </c>
@@ -14044,8 +14109,9 @@
         <f t="shared" si="5"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T55" s="14"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>167</v>
       </c>
@@ -14106,8 +14172,9 @@
         <f t="shared" si="5"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T56" s="14"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
         <v>168</v>
       </c>
@@ -14168,8 +14235,9 @@
         <f t="shared" si="5"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T57" s="14"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
         <v>382</v>
       </c>
@@ -14230,8 +14298,9 @@
         <f t="shared" si="5"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T58" s="14"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
         <v>175</v>
       </c>
@@ -14292,8 +14361,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T59" s="14"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>183</v>
       </c>
@@ -14354,8 +14424,9 @@
         <f t="shared" si="5"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T60" s="14"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>185</v>
       </c>
@@ -14416,8 +14487,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T61" s="14"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
         <v>187</v>
       </c>
@@ -14478,8 +14550,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T62" s="14"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>188</v>
       </c>
@@ -14540,8 +14613,9 @@
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T63" s="14"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
         <v>190</v>
       </c>
@@ -14602,8 +14676,9 @@
         <f t="shared" si="5"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T64" s="14"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
         <v>191</v>
       </c>
@@ -14664,8 +14739,9 @@
         <f t="shared" si="5"/>
         <v>134</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T65" s="14"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
         <v>193</v>
       </c>
@@ -14726,8 +14802,9 @@
         <f t="shared" si="5"/>
         <v>143</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T66" s="14"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
         <v>195</v>
       </c>
@@ -14788,8 +14865,9 @@
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T67" s="14"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
         <v>196</v>
       </c>
@@ -14850,8 +14928,9 @@
         <f t="shared" si="5"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T68" s="14"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
         <v>197</v>
       </c>
@@ -14912,8 +14991,9 @@
         <f t="shared" si="5"/>
         <v>115</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T69" s="14"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
         <v>199</v>
       </c>
@@ -14974,8 +15054,9 @@
         <f t="shared" si="5"/>
         <v>123</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T70" s="14"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
         <v>200</v>
       </c>
@@ -15036,8 +15117,9 @@
         <f t="shared" si="5"/>
         <v>129</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T71" s="14"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
         <v>202</v>
       </c>
@@ -15098,8 +15180,9 @@
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T72" s="14"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
         <v>204</v>
       </c>
@@ -15160,8 +15243,9 @@
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T73" s="14"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
         <v>207</v>
       </c>
@@ -15222,8 +15306,9 @@
         <f t="shared" si="5"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T74" s="14"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
         <v>233</v>
       </c>
@@ -15284,8 +15369,9 @@
         <f t="shared" si="5"/>
         <v>282</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T75" s="14"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
         <v>232</v>
       </c>
@@ -15346,8 +15432,9 @@
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T76" s="14"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
         <v>209</v>
       </c>
@@ -15408,8 +15495,9 @@
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T77" s="14"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
         <v>210</v>
       </c>
@@ -15470,8 +15558,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T78" s="14"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
         <v>212</v>
       </c>
@@ -15532,8 +15621,9 @@
         <f t="shared" si="5"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T79" s="14"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
         <v>218</v>
       </c>
@@ -15594,8 +15684,9 @@
         <f t="shared" si="5"/>
         <v>67</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T80" s="14"/>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
         <v>224</v>
       </c>
@@ -15656,8 +15747,9 @@
         <f t="shared" ref="S81:S127" si="8">LEN(P81)</f>
         <v>133</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T81" s="14"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
         <v>226</v>
       </c>
@@ -15718,8 +15810,9 @@
         <f t="shared" si="8"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T82" s="14"/>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
         <v>227</v>
       </c>
@@ -15780,8 +15873,9 @@
         <f t="shared" si="8"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T83" s="14"/>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
         <v>228</v>
       </c>
@@ -15842,8 +15936,9 @@
         <f t="shared" si="8"/>
         <v>154</v>
       </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T84" s="14"/>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
         <v>841</v>
       </c>
@@ -15904,8 +15999,9 @@
         <f t="shared" si="8"/>
         <v>138</v>
       </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T85" s="14"/>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>231</v>
       </c>
@@ -15966,8 +16062,9 @@
         <f t="shared" si="8"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T86" s="14"/>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
         <v>230</v>
       </c>
@@ -16028,8 +16125,9 @@
         <f t="shared" si="8"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T87" s="14"/>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
         <v>238</v>
       </c>
@@ -16090,8 +16188,9 @@
         <f t="shared" si="8"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T88" s="14"/>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
         <v>239</v>
       </c>
@@ -16152,8 +16251,9 @@
         <f t="shared" si="8"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T89" s="14"/>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
         <v>241</v>
       </c>
@@ -16214,8 +16314,9 @@
         <f t="shared" si="8"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T90" s="14"/>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
         <v>243</v>
       </c>
@@ -16276,8 +16377,9 @@
         <f t="shared" si="8"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T91" s="14"/>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
         <v>245</v>
       </c>
@@ -16338,8 +16440,9 @@
         <f t="shared" si="8"/>
         <v>227</v>
       </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T92" s="14"/>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
         <v>247</v>
       </c>
@@ -16400,8 +16503,9 @@
         <f t="shared" si="8"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T93" s="14"/>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
         <v>248</v>
       </c>
@@ -16462,8 +16566,9 @@
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T94" s="14"/>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
         <v>250</v>
       </c>
@@ -16524,8 +16629,9 @@
         <f t="shared" si="8"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T95" s="14"/>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
         <v>252</v>
       </c>
@@ -16586,8 +16692,9 @@
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T96" s="14"/>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" s="13" t="s">
         <v>254</v>
       </c>
@@ -16648,8 +16755,9 @@
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T97" s="14"/>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
         <v>256</v>
       </c>
@@ -16710,8 +16818,9 @@
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T98" s="14"/>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
         <v>257</v>
       </c>
@@ -16772,8 +16881,9 @@
         <f t="shared" si="8"/>
         <v>126</v>
       </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T99" s="14"/>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="s">
         <v>262</v>
       </c>
@@ -16834,8 +16944,9 @@
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T100" s="14"/>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
         <v>264</v>
       </c>
@@ -16896,8 +17007,9 @@
         <f t="shared" si="8"/>
         <v>168</v>
       </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T101" s="14"/>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
         <v>266</v>
       </c>
@@ -16958,8 +17070,9 @@
         <f t="shared" si="8"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T102" s="14"/>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
         <v>268</v>
       </c>
@@ -17020,8 +17133,9 @@
         <f t="shared" si="8"/>
         <v>205</v>
       </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T103" s="14"/>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
         <v>270</v>
       </c>
@@ -17082,8 +17196,9 @@
         <f t="shared" si="8"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T104" s="14"/>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105" s="13" t="s">
         <v>274</v>
       </c>
@@ -17144,8 +17259,9 @@
         <f t="shared" si="8"/>
         <v>137</v>
       </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T105" s="14"/>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="s">
         <v>272</v>
       </c>
@@ -17206,8 +17322,9 @@
         <f t="shared" si="8"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T106" s="14"/>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
         <v>273</v>
       </c>
@@ -17268,8 +17385,9 @@
         <f t="shared" si="8"/>
         <v>175</v>
       </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T107" s="14"/>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108" s="13" t="s">
         <v>304</v>
       </c>
@@ -17330,8 +17448,9 @@
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T108" s="14"/>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109" s="13" t="s">
         <v>305</v>
       </c>
@@ -17392,8 +17511,9 @@
         <f t="shared" si="8"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T109" s="14"/>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
         <v>308</v>
       </c>
@@ -17454,8 +17574,9 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T110" s="14"/>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
         <v>311</v>
       </c>
@@ -17516,8 +17637,9 @@
         <f t="shared" si="8"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T111" s="14"/>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
         <v>313</v>
       </c>
@@ -17578,8 +17700,9 @@
         <f t="shared" si="8"/>
         <v>115</v>
       </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T112" s="14"/>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>842</v>
       </c>
@@ -17640,8 +17763,9 @@
         <f t="shared" si="8"/>
         <v>126</v>
       </c>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T113" s="14"/>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
         <v>316</v>
       </c>
@@ -17702,8 +17826,9 @@
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T114" s="14"/>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115" s="13" t="s">
         <v>317</v>
       </c>
@@ -17764,8 +17889,9 @@
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T115" s="14"/>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
         <v>320</v>
       </c>
@@ -17826,8 +17952,9 @@
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T116" s="14"/>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117" s="13" t="s">
         <v>321</v>
       </c>
@@ -17888,8 +18015,9 @@
         <f t="shared" si="8"/>
         <v>146</v>
       </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T117" s="14"/>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
         <v>204</v>
       </c>
@@ -17950,8 +18078,9 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T118" s="14"/>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
         <v>322</v>
       </c>
@@ -18012,8 +18141,9 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T119" s="14"/>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
         <v>324</v>
       </c>
@@ -18074,8 +18204,9 @@
         <f t="shared" si="8"/>
         <v>152</v>
       </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T120" s="14"/>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
         <v>423</v>
       </c>
@@ -18135,8 +18266,9 @@
         <f t="shared" si="8"/>
         <v>163</v>
       </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T121" s="14"/>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122" s="13" t="s">
         <v>343</v>
       </c>
@@ -18197,8 +18329,9 @@
         <f t="shared" si="8"/>
         <v>163</v>
       </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T122" s="14"/>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
         <v>345</v>
       </c>
@@ -18259,8 +18392,9 @@
         <f t="shared" si="8"/>
         <v>119</v>
       </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T123" s="14"/>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124" s="13" t="s">
         <v>843</v>
       </c>
@@ -18321,8 +18455,9 @@
         <f t="shared" si="8"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T124" s="14"/>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
         <v>348</v>
       </c>
@@ -18383,8 +18518,9 @@
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T125" s="14"/>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126" s="13" t="s">
         <v>350</v>
       </c>
@@ -18445,8 +18581,9 @@
         <f t="shared" si="8"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T126" s="14"/>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="13" t="s">
         <v>351</v>
       </c>
@@ -18507,8 +18644,9 @@
         <f t="shared" si="8"/>
         <v>242</v>
       </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T127" s="14"/>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128" s="13" t="s">
         <v>339</v>
       </c>
@@ -18569,8 +18707,9 @@
         <f t="shared" ref="S128:S190" si="11">LEN(P128)</f>
         <v>159</v>
       </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T128" s="14"/>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129" s="13" t="s">
         <v>338</v>
       </c>
@@ -18631,8 +18770,9 @@
         <f t="shared" si="11"/>
         <v>183</v>
       </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T129" s="14"/>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130" s="13" t="s">
         <v>341</v>
       </c>
@@ -18693,8 +18833,9 @@
         <f t="shared" si="11"/>
         <v>266</v>
       </c>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T130" s="14"/>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131" s="13" t="s">
         <v>395</v>
       </c>
@@ -18755,8 +18896,9 @@
         <f t="shared" si="11"/>
         <v>382</v>
       </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T131" s="14"/>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132" s="13" t="s">
         <v>340</v>
       </c>
@@ -18817,8 +18959,9 @@
         <f t="shared" si="11"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T132" s="14"/>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133" s="13" t="s">
         <v>342</v>
       </c>
@@ -18879,8 +19022,9 @@
         <f t="shared" si="11"/>
         <v>338</v>
       </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T133" s="14"/>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134" s="13" t="s">
         <v>358</v>
       </c>
@@ -18941,8 +19085,9 @@
         <f t="shared" si="11"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T134" s="14"/>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135" s="13" t="s">
         <v>331</v>
       </c>
@@ -19003,8 +19148,9 @@
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T135" s="14"/>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136" s="13" t="s">
         <v>334</v>
       </c>
@@ -19065,8 +19211,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T136" s="14"/>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137" s="13" t="s">
         <v>335</v>
       </c>
@@ -19127,8 +19274,9 @@
         <f t="shared" si="11"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T137" s="14"/>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
         <v>336</v>
       </c>
@@ -19189,8 +19337,9 @@
         <f t="shared" si="11"/>
         <v>311</v>
       </c>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T138" s="14"/>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
         <v>332</v>
       </c>
@@ -19251,8 +19400,9 @@
         <f t="shared" si="11"/>
         <v>143</v>
       </c>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T139" s="14"/>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140" s="13" t="s">
         <v>337</v>
       </c>
@@ -19313,8 +19463,9 @@
         <f t="shared" si="11"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T140" s="14"/>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141" s="13" t="s">
         <v>333</v>
       </c>
@@ -19375,8 +19526,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T141" s="14"/>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
         <v>399</v>
       </c>
@@ -19437,8 +19589,9 @@
         <f t="shared" si="11"/>
         <v>385</v>
       </c>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T142" s="14"/>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
         <v>401</v>
       </c>
@@ -19499,8 +19652,9 @@
         <f t="shared" si="11"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T143" s="14"/>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
         <v>402</v>
       </c>
@@ -19561,8 +19715,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T144" s="14"/>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
         <v>404</v>
       </c>
@@ -19623,8 +19778,9 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-    </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T145" s="14"/>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
         <v>406</v>
       </c>
@@ -19685,8 +19841,9 @@
         <f t="shared" si="11"/>
         <v>149</v>
       </c>
-    </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T146" s="14"/>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>407</v>
       </c>
@@ -19747,8 +19904,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T147" s="14"/>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
         <v>409</v>
       </c>
@@ -19809,8 +19967,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T148" s="14"/>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
         <v>411</v>
       </c>
@@ -19871,8 +20030,9 @@
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T149" s="14"/>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
         <v>413</v>
       </c>
@@ -19933,8 +20093,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T150" s="14"/>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
         <v>415</v>
       </c>
@@ -19995,8 +20156,9 @@
         <f t="shared" si="11"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T151" s="14"/>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
         <v>416</v>
       </c>
@@ -20057,8 +20219,9 @@
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T152" s="14"/>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
         <v>418</v>
       </c>
@@ -20119,8 +20282,9 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T153" s="14"/>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
         <v>419</v>
       </c>
@@ -20181,8 +20345,9 @@
         <f t="shared" si="11"/>
         <v>164</v>
       </c>
-    </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T154" s="14"/>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
         <v>421</v>
       </c>
@@ -20243,8 +20408,9 @@
         <f t="shared" si="11"/>
         <v>207</v>
       </c>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T155" s="14"/>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
         <v>425</v>
       </c>
@@ -20305,8 +20471,9 @@
         <f t="shared" si="11"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T156" s="14"/>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
         <v>426</v>
       </c>
@@ -20367,8 +20534,9 @@
         <f t="shared" si="11"/>
         <v>221</v>
       </c>
-    </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T157" s="14"/>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A158" s="13" t="s">
         <v>427</v>
       </c>
@@ -20429,8 +20597,9 @@
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T158" s="14"/>
+    </row>
+    <row r="159" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A159" s="13" t="s">
         <v>428</v>
       </c>
@@ -20491,8 +20660,9 @@
         <f t="shared" si="11"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T159" s="14"/>
+    </row>
+    <row r="160" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A160" s="13" t="s">
         <v>429</v>
       </c>
@@ -20553,8 +20723,9 @@
         <f t="shared" si="11"/>
         <v>195</v>
       </c>
-    </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T160" s="14"/>
+    </row>
+    <row r="161" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A161" s="13" t="s">
         <v>430</v>
       </c>
@@ -20615,8 +20786,9 @@
         <f t="shared" si="11"/>
         <v>122</v>
       </c>
-    </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T161" s="14"/>
+    </row>
+    <row r="162" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A162" s="13" t="s">
         <v>431</v>
       </c>
@@ -20677,8 +20849,9 @@
         <f t="shared" si="11"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T162" s="14"/>
+    </row>
+    <row r="163" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A163" s="13" t="s">
         <v>432</v>
       </c>
@@ -20739,8 +20912,9 @@
         <f t="shared" si="11"/>
         <v>201</v>
       </c>
-    </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T163" s="14"/>
+    </row>
+    <row r="164" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A164" s="13" t="s">
         <v>433</v>
       </c>
@@ -20801,8 +20975,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T164" s="14"/>
+    </row>
+    <row r="165" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A165" s="13" t="s">
         <v>434</v>
       </c>
@@ -20863,8 +21038,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T165" s="14"/>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="13" t="s">
         <v>435</v>
       </c>
@@ -20925,8 +21101,9 @@
         <f t="shared" si="11"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T166" s="14"/>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A167" s="13" t="s">
         <v>436</v>
       </c>
@@ -20987,8 +21164,9 @@
         <f t="shared" si="11"/>
         <v>137</v>
       </c>
-    </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T167" s="14"/>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A168" s="13" t="s">
         <v>437</v>
       </c>
@@ -21049,8 +21227,9 @@
         <f t="shared" si="11"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T168" s="14"/>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A169" s="13" t="s">
         <v>438</v>
       </c>
@@ -21111,8 +21290,9 @@
         <f t="shared" si="11"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T169" s="14"/>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A170" s="13" t="s">
         <v>439</v>
       </c>
@@ -21173,8 +21353,9 @@
         <f t="shared" si="11"/>
         <v>127</v>
       </c>
-    </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T170" s="14"/>
+    </row>
+    <row r="171" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A171" s="13" t="s">
         <v>440</v>
       </c>
@@ -21235,8 +21416,9 @@
         <f t="shared" si="11"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T171" s="14"/>
+    </row>
+    <row r="172" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A172" s="13" t="s">
         <v>441</v>
       </c>
@@ -21297,8 +21479,9 @@
         <f t="shared" si="11"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T172" s="14"/>
+    </row>
+    <row r="173" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A173" s="13" t="s">
         <v>442</v>
       </c>
@@ -21359,8 +21542,9 @@
         <f t="shared" si="11"/>
         <v>295</v>
       </c>
-    </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T173" s="14"/>
+    </row>
+    <row r="174" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A174" s="13" t="s">
         <v>443</v>
       </c>
@@ -21421,8 +21605,9 @@
         <f t="shared" si="11"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T174" s="14"/>
+    </row>
+    <row r="175" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A175" s="13" t="s">
         <v>444</v>
       </c>
@@ -21483,8 +21668,9 @@
         <f t="shared" si="11"/>
         <v>287</v>
       </c>
-    </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T175" s="14"/>
+    </row>
+    <row r="176" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A176" s="13" t="s">
         <v>460</v>
       </c>
@@ -21545,8 +21731,9 @@
         <f t="shared" si="11"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T176" s="14"/>
+    </row>
+    <row r="177" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A177" s="13" t="s">
         <v>462</v>
       </c>
@@ -21607,8 +21794,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T177" s="14"/>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A178" s="13" t="s">
         <v>462</v>
       </c>
@@ -21669,8 +21857,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T178" s="14"/>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A179" s="13" t="s">
         <v>463</v>
       </c>
@@ -21731,8 +21920,9 @@
         <f t="shared" si="11"/>
         <v>208</v>
       </c>
-    </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T179" s="14"/>
+    </row>
+    <row r="180" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A180" s="13" t="s">
         <v>487</v>
       </c>
@@ -21793,8 +21983,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T180" s="14"/>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A181" s="13" t="s">
         <v>488</v>
       </c>
@@ -21855,8 +22046,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T181" s="14"/>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A182" s="13" t="s">
         <v>489</v>
       </c>
@@ -21917,8 +22109,9 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T182" s="14"/>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A183" s="13" t="s">
         <v>491</v>
       </c>
@@ -21979,8 +22172,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T183" s="14"/>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A184" s="13" t="s">
         <v>492</v>
       </c>
@@ -22041,8 +22235,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T184" s="14"/>
+    </row>
+    <row r="185" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A185" s="13" t="s">
         <v>493</v>
       </c>
@@ -22103,8 +22298,9 @@
         <f t="shared" si="11"/>
         <v>242</v>
       </c>
-    </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T185" s="14"/>
+    </row>
+    <row r="186" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A186" s="16" t="s">
         <v>494</v>
       </c>
@@ -22165,8 +22361,9 @@
         <f t="shared" si="11"/>
         <v>292</v>
       </c>
-    </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T186" s="14"/>
+    </row>
+    <row r="187" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A187" s="16" t="s">
         <v>496</v>
       </c>
@@ -22227,8 +22424,9 @@
         <f t="shared" si="11"/>
         <v>260</v>
       </c>
-    </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T187" s="14"/>
+    </row>
+    <row r="188" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A188" s="13" t="s">
         <v>497</v>
       </c>
@@ -22289,8 +22487,9 @@
         <f t="shared" si="11"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T188" s="14"/>
+    </row>
+    <row r="189" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A189" s="13" t="s">
         <v>500</v>
       </c>
@@ -22351,8 +22550,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T189" s="14"/>
+    </row>
+    <row r="190" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A190" s="13" t="s">
         <v>501</v>
       </c>
@@ -22413,8 +22613,9 @@
         <f t="shared" si="11"/>
         <v>186</v>
       </c>
-    </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T190" s="14"/>
+    </row>
+    <row r="191" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A191" s="13" t="s">
         <v>506</v>
       </c>
@@ -22475,8 +22676,9 @@
         <f t="shared" ref="S191:S231" si="16">LEN(P191)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T191" s="14"/>
+    </row>
+    <row r="192" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A192" s="13" t="s">
         <v>507</v>
       </c>
@@ -22537,8 +22739,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T192" s="14"/>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A193" s="13" t="s">
         <v>510</v>
       </c>
@@ -22599,8 +22802,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T193" s="14"/>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A194" s="13" t="s">
         <v>512</v>
       </c>
@@ -22661,8 +22865,9 @@
         <f t="shared" si="16"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T194" s="14"/>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A195" s="13" t="s">
         <v>515</v>
       </c>
@@ -22723,8 +22928,9 @@
         <f t="shared" si="16"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T195" s="14"/>
+    </row>
+    <row r="196" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A196" s="13" t="s">
         <v>517</v>
       </c>
@@ -22785,8 +22991,9 @@
         <f t="shared" si="16"/>
         <v>155</v>
       </c>
-    </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T196" s="14"/>
+    </row>
+    <row r="197" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A197" s="13" t="s">
         <v>520</v>
       </c>
@@ -22847,8 +23054,9 @@
         <f t="shared" si="16"/>
         <v>297</v>
       </c>
-    </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T197" s="14"/>
+    </row>
+    <row r="198" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A198" s="13" t="s">
         <v>554</v>
       </c>
@@ -22909,8 +23117,9 @@
         <f t="shared" si="16"/>
         <v>254</v>
       </c>
-    </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T198" s="14"/>
+    </row>
+    <row r="199" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A199" s="13" t="s">
         <v>556</v>
       </c>
@@ -22971,8 +23180,9 @@
         <f t="shared" si="16"/>
         <v>280</v>
       </c>
-    </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T199" s="14"/>
+    </row>
+    <row r="200" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A200" s="13" t="s">
         <v>558</v>
       </c>
@@ -23033,8 +23243,9 @@
         <f t="shared" si="16"/>
         <v>232</v>
       </c>
-    </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T200" s="14"/>
+    </row>
+    <row r="201" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A201" s="13" t="s">
         <v>561</v>
       </c>
@@ -23095,8 +23306,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T201" s="14"/>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A202" s="13" t="s">
         <v>562</v>
       </c>
@@ -23157,8 +23369,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T202" s="14"/>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A203" s="13" t="s">
         <v>564</v>
       </c>
@@ -23219,8 +23432,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T203" s="14"/>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A204" s="13" t="s">
         <v>565</v>
       </c>
@@ -23281,8 +23495,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T204" s="14"/>
+    </row>
+    <row r="205" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A205" s="13" t="s">
         <v>566</v>
       </c>
@@ -23343,8 +23558,9 @@
         <f t="shared" si="16"/>
         <v>215</v>
       </c>
-    </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T205" s="14"/>
+    </row>
+    <row r="206" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A206" s="13" t="s">
         <v>569</v>
       </c>
@@ -23405,8 +23621,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T206" s="14"/>
+    </row>
+    <row r="207" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A207" s="13" t="s">
         <v>574</v>
       </c>
@@ -23467,8 +23684,9 @@
         <f t="shared" si="16"/>
         <v>254</v>
       </c>
-    </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T207" s="14"/>
+    </row>
+    <row r="208" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A208" s="13" t="s">
         <v>507</v>
       </c>
@@ -23529,8 +23747,9 @@
         <f t="shared" si="16"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T208" s="14"/>
+    </row>
+    <row r="209" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A209" s="13" t="s">
         <v>577</v>
       </c>
@@ -23591,8 +23810,9 @@
         <f t="shared" si="16"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T209" s="14"/>
+    </row>
+    <row r="210" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A210" s="13" t="s">
         <v>578</v>
       </c>
@@ -23653,8 +23873,9 @@
         <f t="shared" si="16"/>
         <v>352</v>
       </c>
-    </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T210" s="14"/>
+    </row>
+    <row r="211" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A211" s="13" t="s">
         <v>579</v>
       </c>
@@ -23715,8 +23936,9 @@
         <f t="shared" si="16"/>
         <v>277</v>
       </c>
-    </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T211" s="14"/>
+    </row>
+    <row r="212" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A212" s="13" t="s">
         <v>580</v>
       </c>
@@ -23777,8 +23999,9 @@
         <f t="shared" si="16"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T212" s="14"/>
+    </row>
+    <row r="213" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A213" s="13" t="s">
         <v>581</v>
       </c>
@@ -23839,8 +24062,9 @@
         <f t="shared" si="16"/>
         <v>149</v>
       </c>
-    </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T213" s="14"/>
+    </row>
+    <row r="214" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A214" s="13" t="s">
         <v>582</v>
       </c>
@@ -23901,8 +24125,9 @@
         <f t="shared" si="16"/>
         <v>195</v>
       </c>
-    </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T214" s="14"/>
+    </row>
+    <row r="215" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A215" s="13" t="s">
         <v>583</v>
       </c>
@@ -23963,8 +24188,9 @@
         <f t="shared" si="16"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T215" s="14"/>
+    </row>
+    <row r="216" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A216" s="13" t="s">
         <v>584</v>
       </c>
@@ -24025,8 +24251,9 @@
         <f t="shared" si="16"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T216" s="14"/>
+    </row>
+    <row r="217" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A217" s="13" t="s">
         <v>585</v>
       </c>
@@ -24087,8 +24314,9 @@
         <f t="shared" si="16"/>
         <v>174</v>
       </c>
-    </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T217" s="14"/>
+    </row>
+    <row r="218" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A218" s="13" t="s">
         <v>586</v>
       </c>
@@ -24149,8 +24377,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T218" s="14"/>
+    </row>
+    <row r="219" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A219" s="13" t="s">
         <v>587</v>
       </c>
@@ -24211,8 +24440,9 @@
         <f t="shared" si="16"/>
         <v>564</v>
       </c>
-    </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T219" s="14"/>
+    </row>
+    <row r="220" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A220" s="13" t="s">
         <v>588</v>
       </c>
@@ -24273,8 +24503,9 @@
         <f t="shared" si="16"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="221" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T220" s="14"/>
+    </row>
+    <row r="221" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A221" s="13" t="s">
         <v>610</v>
       </c>
@@ -24335,8 +24566,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T221" s="14"/>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A222" s="13" t="s">
         <v>612</v>
       </c>
@@ -24397,8 +24629,9 @@
         <f t="shared" si="16"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="223" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T222" s="14"/>
+    </row>
+    <row r="223" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A223" s="13" t="s">
         <v>613</v>
       </c>
@@ -24459,8 +24692,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T223" s="14"/>
+    </row>
+    <row r="224" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A224" s="13" t="s">
         <v>615</v>
       </c>
@@ -24521,8 +24755,9 @@
         <f t="shared" si="16"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T224" s="14"/>
+    </row>
+    <row r="225" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A225" s="13" t="s">
         <v>616</v>
       </c>
@@ -24583,8 +24818,9 @@
         <f t="shared" si="16"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T225" s="14"/>
+    </row>
+    <row r="226" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A226" s="13" t="s">
         <v>618</v>
       </c>
@@ -24645,8 +24881,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T226" s="14"/>
+    </row>
+    <row r="227" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A227" s="13" t="s">
         <v>619</v>
       </c>
@@ -24707,8 +24944,9 @@
         <f t="shared" si="16"/>
         <v>119</v>
       </c>
-    </row>
-    <row r="228" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T227" s="14"/>
+    </row>
+    <row r="228" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A228" s="13" t="s">
         <v>621</v>
       </c>
@@ -24769,8 +25007,9 @@
         <f t="shared" si="16"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="229" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T228" s="14"/>
+    </row>
+    <row r="229" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A229" s="13" t="s">
         <v>622</v>
       </c>
@@ -24831,8 +25070,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T229" s="14"/>
+    </row>
+    <row r="230" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A230" s="13" t="s">
         <v>624</v>
       </c>
@@ -24893,8 +25133,9 @@
         <f t="shared" si="16"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="231" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T230" s="14"/>
+    </row>
+    <row r="231" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A231" s="13" t="s">
         <v>625</v>
       </c>
@@ -24955,8 +25196,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T231" s="14"/>
+    </row>
+    <row r="232" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A232" s="13" t="s">
         <v>650</v>
       </c>
@@ -25017,8 +25259,9 @@
         <f t="shared" ref="S232:S256" si="32">LEN(P232)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="233" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T232" s="14"/>
+    </row>
+    <row r="233" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A233" s="13" t="s">
         <v>652</v>
       </c>
@@ -25079,8 +25322,9 @@
         <f t="shared" si="32"/>
         <v>417</v>
       </c>
-    </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T233" s="14"/>
+    </row>
+    <row r="234" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A234" s="13" t="s">
         <v>273</v>
       </c>
@@ -25141,8 +25385,9 @@
         <f t="shared" si="32"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="235" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T234" s="14"/>
+    </row>
+    <row r="235" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A235" s="13" t="s">
         <v>654</v>
       </c>
@@ -25203,8 +25448,9 @@
         <f t="shared" si="32"/>
         <v>136</v>
       </c>
-    </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T235" s="14"/>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A236" s="13" t="s">
         <v>859</v>
       </c>
@@ -25265,8 +25511,9 @@
         <f t="shared" si="32"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="237" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T236" s="14"/>
+    </row>
+    <row r="237" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A237" s="13" t="s">
         <v>844</v>
       </c>
@@ -25327,8 +25574,9 @@
         <f t="shared" si="32"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="238" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T237" s="14"/>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A238" s="13" t="s">
         <v>847</v>
       </c>
@@ -25389,8 +25637,9 @@
         <f t="shared" si="32"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="239" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T238" s="14"/>
+    </row>
+    <row r="239" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A239" s="13" t="s">
         <v>850</v>
       </c>
@@ -25451,8 +25700,9 @@
         <f t="shared" si="32"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="240" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T239" s="14"/>
+    </row>
+    <row r="240" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A240" s="13" t="s">
         <v>851</v>
       </c>
@@ -25513,8 +25763,9 @@
         <f t="shared" si="32"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="241" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T240" s="14"/>
+    </row>
+    <row r="241" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A241" s="13" t="s">
         <v>852</v>
       </c>
@@ -25575,8 +25826,9 @@
         <f t="shared" si="32"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T241" s="14"/>
+    </row>
+    <row r="242" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A242" s="13" t="s">
         <v>854</v>
       </c>
@@ -25637,8 +25889,9 @@
         <f t="shared" si="32"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T242" s="14"/>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A243" s="13" t="s">
         <v>856</v>
       </c>
@@ -25699,8 +25952,9 @@
         <f t="shared" si="32"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T243" s="14"/>
+    </row>
+    <row r="244" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A244" s="13" t="s">
         <v>863</v>
       </c>
@@ -25761,8 +26015,9 @@
         <f t="shared" si="32"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T244" s="14"/>
+    </row>
+    <row r="245" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A245" s="13" t="s">
         <v>866</v>
       </c>
@@ -25823,8 +26078,9 @@
         <f t="shared" si="32"/>
         <v>325</v>
       </c>
-    </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T245" s="14"/>
+    </row>
+    <row r="246" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A246" s="13" t="s">
         <v>868</v>
       </c>
@@ -25885,8 +26141,9 @@
         <f t="shared" si="32"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T246" s="14"/>
+    </row>
+    <row r="247" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A247" s="13" t="s">
         <v>872</v>
       </c>
@@ -25947,8 +26204,9 @@
         <f t="shared" si="32"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T247" s="14"/>
+    </row>
+    <row r="248" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A248" s="13" t="s">
         <v>880</v>
       </c>
@@ -26009,8 +26267,9 @@
         <f t="shared" si="32"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T248" s="14"/>
+    </row>
+    <row r="249" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A249" s="13" t="s">
         <v>884</v>
       </c>
@@ -26071,8 +26330,9 @@
         <f t="shared" si="32"/>
         <v>231</v>
       </c>
-    </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T249" s="14"/>
+    </row>
+    <row r="250" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
         <v>887</v>
       </c>
@@ -26133,8 +26393,9 @@
         <f t="shared" si="32"/>
         <v>185</v>
       </c>
-    </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T250" s="14"/>
+    </row>
+    <row r="251" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
         <v>890</v>
       </c>
@@ -26195,8 +26456,9 @@
         <f t="shared" si="32"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T251" s="14"/>
+    </row>
+    <row r="252" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
         <v>893</v>
       </c>
@@ -26257,8 +26519,9 @@
         <f t="shared" si="32"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T252" s="14"/>
+    </row>
+    <row r="253" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A253" s="13" t="s">
         <v>895</v>
       </c>
@@ -26319,8 +26582,9 @@
         <f t="shared" si="32"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T253" s="14"/>
+    </row>
+    <row r="254" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A254" s="13" t="s">
         <v>899</v>
       </c>
@@ -26381,8 +26645,9 @@
         <f t="shared" si="32"/>
         <v>137</v>
       </c>
-    </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T254" s="14"/>
+    </row>
+    <row r="255" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A255" s="13" t="s">
         <v>901</v>
       </c>
@@ -26443,8 +26708,9 @@
         <f t="shared" si="32"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T255" s="14"/>
+    </row>
+    <row r="256" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A256" s="13" t="s">
         <v>904</v>
       </c>
@@ -26505,8 +26771,9 @@
         <f t="shared" si="32"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T256" s="14"/>
+    </row>
+    <row r="257" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A257" s="9"/>
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
@@ -26526,8 +26793,9 @@
       <c r="Q257" s="9"/>
       <c r="R257" s="9"/>
       <c r="S257" s="17"/>
-    </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T257" s="14"/>
+    </row>
+    <row r="258" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A258" s="9"/>
       <c r="B258" s="9"/>
       <c r="C258" s="9"/>
@@ -26547,8 +26815,9 @@
       <c r="Q258" s="9"/>
       <c r="R258" s="9"/>
       <c r="S258" s="17"/>
-    </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T258" s="14"/>
+    </row>
+    <row r="259" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A259" s="9"/>
       <c r="B259" s="9"/>
       <c r="C259" s="9"/>
@@ -26568,8 +26837,9 @@
       <c r="Q259" s="9"/>
       <c r="R259" s="9"/>
       <c r="S259" s="17"/>
-    </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T259" s="14"/>
+    </row>
+    <row r="260" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A260" s="9"/>
       <c r="B260" s="9"/>
       <c r="C260" s="9"/>
@@ -26589,8 +26859,9 @@
       <c r="Q260" s="9"/>
       <c r="R260" s="9"/>
       <c r="S260" s="17"/>
-    </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T260" s="14"/>
+    </row>
+    <row r="261" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A261" s="9"/>
       <c r="B261" s="9"/>
       <c r="C261" s="9"/>
@@ -26610,8 +26881,9 @@
       <c r="Q261" s="9"/>
       <c r="R261" s="9"/>
       <c r="S261" s="17"/>
-    </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T261" s="14"/>
+    </row>
+    <row r="262" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A262" s="9"/>
       <c r="B262" s="9"/>
       <c r="C262" s="9"/>
@@ -26631,8 +26903,9 @@
       <c r="Q262" s="9"/>
       <c r="R262" s="9"/>
       <c r="S262" s="17"/>
-    </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T262" s="14"/>
+    </row>
+    <row r="263" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A263" s="9"/>
       <c r="B263" s="9"/>
       <c r="C263" s="9"/>
@@ -26652,6 +26925,7 @@
       <c r="Q263" s="9"/>
       <c r="R263" s="9"/>
       <c r="S263" s="17"/>
+      <c r="T263" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#4 get_books_dataset(): added KBSize field.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -10613,9 +10613,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T263"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="T259" sqref="T259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -10959,7 +10959,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="T5" s="14"/>
+      <c r="T5" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -11022,7 +11024,9 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="T6" s="14"/>
+      <c r="T6" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
@@ -11085,7 +11089,9 @@
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="T7" s="14"/>
+      <c r="T7" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
@@ -11148,7 +11154,9 @@
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-      <c r="T8" s="14"/>
+      <c r="T8" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -11211,7 +11219,9 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="T9" s="14"/>
+      <c r="T9" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
@@ -11274,7 +11284,9 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="T10" s="14"/>
+      <c r="T10" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
@@ -11337,7 +11349,9 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="T11" s="14"/>
+      <c r="T11" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
@@ -11400,7 +11414,9 @@
         <f t="shared" si="2"/>
         <v>93</v>
       </c>
-      <c r="T12" s="14"/>
+      <c r="T12" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
@@ -11463,7 +11479,9 @@
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="T13" s="14"/>
+      <c r="T13" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
@@ -11526,7 +11544,9 @@
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
-      <c r="T14" s="14"/>
+      <c r="T14" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -11589,7 +11609,9 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="T15" s="14"/>
+      <c r="T15" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
@@ -11652,7 +11674,9 @@
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="T16" s="14"/>
+      <c r="T16" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
@@ -11715,7 +11739,9 @@
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="T17" s="14"/>
+      <c r="T17" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
@@ -11778,7 +11804,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="T18" s="14"/>
+      <c r="T18" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
@@ -11841,7 +11869,9 @@
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="T19" s="14"/>
+      <c r="T19" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
@@ -11904,7 +11934,9 @@
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="T20" s="14"/>
+      <c r="T20" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
@@ -11967,7 +11999,9 @@
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="T21" s="14"/>
+      <c r="T21" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
@@ -12030,7 +12064,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="T22" s="14"/>
+      <c r="T22" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
@@ -12093,7 +12129,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="T23" s="14"/>
+      <c r="T23" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
@@ -12156,7 +12194,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="T24" s="14"/>
+      <c r="T24" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
@@ -12219,7 +12259,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="T25" s="14"/>
+      <c r="T25" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
@@ -12282,7 +12324,9 @@
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="T26" s="14"/>
+      <c r="T26" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
@@ -12345,7 +12389,9 @@
         <f t="shared" si="2"/>
         <v>133</v>
       </c>
-      <c r="T27" s="14"/>
+      <c r="T27" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
@@ -12408,7 +12454,9 @@
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="T28" s="14"/>
+      <c r="T28" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
@@ -12471,7 +12519,9 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="T29" s="14"/>
+      <c r="T29" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
@@ -12534,7 +12584,9 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="T30" s="14"/>
+      <c r="T30" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
@@ -12597,7 +12649,9 @@
         <f t="shared" ref="S31:S80" si="5">LEN(P31)</f>
         <v>94</v>
       </c>
-      <c r="T31" s="14"/>
+      <c r="T31" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
@@ -12660,7 +12714,9 @@
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="T32" s="14"/>
+      <c r="T32" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
@@ -12723,7 +12779,9 @@
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="T33" s="14"/>
+      <c r="T33" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
@@ -12786,7 +12844,9 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="T34" s="14"/>
+      <c r="T34" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
@@ -12849,7 +12909,9 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="T35" s="14"/>
+      <c r="T35" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
@@ -12912,7 +12974,9 @@
         <f t="shared" si="5"/>
         <v>38</v>
       </c>
-      <c r="T36" s="14"/>
+      <c r="T36" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
@@ -12975,7 +13039,9 @@
         <f t="shared" si="5"/>
         <v>121</v>
       </c>
-      <c r="T37" s="14"/>
+      <c r="T37" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
@@ -13038,7 +13104,9 @@
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="T38" s="14"/>
+      <c r="T38" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
@@ -13101,7 +13169,9 @@
         <f t="shared" si="5"/>
         <v>78</v>
       </c>
-      <c r="T39" s="14"/>
+      <c r="T39" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
@@ -13164,7 +13234,9 @@
         <f t="shared" si="5"/>
         <v>41</v>
       </c>
-      <c r="T40" s="14"/>
+      <c r="T40" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
@@ -13227,7 +13299,9 @@
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-      <c r="T41" s="14"/>
+      <c r="T41" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
@@ -13290,7 +13364,9 @@
         <f t="shared" si="5"/>
         <v>116</v>
       </c>
-      <c r="T42" s="14"/>
+      <c r="T42" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
@@ -13353,7 +13429,9 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="T43" s="14"/>
+      <c r="T43" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
@@ -13416,7 +13494,9 @@
         <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="T44" s="14"/>
+      <c r="T44" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
@@ -13479,7 +13559,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T45" s="14"/>
+      <c r="T45" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
@@ -13542,7 +13624,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T46" s="14"/>
+      <c r="T46" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
@@ -13605,7 +13689,9 @@
         <f t="shared" si="5"/>
         <v>38</v>
       </c>
-      <c r="T47" s="14"/>
+      <c r="T47" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
@@ -13668,7 +13754,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T48" s="14"/>
+      <c r="T48" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
@@ -13731,7 +13819,9 @@
         <f t="shared" si="5"/>
         <v>174</v>
       </c>
-      <c r="T49" s="14"/>
+      <c r="T49" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
@@ -13794,7 +13884,9 @@
         <f t="shared" si="5"/>
         <v>67</v>
       </c>
-      <c r="T50" s="14"/>
+      <c r="T50" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
@@ -13857,7 +13949,9 @@
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="T51" s="14"/>
+      <c r="T51" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
@@ -13920,7 +14014,9 @@
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
-      <c r="T52" s="14"/>
+      <c r="T52" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
@@ -13983,7 +14079,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T53" s="14"/>
+      <c r="T53" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
@@ -14046,7 +14144,9 @@
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="T54" s="14"/>
+      <c r="T54" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
@@ -14109,7 +14209,9 @@
         <f t="shared" si="5"/>
         <v>59</v>
       </c>
-      <c r="T55" s="14"/>
+      <c r="T55" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
@@ -14172,7 +14274,9 @@
         <f t="shared" si="5"/>
         <v>63</v>
       </c>
-      <c r="T56" s="14"/>
+      <c r="T56" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
@@ -14235,7 +14339,9 @@
         <f t="shared" si="5"/>
         <v>84</v>
       </c>
-      <c r="T57" s="14"/>
+      <c r="T57" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
@@ -14298,7 +14404,9 @@
         <f t="shared" si="5"/>
         <v>26</v>
       </c>
-      <c r="T58" s="14"/>
+      <c r="T58" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
@@ -14361,7 +14469,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T59" s="14"/>
+      <c r="T59" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
@@ -14424,7 +14534,9 @@
         <f t="shared" si="5"/>
         <v>66</v>
       </c>
-      <c r="T60" s="14"/>
+      <c r="T60" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
@@ -14487,7 +14599,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T61" s="14"/>
+      <c r="T61" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
@@ -14550,7 +14664,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T62" s="14"/>
+      <c r="T62" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
@@ -14613,7 +14729,9 @@
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-      <c r="T63" s="14"/>
+      <c r="T63" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
@@ -14676,7 +14794,9 @@
         <f t="shared" si="5"/>
         <v>99</v>
       </c>
-      <c r="T64" s="14"/>
+      <c r="T64" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
@@ -14739,7 +14859,9 @@
         <f t="shared" si="5"/>
         <v>134</v>
       </c>
-      <c r="T65" s="14"/>
+      <c r="T65" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
@@ -14802,7 +14924,9 @@
         <f t="shared" si="5"/>
         <v>143</v>
       </c>
-      <c r="T66" s="14"/>
+      <c r="T66" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
@@ -14865,7 +14989,9 @@
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="T67" s="14"/>
+      <c r="T67" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
@@ -14928,7 +15054,9 @@
         <f t="shared" si="5"/>
         <v>99</v>
       </c>
-      <c r="T68" s="14"/>
+      <c r="T68" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
@@ -14991,7 +15119,9 @@
         <f t="shared" si="5"/>
         <v>115</v>
       </c>
-      <c r="T69" s="14"/>
+      <c r="T69" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
@@ -15054,7 +15184,9 @@
         <f t="shared" si="5"/>
         <v>123</v>
       </c>
-      <c r="T70" s="14"/>
+      <c r="T70" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
@@ -15117,7 +15249,9 @@
         <f t="shared" si="5"/>
         <v>129</v>
       </c>
-      <c r="T71" s="14"/>
+      <c r="T71" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
@@ -15180,7 +15314,9 @@
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-      <c r="T72" s="14"/>
+      <c r="T72" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
@@ -15243,7 +15379,9 @@
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="T73" s="14"/>
+      <c r="T73" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
@@ -15306,7 +15444,9 @@
         <f t="shared" si="5"/>
         <v>57</v>
       </c>
-      <c r="T74" s="14"/>
+      <c r="T74" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
@@ -15369,7 +15509,9 @@
         <f t="shared" si="5"/>
         <v>282</v>
       </c>
-      <c r="T75" s="14"/>
+      <c r="T75" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
@@ -15432,7 +15574,9 @@
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="T76" s="14"/>
+      <c r="T76" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
@@ -15495,7 +15639,9 @@
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="T77" s="14"/>
+      <c r="T77" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
@@ -15558,7 +15704,9 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T78" s="14"/>
+      <c r="T78" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
@@ -15621,7 +15769,9 @@
         <f t="shared" si="5"/>
         <v>65</v>
       </c>
-      <c r="T79" s="14"/>
+      <c r="T79" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
@@ -15684,7 +15834,9 @@
         <f t="shared" si="5"/>
         <v>67</v>
       </c>
-      <c r="T80" s="14"/>
+      <c r="T80" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
@@ -15747,7 +15899,9 @@
         <f t="shared" ref="S81:S127" si="8">LEN(P81)</f>
         <v>133</v>
       </c>
-      <c r="T81" s="14"/>
+      <c r="T81" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
@@ -15810,7 +15964,9 @@
         <f t="shared" si="8"/>
         <v>63</v>
       </c>
-      <c r="T82" s="14"/>
+      <c r="T82" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
@@ -15873,7 +16029,9 @@
         <f t="shared" si="8"/>
         <v>77</v>
       </c>
-      <c r="T83" s="14"/>
+      <c r="T83" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
@@ -15936,7 +16094,9 @@
         <f t="shared" si="8"/>
         <v>154</v>
       </c>
-      <c r="T84" s="14"/>
+      <c r="T84" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
@@ -15999,7 +16159,9 @@
         <f t="shared" si="8"/>
         <v>138</v>
       </c>
-      <c r="T85" s="14"/>
+      <c r="T85" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
@@ -16062,7 +16224,9 @@
         <f t="shared" si="8"/>
         <v>66</v>
       </c>
-      <c r="T86" s="14"/>
+      <c r="T86" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
@@ -16125,7 +16289,9 @@
         <f t="shared" si="8"/>
         <v>85</v>
       </c>
-      <c r="T87" s="14"/>
+      <c r="T87" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
@@ -16188,7 +16354,9 @@
         <f t="shared" si="8"/>
         <v>61</v>
       </c>
-      <c r="T88" s="14"/>
+      <c r="T88" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
@@ -16251,7 +16419,9 @@
         <f t="shared" si="8"/>
         <v>81</v>
       </c>
-      <c r="T89" s="14"/>
+      <c r="T89" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
@@ -16314,7 +16484,9 @@
         <f t="shared" si="8"/>
         <v>106</v>
       </c>
-      <c r="T90" s="14"/>
+      <c r="T90" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
@@ -16377,7 +16549,9 @@
         <f t="shared" si="8"/>
         <v>108</v>
       </c>
-      <c r="T91" s="14"/>
+      <c r="T91" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
@@ -16440,7 +16614,9 @@
         <f t="shared" si="8"/>
         <v>227</v>
       </c>
-      <c r="T92" s="14"/>
+      <c r="T92" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
@@ -16503,7 +16679,9 @@
         <f t="shared" si="8"/>
         <v>44</v>
       </c>
-      <c r="T93" s="14"/>
+      <c r="T93" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
@@ -16566,7 +16744,9 @@
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="T94" s="14"/>
+      <c r="T94" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
@@ -16629,7 +16809,9 @@
         <f t="shared" si="8"/>
         <v>73</v>
       </c>
-      <c r="T95" s="14"/>
+      <c r="T95" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
@@ -16692,7 +16874,9 @@
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="T96" s="14"/>
+      <c r="T96" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" s="13" t="s">
@@ -16755,7 +16939,9 @@
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="T97" s="14"/>
+      <c r="T97" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
@@ -16818,7 +17004,9 @@
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="T98" s="14"/>
+      <c r="T98" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
@@ -16881,7 +17069,9 @@
         <f t="shared" si="8"/>
         <v>126</v>
       </c>
-      <c r="T99" s="14"/>
+      <c r="T99" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="s">
@@ -16944,7 +17134,9 @@
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="T100" s="14"/>
+      <c r="T100" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
@@ -17007,7 +17199,9 @@
         <f t="shared" si="8"/>
         <v>168</v>
       </c>
-      <c r="T101" s="14"/>
+      <c r="T101" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
@@ -17070,7 +17264,9 @@
         <f t="shared" si="8"/>
         <v>108</v>
       </c>
-      <c r="T102" s="14"/>
+      <c r="T102" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
@@ -17133,7 +17329,9 @@
         <f t="shared" si="8"/>
         <v>205</v>
       </c>
-      <c r="T103" s="14"/>
+      <c r="T103" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
@@ -17196,7 +17394,9 @@
         <f t="shared" si="8"/>
         <v>36</v>
       </c>
-      <c r="T104" s="14"/>
+      <c r="T104" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105" s="13" t="s">
@@ -17259,7 +17459,9 @@
         <f t="shared" si="8"/>
         <v>137</v>
       </c>
-      <c r="T105" s="14"/>
+      <c r="T105" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="s">
@@ -17322,7 +17524,9 @@
         <f t="shared" si="8"/>
         <v>93</v>
       </c>
-      <c r="T106" s="14"/>
+      <c r="T106" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
@@ -17385,7 +17589,9 @@
         <f t="shared" si="8"/>
         <v>175</v>
       </c>
-      <c r="T107" s="14"/>
+      <c r="T107" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108" s="13" t="s">
@@ -17448,7 +17654,9 @@
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="T108" s="14"/>
+      <c r="T108" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109" s="13" t="s">
@@ -17511,7 +17719,9 @@
         <f t="shared" si="8"/>
         <v>46</v>
       </c>
-      <c r="T109" s="14"/>
+      <c r="T109" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
@@ -17574,7 +17784,9 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="T110" s="14"/>
+      <c r="T110" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
@@ -17637,7 +17849,9 @@
         <f t="shared" si="8"/>
         <v>33</v>
       </c>
-      <c r="T111" s="14"/>
+      <c r="T111" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
@@ -17700,7 +17914,9 @@
         <f t="shared" si="8"/>
         <v>115</v>
       </c>
-      <c r="T112" s="14"/>
+      <c r="T112" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
@@ -17763,7 +17979,9 @@
         <f t="shared" si="8"/>
         <v>126</v>
       </c>
-      <c r="T113" s="14"/>
+      <c r="T113" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
@@ -17826,7 +18044,9 @@
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="T114" s="14"/>
+      <c r="T114" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115" s="13" t="s">
@@ -17889,7 +18109,9 @@
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
-      <c r="T115" s="14"/>
+      <c r="T115" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
@@ -17952,7 +18174,9 @@
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="T116" s="14"/>
+      <c r="T116" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117" s="13" t="s">
@@ -18015,7 +18239,9 @@
         <f t="shared" si="8"/>
         <v>146</v>
       </c>
-      <c r="T117" s="14"/>
+      <c r="T117" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
@@ -18078,7 +18304,9 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="T118" s="14"/>
+      <c r="T118" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
@@ -18141,7 +18369,9 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="T119" s="14"/>
+      <c r="T119" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
@@ -18204,7 +18434,9 @@
         <f t="shared" si="8"/>
         <v>152</v>
       </c>
-      <c r="T120" s="14"/>
+      <c r="T120" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
@@ -18266,7 +18498,9 @@
         <f t="shared" si="8"/>
         <v>163</v>
       </c>
-      <c r="T121" s="14"/>
+      <c r="T121" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122" s="13" t="s">
@@ -18329,7 +18563,9 @@
         <f t="shared" si="8"/>
         <v>163</v>
       </c>
-      <c r="T122" s="14"/>
+      <c r="T122" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
@@ -18392,7 +18628,9 @@
         <f t="shared" si="8"/>
         <v>119</v>
       </c>
-      <c r="T123" s="14"/>
+      <c r="T123" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124" s="13" t="s">
@@ -18455,7 +18693,9 @@
         <f t="shared" si="8"/>
         <v>56</v>
       </c>
-      <c r="T124" s="14"/>
+      <c r="T124" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
@@ -18518,7 +18758,9 @@
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="T125" s="14"/>
+      <c r="T125" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126" s="13" t="s">
@@ -18581,7 +18823,9 @@
         <f t="shared" si="8"/>
         <v>51</v>
       </c>
-      <c r="T126" s="14"/>
+      <c r="T126" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="13" t="s">
@@ -18644,7 +18888,9 @@
         <f t="shared" si="8"/>
         <v>242</v>
       </c>
-      <c r="T127" s="14"/>
+      <c r="T127" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128" s="13" t="s">
@@ -18707,7 +18953,9 @@
         <f t="shared" ref="S128:S190" si="11">LEN(P128)</f>
         <v>159</v>
       </c>
-      <c r="T128" s="14"/>
+      <c r="T128" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129" s="13" t="s">
@@ -18770,7 +19018,9 @@
         <f t="shared" si="11"/>
         <v>183</v>
       </c>
-      <c r="T129" s="14"/>
+      <c r="T129" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130" s="13" t="s">
@@ -18833,7 +19083,9 @@
         <f t="shared" si="11"/>
         <v>266</v>
       </c>
-      <c r="T130" s="14"/>
+      <c r="T130" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131" s="13" t="s">
@@ -18896,7 +19148,9 @@
         <f t="shared" si="11"/>
         <v>382</v>
       </c>
-      <c r="T131" s="14"/>
+      <c r="T131" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132" s="13" t="s">
@@ -18959,7 +19213,9 @@
         <f t="shared" si="11"/>
         <v>59</v>
       </c>
-      <c r="T132" s="14"/>
+      <c r="T132" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133" s="13" t="s">
@@ -19022,7 +19278,9 @@
         <f t="shared" si="11"/>
         <v>338</v>
       </c>
-      <c r="T133" s="14"/>
+      <c r="T133" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134" s="13" t="s">
@@ -19085,7 +19343,9 @@
         <f t="shared" si="11"/>
         <v>89</v>
       </c>
-      <c r="T134" s="14"/>
+      <c r="T134" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135" s="13" t="s">
@@ -19148,7 +19408,9 @@
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
-      <c r="T135" s="14"/>
+      <c r="T135" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136" s="13" t="s">
@@ -19211,7 +19473,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T136" s="14"/>
+      <c r="T136" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137" s="13" t="s">
@@ -19274,7 +19538,9 @@
         <f t="shared" si="11"/>
         <v>62</v>
       </c>
-      <c r="T137" s="14"/>
+      <c r="T137" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138" s="13" t="s">
@@ -19337,7 +19603,9 @@
         <f t="shared" si="11"/>
         <v>311</v>
       </c>
-      <c r="T138" s="14"/>
+      <c r="T138" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139" s="13" t="s">
@@ -19400,7 +19668,9 @@
         <f t="shared" si="11"/>
         <v>143</v>
       </c>
-      <c r="T139" s="14"/>
+      <c r="T139" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140" s="13" t="s">
@@ -19463,7 +19733,9 @@
         <f t="shared" si="11"/>
         <v>86</v>
       </c>
-      <c r="T140" s="14"/>
+      <c r="T140" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141" s="13" t="s">
@@ -19526,7 +19798,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T141" s="14"/>
+      <c r="T141" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
@@ -19589,7 +19863,9 @@
         <f t="shared" si="11"/>
         <v>385</v>
       </c>
-      <c r="T142" s="14"/>
+      <c r="T142" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143" s="13" t="s">
@@ -19652,7 +19928,9 @@
         <f t="shared" si="11"/>
         <v>107</v>
       </c>
-      <c r="T143" s="14"/>
+      <c r="T143" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144" s="13" t="s">
@@ -19715,7 +19993,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T144" s="14"/>
+      <c r="T144" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145" s="13" t="s">
@@ -19778,7 +20058,9 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="T145" s="14"/>
+      <c r="T145" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A146" s="13" t="s">
@@ -19841,7 +20123,9 @@
         <f t="shared" si="11"/>
         <v>149</v>
       </c>
-      <c r="T146" s="14"/>
+      <c r="T146" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="147" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
@@ -19904,7 +20188,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T147" s="14"/>
+      <c r="T147" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A148" s="13" t="s">
@@ -19967,7 +20253,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T148" s="14"/>
+      <c r="T148" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A149" s="13" t="s">
@@ -20030,7 +20318,9 @@
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="T149" s="14"/>
+      <c r="T149" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
@@ -20093,7 +20383,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T150" s="14"/>
+      <c r="T150" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
@@ -20156,7 +20448,9 @@
         <f t="shared" si="11"/>
         <v>31</v>
       </c>
-      <c r="T151" s="14"/>
+      <c r="T151" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
@@ -20219,7 +20513,9 @@
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-      <c r="T152" s="14"/>
+      <c r="T152" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
@@ -20282,7 +20578,9 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="T153" s="14"/>
+      <c r="T153" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
@@ -20345,7 +20643,9 @@
         <f t="shared" si="11"/>
         <v>164</v>
       </c>
-      <c r="T154" s="14"/>
+      <c r="T154" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
@@ -20408,7 +20708,9 @@
         <f t="shared" si="11"/>
         <v>207</v>
       </c>
-      <c r="T155" s="14"/>
+      <c r="T155" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
@@ -20471,7 +20773,9 @@
         <f t="shared" si="11"/>
         <v>140</v>
       </c>
-      <c r="T156" s="14"/>
+      <c r="T156" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
@@ -20534,7 +20838,9 @@
         <f t="shared" si="11"/>
         <v>221</v>
       </c>
-      <c r="T157" s="14"/>
+      <c r="T157" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A158" s="13" t="s">
@@ -20597,7 +20903,9 @@
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-      <c r="T158" s="14"/>
+      <c r="T158" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A159" s="13" t="s">
@@ -20660,7 +20968,9 @@
         <f t="shared" si="11"/>
         <v>27</v>
       </c>
-      <c r="T159" s="14"/>
+      <c r="T159" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A160" s="13" t="s">
@@ -20723,7 +21033,9 @@
         <f t="shared" si="11"/>
         <v>195</v>
       </c>
-      <c r="T160" s="14"/>
+      <c r="T160" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A161" s="13" t="s">
@@ -20786,7 +21098,9 @@
         <f t="shared" si="11"/>
         <v>122</v>
       </c>
-      <c r="T161" s="14"/>
+      <c r="T161" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A162" s="13" t="s">
@@ -20849,7 +21163,9 @@
         <f t="shared" si="11"/>
         <v>53</v>
       </c>
-      <c r="T162" s="14"/>
+      <c r="T162" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A163" s="13" t="s">
@@ -20912,7 +21228,9 @@
         <f t="shared" si="11"/>
         <v>201</v>
       </c>
-      <c r="T163" s="14"/>
+      <c r="T163" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A164" s="13" t="s">
@@ -20975,7 +21293,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T164" s="14"/>
+      <c r="T164" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A165" s="13" t="s">
@@ -21038,7 +21358,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T165" s="14"/>
+      <c r="T165" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" s="13" t="s">
@@ -21101,7 +21423,9 @@
         <f t="shared" si="11"/>
         <v>33</v>
       </c>
-      <c r="T166" s="14"/>
+      <c r="T166" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A167" s="13" t="s">
@@ -21164,7 +21488,9 @@
         <f t="shared" si="11"/>
         <v>137</v>
       </c>
-      <c r="T167" s="14"/>
+      <c r="T167" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A168" s="13" t="s">
@@ -21227,7 +21553,9 @@
         <f t="shared" si="11"/>
         <v>22</v>
       </c>
-      <c r="T168" s="14"/>
+      <c r="T168" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A169" s="13" t="s">
@@ -21290,7 +21618,9 @@
         <f t="shared" si="11"/>
         <v>45</v>
       </c>
-      <c r="T169" s="14"/>
+      <c r="T169" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A170" s="13" t="s">
@@ -21353,7 +21683,9 @@
         <f t="shared" si="11"/>
         <v>127</v>
       </c>
-      <c r="T170" s="14"/>
+      <c r="T170" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A171" s="13" t="s">
@@ -21416,7 +21748,9 @@
         <f t="shared" si="11"/>
         <v>68</v>
       </c>
-      <c r="T171" s="14"/>
+      <c r="T171" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A172" s="13" t="s">
@@ -21479,7 +21813,9 @@
         <f t="shared" si="11"/>
         <v>89</v>
       </c>
-      <c r="T172" s="14"/>
+      <c r="T172" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A173" s="13" t="s">
@@ -21542,7 +21878,9 @@
         <f t="shared" si="11"/>
         <v>295</v>
       </c>
-      <c r="T173" s="14"/>
+      <c r="T173" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A174" s="13" t="s">
@@ -21605,7 +21943,9 @@
         <f t="shared" si="11"/>
         <v>76</v>
       </c>
-      <c r="T174" s="14"/>
+      <c r="T174" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A175" s="13" t="s">
@@ -21668,7 +22008,9 @@
         <f t="shared" si="11"/>
         <v>287</v>
       </c>
-      <c r="T175" s="14"/>
+      <c r="T175" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A176" s="13" t="s">
@@ -21731,7 +22073,9 @@
         <f t="shared" si="11"/>
         <v>27</v>
       </c>
-      <c r="T176" s="14"/>
+      <c r="T176" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="177" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A177" s="13" t="s">
@@ -21794,7 +22138,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T177" s="14"/>
+      <c r="T177" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="178" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A178" s="13" t="s">
@@ -21857,7 +22203,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T178" s="14"/>
+      <c r="T178" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A179" s="13" t="s">
@@ -21920,7 +22268,9 @@
         <f t="shared" si="11"/>
         <v>208</v>
       </c>
-      <c r="T179" s="14"/>
+      <c r="T179" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A180" s="13" t="s">
@@ -21983,7 +22333,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T180" s="14"/>
+      <c r="T180" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="181" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A181" s="13" t="s">
@@ -22046,7 +22398,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T181" s="14"/>
+      <c r="T181" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="182" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A182" s="13" t="s">
@@ -22109,7 +22463,9 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="T182" s="14"/>
+      <c r="T182" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A183" s="13" t="s">
@@ -22172,7 +22528,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T183" s="14"/>
+      <c r="T183" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="184" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A184" s="13" t="s">
@@ -22235,7 +22593,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T184" s="14"/>
+      <c r="T184" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="185" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A185" s="13" t="s">
@@ -22298,7 +22658,9 @@
         <f t="shared" si="11"/>
         <v>242</v>
       </c>
-      <c r="T185" s="14"/>
+      <c r="T185" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="186" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A186" s="16" t="s">
@@ -22361,7 +22723,9 @@
         <f t="shared" si="11"/>
         <v>292</v>
       </c>
-      <c r="T186" s="14"/>
+      <c r="T186" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="187" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A187" s="16" t="s">
@@ -22424,7 +22788,9 @@
         <f t="shared" si="11"/>
         <v>260</v>
       </c>
-      <c r="T187" s="14"/>
+      <c r="T187" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="188" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A188" s="13" t="s">
@@ -22487,7 +22853,9 @@
         <f t="shared" si="11"/>
         <v>74</v>
       </c>
-      <c r="T188" s="14"/>
+      <c r="T188" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="189" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A189" s="13" t="s">
@@ -22550,7 +22918,9 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="T189" s="14"/>
+      <c r="T189" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A190" s="13" t="s">
@@ -22613,7 +22983,9 @@
         <f t="shared" si="11"/>
         <v>186</v>
       </c>
-      <c r="T190" s="14"/>
+      <c r="T190" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A191" s="13" t="s">
@@ -22676,7 +23048,9 @@
         <f t="shared" ref="S191:S231" si="16">LEN(P191)</f>
         <v>16</v>
       </c>
-      <c r="T191" s="14"/>
+      <c r="T191" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="192" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A192" s="13" t="s">
@@ -22739,7 +23113,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T192" s="14"/>
+      <c r="T192" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="193" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A193" s="13" t="s">
@@ -22802,7 +23178,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="T193" s="14"/>
+      <c r="T193" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="194" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A194" s="13" t="s">
@@ -22865,7 +23243,9 @@
         <f t="shared" si="16"/>
         <v>21</v>
       </c>
-      <c r="T194" s="14"/>
+      <c r="T194" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="195" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A195" s="13" t="s">
@@ -22928,7 +23308,9 @@
         <f t="shared" si="16"/>
         <v>24</v>
       </c>
-      <c r="T195" s="14"/>
+      <c r="T195" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="196" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A196" s="13" t="s">
@@ -22991,7 +23373,9 @@
         <f t="shared" si="16"/>
         <v>155</v>
       </c>
-      <c r="T196" s="14"/>
+      <c r="T196" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A197" s="13" t="s">
@@ -23054,7 +23438,9 @@
         <f t="shared" si="16"/>
         <v>297</v>
       </c>
-      <c r="T197" s="14"/>
+      <c r="T197" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="198" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A198" s="13" t="s">
@@ -23117,7 +23503,9 @@
         <f t="shared" si="16"/>
         <v>254</v>
       </c>
-      <c r="T198" s="14"/>
+      <c r="T198" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="199" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A199" s="13" t="s">
@@ -23180,7 +23568,9 @@
         <f t="shared" si="16"/>
         <v>280</v>
       </c>
-      <c r="T199" s="14"/>
+      <c r="T199" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="200" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A200" s="13" t="s">
@@ -23243,7 +23633,9 @@
         <f t="shared" si="16"/>
         <v>232</v>
       </c>
-      <c r="T200" s="14"/>
+      <c r="T200" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="201" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A201" s="13" t="s">
@@ -23306,7 +23698,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T201" s="14"/>
+      <c r="T201" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="202" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A202" s="13" t="s">
@@ -23369,7 +23763,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T202" s="14"/>
+      <c r="T202" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="203" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A203" s="13" t="s">
@@ -23432,7 +23828,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T203" s="14"/>
+      <c r="T203" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A204" s="13" t="s">
@@ -23495,7 +23893,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T204" s="14"/>
+      <c r="T204" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="205" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A205" s="13" t="s">
@@ -23558,7 +23958,9 @@
         <f t="shared" si="16"/>
         <v>215</v>
       </c>
-      <c r="T205" s="14"/>
+      <c r="T205" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="206" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A206" s="13" t="s">
@@ -23621,7 +24023,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T206" s="14"/>
+      <c r="T206" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A207" s="13" t="s">
@@ -23684,7 +24088,9 @@
         <f t="shared" si="16"/>
         <v>254</v>
       </c>
-      <c r="T207" s="14"/>
+      <c r="T207" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="208" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A208" s="13" t="s">
@@ -23747,7 +24153,9 @@
         <f t="shared" si="16"/>
         <v>17</v>
       </c>
-      <c r="T208" s="14"/>
+      <c r="T208" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="209" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A209" s="13" t="s">
@@ -23810,7 +24218,9 @@
         <f t="shared" si="16"/>
         <v>17</v>
       </c>
-      <c r="T209" s="14"/>
+      <c r="T209" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="210" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A210" s="13" t="s">
@@ -23873,7 +24283,9 @@
         <f t="shared" si="16"/>
         <v>352</v>
       </c>
-      <c r="T210" s="14"/>
+      <c r="T210" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="211" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A211" s="13" t="s">
@@ -23936,7 +24348,9 @@
         <f t="shared" si="16"/>
         <v>277</v>
       </c>
-      <c r="T211" s="14"/>
+      <c r="T211" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="212" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A212" s="13" t="s">
@@ -23999,7 +24413,9 @@
         <f t="shared" si="16"/>
         <v>57</v>
       </c>
-      <c r="T212" s="14"/>
+      <c r="T212" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="213" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A213" s="13" t="s">
@@ -24062,7 +24478,9 @@
         <f t="shared" si="16"/>
         <v>149</v>
       </c>
-      <c r="T213" s="14"/>
+      <c r="T213" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="214" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A214" s="13" t="s">
@@ -24125,7 +24543,9 @@
         <f t="shared" si="16"/>
         <v>195</v>
       </c>
-      <c r="T214" s="14"/>
+      <c r="T214" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="215" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A215" s="13" t="s">
@@ -24188,7 +24608,9 @@
         <f t="shared" si="16"/>
         <v>83</v>
       </c>
-      <c r="T215" s="14"/>
+      <c r="T215" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="216" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A216" s="13" t="s">
@@ -24251,7 +24673,9 @@
         <f t="shared" si="16"/>
         <v>86</v>
       </c>
-      <c r="T216" s="14"/>
+      <c r="T216" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="217" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A217" s="13" t="s">
@@ -24314,7 +24738,9 @@
         <f t="shared" si="16"/>
         <v>174</v>
       </c>
-      <c r="T217" s="14"/>
+      <c r="T217" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="218" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A218" s="13" t="s">
@@ -24377,7 +24803,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T218" s="14"/>
+      <c r="T218" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="219" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A219" s="13" t="s">
@@ -24440,7 +24868,9 @@
         <f t="shared" si="16"/>
         <v>564</v>
       </c>
-      <c r="T219" s="14"/>
+      <c r="T219" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="220" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A220" s="13" t="s">
@@ -24503,7 +24933,9 @@
         <f t="shared" si="16"/>
         <v>77</v>
       </c>
-      <c r="T220" s="14"/>
+      <c r="T220" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="221" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A221" s="13" t="s">
@@ -24566,7 +24998,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="T221" s="14"/>
+      <c r="T221" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="222" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A222" s="13" t="s">
@@ -24629,7 +25063,9 @@
         <f t="shared" si="16"/>
         <v>60</v>
       </c>
-      <c r="T222" s="14"/>
+      <c r="T222" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="223" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A223" s="13" t="s">
@@ -24692,7 +25128,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T223" s="14"/>
+      <c r="T223" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="224" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A224" s="13" t="s">
@@ -24755,7 +25193,9 @@
         <f t="shared" si="16"/>
         <v>56</v>
       </c>
-      <c r="T224" s="14"/>
+      <c r="T224" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="225" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A225" s="13" t="s">
@@ -24818,7 +25258,9 @@
         <f t="shared" si="16"/>
         <v>15</v>
       </c>
-      <c r="T225" s="14"/>
+      <c r="T225" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="226" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A226" s="13" t="s">
@@ -24881,7 +25323,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="T226" s="14"/>
+      <c r="T226" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A227" s="13" t="s">
@@ -24944,7 +25388,9 @@
         <f t="shared" si="16"/>
         <v>119</v>
       </c>
-      <c r="T227" s="14"/>
+      <c r="T227" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A228" s="13" t="s">
@@ -25007,7 +25453,9 @@
         <f t="shared" si="16"/>
         <v>41</v>
       </c>
-      <c r="T228" s="14"/>
+      <c r="T228" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A229" s="13" t="s">
@@ -25070,7 +25518,9 @@
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="T229" s="14"/>
+      <c r="T229" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="230" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A230" s="13" t="s">
@@ -25133,7 +25583,9 @@
         <f t="shared" si="16"/>
         <v>59</v>
       </c>
-      <c r="T230" s="14"/>
+      <c r="T230" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="231" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A231" s="13" t="s">
@@ -25196,7 +25648,9 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="T231" s="14"/>
+      <c r="T231" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="232" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A232" s="13" t="s">
@@ -25259,7 +25713,9 @@
         <f t="shared" ref="S232:S256" si="32">LEN(P232)</f>
         <v>54</v>
       </c>
-      <c r="T232" s="14"/>
+      <c r="T232" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="233" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A233" s="13" t="s">
@@ -25322,7 +25778,9 @@
         <f t="shared" si="32"/>
         <v>417</v>
       </c>
-      <c r="T233" s="14"/>
+      <c r="T233" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A234" s="13" t="s">
@@ -25385,7 +25843,9 @@
         <f t="shared" si="32"/>
         <v>99</v>
       </c>
-      <c r="T234" s="14"/>
+      <c r="T234" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="235" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A235" s="13" t="s">
@@ -25448,7 +25908,9 @@
         <f t="shared" si="32"/>
         <v>136</v>
       </c>
-      <c r="T235" s="14"/>
+      <c r="T235" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A236" s="13" t="s">
@@ -25511,7 +25973,9 @@
         <f t="shared" si="32"/>
         <v>68</v>
       </c>
-      <c r="T236" s="14"/>
+      <c r="T236" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="237" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A237" s="13" t="s">
@@ -25574,7 +26038,9 @@
         <f t="shared" si="32"/>
         <v>37</v>
       </c>
-      <c r="T237" s="14"/>
+      <c r="T237" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="238" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A238" s="13" t="s">
@@ -25637,7 +26103,9 @@
         <f t="shared" si="32"/>
         <v>78</v>
       </c>
-      <c r="T238" s="14"/>
+      <c r="T238" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="239" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A239" s="13" t="s">
@@ -25700,7 +26168,9 @@
         <f t="shared" si="32"/>
         <v>8</v>
       </c>
-      <c r="T239" s="14"/>
+      <c r="T239" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="240" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A240" s="13" t="s">
@@ -25763,7 +26233,9 @@
         <f t="shared" si="32"/>
         <v>7</v>
       </c>
-      <c r="T240" s="14"/>
+      <c r="T240" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="241" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A241" s="13" t="s">
@@ -25826,7 +26298,9 @@
         <f t="shared" si="32"/>
         <v>16</v>
       </c>
-      <c r="T241" s="14"/>
+      <c r="T241" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="242" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A242" s="13" t="s">
@@ -25889,7 +26363,9 @@
         <f t="shared" si="32"/>
         <v>16</v>
       </c>
-      <c r="T242" s="14"/>
+      <c r="T242" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="243" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A243" s="13" t="s">
@@ -25952,7 +26428,9 @@
         <f t="shared" si="32"/>
         <v>91</v>
       </c>
-      <c r="T243" s="14"/>
+      <c r="T243" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A244" s="13" t="s">
@@ -26015,7 +26493,9 @@
         <f t="shared" si="32"/>
         <v>33</v>
       </c>
-      <c r="T244" s="14"/>
+      <c r="T244" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="245" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A245" s="13" t="s">
@@ -26078,7 +26558,9 @@
         <f t="shared" si="32"/>
         <v>325</v>
       </c>
-      <c r="T245" s="14"/>
+      <c r="T245" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="246" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A246" s="13" t="s">
@@ -26141,7 +26623,9 @@
         <f t="shared" si="32"/>
         <v>43</v>
       </c>
-      <c r="T246" s="14"/>
+      <c r="T246" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="247" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A247" s="13" t="s">
@@ -26204,7 +26688,9 @@
         <f t="shared" si="32"/>
         <v>50</v>
       </c>
-      <c r="T247" s="14"/>
+      <c r="T247" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="248" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A248" s="13" t="s">
@@ -26267,7 +26753,9 @@
         <f t="shared" si="32"/>
         <v>144</v>
       </c>
-      <c r="T248" s="14"/>
+      <c r="T248" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="249" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A249" s="13" t="s">
@@ -26330,7 +26818,9 @@
         <f t="shared" si="32"/>
         <v>231</v>
       </c>
-      <c r="T249" s="14"/>
+      <c r="T249" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="250" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
@@ -26393,7 +26883,9 @@
         <f t="shared" si="32"/>
         <v>185</v>
       </c>
-      <c r="T250" s="14"/>
+      <c r="T250" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="251" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
@@ -26456,7 +26948,9 @@
         <f t="shared" si="32"/>
         <v>80</v>
       </c>
-      <c r="T251" s="14"/>
+      <c r="T251" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
@@ -26519,7 +27013,9 @@
         <f t="shared" si="32"/>
         <v>78</v>
       </c>
-      <c r="T252" s="14"/>
+      <c r="T252" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="253" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A253" s="13" t="s">
@@ -26582,7 +27078,9 @@
         <f t="shared" si="32"/>
         <v>60</v>
       </c>
-      <c r="T253" s="14"/>
+      <c r="T253" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="254" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A254" s="13" t="s">
@@ -26645,7 +27143,9 @@
         <f t="shared" si="32"/>
         <v>137</v>
       </c>
-      <c r="T254" s="14"/>
+      <c r="T254" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="255" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A255" s="13" t="s">
@@ -26708,7 +27208,9 @@
         <f t="shared" si="32"/>
         <v>105</v>
       </c>
-      <c r="T255" s="14"/>
+      <c r="T255" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="256" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A256" s="13" t="s">
@@ -26771,7 +27273,9 @@
         <f t="shared" si="32"/>
         <v>94</v>
       </c>
-      <c r="T256" s="14"/>
+      <c r="T256" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A257" s="9"/>

</xml_diff>

<commit_message>
#8 Reading List.xlsx, "Producing Open Source Software": increased Rating from 1 to 2 because inconsistent with KBSize (5).
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -10607,9 +10607,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -13142,7 +13142,7 @@
         <v>367</v>
       </c>
       <c r="M39" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N39" s="43">
         <v>20.97</v>

</xml_diff>

<commit_message>
Reading List.xlsx: updated to 2023-12-30.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4266" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="912">
   <si>
     <t>Format</t>
   </si>
@@ -2762,6 +2762,21 @@
   </si>
   <si>
     <t>KBSize</t>
+  </si>
+  <si>
+    <t>Learning AWS IoT</t>
+  </si>
+  <si>
+    <t>2023-12-21</t>
+  </si>
+  <si>
+    <t>Useful. Ok as a "Getting Started" guide.</t>
+  </si>
+  <si>
+    <t>Building Python Web APIs with FastAPI</t>
+  </si>
+  <si>
+    <t>Useful. A concise but comprehensive book.</t>
   </si>
 </sst>
 </file>
@@ -10607,9 +10622,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K260" sqref="K260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -25604,11 +25619,11 @@
         <v>650</v>
       </c>
       <c r="H231" s="9">
-        <f t="shared" ref="H231:H255" si="30">YEAR(G231)</f>
+        <f t="shared" ref="H231:H256" si="30">YEAR(G231)</f>
         <v>2021</v>
       </c>
       <c r="I231" s="9">
-        <f t="shared" ref="I231:I255" si="31">MONTH(G231)</f>
+        <f t="shared" ref="I231:I256" si="31">MONTH(G231)</f>
         <v>3</v>
       </c>
       <c r="J231" s="9" t="s">
@@ -25639,7 +25654,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S255" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S257" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -27207,51 +27222,137 @@
       </c>
     </row>
     <row r="256" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A256" s="9"/>
-      <c r="B256" s="9"/>
-      <c r="C256" s="9"/>
-      <c r="D256" s="9"/>
-      <c r="E256" s="9"/>
-      <c r="F256" s="9"/>
-      <c r="G256" s="9"/>
-      <c r="H256" s="9"/>
-      <c r="I256" s="9"/>
-      <c r="J256" s="9"/>
-      <c r="K256" s="9"/>
-      <c r="L256" s="9"/>
-      <c r="M256" s="9"/>
-      <c r="N256" s="9"/>
-      <c r="O256" s="9"/>
-      <c r="P256" s="9"/>
-      <c r="Q256" s="9"/>
-      <c r="R256" s="9"/>
-      <c r="S256" s="17"/>
-      <c r="T256" s="14"/>
+      <c r="A256" s="13" t="s">
+        <v>907</v>
+      </c>
+      <c r="B256" s="17">
+        <v>2018</v>
+      </c>
+      <c r="C256" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D256" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E256" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F256" s="17">
+        <v>229</v>
+      </c>
+      <c r="G256" s="9" t="s">
+        <v>908</v>
+      </c>
+      <c r="H256" s="17">
+        <f t="shared" si="30"/>
+        <v>2023</v>
+      </c>
+      <c r="I256" s="17">
+        <f t="shared" si="31"/>
+        <v>12</v>
+      </c>
+      <c r="J256" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K256" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L256" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M256" s="17">
+        <v>3</v>
+      </c>
+      <c r="N256" s="17">
+        <v>43.99</v>
+      </c>
+      <c r="O256" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P256" s="13" t="s">
+        <v>909</v>
+      </c>
+      <c r="Q256" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="R256" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S256" s="17">
+        <f t="shared" si="32"/>
+        <v>40</v>
+      </c>
+      <c r="T256" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A257" s="9"/>
-      <c r="B257" s="9"/>
-      <c r="C257" s="9"/>
-      <c r="D257" s="9"/>
-      <c r="E257" s="9"/>
-      <c r="F257" s="9"/>
-      <c r="G257" s="9"/>
-      <c r="H257" s="9"/>
-      <c r="I257" s="9"/>
-      <c r="J257" s="9"/>
-      <c r="K257" s="9"/>
-      <c r="L257" s="9"/>
-      <c r="M257" s="9"/>
-      <c r="N257" s="9"/>
-      <c r="O257" s="9"/>
-      <c r="P257" s="9"/>
-      <c r="Q257" s="9"/>
-      <c r="R257" s="9"/>
-      <c r="S257" s="17"/>
-      <c r="T257" s="14"/>
+      <c r="A257" s="13" t="s">
+        <v>910</v>
+      </c>
+      <c r="B257" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C257" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D257" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E257" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F257" s="17">
+        <v>94</v>
+      </c>
+      <c r="G257" s="9" t="s">
+        <v>908</v>
+      </c>
+      <c r="H257" s="17">
+        <f t="shared" ref="H257" si="33">YEAR(G257)</f>
+        <v>2023</v>
+      </c>
+      <c r="I257" s="17">
+        <f t="shared" ref="I257" si="34">MONTH(G257)</f>
+        <v>12</v>
+      </c>
+      <c r="J257" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K257" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L257" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M257" s="17">
+        <v>4</v>
+      </c>
+      <c r="N257" s="17">
+        <v>41.99</v>
+      </c>
+      <c r="O257" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P257" s="13" t="s">
+        <v>911</v>
+      </c>
+      <c r="Q257" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R257" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S257" s="17">
+        <f t="shared" si="32"/>
+        <v>41</v>
+      </c>
+      <c r="T257" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A258" s="9"/>
+      <c r="A258" s="13"/>
       <c r="B258" s="9"/>
       <c r="C258" s="9"/>
       <c r="D258" s="9"/>
@@ -27266,14 +27367,14 @@
       <c r="M258" s="9"/>
       <c r="N258" s="9"/>
       <c r="O258" s="9"/>
-      <c r="P258" s="9"/>
+      <c r="P258" s="13"/>
       <c r="Q258" s="9"/>
       <c r="R258" s="9"/>
       <c r="S258" s="17"/>
       <c r="T258" s="14"/>
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A259" s="9"/>
+      <c r="A259" s="13"/>
       <c r="B259" s="9"/>
       <c r="C259" s="9"/>
       <c r="D259" s="9"/>
@@ -27288,14 +27389,14 @@
       <c r="M259" s="9"/>
       <c r="N259" s="9"/>
       <c r="O259" s="9"/>
-      <c r="P259" s="9"/>
+      <c r="P259" s="13"/>
       <c r="Q259" s="9"/>
       <c r="R259" s="9"/>
       <c r="S259" s="17"/>
       <c r="T259" s="14"/>
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A260" s="9"/>
+      <c r="A260" s="13"/>
       <c r="B260" s="9"/>
       <c r="C260" s="9"/>
       <c r="D260" s="9"/>
@@ -27310,14 +27411,14 @@
       <c r="M260" s="9"/>
       <c r="N260" s="9"/>
       <c r="O260" s="9"/>
-      <c r="P260" s="9"/>
+      <c r="P260" s="13"/>
       <c r="Q260" s="9"/>
       <c r="R260" s="9"/>
       <c r="S260" s="17"/>
       <c r="T260" s="14"/>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A261" s="9"/>
+      <c r="A261" s="13"/>
       <c r="B261" s="9"/>
       <c r="C261" s="9"/>
       <c r="D261" s="9"/>
@@ -27332,14 +27433,14 @@
       <c r="M261" s="9"/>
       <c r="N261" s="9"/>
       <c r="O261" s="9"/>
-      <c r="P261" s="9"/>
+      <c r="P261" s="13"/>
       <c r="Q261" s="9"/>
       <c r="R261" s="9"/>
       <c r="S261" s="17"/>
       <c r="T261" s="14"/>
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A262" s="9"/>
+      <c r="A262" s="13"/>
       <c r="B262" s="9"/>
       <c r="C262" s="9"/>
       <c r="D262" s="9"/>
@@ -27354,7 +27455,7 @@
       <c r="M262" s="9"/>
       <c r="N262" s="9"/>
       <c r="O262" s="9"/>
-      <c r="P262" s="9"/>
+      <c r="P262" s="13"/>
       <c r="Q262" s="9"/>
       <c r="R262" s="9"/>
       <c r="S262" s="17"/>

</xml_diff>

<commit_message>
Reading List.xlsx: updated to 2023-12-31.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4302" uniqueCount="915">
   <si>
     <t>Format</t>
   </si>
@@ -2777,6 +2777,15 @@
   </si>
   <si>
     <t>Useful. A concise but comprehensive book.</t>
+  </si>
+  <si>
+    <t>Building Python Microservices with FastAPI (1st Ed.)</t>
+  </si>
+  <si>
+    <t>2023-12-31</t>
+  </si>
+  <si>
+    <t>Useful. It's unstructed and caotic like most of the Packt books, but it contains some useful bits of information.</t>
   </si>
 </sst>
 </file>
@@ -10624,7 +10633,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K260" sqref="K260"/>
+      <selection pane="bottomLeft" activeCell="F260" sqref="F260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -25654,7 +25663,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S257" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S258" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -27309,11 +27318,11 @@
         <v>908</v>
       </c>
       <c r="H257" s="17">
-        <f t="shared" ref="H257" si="33">YEAR(G257)</f>
+        <f t="shared" ref="H257:H258" si="33">YEAR(G257)</f>
         <v>2023</v>
       </c>
       <c r="I257" s="17">
-        <f t="shared" ref="I257" si="34">MONTH(G257)</f>
+        <f t="shared" ref="I257:I258" si="34">MONTH(G257)</f>
         <v>12</v>
       </c>
       <c r="J257" s="9" t="s">
@@ -27352,26 +27361,69 @@
       </c>
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A258" s="13"/>
-      <c r="B258" s="9"/>
-      <c r="C258" s="9"/>
-      <c r="D258" s="9"/>
-      <c r="E258" s="9"/>
-      <c r="F258" s="9"/>
-      <c r="G258" s="9"/>
-      <c r="H258" s="9"/>
-      <c r="I258" s="9"/>
-      <c r="J258" s="9"/>
-      <c r="K258" s="9"/>
-      <c r="L258" s="9"/>
-      <c r="M258" s="9"/>
-      <c r="N258" s="9"/>
-      <c r="O258" s="9"/>
-      <c r="P258" s="13"/>
-      <c r="Q258" s="9"/>
-      <c r="R258" s="9"/>
-      <c r="S258" s="17"/>
-      <c r="T258" s="14"/>
+      <c r="A258" s="13" t="s">
+        <v>912</v>
+      </c>
+      <c r="B258" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C258" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D258" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E258" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F258" s="17">
+        <v>265</v>
+      </c>
+      <c r="G258" s="9" t="s">
+        <v>913</v>
+      </c>
+      <c r="H258" s="17">
+        <f t="shared" si="33"/>
+        <v>2023</v>
+      </c>
+      <c r="I258" s="17">
+        <f t="shared" si="34"/>
+        <v>12</v>
+      </c>
+      <c r="J258" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K258" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L258" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M258" s="17">
+        <v>3</v>
+      </c>
+      <c r="N258" s="17">
+        <v>46.99</v>
+      </c>
+      <c r="O258" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P258" s="16" t="s">
+        <v>914</v>
+      </c>
+      <c r="Q258" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R258" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S258" s="17">
+        <f t="shared" si="32"/>
+        <v>113</v>
+      </c>
+      <c r="T258" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A259" s="13"/>

</xml_diff>

<commit_message>
Reading List*: update 08.01.2024.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4302" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4338" uniqueCount="923">
   <si>
     <t>Format</t>
   </si>
@@ -2786,6 +2786,30 @@
   </si>
   <si>
     <t>Useful. It's unstructed and caotic like most of the Packt books, but it contains some useful bits of information.</t>
+  </si>
+  <si>
+    <t>Building Sata Science Applications with FastAPI</t>
+  </si>
+  <si>
+    <t>Useful. It contains some useful information, but it's unstructured and it has a low readiblity layout due of the Github links at the bottom of every code example.</t>
+  </si>
+  <si>
+    <t>2024-01-04</t>
+  </si>
+  <si>
+    <t>The Rules of Programming (Early Release)</t>
+  </si>
+  <si>
+    <t>2024-01-06</t>
+  </si>
+  <si>
+    <t>Useless. Well written, but nothing new under the sun. Pretty useless book.</t>
+  </si>
+  <si>
+    <t>Concise Guide to Software Engineering</t>
+  </si>
+  <si>
+    <t>Useless. I guess that for a beginner this book could have a certain degree of usefullness, but for a software developer with some years of experience it has none.</t>
   </si>
 </sst>
 </file>
@@ -10629,11 +10653,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T262"/>
+  <dimension ref="A1:T269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F260" sqref="F260"/>
+      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -25663,7 +25687,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S258" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S261" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -27318,11 +27342,11 @@
         <v>908</v>
       </c>
       <c r="H257" s="17">
-        <f t="shared" ref="H257:H258" si="33">YEAR(G257)</f>
+        <f t="shared" ref="H257:H259" si="33">YEAR(G257)</f>
         <v>2023</v>
       </c>
       <c r="I257" s="17">
-        <f t="shared" ref="I257:I258" si="34">MONTH(G257)</f>
+        <f t="shared" ref="I257:I259" si="34">MONTH(G257)</f>
         <v>12</v>
       </c>
       <c r="J257" s="9" t="s">
@@ -27426,70 +27450,199 @@
       </c>
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A259" s="13"/>
-      <c r="B259" s="9"/>
-      <c r="C259" s="9"/>
-      <c r="D259" s="9"/>
-      <c r="E259" s="9"/>
-      <c r="F259" s="9"/>
-      <c r="G259" s="9"/>
-      <c r="H259" s="9"/>
-      <c r="I259" s="9"/>
-      <c r="J259" s="9"/>
-      <c r="K259" s="9"/>
-      <c r="L259" s="9"/>
-      <c r="M259" s="9"/>
-      <c r="N259" s="9"/>
-      <c r="O259" s="9"/>
-      <c r="P259" s="13"/>
-      <c r="Q259" s="9"/>
-      <c r="R259" s="9"/>
-      <c r="S259" s="17"/>
-      <c r="T259" s="14"/>
+      <c r="A259" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="B259" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C259" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D259" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E259" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F259" s="17">
+        <v>288</v>
+      </c>
+      <c r="G259" s="9" t="s">
+        <v>917</v>
+      </c>
+      <c r="H259" s="9">
+        <f t="shared" si="33"/>
+        <v>2024</v>
+      </c>
+      <c r="I259" s="9">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="J259" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K259" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L259" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M259" s="17">
+        <v>2</v>
+      </c>
+      <c r="N259" s="17">
+        <v>51.99</v>
+      </c>
+      <c r="O259" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P259" s="16" t="s">
+        <v>916</v>
+      </c>
+      <c r="Q259" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R259" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S259" s="17">
+        <f t="shared" si="32"/>
+        <v>162</v>
+      </c>
+      <c r="T259" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A260" s="13"/>
-      <c r="B260" s="9"/>
-      <c r="C260" s="9"/>
-      <c r="D260" s="9"/>
-      <c r="E260" s="9"/>
-      <c r="F260" s="9"/>
-      <c r="G260" s="9"/>
-      <c r="H260" s="9"/>
-      <c r="I260" s="9"/>
-      <c r="J260" s="9"/>
-      <c r="K260" s="9"/>
-      <c r="L260" s="9"/>
-      <c r="M260" s="9"/>
-      <c r="N260" s="9"/>
-      <c r="O260" s="9"/>
-      <c r="P260" s="13"/>
-      <c r="Q260" s="9"/>
-      <c r="R260" s="9"/>
-      <c r="S260" s="17"/>
-      <c r="T260" s="14"/>
+      <c r="A260" s="13" t="s">
+        <v>918</v>
+      </c>
+      <c r="B260" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C260" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D260" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E260" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F260" s="17">
+        <v>151</v>
+      </c>
+      <c r="G260" s="9" t="s">
+        <v>919</v>
+      </c>
+      <c r="H260" s="9">
+        <f t="shared" ref="H260" si="35">YEAR(G260)</f>
+        <v>2024</v>
+      </c>
+      <c r="I260" s="9">
+        <f t="shared" ref="I260" si="36">MONTH(G260)</f>
+        <v>1</v>
+      </c>
+      <c r="J260" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K260" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L260" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M260" s="17">
+        <v>1</v>
+      </c>
+      <c r="N260" s="17">
+        <v>30.49</v>
+      </c>
+      <c r="O260" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P260" s="13" t="s">
+        <v>920</v>
+      </c>
+      <c r="Q260" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R260" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S260" s="17">
+        <f t="shared" si="32"/>
+        <v>74</v>
+      </c>
+      <c r="T260" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A261" s="13"/>
-      <c r="B261" s="9"/>
-      <c r="C261" s="9"/>
-      <c r="D261" s="9"/>
-      <c r="E261" s="9"/>
-      <c r="F261" s="9"/>
-      <c r="G261" s="9"/>
-      <c r="H261" s="9"/>
-      <c r="I261" s="9"/>
-      <c r="J261" s="9"/>
-      <c r="K261" s="9"/>
-      <c r="L261" s="9"/>
-      <c r="M261" s="9"/>
-      <c r="N261" s="9"/>
-      <c r="O261" s="9"/>
-      <c r="P261" s="13"/>
-      <c r="Q261" s="9"/>
-      <c r="R261" s="9"/>
-      <c r="S261" s="17"/>
-      <c r="T261" s="14"/>
+      <c r="A261" s="13" t="s">
+        <v>921</v>
+      </c>
+      <c r="B261" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C261" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D261" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E261" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F261" s="17">
+        <v>416</v>
+      </c>
+      <c r="G261" s="9" t="s">
+        <v>919</v>
+      </c>
+      <c r="H261" s="9">
+        <f t="shared" ref="H261" si="37">YEAR(G261)</f>
+        <v>2024</v>
+      </c>
+      <c r="I261" s="9">
+        <f t="shared" ref="I261" si="38">MONTH(G261)</f>
+        <v>1</v>
+      </c>
+      <c r="J261" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K261" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L261" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="M261" s="17">
+        <v>1</v>
+      </c>
+      <c r="N261" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O261" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P261" s="13" t="s">
+        <v>922</v>
+      </c>
+      <c r="Q261" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R261" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S261" s="17">
+        <f t="shared" si="32"/>
+        <v>162</v>
+      </c>
+      <c r="T261" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A262" s="13"/>
@@ -27512,6 +27665,160 @@
       <c r="R262" s="9"/>
       <c r="S262" s="17"/>
       <c r="T262" s="14"/>
+    </row>
+    <row r="263" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A263" s="9"/>
+      <c r="B263" s="9"/>
+      <c r="C263" s="9"/>
+      <c r="D263" s="9"/>
+      <c r="E263" s="9"/>
+      <c r="F263" s="9"/>
+      <c r="G263" s="9"/>
+      <c r="H263" s="9"/>
+      <c r="I263" s="9"/>
+      <c r="J263" s="9"/>
+      <c r="K263" s="9"/>
+      <c r="L263" s="9"/>
+      <c r="M263" s="9"/>
+      <c r="N263" s="9"/>
+      <c r="O263" s="9"/>
+      <c r="P263" s="9"/>
+      <c r="Q263" s="9"/>
+      <c r="R263" s="9"/>
+      <c r="S263" s="17"/>
+      <c r="T263" s="9"/>
+    </row>
+    <row r="264" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A264" s="9"/>
+      <c r="B264" s="9"/>
+      <c r="C264" s="9"/>
+      <c r="D264" s="9"/>
+      <c r="E264" s="9"/>
+      <c r="F264" s="9"/>
+      <c r="G264" s="9"/>
+      <c r="H264" s="9"/>
+      <c r="I264" s="9"/>
+      <c r="J264" s="9"/>
+      <c r="K264" s="9"/>
+      <c r="L264" s="9"/>
+      <c r="M264" s="9"/>
+      <c r="N264" s="9"/>
+      <c r="O264" s="9"/>
+      <c r="P264" s="9"/>
+      <c r="Q264" s="9"/>
+      <c r="R264" s="9"/>
+      <c r="S264" s="17"/>
+      <c r="T264" s="9"/>
+    </row>
+    <row r="265" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A265" s="9"/>
+      <c r="B265" s="9"/>
+      <c r="C265" s="9"/>
+      <c r="D265" s="9"/>
+      <c r="E265" s="9"/>
+      <c r="F265" s="9"/>
+      <c r="G265" s="9"/>
+      <c r="H265" s="9"/>
+      <c r="I265" s="9"/>
+      <c r="J265" s="9"/>
+      <c r="K265" s="9"/>
+      <c r="L265" s="9"/>
+      <c r="M265" s="9"/>
+      <c r="N265" s="9"/>
+      <c r="O265" s="9"/>
+      <c r="P265" s="9"/>
+      <c r="Q265" s="9"/>
+      <c r="R265" s="9"/>
+      <c r="S265" s="17"/>
+      <c r="T265" s="9"/>
+    </row>
+    <row r="266" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A266" s="9"/>
+      <c r="B266" s="9"/>
+      <c r="C266" s="9"/>
+      <c r="D266" s="9"/>
+      <c r="E266" s="9"/>
+      <c r="F266" s="9"/>
+      <c r="G266" s="9"/>
+      <c r="H266" s="9"/>
+      <c r="I266" s="9"/>
+      <c r="J266" s="9"/>
+      <c r="K266" s="9"/>
+      <c r="L266" s="9"/>
+      <c r="M266" s="9"/>
+      <c r="N266" s="9"/>
+      <c r="O266" s="9"/>
+      <c r="P266" s="9"/>
+      <c r="Q266" s="9"/>
+      <c r="R266" s="9"/>
+      <c r="S266" s="17"/>
+      <c r="T266" s="9"/>
+    </row>
+    <row r="267" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A267" s="9"/>
+      <c r="B267" s="9"/>
+      <c r="C267" s="9"/>
+      <c r="D267" s="9"/>
+      <c r="E267" s="9"/>
+      <c r="F267" s="9"/>
+      <c r="G267" s="9"/>
+      <c r="H267" s="9"/>
+      <c r="I267" s="9"/>
+      <c r="J267" s="9"/>
+      <c r="K267" s="9"/>
+      <c r="L267" s="9"/>
+      <c r="M267" s="9"/>
+      <c r="N267" s="9"/>
+      <c r="O267" s="9"/>
+      <c r="P267" s="9"/>
+      <c r="Q267" s="9"/>
+      <c r="R267" s="9"/>
+      <c r="S267" s="17"/>
+      <c r="T267" s="9"/>
+    </row>
+    <row r="268" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A268" s="9"/>
+      <c r="B268" s="9"/>
+      <c r="C268" s="9"/>
+      <c r="D268" s="9"/>
+      <c r="E268" s="9"/>
+      <c r="F268" s="9"/>
+      <c r="G268" s="9"/>
+      <c r="H268" s="9"/>
+      <c r="I268" s="9"/>
+      <c r="J268" s="9"/>
+      <c r="K268" s="9"/>
+      <c r="L268" s="9"/>
+      <c r="M268" s="9"/>
+      <c r="N268" s="9"/>
+      <c r="O268" s="9"/>
+      <c r="P268" s="9"/>
+      <c r="Q268" s="9"/>
+      <c r="R268" s="9"/>
+      <c r="S268" s="17"/>
+      <c r="T268" s="9"/>
+    </row>
+    <row r="269" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A269" s="9"/>
+      <c r="B269" s="9"/>
+      <c r="C269" s="9"/>
+      <c r="D269" s="9"/>
+      <c r="E269" s="9"/>
+      <c r="F269" s="9"/>
+      <c r="G269" s="9"/>
+      <c r="H269" s="9"/>
+      <c r="I269" s="9"/>
+      <c r="J269" s="9"/>
+      <c r="K269" s="9"/>
+      <c r="L269" s="9"/>
+      <c r="M269" s="9"/>
+      <c r="N269" s="9"/>
+      <c r="O269" s="9"/>
+      <c r="P269" s="9"/>
+      <c r="Q269" s="9"/>
+      <c r="R269" s="9"/>
+      <c r="S269" s="17"/>
+      <c r="T269" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#11 Reading List: updated to 2024-01-28.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -10655,9 +10655,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A266" sqref="A266"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R257" sqref="R257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -26471,7 +26471,7 @@
         <v>33</v>
       </c>
       <c r="T243" s="14">
-        <v>0</v>
+        <v>488</v>
       </c>
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.2">
@@ -26536,7 +26536,7 @@
         <v>325</v>
       </c>
       <c r="T244" s="14">
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="245" spans="1:20" x14ac:dyDescent="0.2">
@@ -26666,7 +26666,7 @@
         <v>50</v>
       </c>
       <c r="T246" s="14">
-        <v>0</v>
+        <v>367</v>
       </c>
     </row>
     <row r="247" spans="1:20" x14ac:dyDescent="0.2">
@@ -26731,7 +26731,7 @@
         <v>144</v>
       </c>
       <c r="T247" s="14">
-        <v>0</v>
+        <v>431</v>
       </c>
     </row>
     <row r="248" spans="1:20" x14ac:dyDescent="0.2">
@@ -26796,7 +26796,7 @@
         <v>231</v>
       </c>
       <c r="T248" s="14">
-        <v>0</v>
+        <v>380</v>
       </c>
     </row>
     <row r="249" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Reading List: updated 05.02.2024.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -10657,7 +10657,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R257" sqref="R257"/>
+      <selection pane="bottomLeft" activeCell="S265" sqref="S265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -26861,7 +26861,7 @@
         <v>185</v>
       </c>
       <c r="T249" s="14">
-        <v>0</v>
+        <v>280</v>
       </c>
     </row>
     <row r="250" spans="1:20" x14ac:dyDescent="0.2">
@@ -26926,7 +26926,7 @@
         <v>80</v>
       </c>
       <c r="T250" s="14">
-        <v>0</v>
+        <v>230</v>
       </c>
     </row>
     <row r="251" spans="1:20" x14ac:dyDescent="0.2">
@@ -26991,7 +26991,7 @@
         <v>78</v>
       </c>
       <c r="T251" s="14">
-        <v>0</v>
+        <v>194</v>
       </c>
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.2">
@@ -27056,7 +27056,7 @@
         <v>60</v>
       </c>
       <c r="T252" s="14">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="253" spans="1:20" x14ac:dyDescent="0.2">
@@ -27121,7 +27121,7 @@
         <v>137</v>
       </c>
       <c r="T253" s="14">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="254" spans="1:20" x14ac:dyDescent="0.2">
@@ -27186,7 +27186,7 @@
         <v>105</v>
       </c>
       <c r="T254" s="14">
-        <v>0</v>
+        <v>154</v>
       </c>
     </row>
     <row r="255" spans="1:20" x14ac:dyDescent="0.2">
@@ -27251,7 +27251,7 @@
         <v>94</v>
       </c>
       <c r="T255" s="14">
-        <v>0</v>
+        <v>164</v>
       </c>
     </row>
     <row r="256" spans="1:20" x14ac:dyDescent="0.2">
@@ -27316,7 +27316,7 @@
         <v>40</v>
       </c>
       <c r="T256" s="14">
-        <v>0</v>
+        <v>330</v>
       </c>
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.2">
@@ -27381,7 +27381,7 @@
         <v>41</v>
       </c>
       <c r="T257" s="14">
-        <v>0</v>
+        <v>747</v>
       </c>
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#11 Reading List: update 18.02.2024
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -2788,9 +2788,6 @@
     <t>Useful. It's unstructed and caotic like most of the Packt books, but it contains some useful bits of information.</t>
   </si>
   <si>
-    <t>Building Sata Science Applications with FastAPI</t>
-  </si>
-  <si>
     <t>Useful. It contains some useful information, but it's unstructured and it has a low readiblity layout due of the Github links at the bottom of every code example.</t>
   </si>
   <si>
@@ -2810,6 +2807,9 @@
   </si>
   <si>
     <t>Useless. I guess that for a beginner this book could have a certain degree of usefullness, but for a software developer with some years of experience it has none.</t>
+  </si>
+  <si>
+    <t>Building Data Science Applications with FastAPI</t>
   </si>
 </sst>
 </file>
@@ -10655,9 +10655,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S265" sqref="S265"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A261" sqref="A261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -27446,12 +27446,12 @@
         <v>113</v>
       </c>
       <c r="T258" s="14">
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A259" s="13" t="s">
-        <v>915</v>
+        <v>922</v>
       </c>
       <c r="B259" s="17">
         <v>2023</v>
@@ -27469,7 +27469,7 @@
         <v>288</v>
       </c>
       <c r="G259" s="9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H259" s="9">
         <f t="shared" si="33"/>
@@ -27498,7 +27498,7 @@
         <v>664</v>
       </c>
       <c r="P259" s="16" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Q259" s="9" t="s">
         <v>569</v>
@@ -27511,12 +27511,12 @@
         <v>162</v>
       </c>
       <c r="T259" s="14">
-        <v>0</v>
+        <v>326</v>
       </c>
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A260" s="13" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B260" s="17">
         <v>2023</v>
@@ -27534,7 +27534,7 @@
         <v>151</v>
       </c>
       <c r="G260" s="9" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="H260" s="9">
         <f t="shared" ref="H260" si="35">YEAR(G260)</f>
@@ -27563,7 +27563,7 @@
         <v>664</v>
       </c>
       <c r="P260" s="13" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="Q260" s="9" t="s">
         <v>469</v>
@@ -27576,12 +27576,12 @@
         <v>74</v>
       </c>
       <c r="T260" s="14">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A261" s="13" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B261" s="17">
         <v>2022</v>
@@ -27599,7 +27599,7 @@
         <v>416</v>
       </c>
       <c r="G261" s="9" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="H261" s="9">
         <f t="shared" ref="H261" si="37">YEAR(G261)</f>
@@ -27628,7 +27628,7 @@
         <v>664</v>
       </c>
       <c r="P261" s="13" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="Q261" s="9" t="s">
         <v>469</v>
@@ -27641,7 +27641,7 @@
         <v>162</v>
       </c>
       <c r="T261" s="14">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Reading List, update: 2024.02.26.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4338" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4506" uniqueCount="957">
   <si>
     <t>Format</t>
   </si>
@@ -2779,9 +2779,6 @@
     <t>Useful. A concise but comprehensive book.</t>
   </si>
   <si>
-    <t>Building Python Microservices with FastAPI (1st Ed.)</t>
-  </si>
-  <si>
     <t>2023-12-31</t>
   </si>
   <si>
@@ -2809,7 +2806,112 @@
     <t>Useless. I guess that for a beginner this book could have a certain degree of usefullness, but for a software developer with some years of experience it has none.</t>
   </si>
   <si>
-    <t>Building Data Science Applications with FastAPI</t>
+    <t>Building Data Science Applications with FastAPI (2nd Edition)</t>
+  </si>
+  <si>
+    <t>Building Python Microservices with FastAPI (1st Edition)</t>
+  </si>
+  <si>
+    <t>ProxMox VE Administration Guide - Release 7.2</t>
+  </si>
+  <si>
+    <t>2024-02-19</t>
+  </si>
+  <si>
+    <t>Useful. It shows how well ProxMox has been designed.</t>
+  </si>
+  <si>
+    <t>Clean Architecture</t>
+  </si>
+  <si>
+    <t>Useful. A good book for beginners, well-written and clear. The last part about the history of computers could be easily removed.</t>
+  </si>
+  <si>
+    <t>Python How-To</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>Useless. Well-written, but it contains no original nor well-structured knowledge. In addition, the second half of the book is not about Python but about Flask. Totally useless book.</t>
+  </si>
+  <si>
+    <t>Python Foundation</t>
+  </si>
+  <si>
+    <t>Useless. Very basic overview about multiple Python-related topics. The layout of the book is horrible (dense, lack of bold face, ...).</t>
+  </si>
+  <si>
+    <t>Python Unit Test Automation (2nd Edition)</t>
+  </si>
+  <si>
+    <t>Useless. Just a walkthrough of Python unit test frameworks. No original content.</t>
+  </si>
+  <si>
+    <t>Testing in Python</t>
+  </si>
+  <si>
+    <t>Useless. Too much opinionated towards pytest, not able to explain why pytest is better than unittest in a convincing way.</t>
+  </si>
+  <si>
+    <t>2024-02-25</t>
+  </si>
+  <si>
+    <t>Python Object-Oriented Programming (4th Edition)</t>
+  </si>
+  <si>
+    <t>Useful. An ok getting started guide for whom wants to learn OOP and Python from scratch at the same time.</t>
+  </si>
+  <si>
+    <t>Intermediate Python [MLI]</t>
+  </si>
+  <si>
+    <t>MLI</t>
+  </si>
+  <si>
+    <t>Useless. Well-written (organized like a recipe book and without ramblings), but contains no different knowledge than hundreds of Python books.</t>
+  </si>
+  <si>
+    <t>Learning Advanced Python By Studying Open-Source Projects</t>
+  </si>
+  <si>
+    <t>CRC Press</t>
+  </si>
+  <si>
+    <t>Useless. The book title is misleading: the author doesn't study any open-source project. It's just a Python cookbook like hundreds others.</t>
+  </si>
+  <si>
+    <t>Python in a Nutshell (4th Edition)</t>
+  </si>
+  <si>
+    <t>Useful. Well-written and comprehensive, it contains few bits of information I didn't know.</t>
+  </si>
+  <si>
+    <t>Python 3 And Feature Engineering</t>
+  </si>
+  <si>
+    <t>Useful. No-frills introduction to feature engineering in a cookbook format.</t>
+  </si>
+  <si>
+    <t>Python Testing Cookbook (2nd Edition)</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
+  </si>
+  <si>
+    <t>Useful. It's a long list of testing techniques and Python tools to perform them. Good to have all collected in the same book.</t>
+  </si>
+  <si>
+    <t>Python Testing with pytest (2nd Edition)</t>
+  </si>
+  <si>
+    <t>Useful. A well-written and comprehensive book about pytest.</t>
+  </si>
+  <si>
+    <t>Python Packages</t>
+  </si>
+  <si>
+    <t>Useful. Excellent book about the topic. It's well-written, comprehensive and pragmatic. It would become perfect by removing the repetitions.</t>
   </si>
 </sst>
 </file>
@@ -10653,11 +10755,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T269"/>
+  <dimension ref="A1:T288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A261" sqref="A261"/>
+      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C277" sqref="C277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -25687,7 +25789,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S261" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S275" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -27386,7 +27488,7 @@
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A258" s="13" t="s">
-        <v>912</v>
+        <v>922</v>
       </c>
       <c r="B258" s="17">
         <v>2022</v>
@@ -27404,7 +27506,7 @@
         <v>265</v>
       </c>
       <c r="G258" s="9" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="H258" s="17">
         <f t="shared" si="33"/>
@@ -27433,7 +27535,7 @@
         <v>664</v>
       </c>
       <c r="P258" s="16" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q258" s="9" t="s">
         <v>569</v>
@@ -27451,7 +27553,7 @@
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A259" s="13" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B259" s="17">
         <v>2023</v>
@@ -27469,7 +27571,7 @@
         <v>288</v>
       </c>
       <c r="G259" s="9" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H259" s="9">
         <f t="shared" si="33"/>
@@ -27498,7 +27600,7 @@
         <v>664</v>
       </c>
       <c r="P259" s="16" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q259" s="9" t="s">
         <v>569</v>
@@ -27516,7 +27618,7 @@
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A260" s="13" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B260" s="17">
         <v>2023</v>
@@ -27534,7 +27636,7 @@
         <v>151</v>
       </c>
       <c r="G260" s="9" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="H260" s="9">
         <f t="shared" ref="H260" si="35">YEAR(G260)</f>
@@ -27563,7 +27665,7 @@
         <v>664</v>
       </c>
       <c r="P260" s="13" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="Q260" s="9" t="s">
         <v>469</v>
@@ -27581,7 +27683,7 @@
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A261" s="13" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B261" s="17">
         <v>2022</v>
@@ -27599,14 +27701,14 @@
         <v>416</v>
       </c>
       <c r="G261" s="9" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="H261" s="9">
-        <f t="shared" ref="H261" si="37">YEAR(G261)</f>
+        <f t="shared" ref="H261:H263" si="37">YEAR(G261)</f>
         <v>2024</v>
       </c>
       <c r="I261" s="9">
-        <f t="shared" ref="I261" si="38">MONTH(G261)</f>
+        <f t="shared" ref="I261:I263" si="38">MONTH(G261)</f>
         <v>1</v>
       </c>
       <c r="J261" s="9" t="s">
@@ -27628,7 +27730,7 @@
         <v>664</v>
       </c>
       <c r="P261" s="13" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="Q261" s="9" t="s">
         <v>469</v>
@@ -27645,180 +27747,1200 @@
       </c>
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A262" s="13"/>
-      <c r="B262" s="9"/>
-      <c r="C262" s="9"/>
-      <c r="D262" s="9"/>
-      <c r="E262" s="9"/>
-      <c r="F262" s="9"/>
-      <c r="G262" s="9"/>
-      <c r="H262" s="9"/>
-      <c r="I262" s="9"/>
-      <c r="J262" s="9"/>
-      <c r="K262" s="9"/>
-      <c r="L262" s="9"/>
-      <c r="M262" s="9"/>
-      <c r="N262" s="9"/>
-      <c r="O262" s="9"/>
-      <c r="P262" s="13"/>
-      <c r="Q262" s="9"/>
-      <c r="R262" s="9"/>
-      <c r="S262" s="17"/>
-      <c r="T262" s="14"/>
+      <c r="A262" s="13" t="s">
+        <v>923</v>
+      </c>
+      <c r="B262" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C262" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D262" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E262" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F262" s="17">
+        <v>535</v>
+      </c>
+      <c r="G262" s="9" t="s">
+        <v>924</v>
+      </c>
+      <c r="H262" s="9">
+        <f t="shared" si="37"/>
+        <v>2024</v>
+      </c>
+      <c r="I262" s="9">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="J262" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K262" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L262" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M262" s="17">
+        <v>2</v>
+      </c>
+      <c r="N262" s="43">
+        <v>0</v>
+      </c>
+      <c r="O262" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P262" s="13" t="s">
+        <v>925</v>
+      </c>
+      <c r="Q262" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="R262" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S262" s="17">
+        <f t="shared" si="32"/>
+        <v>52</v>
+      </c>
+      <c r="T262" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="263" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A263" s="9"/>
-      <c r="B263" s="9"/>
-      <c r="C263" s="9"/>
-      <c r="D263" s="9"/>
-      <c r="E263" s="9"/>
-      <c r="F263" s="9"/>
-      <c r="G263" s="9"/>
-      <c r="H263" s="9"/>
-      <c r="I263" s="9"/>
-      <c r="J263" s="9"/>
-      <c r="K263" s="9"/>
-      <c r="L263" s="9"/>
-      <c r="M263" s="9"/>
-      <c r="N263" s="9"/>
-      <c r="O263" s="9"/>
-      <c r="P263" s="9"/>
-      <c r="Q263" s="9"/>
-      <c r="R263" s="9"/>
-      <c r="S263" s="17"/>
-      <c r="T263" s="9"/>
+      <c r="A263" s="13" t="s">
+        <v>926</v>
+      </c>
+      <c r="B263" s="17">
+        <v>2018</v>
+      </c>
+      <c r="C263" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D263" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E263" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F263" s="17">
+        <v>429</v>
+      </c>
+      <c r="G263" s="9" t="s">
+        <v>924</v>
+      </c>
+      <c r="H263" s="9">
+        <f t="shared" si="37"/>
+        <v>2024</v>
+      </c>
+      <c r="I263" s="9">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="J263" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K263" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L263" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="M263" s="17">
+        <v>3</v>
+      </c>
+      <c r="N263" s="17">
+        <v>30.39</v>
+      </c>
+      <c r="O263" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P263" s="16" t="s">
+        <v>927</v>
+      </c>
+      <c r="Q263" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R263" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S263" s="17">
+        <f t="shared" si="32"/>
+        <v>128</v>
+      </c>
+      <c r="T263" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="264" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A264" s="9"/>
-      <c r="B264" s="9"/>
-      <c r="C264" s="9"/>
-      <c r="D264" s="9"/>
-      <c r="E264" s="9"/>
-      <c r="F264" s="9"/>
-      <c r="G264" s="9"/>
-      <c r="H264" s="9"/>
-      <c r="I264" s="9"/>
-      <c r="J264" s="9"/>
-      <c r="K264" s="9"/>
-      <c r="L264" s="9"/>
-      <c r="M264" s="9"/>
-      <c r="N264" s="9"/>
-      <c r="O264" s="9"/>
-      <c r="P264" s="9"/>
-      <c r="Q264" s="9"/>
-      <c r="R264" s="9"/>
-      <c r="S264" s="17"/>
-      <c r="T264" s="9"/>
+      <c r="A264" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="B264" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C264" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D264" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E264" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F264" s="17">
+        <v>455</v>
+      </c>
+      <c r="G264" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="H264" s="9">
+        <f t="shared" ref="H264" si="39">YEAR(G264)</f>
+        <v>2024</v>
+      </c>
+      <c r="I264" s="9">
+        <f t="shared" ref="I264" si="40">MONTH(G264)</f>
+        <v>2</v>
+      </c>
+      <c r="J264" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K264" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L264" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M264" s="17">
+        <v>1</v>
+      </c>
+      <c r="N264" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O264" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P264" s="16" t="s">
+        <v>930</v>
+      </c>
+      <c r="Q264" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R264" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S264" s="17">
+        <f t="shared" si="32"/>
+        <v>181</v>
+      </c>
+      <c r="T264" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="265" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A265" s="9"/>
-      <c r="B265" s="9"/>
-      <c r="C265" s="9"/>
-      <c r="D265" s="9"/>
-      <c r="E265" s="9"/>
-      <c r="F265" s="9"/>
-      <c r="G265" s="9"/>
-      <c r="H265" s="9"/>
-      <c r="I265" s="9"/>
-      <c r="J265" s="9"/>
-      <c r="K265" s="9"/>
-      <c r="L265" s="9"/>
-      <c r="M265" s="9"/>
-      <c r="N265" s="9"/>
-      <c r="O265" s="9"/>
-      <c r="P265" s="9"/>
-      <c r="Q265" s="9"/>
-      <c r="R265" s="9"/>
-      <c r="S265" s="17"/>
-      <c r="T265" s="9"/>
+      <c r="A265" s="13" t="s">
+        <v>931</v>
+      </c>
+      <c r="B265" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C265" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D265" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E265" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F265" s="17">
+        <v>205</v>
+      </c>
+      <c r="G265" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="H265" s="9">
+        <f t="shared" ref="H265" si="41">YEAR(G265)</f>
+        <v>2024</v>
+      </c>
+      <c r="I265" s="9">
+        <f t="shared" ref="I265" si="42">MONTH(G265)</f>
+        <v>2</v>
+      </c>
+      <c r="J265" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K265" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L265" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M265" s="17">
+        <v>1</v>
+      </c>
+      <c r="N265" s="17">
+        <v>22.49</v>
+      </c>
+      <c r="O265" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P265" s="16" t="s">
+        <v>932</v>
+      </c>
+      <c r="Q265" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R265" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S265" s="17">
+        <f t="shared" si="32"/>
+        <v>134</v>
+      </c>
+      <c r="T265" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="266" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A266" s="9"/>
-      <c r="B266" s="9"/>
-      <c r="C266" s="9"/>
-      <c r="D266" s="9"/>
-      <c r="E266" s="9"/>
-      <c r="F266" s="9"/>
-      <c r="G266" s="9"/>
-      <c r="H266" s="9"/>
-      <c r="I266" s="9"/>
-      <c r="J266" s="9"/>
-      <c r="K266" s="9"/>
-      <c r="L266" s="9"/>
-      <c r="M266" s="9"/>
-      <c r="N266" s="9"/>
-      <c r="O266" s="9"/>
-      <c r="P266" s="9"/>
-      <c r="Q266" s="9"/>
-      <c r="R266" s="9"/>
-      <c r="S266" s="17"/>
-      <c r="T266" s="9"/>
+      <c r="A266" s="13" t="s">
+        <v>933</v>
+      </c>
+      <c r="B266" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C266" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D266" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E266" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F266" s="17">
+        <v>94</v>
+      </c>
+      <c r="G266" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="H266" s="9">
+        <f t="shared" ref="H266" si="43">YEAR(G266)</f>
+        <v>2024</v>
+      </c>
+      <c r="I266" s="9">
+        <f t="shared" ref="I266" si="44">MONTH(G266)</f>
+        <v>2</v>
+      </c>
+      <c r="J266" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K266" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L266" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="M266" s="17">
+        <v>1</v>
+      </c>
+      <c r="N266" s="17">
+        <v>38.880000000000003</v>
+      </c>
+      <c r="O266" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P266" s="13" t="s">
+        <v>934</v>
+      </c>
+      <c r="Q266" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R266" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S266" s="17">
+        <f t="shared" si="32"/>
+        <v>80</v>
+      </c>
+      <c r="T266" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="267" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A267" s="9"/>
-      <c r="B267" s="9"/>
-      <c r="C267" s="9"/>
-      <c r="D267" s="9"/>
-      <c r="E267" s="9"/>
-      <c r="F267" s="9"/>
-      <c r="G267" s="9"/>
-      <c r="H267" s="9"/>
-      <c r="I267" s="9"/>
-      <c r="J267" s="9"/>
-      <c r="K267" s="9"/>
-      <c r="L267" s="9"/>
-      <c r="M267" s="9"/>
-      <c r="N267" s="9"/>
-      <c r="O267" s="9"/>
-      <c r="P267" s="9"/>
-      <c r="Q267" s="9"/>
-      <c r="R267" s="9"/>
-      <c r="S267" s="17"/>
-      <c r="T267" s="9"/>
+      <c r="A267" s="13" t="s">
+        <v>935</v>
+      </c>
+      <c r="B267" s="17">
+        <v>2020</v>
+      </c>
+      <c r="C267" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D267" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E267" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F267" s="17">
+        <v>132</v>
+      </c>
+      <c r="G267" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="H267" s="9">
+        <f t="shared" ref="H267:H268" si="45">YEAR(G267)</f>
+        <v>2024</v>
+      </c>
+      <c r="I267" s="9">
+        <f t="shared" ref="I267:I268" si="46">MONTH(G267)</f>
+        <v>2</v>
+      </c>
+      <c r="J267" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K267" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L267" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M267" s="17">
+        <v>1</v>
+      </c>
+      <c r="N267" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O267" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P267" s="13" t="s">
+        <v>936</v>
+      </c>
+      <c r="Q267" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R267" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S267" s="17">
+        <f t="shared" si="32"/>
+        <v>121</v>
+      </c>
+      <c r="T267" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="268" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A268" s="9"/>
-      <c r="B268" s="9"/>
-      <c r="C268" s="9"/>
-      <c r="D268" s="9"/>
-      <c r="E268" s="9"/>
-      <c r="F268" s="9"/>
-      <c r="G268" s="9"/>
-      <c r="H268" s="9"/>
-      <c r="I268" s="9"/>
-      <c r="J268" s="9"/>
-      <c r="K268" s="9"/>
-      <c r="L268" s="9"/>
-      <c r="M268" s="9"/>
-      <c r="N268" s="9"/>
-      <c r="O268" s="9"/>
-      <c r="P268" s="9"/>
-      <c r="Q268" s="9"/>
-      <c r="R268" s="9"/>
-      <c r="S268" s="17"/>
-      <c r="T268" s="9"/>
+      <c r="A268" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="B268" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C268" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D268" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E268" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F268" s="17">
+        <v>715</v>
+      </c>
+      <c r="G268" s="9" t="s">
+        <v>937</v>
+      </c>
+      <c r="H268" s="9">
+        <f t="shared" si="45"/>
+        <v>2024</v>
+      </c>
+      <c r="I268" s="9">
+        <f t="shared" si="46"/>
+        <v>2</v>
+      </c>
+      <c r="J268" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K268" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L268" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M268" s="17">
+        <v>2</v>
+      </c>
+      <c r="N268" s="17">
+        <v>38.24</v>
+      </c>
+      <c r="O268" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P268" s="13" t="s">
+        <v>939</v>
+      </c>
+      <c r="Q268" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R268" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S268" s="17">
+        <f t="shared" si="32"/>
+        <v>105</v>
+      </c>
+      <c r="T268" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="269" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A269" s="9"/>
-      <c r="B269" s="9"/>
-      <c r="C269" s="9"/>
-      <c r="D269" s="9"/>
-      <c r="E269" s="9"/>
-      <c r="F269" s="9"/>
-      <c r="G269" s="9"/>
-      <c r="H269" s="9"/>
-      <c r="I269" s="9"/>
-      <c r="J269" s="9"/>
-      <c r="K269" s="9"/>
-      <c r="L269" s="9"/>
-      <c r="M269" s="9"/>
-      <c r="N269" s="9"/>
-      <c r="O269" s="9"/>
-      <c r="P269" s="9"/>
-      <c r="Q269" s="9"/>
-      <c r="R269" s="9"/>
-      <c r="S269" s="17"/>
-      <c r="T269" s="9"/>
+      <c r="A269" s="13" t="s">
+        <v>940</v>
+      </c>
+      <c r="B269" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C269" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D269" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E269" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F269" s="17">
+        <v>192</v>
+      </c>
+      <c r="G269" s="9" t="s">
+        <v>937</v>
+      </c>
+      <c r="H269" s="9">
+        <f t="shared" ref="H269" si="47">YEAR(G269)</f>
+        <v>2024</v>
+      </c>
+      <c r="I269" s="9">
+        <f t="shared" ref="I269" si="48">MONTH(G269)</f>
+        <v>2</v>
+      </c>
+      <c r="J269" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K269" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L269" s="9" t="s">
+        <v>941</v>
+      </c>
+      <c r="M269" s="17">
+        <v>1</v>
+      </c>
+      <c r="N269" s="17">
+        <v>54.99</v>
+      </c>
+      <c r="O269" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P269" s="13" t="s">
+        <v>942</v>
+      </c>
+      <c r="Q269" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R269" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S269" s="17">
+        <f t="shared" si="32"/>
+        <v>142</v>
+      </c>
+      <c r="T269" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A270" s="13" t="s">
+        <v>943</v>
+      </c>
+      <c r="B270" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C270" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D270" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E270" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F270" s="17">
+        <v>139</v>
+      </c>
+      <c r="G270" s="9" t="s">
+        <v>937</v>
+      </c>
+      <c r="H270" s="9">
+        <f t="shared" ref="H270" si="49">YEAR(G270)</f>
+        <v>2024</v>
+      </c>
+      <c r="I270" s="9">
+        <f t="shared" ref="I270" si="50">MONTH(G270)</f>
+        <v>2</v>
+      </c>
+      <c r="J270" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K270" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L270" s="9" t="s">
+        <v>944</v>
+      </c>
+      <c r="M270" s="17">
+        <v>1</v>
+      </c>
+      <c r="N270" s="17">
+        <v>59.95</v>
+      </c>
+      <c r="O270" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P270" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="Q270" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R270" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S270" s="17">
+        <f t="shared" si="32"/>
+        <v>138</v>
+      </c>
+      <c r="T270" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A271" s="13" t="s">
+        <v>946</v>
+      </c>
+      <c r="B271" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C271" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D271" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E271" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F271" s="17">
+        <v>963</v>
+      </c>
+      <c r="G271" s="9" t="s">
+        <v>937</v>
+      </c>
+      <c r="H271" s="9">
+        <f t="shared" ref="H271" si="51">YEAR(G271)</f>
+        <v>2024</v>
+      </c>
+      <c r="I271" s="9">
+        <f t="shared" ref="I271" si="52">MONTH(G271)</f>
+        <v>2</v>
+      </c>
+      <c r="J271" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K271" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L271" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M271" s="17">
+        <v>3</v>
+      </c>
+      <c r="N271" s="17">
+        <v>65.23</v>
+      </c>
+      <c r="O271" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P271" s="13" t="s">
+        <v>947</v>
+      </c>
+      <c r="Q271" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R271" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S271" s="17">
+        <f t="shared" si="32"/>
+        <v>90</v>
+      </c>
+      <c r="T271" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A272" s="13" t="s">
+        <v>948</v>
+      </c>
+      <c r="B272" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C272" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D272" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E272" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F272" s="17">
+        <v>229</v>
+      </c>
+      <c r="G272" s="9" t="s">
+        <v>937</v>
+      </c>
+      <c r="H272" s="9">
+        <f t="shared" ref="H272:H273" si="53">YEAR(G272)</f>
+        <v>2024</v>
+      </c>
+      <c r="I272" s="9">
+        <f t="shared" ref="I272:I273" si="54">MONTH(G272)</f>
+        <v>2</v>
+      </c>
+      <c r="J272" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K272" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L272" s="9" t="s">
+        <v>941</v>
+      </c>
+      <c r="M272" s="17">
+        <v>2</v>
+      </c>
+      <c r="N272" s="17">
+        <v>54.99</v>
+      </c>
+      <c r="O272" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P272" s="13" t="s">
+        <v>949</v>
+      </c>
+      <c r="Q272" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R272" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S272" s="17">
+        <f t="shared" si="32"/>
+        <v>75</v>
+      </c>
+      <c r="T272" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A273" s="13" t="s">
+        <v>950</v>
+      </c>
+      <c r="B273" s="17">
+        <v>2018</v>
+      </c>
+      <c r="C273" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D273" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E273" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F273" s="17">
+        <v>978</v>
+      </c>
+      <c r="G273" s="9" t="s">
+        <v>951</v>
+      </c>
+      <c r="H273" s="9">
+        <f t="shared" si="53"/>
+        <v>2024</v>
+      </c>
+      <c r="I273" s="9">
+        <f t="shared" si="54"/>
+        <v>2</v>
+      </c>
+      <c r="J273" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K273" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L273" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M273" s="17">
+        <v>2</v>
+      </c>
+      <c r="N273" s="17">
+        <v>33.99</v>
+      </c>
+      <c r="O273" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P273" s="13" t="s">
+        <v>952</v>
+      </c>
+      <c r="Q273" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R273" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S273" s="17">
+        <f t="shared" si="32"/>
+        <v>125</v>
+      </c>
+      <c r="T273" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A274" s="13" t="s">
+        <v>953</v>
+      </c>
+      <c r="B274" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C274" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D274" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E274" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F274" s="17">
+        <v>264</v>
+      </c>
+      <c r="G274" s="9" t="s">
+        <v>951</v>
+      </c>
+      <c r="H274" s="9">
+        <f t="shared" ref="H274" si="55">YEAR(G274)</f>
+        <v>2024</v>
+      </c>
+      <c r="I274" s="9">
+        <f t="shared" ref="I274" si="56">MONTH(G274)</f>
+        <v>2</v>
+      </c>
+      <c r="J274" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K274" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L274" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="M274" s="17">
+        <v>3</v>
+      </c>
+      <c r="N274" s="17">
+        <v>39.49</v>
+      </c>
+      <c r="O274" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P274" s="13" t="s">
+        <v>954</v>
+      </c>
+      <c r="Q274" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R274" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S274" s="17">
+        <f t="shared" si="32"/>
+        <v>59</v>
+      </c>
+      <c r="T274" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A275" s="13" t="s">
+        <v>955</v>
+      </c>
+      <c r="B275" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C275" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D275" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E275" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F275" s="17">
+        <v>243</v>
+      </c>
+      <c r="G275" s="9" t="s">
+        <v>951</v>
+      </c>
+      <c r="H275" s="9">
+        <f t="shared" ref="H275" si="57">YEAR(G275)</f>
+        <v>2024</v>
+      </c>
+      <c r="I275" s="9">
+        <f t="shared" ref="I275" si="58">MONTH(G275)</f>
+        <v>2</v>
+      </c>
+      <c r="J275" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K275" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L275" s="9" t="s">
+        <v>944</v>
+      </c>
+      <c r="M275" s="17">
+        <v>4</v>
+      </c>
+      <c r="N275" s="17">
+        <v>48.95</v>
+      </c>
+      <c r="O275" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P275" s="13" t="s">
+        <v>956</v>
+      </c>
+      <c r="Q275" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R275" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S275" s="17">
+        <f t="shared" si="32"/>
+        <v>140</v>
+      </c>
+      <c r="T275" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A276" s="13"/>
+      <c r="B276" s="9"/>
+      <c r="C276" s="9"/>
+      <c r="D276" s="9"/>
+      <c r="E276" s="9"/>
+      <c r="F276" s="9"/>
+      <c r="G276" s="9"/>
+      <c r="H276" s="9"/>
+      <c r="I276" s="9"/>
+      <c r="J276" s="9"/>
+      <c r="K276" s="9"/>
+      <c r="L276" s="9"/>
+      <c r="M276" s="9"/>
+      <c r="N276" s="9"/>
+      <c r="O276" s="9"/>
+      <c r="P276" s="13"/>
+      <c r="Q276" s="9"/>
+      <c r="R276" s="9"/>
+      <c r="S276" s="17"/>
+      <c r="T276" s="9"/>
+    </row>
+    <row r="277" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A277" s="13"/>
+      <c r="B277" s="9"/>
+      <c r="C277" s="9"/>
+      <c r="D277" s="9"/>
+      <c r="E277" s="9"/>
+      <c r="F277" s="9"/>
+      <c r="G277" s="9"/>
+      <c r="H277" s="9"/>
+      <c r="I277" s="9"/>
+      <c r="J277" s="9"/>
+      <c r="K277" s="9"/>
+      <c r="L277" s="9"/>
+      <c r="M277" s="9"/>
+      <c r="N277" s="9"/>
+      <c r="O277" s="9"/>
+      <c r="P277" s="13"/>
+      <c r="Q277" s="9"/>
+      <c r="R277" s="9"/>
+      <c r="S277" s="17"/>
+      <c r="T277" s="9"/>
+    </row>
+    <row r="278" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A278" s="13"/>
+      <c r="B278" s="9"/>
+      <c r="C278" s="9"/>
+      <c r="D278" s="9"/>
+      <c r="E278" s="9"/>
+      <c r="F278" s="9"/>
+      <c r="G278" s="9"/>
+      <c r="H278" s="9"/>
+      <c r="I278" s="9"/>
+      <c r="J278" s="9"/>
+      <c r="K278" s="9"/>
+      <c r="L278" s="9"/>
+      <c r="M278" s="9"/>
+      <c r="N278" s="9"/>
+      <c r="O278" s="9"/>
+      <c r="P278" s="13"/>
+      <c r="Q278" s="9"/>
+      <c r="R278" s="9"/>
+      <c r="S278" s="17"/>
+      <c r="T278" s="9"/>
+    </row>
+    <row r="279" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A279" s="13"/>
+      <c r="B279" s="9"/>
+      <c r="C279" s="9"/>
+      <c r="D279" s="9"/>
+      <c r="E279" s="9"/>
+      <c r="F279" s="9"/>
+      <c r="G279" s="9"/>
+      <c r="H279" s="9"/>
+      <c r="I279" s="9"/>
+      <c r="J279" s="9"/>
+      <c r="K279" s="9"/>
+      <c r="L279" s="9"/>
+      <c r="M279" s="9"/>
+      <c r="N279" s="9"/>
+      <c r="O279" s="9"/>
+      <c r="P279" s="13"/>
+      <c r="Q279" s="9"/>
+      <c r="R279" s="9"/>
+      <c r="S279" s="17"/>
+      <c r="T279" s="9"/>
+    </row>
+    <row r="280" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A280" s="13"/>
+      <c r="B280" s="9"/>
+      <c r="C280" s="9"/>
+      <c r="D280" s="9"/>
+      <c r="E280" s="9"/>
+      <c r="F280" s="9"/>
+      <c r="G280" s="9"/>
+      <c r="H280" s="9"/>
+      <c r="I280" s="9"/>
+      <c r="J280" s="9"/>
+      <c r="K280" s="9"/>
+      <c r="L280" s="9"/>
+      <c r="M280" s="9"/>
+      <c r="N280" s="9"/>
+      <c r="O280" s="9"/>
+      <c r="P280" s="13"/>
+      <c r="Q280" s="9"/>
+      <c r="R280" s="9"/>
+      <c r="S280" s="17"/>
+      <c r="T280" s="9"/>
+    </row>
+    <row r="281" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A281" s="13"/>
+      <c r="B281" s="9"/>
+      <c r="C281" s="9"/>
+      <c r="D281" s="9"/>
+      <c r="E281" s="9"/>
+      <c r="F281" s="9"/>
+      <c r="G281" s="9"/>
+      <c r="H281" s="9"/>
+      <c r="I281" s="9"/>
+      <c r="J281" s="9"/>
+      <c r="K281" s="9"/>
+      <c r="L281" s="9"/>
+      <c r="M281" s="9"/>
+      <c r="N281" s="9"/>
+      <c r="O281" s="9"/>
+      <c r="P281" s="13"/>
+      <c r="Q281" s="9"/>
+      <c r="R281" s="9"/>
+      <c r="S281" s="17"/>
+      <c r="T281" s="9"/>
+    </row>
+    <row r="282" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A282" s="13"/>
+      <c r="B282" s="9"/>
+      <c r="C282" s="9"/>
+      <c r="D282" s="9"/>
+      <c r="E282" s="9"/>
+      <c r="F282" s="9"/>
+      <c r="G282" s="9"/>
+      <c r="H282" s="9"/>
+      <c r="I282" s="9"/>
+      <c r="J282" s="9"/>
+      <c r="K282" s="9"/>
+      <c r="L282" s="9"/>
+      <c r="M282" s="9"/>
+      <c r="N282" s="9"/>
+      <c r="O282" s="9"/>
+      <c r="P282" s="13"/>
+      <c r="Q282" s="9"/>
+      <c r="R282" s="9"/>
+      <c r="S282" s="17"/>
+      <c r="T282" s="9"/>
+    </row>
+    <row r="283" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A283" s="13"/>
+      <c r="B283" s="9"/>
+      <c r="C283" s="9"/>
+      <c r="D283" s="9"/>
+      <c r="E283" s="9"/>
+      <c r="F283" s="9"/>
+      <c r="G283" s="9"/>
+      <c r="H283" s="9"/>
+      <c r="I283" s="9"/>
+      <c r="J283" s="9"/>
+      <c r="K283" s="9"/>
+      <c r="L283" s="9"/>
+      <c r="M283" s="9"/>
+      <c r="N283" s="9"/>
+      <c r="O283" s="9"/>
+      <c r="P283" s="13"/>
+      <c r="Q283" s="9"/>
+      <c r="R283" s="9"/>
+      <c r="S283" s="17"/>
+      <c r="T283" s="9"/>
+    </row>
+    <row r="284" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A284" s="13"/>
+      <c r="B284" s="9"/>
+      <c r="C284" s="9"/>
+      <c r="D284" s="9"/>
+      <c r="E284" s="9"/>
+      <c r="F284" s="9"/>
+      <c r="G284" s="9"/>
+      <c r="H284" s="9"/>
+      <c r="I284" s="9"/>
+      <c r="J284" s="9"/>
+      <c r="K284" s="9"/>
+      <c r="L284" s="9"/>
+      <c r="M284" s="9"/>
+      <c r="N284" s="9"/>
+      <c r="O284" s="9"/>
+      <c r="P284" s="13"/>
+      <c r="Q284" s="9"/>
+      <c r="R284" s="9"/>
+      <c r="S284" s="17"/>
+      <c r="T284" s="9"/>
+    </row>
+    <row r="285" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A285" s="13"/>
+      <c r="B285" s="9"/>
+      <c r="C285" s="9"/>
+      <c r="D285" s="9"/>
+      <c r="E285" s="9"/>
+      <c r="F285" s="9"/>
+      <c r="G285" s="9"/>
+      <c r="H285" s="9"/>
+      <c r="I285" s="9"/>
+      <c r="J285" s="9"/>
+      <c r="K285" s="9"/>
+      <c r="L285" s="9"/>
+      <c r="M285" s="9"/>
+      <c r="N285" s="9"/>
+      <c r="O285" s="9"/>
+      <c r="P285" s="13"/>
+      <c r="Q285" s="9"/>
+      <c r="R285" s="9"/>
+      <c r="S285" s="17"/>
+      <c r="T285" s="9"/>
+    </row>
+    <row r="286" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A286" s="13"/>
+      <c r="B286" s="9"/>
+      <c r="C286" s="9"/>
+      <c r="D286" s="9"/>
+      <c r="E286" s="9"/>
+      <c r="F286" s="9"/>
+      <c r="G286" s="9"/>
+      <c r="H286" s="9"/>
+      <c r="I286" s="9"/>
+      <c r="J286" s="9"/>
+      <c r="K286" s="9"/>
+      <c r="L286" s="9"/>
+      <c r="M286" s="9"/>
+      <c r="N286" s="9"/>
+      <c r="O286" s="9"/>
+      <c r="P286" s="13"/>
+      <c r="Q286" s="9"/>
+      <c r="R286" s="9"/>
+      <c r="S286" s="17"/>
+      <c r="T286" s="9"/>
+    </row>
+    <row r="287" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A287" s="13"/>
+      <c r="B287" s="9"/>
+      <c r="C287" s="9"/>
+      <c r="D287" s="9"/>
+      <c r="E287" s="9"/>
+      <c r="F287" s="9"/>
+      <c r="G287" s="9"/>
+      <c r="H287" s="9"/>
+      <c r="I287" s="9"/>
+      <c r="J287" s="9"/>
+      <c r="K287" s="9"/>
+      <c r="L287" s="9"/>
+      <c r="M287" s="9"/>
+      <c r="N287" s="9"/>
+      <c r="O287" s="9"/>
+      <c r="P287" s="13"/>
+      <c r="Q287" s="9"/>
+      <c r="R287" s="9"/>
+      <c r="S287" s="17"/>
+      <c r="T287" s="9"/>
+    </row>
+    <row r="288" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A288" s="13"/>
+      <c r="B288" s="9"/>
+      <c r="C288" s="9"/>
+      <c r="D288" s="9"/>
+      <c r="E288" s="9"/>
+      <c r="F288" s="9"/>
+      <c r="G288" s="9"/>
+      <c r="H288" s="9"/>
+      <c r="I288" s="9"/>
+      <c r="J288" s="9"/>
+      <c r="K288" s="9"/>
+      <c r="L288" s="9"/>
+      <c r="M288" s="9"/>
+      <c r="N288" s="9"/>
+      <c r="O288" s="9"/>
+      <c r="P288" s="13"/>
+      <c r="Q288" s="9"/>
+      <c r="R288" s="9"/>
+      <c r="S288" s="17"/>
+      <c r="T288" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#23 Reading List.xslx: updated to 2024-05-19.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Repositories\jupnb-nwreadinglistmanager\nwreadinglistmanager\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Repositories\jupnb-nwreadinglist\nwreadinglist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4506" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4530" uniqueCount="963">
   <si>
     <t>Format</t>
   </si>
@@ -2912,6 +2912,24 @@
   </si>
   <si>
     <t>Useful. Excellent book about the topic. It's well-written, comprehensive and pragmatic. It would become perfect by removing the repetitions.</t>
+  </si>
+  <si>
+    <t>The Quick Guide to Prompt Engineering</t>
+  </si>
+  <si>
+    <t>2024-05-19</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Useless. Extremely repetitive, the same content could have been written in 40 pages. No practical or hands-on knowledge, just obvious and superficial statements. Avoid.</t>
+  </si>
+  <si>
+    <t>Writing AI Prompts For Dummies</t>
+  </si>
+  <si>
+    <t>Useless. It's a list of online AI services and a soup of obvious statements. No hands-on knowledge.</t>
   </si>
 </sst>
 </file>
@@ -10758,8 +10776,8 @@
   <dimension ref="A1:T288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C277" sqref="C277"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -25789,7 +25807,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S275" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S277" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -28614,11 +28632,11 @@
         <v>951</v>
       </c>
       <c r="H275" s="9">
-        <f t="shared" ref="H275" si="57">YEAR(G275)</f>
+        <f t="shared" ref="H275:H277" si="57">YEAR(G275)</f>
         <v>2024</v>
       </c>
       <c r="I275" s="9">
-        <f t="shared" ref="I275" si="58">MONTH(G275)</f>
+        <f t="shared" ref="I275:I276" si="58">MONTH(G275)</f>
         <v>2</v>
       </c>
       <c r="J275" s="9" t="s">
@@ -28657,48 +28675,134 @@
       </c>
     </row>
     <row r="276" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A276" s="13"/>
-      <c r="B276" s="9"/>
-      <c r="C276" s="9"/>
-      <c r="D276" s="9"/>
-      <c r="E276" s="9"/>
-      <c r="F276" s="9"/>
-      <c r="G276" s="9"/>
-      <c r="H276" s="9"/>
-      <c r="I276" s="9"/>
-      <c r="J276" s="9"/>
-      <c r="K276" s="9"/>
-      <c r="L276" s="9"/>
-      <c r="M276" s="9"/>
-      <c r="N276" s="9"/>
-      <c r="O276" s="9"/>
-      <c r="P276" s="13"/>
-      <c r="Q276" s="9"/>
-      <c r="R276" s="9"/>
-      <c r="S276" s="17"/>
-      <c r="T276" s="9"/>
+      <c r="A276" s="13" t="s">
+        <v>957</v>
+      </c>
+      <c r="B276" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C276" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D276" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E276" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F276" s="17">
+        <v>337</v>
+      </c>
+      <c r="G276" s="9" t="s">
+        <v>958</v>
+      </c>
+      <c r="H276" s="9">
+        <f t="shared" si="57"/>
+        <v>2024</v>
+      </c>
+      <c r="I276" s="9">
+        <f>MONTH(G276)</f>
+        <v>5</v>
+      </c>
+      <c r="J276" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K276" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L276" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="M276" s="17">
+        <v>1</v>
+      </c>
+      <c r="N276" s="17">
+        <v>24.99</v>
+      </c>
+      <c r="O276" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P276" s="13" t="s">
+        <v>960</v>
+      </c>
+      <c r="Q276" s="9" t="s">
+        <v>959</v>
+      </c>
+      <c r="R276" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S276" s="17">
+        <f t="shared" si="32"/>
+        <v>168</v>
+      </c>
+      <c r="T276" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="277" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A277" s="13"/>
-      <c r="B277" s="9"/>
-      <c r="C277" s="9"/>
-      <c r="D277" s="9"/>
-      <c r="E277" s="9"/>
-      <c r="F277" s="9"/>
-      <c r="G277" s="9"/>
-      <c r="H277" s="9"/>
-      <c r="I277" s="9"/>
-      <c r="J277" s="9"/>
-      <c r="K277" s="9"/>
-      <c r="L277" s="9"/>
-      <c r="M277" s="9"/>
-      <c r="N277" s="9"/>
-      <c r="O277" s="9"/>
-      <c r="P277" s="13"/>
-      <c r="Q277" s="9"/>
-      <c r="R277" s="9"/>
-      <c r="S277" s="17"/>
-      <c r="T277" s="9"/>
+      <c r="A277" s="13" t="s">
+        <v>961</v>
+      </c>
+      <c r="B277" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C277" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D277" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E277" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F277" s="17">
+        <v>253</v>
+      </c>
+      <c r="G277" s="9" t="s">
+        <v>958</v>
+      </c>
+      <c r="H277" s="9">
+        <f t="shared" si="57"/>
+        <v>2024</v>
+      </c>
+      <c r="I277" s="9">
+        <f>MONTH(G277)</f>
+        <v>5</v>
+      </c>
+      <c r="J277" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K277" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L277" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="M277" s="17">
+        <v>1</v>
+      </c>
+      <c r="N277" s="17">
+        <v>24.99</v>
+      </c>
+      <c r="O277" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P277" s="13" t="s">
+        <v>962</v>
+      </c>
+      <c r="Q277" s="9" t="s">
+        <v>959</v>
+      </c>
+      <c r="R277" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S277" s="17">
+        <f t="shared" si="32"/>
+        <v>99</v>
+      </c>
+      <c r="T277" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="278" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A278" s="13"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated to 2024-06-25.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4530" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4566" uniqueCount="971">
   <si>
     <t>Format</t>
   </si>
@@ -2930,6 +2930,30 @@
   </si>
   <si>
     <t>Useless. It's a list of online AI services and a soup of obvious statements. No hands-on knowledge.</t>
+  </si>
+  <si>
+    <t>Product Management</t>
+  </si>
+  <si>
+    <t>Unlocking The Secrets of Prompt Engineering</t>
+  </si>
+  <si>
+    <t>2024-06-25</t>
+  </si>
+  <si>
+    <t>Useful. Despite being a book published by Packt, it's reasonably well written, clear and structured, and not the usual copy&amp;paste of random blocks of text taken from the internet. It's not a masterpiece, but it contains a couple of use cases that stimulate your critical thinking.</t>
+  </si>
+  <si>
+    <t>API as a Product</t>
+  </si>
+  <si>
+    <t>Useful. Concise and comprehensive book about product management and API development.</t>
+  </si>
+  <si>
+    <t>Building an API Product</t>
+  </si>
+  <si>
+    <t>Useful. Decent book, but as many published by Packt contains many repetitions and redundancy. It could be easily shrinked be 1/3 without losing content.</t>
   </si>
 </sst>
 </file>
@@ -10776,8 +10800,8 @@
   <dimension ref="A1:T288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A282" sqref="A282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -24696,7 +24720,7 @@
         <v>825</v>
       </c>
       <c r="Q214" s="9" t="s">
-        <v>469</v>
+        <v>963</v>
       </c>
       <c r="R214" s="9" t="s">
         <v>159</v>
@@ -25807,7 +25831,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S277" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S280" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -28632,11 +28656,11 @@
         <v>951</v>
       </c>
       <c r="H275" s="9">
-        <f t="shared" ref="H275:H277" si="57">YEAR(G275)</f>
+        <f t="shared" ref="H275:H278" si="57">YEAR(G275)</f>
         <v>2024</v>
       </c>
       <c r="I275" s="9">
-        <f t="shared" ref="I275:I276" si="58">MONTH(G275)</f>
+        <f t="shared" ref="I275" si="58">MONTH(G275)</f>
         <v>2</v>
       </c>
       <c r="J275" s="9" t="s">
@@ -28805,70 +28829,199 @@
       </c>
     </row>
     <row r="278" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A278" s="13"/>
-      <c r="B278" s="9"/>
-      <c r="C278" s="9"/>
-      <c r="D278" s="9"/>
-      <c r="E278" s="9"/>
-      <c r="F278" s="9"/>
-      <c r="G278" s="9"/>
-      <c r="H278" s="9"/>
-      <c r="I278" s="9"/>
-      <c r="J278" s="9"/>
-      <c r="K278" s="9"/>
-      <c r="L278" s="9"/>
-      <c r="M278" s="9"/>
-      <c r="N278" s="9"/>
-      <c r="O278" s="9"/>
-      <c r="P278" s="13"/>
-      <c r="Q278" s="9"/>
-      <c r="R278" s="9"/>
-      <c r="S278" s="17"/>
-      <c r="T278" s="9"/>
+      <c r="A278" s="13" t="s">
+        <v>964</v>
+      </c>
+      <c r="B278" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C278" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D278" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E278" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F278" s="17">
+        <v>316</v>
+      </c>
+      <c r="G278" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="H278" s="9">
+        <f t="shared" si="57"/>
+        <v>2024</v>
+      </c>
+      <c r="I278" s="9">
+        <f>MONTH(G278)</f>
+        <v>6</v>
+      </c>
+      <c r="J278" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K278" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L278" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M278" s="17">
+        <v>3</v>
+      </c>
+      <c r="N278" s="17">
+        <v>44.99</v>
+      </c>
+      <c r="O278" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P278" s="13" t="s">
+        <v>966</v>
+      </c>
+      <c r="Q278" s="9" t="s">
+        <v>959</v>
+      </c>
+      <c r="R278" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S278" s="17">
+        <f t="shared" si="32"/>
+        <v>280</v>
+      </c>
+      <c r="T278" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="279" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A279" s="13"/>
-      <c r="B279" s="9"/>
-      <c r="C279" s="9"/>
-      <c r="D279" s="9"/>
-      <c r="E279" s="9"/>
-      <c r="F279" s="9"/>
-      <c r="G279" s="9"/>
-      <c r="H279" s="9"/>
-      <c r="I279" s="9"/>
-      <c r="J279" s="9"/>
-      <c r="K279" s="9"/>
-      <c r="L279" s="9"/>
-      <c r="M279" s="9"/>
-      <c r="N279" s="9"/>
-      <c r="O279" s="9"/>
-      <c r="P279" s="13"/>
-      <c r="Q279" s="9"/>
-      <c r="R279" s="9"/>
-      <c r="S279" s="17"/>
-      <c r="T279" s="9"/>
+      <c r="A279" s="13" t="s">
+        <v>967</v>
+      </c>
+      <c r="B279" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C279" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D279" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E279" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F279" s="17">
+        <v>112</v>
+      </c>
+      <c r="G279" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="H279" s="9">
+        <f t="shared" ref="H279" si="59">YEAR(G279)</f>
+        <v>2024</v>
+      </c>
+      <c r="I279" s="9">
+        <f>MONTH(G279)</f>
+        <v>6</v>
+      </c>
+      <c r="J279" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K279" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L279" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M279" s="17">
+        <v>3</v>
+      </c>
+      <c r="N279" s="43">
+        <v>0</v>
+      </c>
+      <c r="O279" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P279" s="13" t="s">
+        <v>968</v>
+      </c>
+      <c r="Q279" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R279" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S279" s="17">
+        <f t="shared" si="32"/>
+        <v>84</v>
+      </c>
+      <c r="T279" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="280" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A280" s="13"/>
-      <c r="B280" s="9"/>
-      <c r="C280" s="9"/>
-      <c r="D280" s="9"/>
-      <c r="E280" s="9"/>
-      <c r="F280" s="9"/>
-      <c r="G280" s="9"/>
-      <c r="H280" s="9"/>
-      <c r="I280" s="9"/>
-      <c r="J280" s="9"/>
-      <c r="K280" s="9"/>
-      <c r="L280" s="9"/>
-      <c r="M280" s="9"/>
-      <c r="N280" s="9"/>
-      <c r="O280" s="9"/>
-      <c r="P280" s="13"/>
-      <c r="Q280" s="9"/>
-      <c r="R280" s="9"/>
-      <c r="S280" s="17"/>
-      <c r="T280" s="9"/>
+      <c r="A280" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="B280" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C280" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D280" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E280" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F280" s="17">
+        <v>1779</v>
+      </c>
+      <c r="G280" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="H280" s="9">
+        <f t="shared" ref="H280" si="60">YEAR(G280)</f>
+        <v>2024</v>
+      </c>
+      <c r="I280" s="9">
+        <f>MONTH(G280)</f>
+        <v>6</v>
+      </c>
+      <c r="J280" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K280" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L280" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M280" s="17">
+        <v>3</v>
+      </c>
+      <c r="N280" s="17">
+        <v>40.549999999999997</v>
+      </c>
+      <c r="O280" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P280" s="13" t="s">
+        <v>970</v>
+      </c>
+      <c r="Q280" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R280" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S280" s="17">
+        <f t="shared" si="32"/>
+        <v>152</v>
+      </c>
+      <c r="T280" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="281" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A281" s="13"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated to 2024-07-05.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4566" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4598" uniqueCount="978">
   <si>
     <t>Format</t>
   </si>
@@ -2954,6 +2954,27 @@
   </si>
   <si>
     <t>Useful. Decent book, but as many published by Packt contains many repetitions and redundancy. It could be easily shrinked be 1/3 without losing content.</t>
+  </si>
+  <si>
+    <t>The Kaggle Book</t>
+  </si>
+  <si>
+    <t>2024-06-27</t>
+  </si>
+  <si>
+    <t>Useless. No actionable knowledge, just a very wordy description of how Kaggle works, with a bunch of random data science theory blocks in the mix. [STOPPED 152]</t>
+  </si>
+  <si>
+    <t>Microservice API</t>
+  </si>
+  <si>
+    <t>2024-07-04</t>
+  </si>
+  <si>
+    <t>Useful. It contains some useful bits of knowledge about FastAPI.</t>
+  </si>
+  <si>
+    <t>Building and Delivering Microservices on AWS</t>
   </si>
 </sst>
 </file>
@@ -10797,11 +10818,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T288"/>
+  <dimension ref="A1:T300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A282" sqref="A282"/>
+      <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A284" sqref="A284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -25831,7 +25852,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S280" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S282" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -28981,7 +29002,7 @@
         <v>965</v>
       </c>
       <c r="H280" s="9">
-        <f t="shared" ref="H280" si="60">YEAR(G280)</f>
+        <f t="shared" ref="H280:H282" si="60">YEAR(G280)</f>
         <v>2024</v>
       </c>
       <c r="I280" s="9">
@@ -29024,68 +29045,176 @@
       </c>
     </row>
     <row r="281" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A281" s="13"/>
-      <c r="B281" s="9"/>
-      <c r="C281" s="9"/>
-      <c r="D281" s="9"/>
-      <c r="E281" s="9"/>
-      <c r="F281" s="9"/>
-      <c r="G281" s="9"/>
-      <c r="H281" s="9"/>
-      <c r="I281" s="9"/>
-      <c r="J281" s="9"/>
-      <c r="K281" s="9"/>
-      <c r="L281" s="9"/>
-      <c r="M281" s="9"/>
-      <c r="N281" s="9"/>
-      <c r="O281" s="9"/>
-      <c r="P281" s="13"/>
-      <c r="Q281" s="9"/>
-      <c r="R281" s="9"/>
-      <c r="S281" s="17"/>
-      <c r="T281" s="9"/>
+      <c r="A281" s="13" t="s">
+        <v>971</v>
+      </c>
+      <c r="B281" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C281" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D281" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E281" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F281" s="17">
+        <v>365</v>
+      </c>
+      <c r="G281" s="9" t="s">
+        <v>972</v>
+      </c>
+      <c r="H281" s="9">
+        <f t="shared" si="60"/>
+        <v>2024</v>
+      </c>
+      <c r="I281" s="9">
+        <f>MONTH(G281)</f>
+        <v>6</v>
+      </c>
+      <c r="J281" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K281" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L281" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M281" s="17">
+        <v>1</v>
+      </c>
+      <c r="N281" s="17">
+        <v>49.15</v>
+      </c>
+      <c r="O281" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P281" s="16" t="s">
+        <v>973</v>
+      </c>
+      <c r="Q281" s="9" t="s">
+        <v>904</v>
+      </c>
+      <c r="R281" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S281" s="17">
+        <f t="shared" si="32"/>
+        <v>160</v>
+      </c>
+      <c r="T281" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="282" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A282" s="13"/>
-      <c r="B282" s="9"/>
-      <c r="C282" s="9"/>
-      <c r="D282" s="9"/>
-      <c r="E282" s="9"/>
-      <c r="F282" s="9"/>
-      <c r="G282" s="9"/>
-      <c r="H282" s="9"/>
-      <c r="I282" s="9"/>
-      <c r="J282" s="9"/>
-      <c r="K282" s="9"/>
-      <c r="L282" s="9"/>
-      <c r="M282" s="9"/>
-      <c r="N282" s="9"/>
-      <c r="O282" s="9"/>
-      <c r="P282" s="13"/>
-      <c r="Q282" s="9"/>
-      <c r="R282" s="9"/>
-      <c r="S282" s="17"/>
-      <c r="T282" s="9"/>
+      <c r="A282" s="13" t="s">
+        <v>974</v>
+      </c>
+      <c r="B282" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C282" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D282" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E282" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F282" s="17">
+        <v>340</v>
+      </c>
+      <c r="G282" s="9" t="s">
+        <v>975</v>
+      </c>
+      <c r="H282" s="9">
+        <f t="shared" si="60"/>
+        <v>2024</v>
+      </c>
+      <c r="I282" s="9">
+        <f>MONTH(G282)</f>
+        <v>7</v>
+      </c>
+      <c r="J282" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K282" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L282" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M282" s="17">
+        <v>2</v>
+      </c>
+      <c r="N282" s="17">
+        <v>50.21</v>
+      </c>
+      <c r="O282" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P282" s="13" t="s">
+        <v>976</v>
+      </c>
+      <c r="Q282" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R282" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S282" s="17">
+        <f t="shared" si="32"/>
+        <v>64</v>
+      </c>
+      <c r="T282" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="283" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A283" s="13"/>
-      <c r="B283" s="9"/>
-      <c r="C283" s="9"/>
-      <c r="D283" s="9"/>
-      <c r="E283" s="9"/>
-      <c r="F283" s="9"/>
+      <c r="A283" s="13" t="s">
+        <v>977</v>
+      </c>
+      <c r="B283" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C283" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D283" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E283" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F283" s="17">
+        <v>600</v>
+      </c>
       <c r="G283" s="9"/>
       <c r="H283" s="9"/>
       <c r="I283" s="9"/>
       <c r="J283" s="9"/>
       <c r="K283" s="9"/>
-      <c r="L283" s="9"/>
+      <c r="L283" s="9" t="s">
+        <v>365</v>
+      </c>
       <c r="M283" s="9"/>
-      <c r="N283" s="9"/>
-      <c r="O283" s="9"/>
+      <c r="N283" s="17">
+        <v>43.13</v>
+      </c>
+      <c r="O283" s="9" t="s">
+        <v>664</v>
+      </c>
       <c r="P283" s="13"/>
-      <c r="Q283" s="9"/>
-      <c r="R283" s="9"/>
+      <c r="Q283" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R283" s="9" t="s">
+        <v>159</v>
+      </c>
       <c r="S283" s="17"/>
       <c r="T283" s="9"/>
     </row>
@@ -29198,6 +29327,270 @@
       <c r="R288" s="9"/>
       <c r="S288" s="17"/>
       <c r="T288" s="9"/>
+    </row>
+    <row r="289" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A289" s="9"/>
+      <c r="B289" s="9"/>
+      <c r="C289" s="9"/>
+      <c r="D289" s="9"/>
+      <c r="E289" s="9"/>
+      <c r="F289" s="9"/>
+      <c r="G289" s="9"/>
+      <c r="H289" s="9"/>
+      <c r="I289" s="9"/>
+      <c r="J289" s="9"/>
+      <c r="K289" s="9"/>
+      <c r="L289" s="9"/>
+      <c r="M289" s="9"/>
+      <c r="N289" s="9"/>
+      <c r="O289" s="9"/>
+      <c r="P289" s="9"/>
+      <c r="Q289" s="9"/>
+      <c r="R289" s="9"/>
+      <c r="S289" s="17"/>
+      <c r="T289" s="9"/>
+    </row>
+    <row r="290" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A290" s="9"/>
+      <c r="B290" s="9"/>
+      <c r="C290" s="9"/>
+      <c r="D290" s="9"/>
+      <c r="E290" s="9"/>
+      <c r="F290" s="9"/>
+      <c r="G290" s="9"/>
+      <c r="H290" s="9"/>
+      <c r="I290" s="9"/>
+      <c r="J290" s="9"/>
+      <c r="K290" s="9"/>
+      <c r="L290" s="9"/>
+      <c r="M290" s="9"/>
+      <c r="N290" s="9"/>
+      <c r="O290" s="9"/>
+      <c r="P290" s="9"/>
+      <c r="Q290" s="9"/>
+      <c r="R290" s="9"/>
+      <c r="S290" s="17"/>
+      <c r="T290" s="9"/>
+    </row>
+    <row r="291" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A291" s="9"/>
+      <c r="B291" s="9"/>
+      <c r="C291" s="9"/>
+      <c r="D291" s="9"/>
+      <c r="E291" s="9"/>
+      <c r="F291" s="9"/>
+      <c r="G291" s="9"/>
+      <c r="H291" s="9"/>
+      <c r="I291" s="9"/>
+      <c r="J291" s="9"/>
+      <c r="K291" s="9"/>
+      <c r="L291" s="9"/>
+      <c r="M291" s="9"/>
+      <c r="N291" s="9"/>
+      <c r="O291" s="9"/>
+      <c r="P291" s="9"/>
+      <c r="Q291" s="9"/>
+      <c r="R291" s="9"/>
+      <c r="S291" s="17"/>
+      <c r="T291" s="9"/>
+    </row>
+    <row r="292" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A292" s="9"/>
+      <c r="B292" s="9"/>
+      <c r="C292" s="9"/>
+      <c r="D292" s="9"/>
+      <c r="E292" s="9"/>
+      <c r="F292" s="9"/>
+      <c r="G292" s="9"/>
+      <c r="H292" s="9"/>
+      <c r="I292" s="9"/>
+      <c r="J292" s="9"/>
+      <c r="K292" s="9"/>
+      <c r="L292" s="9"/>
+      <c r="M292" s="9"/>
+      <c r="N292" s="9"/>
+      <c r="O292" s="9"/>
+      <c r="P292" s="9"/>
+      <c r="Q292" s="9"/>
+      <c r="R292" s="9"/>
+      <c r="S292" s="17"/>
+      <c r="T292" s="9"/>
+    </row>
+    <row r="293" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A293" s="9"/>
+      <c r="B293" s="9"/>
+      <c r="C293" s="9"/>
+      <c r="D293" s="9"/>
+      <c r="E293" s="9"/>
+      <c r="F293" s="9"/>
+      <c r="G293" s="9"/>
+      <c r="H293" s="9"/>
+      <c r="I293" s="9"/>
+      <c r="J293" s="9"/>
+      <c r="K293" s="9"/>
+      <c r="L293" s="9"/>
+      <c r="M293" s="9"/>
+      <c r="N293" s="9"/>
+      <c r="O293" s="9"/>
+      <c r="P293" s="9"/>
+      <c r="Q293" s="9"/>
+      <c r="R293" s="9"/>
+      <c r="S293" s="17"/>
+      <c r="T293" s="9"/>
+    </row>
+    <row r="294" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A294" s="9"/>
+      <c r="B294" s="9"/>
+      <c r="C294" s="9"/>
+      <c r="D294" s="9"/>
+      <c r="E294" s="9"/>
+      <c r="F294" s="9"/>
+      <c r="G294" s="9"/>
+      <c r="H294" s="9"/>
+      <c r="I294" s="9"/>
+      <c r="J294" s="9"/>
+      <c r="K294" s="9"/>
+      <c r="L294" s="9"/>
+      <c r="M294" s="9"/>
+      <c r="N294" s="9"/>
+      <c r="O294" s="9"/>
+      <c r="P294" s="9"/>
+      <c r="Q294" s="9"/>
+      <c r="R294" s="9"/>
+      <c r="S294" s="17"/>
+      <c r="T294" s="9"/>
+    </row>
+    <row r="295" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A295" s="9"/>
+      <c r="B295" s="9"/>
+      <c r="C295" s="9"/>
+      <c r="D295" s="9"/>
+      <c r="E295" s="9"/>
+      <c r="F295" s="9"/>
+      <c r="G295" s="9"/>
+      <c r="H295" s="9"/>
+      <c r="I295" s="9"/>
+      <c r="J295" s="9"/>
+      <c r="K295" s="9"/>
+      <c r="L295" s="9"/>
+      <c r="M295" s="9"/>
+      <c r="N295" s="9"/>
+      <c r="O295" s="9"/>
+      <c r="P295" s="9"/>
+      <c r="Q295" s="9"/>
+      <c r="R295" s="9"/>
+      <c r="S295" s="17"/>
+      <c r="T295" s="9"/>
+    </row>
+    <row r="296" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A296" s="9"/>
+      <c r="B296" s="9"/>
+      <c r="C296" s="9"/>
+      <c r="D296" s="9"/>
+      <c r="E296" s="9"/>
+      <c r="F296" s="9"/>
+      <c r="G296" s="9"/>
+      <c r="H296" s="9"/>
+      <c r="I296" s="9"/>
+      <c r="J296" s="9"/>
+      <c r="K296" s="9"/>
+      <c r="L296" s="9"/>
+      <c r="M296" s="9"/>
+      <c r="N296" s="9"/>
+      <c r="O296" s="9"/>
+      <c r="P296" s="9"/>
+      <c r="Q296" s="9"/>
+      <c r="R296" s="9"/>
+      <c r="S296" s="17"/>
+      <c r="T296" s="9"/>
+    </row>
+    <row r="297" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A297" s="9"/>
+      <c r="B297" s="9"/>
+      <c r="C297" s="9"/>
+      <c r="D297" s="9"/>
+      <c r="E297" s="9"/>
+      <c r="F297" s="9"/>
+      <c r="G297" s="9"/>
+      <c r="H297" s="9"/>
+      <c r="I297" s="9"/>
+      <c r="J297" s="9"/>
+      <c r="K297" s="9"/>
+      <c r="L297" s="9"/>
+      <c r="M297" s="9"/>
+      <c r="N297" s="9"/>
+      <c r="O297" s="9"/>
+      <c r="P297" s="9"/>
+      <c r="Q297" s="9"/>
+      <c r="R297" s="9"/>
+      <c r="S297" s="17"/>
+      <c r="T297" s="9"/>
+    </row>
+    <row r="298" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A298" s="9"/>
+      <c r="B298" s="9"/>
+      <c r="C298" s="9"/>
+      <c r="D298" s="9"/>
+      <c r="E298" s="9"/>
+      <c r="F298" s="9"/>
+      <c r="G298" s="9"/>
+      <c r="H298" s="9"/>
+      <c r="I298" s="9"/>
+      <c r="J298" s="9"/>
+      <c r="K298" s="9"/>
+      <c r="L298" s="9"/>
+      <c r="M298" s="9"/>
+      <c r="N298" s="9"/>
+      <c r="O298" s="9"/>
+      <c r="P298" s="9"/>
+      <c r="Q298" s="9"/>
+      <c r="R298" s="9"/>
+      <c r="S298" s="17"/>
+      <c r="T298" s="9"/>
+    </row>
+    <row r="299" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A299" s="9"/>
+      <c r="B299" s="9"/>
+      <c r="C299" s="9"/>
+      <c r="D299" s="9"/>
+      <c r="E299" s="9"/>
+      <c r="F299" s="9"/>
+      <c r="G299" s="9"/>
+      <c r="H299" s="9"/>
+      <c r="I299" s="9"/>
+      <c r="J299" s="9"/>
+      <c r="K299" s="9"/>
+      <c r="L299" s="9"/>
+      <c r="M299" s="9"/>
+      <c r="N299" s="9"/>
+      <c r="O299" s="9"/>
+      <c r="P299" s="9"/>
+      <c r="Q299" s="9"/>
+      <c r="R299" s="9"/>
+      <c r="S299" s="17"/>
+      <c r="T299" s="9"/>
+    </row>
+    <row r="300" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A300" s="9"/>
+      <c r="B300" s="9"/>
+      <c r="C300" s="9"/>
+      <c r="D300" s="9"/>
+      <c r="E300" s="9"/>
+      <c r="F300" s="9"/>
+      <c r="G300" s="9"/>
+      <c r="H300" s="9"/>
+      <c r="I300" s="9"/>
+      <c r="J300" s="9"/>
+      <c r="K300" s="9"/>
+      <c r="L300" s="9"/>
+      <c r="M300" s="9"/>
+      <c r="N300" s="9"/>
+      <c r="O300" s="9"/>
+      <c r="P300" s="9"/>
+      <c r="Q300" s="9"/>
+      <c r="R300" s="9"/>
+      <c r="S300" s="17"/>
+      <c r="T300" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated to 2024-07-09.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4598" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4638" uniqueCount="986">
   <si>
     <t>Format</t>
   </si>
@@ -2975,6 +2975,30 @@
   </si>
   <si>
     <t>Building and Delivering Microservices on AWS</t>
+  </si>
+  <si>
+    <t>2024-07-09</t>
+  </si>
+  <si>
+    <t>Useful. A soup of different topics as every Packt book, but it contains some actionable bits of knowledge.</t>
+  </si>
+  <si>
+    <t>Better Python Code</t>
+  </si>
+  <si>
+    <t>Useless. For the author of this book, writing "better" code is often equal to write terse and less readable code, just because according to him, it's more "pythonic" that way - i.e. enumerate() instead of for...range(len()).</t>
+  </si>
+  <si>
+    <t>The Art of Leadership: Small Things, Done Well</t>
+  </si>
+  <si>
+    <t>Useful. It contains soem good advices, but it's a very wordy and painful-to-read book. Its readability could be massively improved by adopting a recipe book layout and cut 4/5 of the content. If I want to read a novel, I buy a novel.</t>
+  </si>
+  <si>
+    <t>Think One Team</t>
+  </si>
+  <si>
+    <t>Useless. Very wordy and repetitive, the exact same content coulkd have been expressed in 50 pages. It contains very idealistic and unrealistic advices that purposely ignore human nature.</t>
   </si>
 </sst>
 </file>
@@ -10822,7 +10846,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A284" sqref="A284"/>
+      <selection pane="bottomLeft" activeCell="A287" sqref="A287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -25852,7 +25876,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S282" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S286" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -28746,7 +28770,7 @@
         <v>2024</v>
       </c>
       <c r="I276" s="9">
-        <f>MONTH(G276)</f>
+        <f t="shared" ref="I276:I282" si="59">MONTH(G276)</f>
         <v>5</v>
       </c>
       <c r="J276" s="9" t="s">
@@ -28811,7 +28835,7 @@
         <v>2024</v>
       </c>
       <c r="I277" s="9">
-        <f>MONTH(G277)</f>
+        <f t="shared" si="59"/>
         <v>5</v>
       </c>
       <c r="J277" s="9" t="s">
@@ -28876,7 +28900,7 @@
         <v>2024</v>
       </c>
       <c r="I278" s="9">
-        <f>MONTH(G278)</f>
+        <f t="shared" si="59"/>
         <v>6</v>
       </c>
       <c r="J278" s="9" t="s">
@@ -28937,11 +28961,11 @@
         <v>965</v>
       </c>
       <c r="H279" s="9">
-        <f t="shared" ref="H279" si="59">YEAR(G279)</f>
+        <f t="shared" ref="H279" si="60">YEAR(G279)</f>
         <v>2024</v>
       </c>
       <c r="I279" s="9">
-        <f>MONTH(G279)</f>
+        <f t="shared" si="59"/>
         <v>6</v>
       </c>
       <c r="J279" s="9" t="s">
@@ -29002,11 +29026,11 @@
         <v>965</v>
       </c>
       <c r="H280" s="9">
-        <f t="shared" ref="H280:H282" si="60">YEAR(G280)</f>
+        <f t="shared" ref="H280:H282" si="61">YEAR(G280)</f>
         <v>2024</v>
       </c>
       <c r="I280" s="9">
-        <f>MONTH(G280)</f>
+        <f t="shared" si="59"/>
         <v>6</v>
       </c>
       <c r="J280" s="9" t="s">
@@ -29067,11 +29091,11 @@
         <v>972</v>
       </c>
       <c r="H281" s="9">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>2024</v>
       </c>
       <c r="I281" s="9">
-        <f>MONTH(G281)</f>
+        <f t="shared" si="59"/>
         <v>6</v>
       </c>
       <c r="J281" s="9" t="s">
@@ -29132,11 +29156,11 @@
         <v>975</v>
       </c>
       <c r="H282" s="9">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>2024</v>
       </c>
       <c r="I282" s="9">
-        <f>MONTH(G282)</f>
+        <f t="shared" si="59"/>
         <v>7</v>
       </c>
       <c r="J282" s="9" t="s">
@@ -29193,96 +29217,246 @@
       <c r="F283" s="17">
         <v>600</v>
       </c>
-      <c r="G283" s="9"/>
-      <c r="H283" s="9"/>
-      <c r="I283" s="9"/>
-      <c r="J283" s="9"/>
-      <c r="K283" s="9"/>
+      <c r="G283" s="9" t="s">
+        <v>978</v>
+      </c>
+      <c r="H283" s="9">
+        <f t="shared" ref="H283" si="62">YEAR(G283)</f>
+        <v>2024</v>
+      </c>
+      <c r="I283" s="9">
+        <f t="shared" ref="I283" si="63">MONTH(G283)</f>
+        <v>7</v>
+      </c>
+      <c r="J283" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K283" s="9" t="s">
+        <v>159</v>
+      </c>
       <c r="L283" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="M283" s="9"/>
+      <c r="M283" s="17">
+        <v>2</v>
+      </c>
       <c r="N283" s="17">
         <v>43.13</v>
       </c>
       <c r="O283" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P283" s="13"/>
+      <c r="P283" s="13" t="s">
+        <v>979</v>
+      </c>
       <c r="Q283" s="9" t="s">
         <v>469</v>
       </c>
       <c r="R283" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="S283" s="17"/>
-      <c r="T283" s="9"/>
+      <c r="S283" s="17">
+        <f t="shared" si="32"/>
+        <v>106</v>
+      </c>
+      <c r="T283" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="284" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A284" s="13"/>
-      <c r="B284" s="9"/>
-      <c r="C284" s="9"/>
-      <c r="D284" s="9"/>
-      <c r="E284" s="9"/>
-      <c r="F284" s="9"/>
-      <c r="G284" s="9"/>
-      <c r="H284" s="9"/>
-      <c r="I284" s="9"/>
-      <c r="J284" s="9"/>
-      <c r="K284" s="9"/>
-      <c r="L284" s="9"/>
-      <c r="M284" s="9"/>
-      <c r="N284" s="9"/>
-      <c r="O284" s="9"/>
-      <c r="P284" s="13"/>
-      <c r="Q284" s="9"/>
-      <c r="R284" s="9"/>
-      <c r="S284" s="17"/>
-      <c r="T284" s="9"/>
+      <c r="A284" s="13" t="s">
+        <v>980</v>
+      </c>
+      <c r="B284" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C284" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D284" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E284" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F284" s="17">
+        <v>289</v>
+      </c>
+      <c r="G284" s="9" t="s">
+        <v>978</v>
+      </c>
+      <c r="H284" s="9">
+        <f t="shared" ref="H284" si="64">YEAR(G284)</f>
+        <v>2024</v>
+      </c>
+      <c r="I284" s="9">
+        <f t="shared" ref="I284" si="65">MONTH(G284)</f>
+        <v>7</v>
+      </c>
+      <c r="J284" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K284" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L284" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="M284" s="17">
+        <v>1</v>
+      </c>
+      <c r="N284" s="17">
+        <v>49.71</v>
+      </c>
+      <c r="O284" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P284" s="13" t="s">
+        <v>981</v>
+      </c>
+      <c r="Q284" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R284" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S284" s="17">
+        <f t="shared" si="32"/>
+        <v>224</v>
+      </c>
+      <c r="T284" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="285" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A285" s="13"/>
-      <c r="B285" s="9"/>
-      <c r="C285" s="9"/>
-      <c r="D285" s="9"/>
-      <c r="E285" s="9"/>
-      <c r="F285" s="9"/>
-      <c r="G285" s="9"/>
-      <c r="H285" s="9"/>
-      <c r="I285" s="9"/>
-      <c r="J285" s="9"/>
-      <c r="K285" s="9"/>
-      <c r="L285" s="9"/>
-      <c r="M285" s="9"/>
-      <c r="N285" s="9"/>
-      <c r="O285" s="9"/>
-      <c r="P285" s="13"/>
-      <c r="Q285" s="9"/>
-      <c r="R285" s="9"/>
-      <c r="S285" s="17"/>
-      <c r="T285" s="9"/>
+      <c r="A285" s="13" t="s">
+        <v>982</v>
+      </c>
+      <c r="B285" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C285" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D285" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E285" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F285" s="17">
+        <v>198</v>
+      </c>
+      <c r="G285" s="9" t="s">
+        <v>978</v>
+      </c>
+      <c r="H285" s="9">
+        <f t="shared" ref="H285" si="66">YEAR(G285)</f>
+        <v>2024</v>
+      </c>
+      <c r="I285" s="9">
+        <f t="shared" ref="I285" si="67">MONTH(G285)</f>
+        <v>7</v>
+      </c>
+      <c r="J285" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K285" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L285" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M285" s="17">
+        <v>2</v>
+      </c>
+      <c r="N285" s="17">
+        <v>22.94</v>
+      </c>
+      <c r="O285" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P285" s="16" t="s">
+        <v>983</v>
+      </c>
+      <c r="Q285" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R285" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S285" s="17">
+        <f t="shared" si="32"/>
+        <v>233</v>
+      </c>
+      <c r="T285" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="286" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A286" s="13"/>
-      <c r="B286" s="9"/>
-      <c r="C286" s="9"/>
-      <c r="D286" s="9"/>
-      <c r="E286" s="9"/>
-      <c r="F286" s="9"/>
-      <c r="G286" s="9"/>
-      <c r="H286" s="9"/>
-      <c r="I286" s="9"/>
-      <c r="J286" s="9"/>
-      <c r="K286" s="9"/>
-      <c r="L286" s="9"/>
-      <c r="M286" s="9"/>
-      <c r="N286" s="9"/>
-      <c r="O286" s="9"/>
-      <c r="P286" s="13"/>
-      <c r="Q286" s="9"/>
-      <c r="R286" s="9"/>
-      <c r="S286" s="17"/>
-      <c r="T286" s="9"/>
+      <c r="A286" s="13" t="s">
+        <v>984</v>
+      </c>
+      <c r="B286" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C286" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D286" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E286" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F286" s="17">
+        <v>224</v>
+      </c>
+      <c r="G286" s="9" t="s">
+        <v>978</v>
+      </c>
+      <c r="H286" s="9">
+        <f t="shared" ref="H286" si="68">YEAR(G286)</f>
+        <v>2024</v>
+      </c>
+      <c r="I286" s="9">
+        <f t="shared" ref="I286" si="69">MONTH(G286)</f>
+        <v>7</v>
+      </c>
+      <c r="J286" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K286" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L286" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="M286" s="17">
+        <v>1</v>
+      </c>
+      <c r="N286" s="17">
+        <v>16.690000000000001</v>
+      </c>
+      <c r="O286" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P286" s="16" t="s">
+        <v>985</v>
+      </c>
+      <c r="Q286" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R286" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S286" s="17">
+        <f t="shared" si="32"/>
+        <v>186</v>
+      </c>
+      <c r="T286" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A287" s="13"/>
@@ -29300,7 +29474,7 @@
       <c r="M287" s="9"/>
       <c r="N287" s="9"/>
       <c r="O287" s="9"/>
-      <c r="P287" s="13"/>
+      <c r="P287" s="16"/>
       <c r="Q287" s="9"/>
       <c r="R287" s="9"/>
       <c r="S287" s="17"/>
@@ -29322,7 +29496,7 @@
       <c r="M288" s="9"/>
       <c r="N288" s="9"/>
       <c r="O288" s="9"/>
-      <c r="P288" s="13"/>
+      <c r="P288" s="16"/>
       <c r="Q288" s="9"/>
       <c r="R288" s="9"/>
       <c r="S288" s="17"/>
@@ -29344,7 +29518,7 @@
       <c r="M289" s="9"/>
       <c r="N289" s="9"/>
       <c r="O289" s="9"/>
-      <c r="P289" s="9"/>
+      <c r="P289" s="16"/>
       <c r="Q289" s="9"/>
       <c r="R289" s="9"/>
       <c r="S289" s="17"/>
@@ -29366,7 +29540,7 @@
       <c r="M290" s="9"/>
       <c r="N290" s="9"/>
       <c r="O290" s="9"/>
-      <c r="P290" s="9"/>
+      <c r="P290" s="16"/>
       <c r="Q290" s="9"/>
       <c r="R290" s="9"/>
       <c r="S290" s="17"/>
@@ -29388,7 +29562,7 @@
       <c r="M291" s="9"/>
       <c r="N291" s="9"/>
       <c r="O291" s="9"/>
-      <c r="P291" s="9"/>
+      <c r="P291" s="16"/>
       <c r="Q291" s="9"/>
       <c r="R291" s="9"/>
       <c r="S291" s="17"/>
@@ -29410,7 +29584,7 @@
       <c r="M292" s="9"/>
       <c r="N292" s="9"/>
       <c r="O292" s="9"/>
-      <c r="P292" s="9"/>
+      <c r="P292" s="16"/>
       <c r="Q292" s="9"/>
       <c r="R292" s="9"/>
       <c r="S292" s="17"/>
@@ -29432,7 +29606,7 @@
       <c r="M293" s="9"/>
       <c r="N293" s="9"/>
       <c r="O293" s="9"/>
-      <c r="P293" s="9"/>
+      <c r="P293" s="16"/>
       <c r="Q293" s="9"/>
       <c r="R293" s="9"/>
       <c r="S293" s="17"/>
@@ -29454,7 +29628,7 @@
       <c r="M294" s="9"/>
       <c r="N294" s="9"/>
       <c r="O294" s="9"/>
-      <c r="P294" s="9"/>
+      <c r="P294" s="16"/>
       <c r="Q294" s="9"/>
       <c r="R294" s="9"/>
       <c r="S294" s="17"/>
@@ -29476,7 +29650,7 @@
       <c r="M295" s="9"/>
       <c r="N295" s="9"/>
       <c r="O295" s="9"/>
-      <c r="P295" s="9"/>
+      <c r="P295" s="16"/>
       <c r="Q295" s="9"/>
       <c r="R295" s="9"/>
       <c r="S295" s="17"/>
@@ -29498,7 +29672,7 @@
       <c r="M296" s="9"/>
       <c r="N296" s="9"/>
       <c r="O296" s="9"/>
-      <c r="P296" s="9"/>
+      <c r="P296" s="16"/>
       <c r="Q296" s="9"/>
       <c r="R296" s="9"/>
       <c r="S296" s="17"/>
@@ -29520,7 +29694,7 @@
       <c r="M297" s="9"/>
       <c r="N297" s="9"/>
       <c r="O297" s="9"/>
-      <c r="P297" s="9"/>
+      <c r="P297" s="16"/>
       <c r="Q297" s="9"/>
       <c r="R297" s="9"/>
       <c r="S297" s="17"/>
@@ -29542,7 +29716,7 @@
       <c r="M298" s="9"/>
       <c r="N298" s="9"/>
       <c r="O298" s="9"/>
-      <c r="P298" s="9"/>
+      <c r="P298" s="16"/>
       <c r="Q298" s="9"/>
       <c r="R298" s="9"/>
       <c r="S298" s="17"/>
@@ -29564,7 +29738,7 @@
       <c r="M299" s="9"/>
       <c r="N299" s="9"/>
       <c r="O299" s="9"/>
-      <c r="P299" s="9"/>
+      <c r="P299" s="16"/>
       <c r="Q299" s="9"/>
       <c r="R299" s="9"/>
       <c r="S299" s="17"/>
@@ -29586,7 +29760,7 @@
       <c r="M300" s="9"/>
       <c r="N300" s="9"/>
       <c r="O300" s="9"/>
-      <c r="P300" s="9"/>
+      <c r="P300" s="16"/>
       <c r="Q300" s="9"/>
       <c r="R300" s="9"/>
       <c r="S300" s="17"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated to 2024-07-13.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4638" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4698" uniqueCount="998">
   <si>
     <t>Format</t>
   </si>
@@ -2999,6 +2999,42 @@
   </si>
   <si>
     <t>Useless. Very wordy and repetitive, the exact same content coulkd have been expressed in 50 pages. It contains very idealistic and unrealistic advices that purposely ignore human nature.</t>
+  </si>
+  <si>
+    <t>Product Management In Practice (2nd Edition)</t>
+  </si>
+  <si>
+    <t>2024-07-11</t>
+  </si>
+  <si>
+    <t>Useful. Well written but very wordy, the exact same content could have been expressed in 50 pages.</t>
+  </si>
+  <si>
+    <t>Software Requirements Essentials</t>
+  </si>
+  <si>
+    <t>2024-07-13</t>
+  </si>
+  <si>
+    <t>Useful. A valid book for beginners in product management.</t>
+  </si>
+  <si>
+    <t>Senior Engineer Mindset</t>
+  </si>
+  <si>
+    <t>Nordic APIs</t>
+  </si>
+  <si>
+    <t>Useful. Nothing new, but a good summary written in a straight-to-the-point language.</t>
+  </si>
+  <si>
+    <t>The Art of Crafting User Stories</t>
+  </si>
+  <si>
+    <t>Useless. It's well written, but it's very repetitive. The same content could have been written in 1/3 of the pages. Packt's book lack of proper editing.</t>
+  </si>
+  <si>
+    <t>Developing the API Mindset</t>
   </si>
 </sst>
 </file>
@@ -10845,8 +10881,8 @@
   <dimension ref="A1:T300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A287" sqref="A287"/>
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A292" sqref="A292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -28975,7 +29011,7 @@
         <v>159</v>
       </c>
       <c r="L279" s="9" t="s">
-        <v>602</v>
+        <v>993</v>
       </c>
       <c r="M279" s="17">
         <v>3</v>
@@ -29459,117 +29495,332 @@
       </c>
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A287" s="13"/>
-      <c r="B287" s="9"/>
-      <c r="C287" s="9"/>
-      <c r="D287" s="9"/>
-      <c r="E287" s="9"/>
-      <c r="F287" s="9"/>
-      <c r="G287" s="9"/>
-      <c r="H287" s="9"/>
-      <c r="I287" s="9"/>
-      <c r="J287" s="9"/>
-      <c r="K287" s="9"/>
-      <c r="L287" s="9"/>
-      <c r="M287" s="9"/>
-      <c r="N287" s="9"/>
-      <c r="O287" s="9"/>
-      <c r="P287" s="16"/>
-      <c r="Q287" s="9"/>
-      <c r="R287" s="9"/>
-      <c r="S287" s="17"/>
-      <c r="T287" s="9"/>
+      <c r="A287" s="13" t="s">
+        <v>986</v>
+      </c>
+      <c r="B287" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C287" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D287" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E287" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F287" s="17">
+        <v>296</v>
+      </c>
+      <c r="G287" s="9" t="s">
+        <v>987</v>
+      </c>
+      <c r="H287" s="9">
+        <f t="shared" ref="H287" si="70">YEAR(G287)</f>
+        <v>2024</v>
+      </c>
+      <c r="I287" s="9">
+        <f t="shared" ref="I287" si="71">MONTH(G287)</f>
+        <v>7</v>
+      </c>
+      <c r="J287" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K287" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L287" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M287" s="17">
+        <v>3</v>
+      </c>
+      <c r="N287" s="17">
+        <v>31.99</v>
+      </c>
+      <c r="O287" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P287" s="16" t="s">
+        <v>988</v>
+      </c>
+      <c r="Q287" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R287" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S287" s="17">
+        <f t="shared" ref="S287" si="72">LEN(P287)</f>
+        <v>98</v>
+      </c>
+      <c r="T287" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="288" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A288" s="13"/>
-      <c r="B288" s="9"/>
-      <c r="C288" s="9"/>
-      <c r="D288" s="9"/>
-      <c r="E288" s="9"/>
-      <c r="F288" s="9"/>
-      <c r="G288" s="9"/>
-      <c r="H288" s="9"/>
-      <c r="I288" s="9"/>
-      <c r="J288" s="9"/>
-      <c r="K288" s="9"/>
-      <c r="L288" s="9"/>
-      <c r="M288" s="9"/>
-      <c r="N288" s="9"/>
-      <c r="O288" s="9"/>
-      <c r="P288" s="16"/>
-      <c r="Q288" s="9"/>
-      <c r="R288" s="9"/>
-      <c r="S288" s="17"/>
-      <c r="T288" s="9"/>
+      <c r="A288" s="13" t="s">
+        <v>989</v>
+      </c>
+      <c r="B288" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C288" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D288" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E288" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F288" s="17">
+        <v>200</v>
+      </c>
+      <c r="G288" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="H288" s="9">
+        <f t="shared" ref="H288" si="73">YEAR(G288)</f>
+        <v>2024</v>
+      </c>
+      <c r="I288" s="9">
+        <f t="shared" ref="I288" si="74">MONTH(G288)</f>
+        <v>7</v>
+      </c>
+      <c r="J288" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K288" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L288" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="M288" s="17">
+        <v>3</v>
+      </c>
+      <c r="N288" s="17">
+        <v>27.99</v>
+      </c>
+      <c r="O288" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P288" s="16" t="s">
+        <v>991</v>
+      </c>
+      <c r="Q288" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R288" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S288" s="17">
+        <f t="shared" ref="S288:S289" si="75">LEN(P288)</f>
+        <v>57</v>
+      </c>
+      <c r="T288" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="289" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A289" s="9"/>
-      <c r="B289" s="9"/>
-      <c r="C289" s="9"/>
-      <c r="D289" s="9"/>
-      <c r="E289" s="9"/>
-      <c r="F289" s="9"/>
-      <c r="G289" s="9"/>
-      <c r="H289" s="9"/>
-      <c r="I289" s="9"/>
-      <c r="J289" s="9"/>
-      <c r="K289" s="9"/>
-      <c r="L289" s="9"/>
-      <c r="M289" s="9"/>
-      <c r="N289" s="9"/>
-      <c r="O289" s="9"/>
-      <c r="P289" s="16"/>
-      <c r="Q289" s="9"/>
-      <c r="R289" s="9"/>
-      <c r="S289" s="17"/>
-      <c r="T289" s="9"/>
+      <c r="A289" s="13" t="s">
+        <v>992</v>
+      </c>
+      <c r="B289" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C289" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D289" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E289" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F289" s="17">
+        <v>255</v>
+      </c>
+      <c r="G289" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="H289" s="9">
+        <f t="shared" ref="H289" si="76">YEAR(G289)</f>
+        <v>2024</v>
+      </c>
+      <c r="I289" s="9">
+        <f t="shared" ref="I289" si="77">MONTH(G289)</f>
+        <v>7</v>
+      </c>
+      <c r="J289" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K289" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L289" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M289" s="17">
+        <v>3</v>
+      </c>
+      <c r="N289" s="43">
+        <v>49</v>
+      </c>
+      <c r="O289" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P289" s="16" t="s">
+        <v>994</v>
+      </c>
+      <c r="Q289" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R289" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S289" s="17">
+        <f t="shared" ref="S289" si="78">LEN(P289)</f>
+        <v>84</v>
+      </c>
+      <c r="T289" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="290" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A290" s="9"/>
-      <c r="B290" s="9"/>
-      <c r="C290" s="9"/>
-      <c r="D290" s="9"/>
-      <c r="E290" s="9"/>
-      <c r="F290" s="9"/>
-      <c r="G290" s="9"/>
-      <c r="H290" s="9"/>
-      <c r="I290" s="9"/>
-      <c r="J290" s="9"/>
-      <c r="K290" s="9"/>
-      <c r="L290" s="9"/>
-      <c r="M290" s="9"/>
-      <c r="N290" s="9"/>
-      <c r="O290" s="9"/>
-      <c r="P290" s="16"/>
-      <c r="Q290" s="9"/>
-      <c r="R290" s="9"/>
-      <c r="S290" s="17"/>
-      <c r="T290" s="9"/>
+      <c r="A290" s="13" t="s">
+        <v>995</v>
+      </c>
+      <c r="B290" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C290" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D290" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E290" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F290" s="17">
+        <v>192</v>
+      </c>
+      <c r="G290" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="H290" s="9">
+        <f t="shared" ref="H290" si="79">YEAR(G290)</f>
+        <v>2024</v>
+      </c>
+      <c r="I290" s="9">
+        <f t="shared" ref="I290" si="80">MONTH(G290)</f>
+        <v>7</v>
+      </c>
+      <c r="J290" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K290" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L290" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M290" s="17">
+        <v>2</v>
+      </c>
+      <c r="N290" s="17">
+        <v>26.01</v>
+      </c>
+      <c r="O290" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P290" s="16" t="s">
+        <v>996</v>
+      </c>
+      <c r="Q290" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R290" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S290" s="17">
+        <f t="shared" ref="S290:S291" si="81">LEN(P290)</f>
+        <v>152</v>
+      </c>
+      <c r="T290" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="291" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A291" s="9"/>
-      <c r="B291" s="9"/>
-      <c r="C291" s="9"/>
-      <c r="D291" s="9"/>
-      <c r="E291" s="9"/>
-      <c r="F291" s="9"/>
-      <c r="G291" s="9"/>
-      <c r="H291" s="9"/>
-      <c r="I291" s="9"/>
-      <c r="J291" s="9"/>
-      <c r="K291" s="9"/>
-      <c r="L291" s="9"/>
-      <c r="M291" s="9"/>
-      <c r="N291" s="9"/>
-      <c r="O291" s="9"/>
-      <c r="P291" s="16"/>
-      <c r="Q291" s="9"/>
-      <c r="R291" s="9"/>
-      <c r="S291" s="17"/>
-      <c r="T291" s="9"/>
+      <c r="A291" s="13" t="s">
+        <v>997</v>
+      </c>
+      <c r="B291" s="17">
+        <v>2015</v>
+      </c>
+      <c r="C291" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D291" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E291" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F291" s="17">
+        <v>96</v>
+      </c>
+      <c r="G291" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="H291" s="9">
+        <f t="shared" ref="H291" si="82">YEAR(G291)</f>
+        <v>2024</v>
+      </c>
+      <c r="I291" s="9">
+        <f t="shared" ref="I291" si="83">MONTH(G291)</f>
+        <v>7</v>
+      </c>
+      <c r="J291" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K291" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L291" s="9" t="s">
+        <v>993</v>
+      </c>
+      <c r="M291" s="17">
+        <v>3</v>
+      </c>
+      <c r="N291" s="43">
+        <v>0</v>
+      </c>
+      <c r="O291" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P291" s="28" t="s">
+        <v>707</v>
+      </c>
+      <c r="Q291" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R291" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S291" s="17">
+        <f t="shared" si="81"/>
+        <v>26</v>
+      </c>
+      <c r="T291" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="292" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A292" s="9"/>
+      <c r="A292" s="13"/>
       <c r="B292" s="9"/>
       <c r="C292" s="9"/>
       <c r="D292" s="9"/>
@@ -29591,7 +29842,7 @@
       <c r="T292" s="9"/>
     </row>
     <row r="293" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A293" s="9"/>
+      <c r="A293" s="13"/>
       <c r="B293" s="9"/>
       <c r="C293" s="9"/>
       <c r="D293" s="9"/>
@@ -29613,7 +29864,7 @@
       <c r="T293" s="9"/>
     </row>
     <row r="294" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A294" s="9"/>
+      <c r="A294" s="13"/>
       <c r="B294" s="9"/>
       <c r="C294" s="9"/>
       <c r="D294" s="9"/>
@@ -29635,7 +29886,7 @@
       <c r="T294" s="9"/>
     </row>
     <row r="295" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A295" s="9"/>
+      <c r="A295" s="13"/>
       <c r="B295" s="9"/>
       <c r="C295" s="9"/>
       <c r="D295" s="9"/>
@@ -29657,7 +29908,7 @@
       <c r="T295" s="9"/>
     </row>
     <row r="296" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A296" s="9"/>
+      <c r="A296" s="13"/>
       <c r="B296" s="9"/>
       <c r="C296" s="9"/>
       <c r="D296" s="9"/>
@@ -29679,7 +29930,7 @@
       <c r="T296" s="9"/>
     </row>
     <row r="297" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A297" s="9"/>
+      <c r="A297" s="13"/>
       <c r="B297" s="9"/>
       <c r="C297" s="9"/>
       <c r="D297" s="9"/>
@@ -29701,7 +29952,7 @@
       <c r="T297" s="9"/>
     </row>
     <row r="298" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A298" s="9"/>
+      <c r="A298" s="13"/>
       <c r="B298" s="9"/>
       <c r="C298" s="9"/>
       <c r="D298" s="9"/>
@@ -29723,7 +29974,7 @@
       <c r="T298" s="9"/>
     </row>
     <row r="299" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A299" s="9"/>
+      <c r="A299" s="13"/>
       <c r="B299" s="9"/>
       <c r="C299" s="9"/>
       <c r="D299" s="9"/>
@@ -29745,7 +29996,7 @@
       <c r="T299" s="9"/>
     </row>
     <row r="300" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A300" s="9"/>
+      <c r="A300" s="13"/>
       <c r="B300" s="9"/>
       <c r="C300" s="9"/>
       <c r="D300" s="9"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated to 2024-07-19.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4698" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="1014">
   <si>
     <t>Format</t>
   </si>
@@ -3035,6 +3035,54 @@
   </si>
   <si>
     <t>Developing the API Mindset</t>
+  </si>
+  <si>
+    <t>How To Successfully Market an API</t>
+  </si>
+  <si>
+    <t>2024-07-14</t>
+  </si>
+  <si>
+    <t>Useful. An ok summary about the topic.</t>
+  </si>
+  <si>
+    <t>A Philosophy of Software Design</t>
+  </si>
+  <si>
+    <t>2024-07-16</t>
+  </si>
+  <si>
+    <t>Yaknyam Press</t>
+  </si>
+  <si>
+    <t>Useful. Finally an author who writes about a topic using his own words and examples, and not by copy'n'paste. It's clear that the author has plenty of experience and critical thinking, and he used both to summarize all the root causes of complexity in software design.</t>
+  </si>
+  <si>
+    <t>Expert Python Programming (4th Edition)</t>
+  </si>
+  <si>
+    <t>2024-07-17</t>
+  </si>
+  <si>
+    <t>Useful. It's repetitive and redundant, but it contains some pieces of knowledge that I didn't read in any other Python book so far.</t>
+  </si>
+  <si>
+    <t>Modern Data Architectures with Python</t>
+  </si>
+  <si>
+    <t>2024-07-18</t>
+  </si>
+  <si>
+    <t>Useless. Random showcase of different technologies without telling any story.</t>
+  </si>
+  <si>
+    <t>Cost-Effective Data Pipelines</t>
+  </si>
+  <si>
+    <t>2024-07-19</t>
+  </si>
+  <si>
+    <t>Useless. A soup of different technologies and concepts.</t>
   </si>
 </sst>
 </file>
@@ -10878,11 +10926,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T300"/>
+  <dimension ref="A1:T307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A292" sqref="A292"/>
+      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A297" sqref="A297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -29617,7 +29665,7 @@
         <v>159</v>
       </c>
       <c r="S288" s="17">
-        <f t="shared" ref="S288:S289" si="75">LEN(P288)</f>
+        <f t="shared" ref="S288" si="75">LEN(P288)</f>
         <v>57</v>
       </c>
       <c r="T288" s="14">
@@ -29747,7 +29795,7 @@
         <v>159</v>
       </c>
       <c r="S290" s="17">
-        <f t="shared" ref="S290:S291" si="81">LEN(P290)</f>
+        <f t="shared" ref="S290:S296" si="81">LEN(P290)</f>
         <v>152</v>
       </c>
       <c r="T290" s="14">
@@ -29820,114 +29868,329 @@
       </c>
     </row>
     <row r="292" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A292" s="13"/>
-      <c r="B292" s="9"/>
-      <c r="C292" s="9"/>
-      <c r="D292" s="9"/>
-      <c r="E292" s="9"/>
-      <c r="F292" s="9"/>
-      <c r="G292" s="9"/>
-      <c r="H292" s="9"/>
-      <c r="I292" s="9"/>
-      <c r="J292" s="9"/>
-      <c r="K292" s="9"/>
-      <c r="L292" s="9"/>
-      <c r="M292" s="9"/>
-      <c r="N292" s="9"/>
-      <c r="O292" s="9"/>
-      <c r="P292" s="16"/>
-      <c r="Q292" s="9"/>
-      <c r="R292" s="9"/>
-      <c r="S292" s="17"/>
-      <c r="T292" s="9"/>
+      <c r="A292" s="13" t="s">
+        <v>998</v>
+      </c>
+      <c r="B292" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C292" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D292" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E292" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F292" s="17">
+        <v>194</v>
+      </c>
+      <c r="G292" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="H292" s="9">
+        <f t="shared" ref="H292" si="84">YEAR(G292)</f>
+        <v>2024</v>
+      </c>
+      <c r="I292" s="9">
+        <f t="shared" ref="I292" si="85">MONTH(G292)</f>
+        <v>7</v>
+      </c>
+      <c r="J292" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K292" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L292" s="9" t="s">
+        <v>993</v>
+      </c>
+      <c r="M292" s="17">
+        <v>3</v>
+      </c>
+      <c r="N292" s="43">
+        <v>0</v>
+      </c>
+      <c r="O292" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P292" s="28" t="s">
+        <v>1000</v>
+      </c>
+      <c r="Q292" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R292" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S292" s="17">
+        <f t="shared" si="81"/>
+        <v>38</v>
+      </c>
+      <c r="T292" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="293" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A293" s="13"/>
-      <c r="B293" s="9"/>
-      <c r="C293" s="9"/>
-      <c r="D293" s="9"/>
-      <c r="E293" s="9"/>
-      <c r="F293" s="9"/>
-      <c r="G293" s="9"/>
-      <c r="H293" s="9"/>
-      <c r="I293" s="9"/>
-      <c r="J293" s="9"/>
-      <c r="K293" s="9"/>
-      <c r="L293" s="9"/>
-      <c r="M293" s="9"/>
-      <c r="N293" s="9"/>
-      <c r="O293" s="9"/>
-      <c r="P293" s="16"/>
-      <c r="Q293" s="9"/>
-      <c r="R293" s="9"/>
-      <c r="S293" s="17"/>
-      <c r="T293" s="9"/>
+      <c r="A293" s="13" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B293" s="17">
+        <v>2018</v>
+      </c>
+      <c r="C293" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D293" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E293" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F293" s="17">
+        <v>188</v>
+      </c>
+      <c r="G293" s="9" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H293" s="9">
+        <f t="shared" ref="H293:H295" si="86">YEAR(G293)</f>
+        <v>2024</v>
+      </c>
+      <c r="I293" s="9">
+        <f t="shared" ref="I293:I295" si="87">MONTH(G293)</f>
+        <v>7</v>
+      </c>
+      <c r="J293" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K293" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L293" s="9" t="s">
+        <v>1003</v>
+      </c>
+      <c r="M293" s="17">
+        <v>4</v>
+      </c>
+      <c r="N293" s="43">
+        <v>48</v>
+      </c>
+      <c r="O293" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P293" s="16" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Q293" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R293" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S293" s="17">
+        <f t="shared" si="81"/>
+        <v>268</v>
+      </c>
+      <c r="T293" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="294" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A294" s="13"/>
-      <c r="B294" s="9"/>
-      <c r="C294" s="9"/>
-      <c r="D294" s="9"/>
-      <c r="E294" s="9"/>
-      <c r="F294" s="9"/>
-      <c r="G294" s="9"/>
-      <c r="H294" s="9"/>
-      <c r="I294" s="9"/>
-      <c r="J294" s="9"/>
-      <c r="K294" s="9"/>
-      <c r="L294" s="9"/>
-      <c r="M294" s="9"/>
-      <c r="N294" s="9"/>
-      <c r="O294" s="9"/>
-      <c r="P294" s="16"/>
-      <c r="Q294" s="9"/>
-      <c r="R294" s="9"/>
-      <c r="S294" s="17"/>
-      <c r="T294" s="9"/>
+      <c r="A294" s="13" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B294" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C294" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D294" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E294" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F294" s="17">
+        <v>631</v>
+      </c>
+      <c r="G294" s="9" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H294" s="9">
+        <f t="shared" si="86"/>
+        <v>2024</v>
+      </c>
+      <c r="I294" s="9">
+        <f t="shared" si="87"/>
+        <v>7</v>
+      </c>
+      <c r="J294" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K294" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L294" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M294" s="17">
+        <v>3</v>
+      </c>
+      <c r="N294" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O294" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P294" s="16" t="s">
+        <v>1007</v>
+      </c>
+      <c r="Q294" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R294" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S294" s="17">
+        <f t="shared" si="81"/>
+        <v>131</v>
+      </c>
+      <c r="T294" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="295" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A295" s="13"/>
-      <c r="B295" s="9"/>
-      <c r="C295" s="9"/>
-      <c r="D295" s="9"/>
-      <c r="E295" s="9"/>
-      <c r="F295" s="9"/>
-      <c r="G295" s="9"/>
-      <c r="H295" s="9"/>
-      <c r="I295" s="9"/>
-      <c r="J295" s="9"/>
-      <c r="K295" s="9"/>
-      <c r="L295" s="9"/>
-      <c r="M295" s="9"/>
-      <c r="N295" s="9"/>
-      <c r="O295" s="9"/>
-      <c r="P295" s="16"/>
-      <c r="Q295" s="9"/>
-      <c r="R295" s="9"/>
-      <c r="S295" s="17"/>
-      <c r="T295" s="9"/>
+      <c r="A295" s="13" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B295" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C295" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D295" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E295" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F295" s="17">
+        <v>318</v>
+      </c>
+      <c r="G295" s="9" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H295" s="9">
+        <f t="shared" si="86"/>
+        <v>2024</v>
+      </c>
+      <c r="I295" s="9">
+        <f t="shared" si="87"/>
+        <v>7</v>
+      </c>
+      <c r="J295" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K295" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L295" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M295" s="17">
+        <v>1</v>
+      </c>
+      <c r="N295" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O295" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P295" s="16" t="s">
+        <v>1010</v>
+      </c>
+      <c r="Q295" s="9" t="s">
+        <v>874</v>
+      </c>
+      <c r="R295" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S295" s="17">
+        <f t="shared" si="81"/>
+        <v>77</v>
+      </c>
+      <c r="T295" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="296" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A296" s="13"/>
-      <c r="B296" s="9"/>
-      <c r="C296" s="9"/>
-      <c r="D296" s="9"/>
-      <c r="E296" s="9"/>
-      <c r="F296" s="9"/>
-      <c r="G296" s="9"/>
-      <c r="H296" s="9"/>
-      <c r="I296" s="9"/>
-      <c r="J296" s="9"/>
-      <c r="K296" s="9"/>
-      <c r="L296" s="9"/>
-      <c r="M296" s="9"/>
-      <c r="N296" s="9"/>
-      <c r="O296" s="9"/>
-      <c r="P296" s="16"/>
-      <c r="Q296" s="9"/>
-      <c r="R296" s="9"/>
-      <c r="S296" s="17"/>
-      <c r="T296" s="9"/>
+      <c r="A296" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B296" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C296" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D296" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E296" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F296" s="17">
+        <v>298</v>
+      </c>
+      <c r="G296" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H296" s="9">
+        <f t="shared" ref="H296" si="88">YEAR(G296)</f>
+        <v>2024</v>
+      </c>
+      <c r="I296" s="9">
+        <f t="shared" ref="I296" si="89">MONTH(G296)</f>
+        <v>7</v>
+      </c>
+      <c r="J296" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K296" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L296" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M296" s="17">
+        <v>1</v>
+      </c>
+      <c r="N296" s="17">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="O296" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P296" s="16" t="s">
+        <v>1013</v>
+      </c>
+      <c r="Q296" s="9" t="s">
+        <v>874</v>
+      </c>
+      <c r="R296" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S296" s="17">
+        <f t="shared" si="81"/>
+        <v>55</v>
+      </c>
+      <c r="T296" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="297" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A297" s="13"/>
@@ -30016,6 +30279,160 @@
       <c r="R300" s="9"/>
       <c r="S300" s="17"/>
       <c r="T300" s="9"/>
+    </row>
+    <row r="301" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A301" s="9"/>
+      <c r="B301" s="9"/>
+      <c r="C301" s="9"/>
+      <c r="D301" s="9"/>
+      <c r="E301" s="9"/>
+      <c r="F301" s="9"/>
+      <c r="G301" s="9"/>
+      <c r="H301" s="9"/>
+      <c r="I301" s="9"/>
+      <c r="J301" s="9"/>
+      <c r="K301" s="9"/>
+      <c r="L301" s="9"/>
+      <c r="M301" s="9"/>
+      <c r="N301" s="9"/>
+      <c r="O301" s="9"/>
+      <c r="P301" s="9"/>
+      <c r="Q301" s="9"/>
+      <c r="R301" s="9"/>
+      <c r="S301" s="17"/>
+      <c r="T301" s="9"/>
+    </row>
+    <row r="302" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A302" s="9"/>
+      <c r="B302" s="9"/>
+      <c r="C302" s="9"/>
+      <c r="D302" s="9"/>
+      <c r="E302" s="9"/>
+      <c r="F302" s="9"/>
+      <c r="G302" s="9"/>
+      <c r="H302" s="9"/>
+      <c r="I302" s="9"/>
+      <c r="J302" s="9"/>
+      <c r="K302" s="9"/>
+      <c r="L302" s="9"/>
+      <c r="M302" s="9"/>
+      <c r="N302" s="9"/>
+      <c r="O302" s="9"/>
+      <c r="P302" s="9"/>
+      <c r="Q302" s="9"/>
+      <c r="R302" s="9"/>
+      <c r="S302" s="17"/>
+      <c r="T302" s="9"/>
+    </row>
+    <row r="303" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A303" s="9"/>
+      <c r="B303" s="9"/>
+      <c r="C303" s="9"/>
+      <c r="D303" s="9"/>
+      <c r="E303" s="9"/>
+      <c r="F303" s="9"/>
+      <c r="G303" s="9"/>
+      <c r="H303" s="9"/>
+      <c r="I303" s="9"/>
+      <c r="J303" s="9"/>
+      <c r="K303" s="9"/>
+      <c r="L303" s="9"/>
+      <c r="M303" s="9"/>
+      <c r="N303" s="9"/>
+      <c r="O303" s="9"/>
+      <c r="P303" s="9"/>
+      <c r="Q303" s="9"/>
+      <c r="R303" s="9"/>
+      <c r="S303" s="17"/>
+      <c r="T303" s="9"/>
+    </row>
+    <row r="304" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A304" s="9"/>
+      <c r="B304" s="9"/>
+      <c r="C304" s="9"/>
+      <c r="D304" s="9"/>
+      <c r="E304" s="9"/>
+      <c r="F304" s="9"/>
+      <c r="G304" s="9"/>
+      <c r="H304" s="9"/>
+      <c r="I304" s="9"/>
+      <c r="J304" s="9"/>
+      <c r="K304" s="9"/>
+      <c r="L304" s="9"/>
+      <c r="M304" s="9"/>
+      <c r="N304" s="9"/>
+      <c r="O304" s="9"/>
+      <c r="P304" s="9"/>
+      <c r="Q304" s="9"/>
+      <c r="R304" s="9"/>
+      <c r="S304" s="17"/>
+      <c r="T304" s="9"/>
+    </row>
+    <row r="305" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A305" s="9"/>
+      <c r="B305" s="9"/>
+      <c r="C305" s="9"/>
+      <c r="D305" s="9"/>
+      <c r="E305" s="9"/>
+      <c r="F305" s="9"/>
+      <c r="G305" s="9"/>
+      <c r="H305" s="9"/>
+      <c r="I305" s="9"/>
+      <c r="J305" s="9"/>
+      <c r="K305" s="9"/>
+      <c r="L305" s="9"/>
+      <c r="M305" s="9"/>
+      <c r="N305" s="9"/>
+      <c r="O305" s="9"/>
+      <c r="P305" s="9"/>
+      <c r="Q305" s="9"/>
+      <c r="R305" s="9"/>
+      <c r="S305" s="17"/>
+      <c r="T305" s="9"/>
+    </row>
+    <row r="306" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A306" s="9"/>
+      <c r="B306" s="9"/>
+      <c r="C306" s="9"/>
+      <c r="D306" s="9"/>
+      <c r="E306" s="9"/>
+      <c r="F306" s="9"/>
+      <c r="G306" s="9"/>
+      <c r="H306" s="9"/>
+      <c r="I306" s="9"/>
+      <c r="J306" s="9"/>
+      <c r="K306" s="9"/>
+      <c r="L306" s="9"/>
+      <c r="M306" s="9"/>
+      <c r="N306" s="9"/>
+      <c r="O306" s="9"/>
+      <c r="P306" s="9"/>
+      <c r="Q306" s="9"/>
+      <c r="R306" s="9"/>
+      <c r="S306" s="17"/>
+      <c r="T306" s="9"/>
+    </row>
+    <row r="307" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A307" s="9"/>
+      <c r="B307" s="9"/>
+      <c r="C307" s="9"/>
+      <c r="D307" s="9"/>
+      <c r="E307" s="9"/>
+      <c r="F307" s="9"/>
+      <c r="G307" s="9"/>
+      <c r="H307" s="9"/>
+      <c r="I307" s="9"/>
+      <c r="J307" s="9"/>
+      <c r="K307" s="9"/>
+      <c r="L307" s="9"/>
+      <c r="M307" s="9"/>
+      <c r="N307" s="9"/>
+      <c r="O307" s="9"/>
+      <c r="P307" s="9"/>
+      <c r="Q307" s="9"/>
+      <c r="R307" s="9"/>
+      <c r="S307" s="17"/>
+      <c r="T307" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated to 2024-07-23.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4830" uniqueCount="1027">
   <si>
     <t>Format</t>
   </si>
@@ -3083,6 +3083,45 @@
   </si>
   <si>
     <t>Useless. A soup of different technologies and concepts.</t>
+  </si>
+  <si>
+    <t>Learn Enough Python To Be Dangerous</t>
+  </si>
+  <si>
+    <t>2024-07-22</t>
+  </si>
+  <si>
+    <t>Professional Python: Object-Oriented Approaches To Efficient Software Development</t>
+  </si>
+  <si>
+    <t>Useless. A book for beginners that has nothing to do with the term "professional", and with an awfully colored layout that it's very difficult to read. One positive aspect: it contains concise code examples to illustrate design patterns in Python.</t>
+  </si>
+  <si>
+    <t>The Pythonic Way</t>
+  </si>
+  <si>
+    <t>2024-07-23</t>
+  </si>
+  <si>
+    <t>Useful. This book follows an approach very unique and personal to talk about Python. The author built the book around PEP documents and other conventions. On the contrary to dozens of Python books, this contains original content.</t>
+  </si>
+  <si>
+    <t>LangChain: A Hands-On Guide To Modern AI Applications</t>
+  </si>
+  <si>
+    <t>Useful. A short introduction about Langchain.</t>
+  </si>
+  <si>
+    <t>Data Analysis: A Gentle Introduction For Future Data Scientists</t>
+  </si>
+  <si>
+    <t>Useful. This book starts well, but then it loses itself into too much theory and no practical examples.</t>
+  </si>
+  <si>
+    <t>The Creative Programmer</t>
+  </si>
+  <si>
+    <t>Useless. Well written, but the author didn't write any original content, but just listed theories and concepts written by others. This book is below the Manning's average rate.</t>
   </si>
 </sst>
 </file>
@@ -10926,11 +10965,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T307"/>
+  <dimension ref="A1:T314"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A297" sqref="A297"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A303" sqref="A303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -29795,7 +29834,7 @@
         <v>159</v>
       </c>
       <c r="S290" s="17">
-        <f t="shared" ref="S290:S296" si="81">LEN(P290)</f>
+        <f t="shared" ref="S290:S302" si="81">LEN(P290)</f>
         <v>152</v>
       </c>
       <c r="T290" s="14">
@@ -30193,139 +30232,397 @@
       </c>
     </row>
     <row r="297" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A297" s="13"/>
-      <c r="B297" s="9"/>
-      <c r="C297" s="9"/>
-      <c r="D297" s="9"/>
-      <c r="E297" s="9"/>
-      <c r="F297" s="9"/>
-      <c r="G297" s="9"/>
-      <c r="H297" s="9"/>
-      <c r="I297" s="9"/>
-      <c r="J297" s="9"/>
-      <c r="K297" s="9"/>
-      <c r="L297" s="9"/>
-      <c r="M297" s="9"/>
-      <c r="N297" s="9"/>
-      <c r="O297" s="9"/>
-      <c r="P297" s="16"/>
-      <c r="Q297" s="9"/>
-      <c r="R297" s="9"/>
-      <c r="S297" s="17"/>
-      <c r="T297" s="9"/>
+      <c r="A297" s="13" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B297" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C297" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D297" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E297" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F297" s="17">
+        <v>636</v>
+      </c>
+      <c r="G297" s="9" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H297" s="9">
+        <f t="shared" ref="H297" si="90">YEAR(G297)</f>
+        <v>2024</v>
+      </c>
+      <c r="I297" s="9">
+        <f t="shared" ref="I297" si="91">MONTH(G297)</f>
+        <v>7</v>
+      </c>
+      <c r="J297" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K297" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L297" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="M297" s="17">
+        <v>1</v>
+      </c>
+      <c r="N297" s="17">
+        <v>39.99</v>
+      </c>
+      <c r="O297" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P297" s="16" t="s">
+        <v>1013</v>
+      </c>
+      <c r="Q297" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R297" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S297" s="17">
+        <f t="shared" si="81"/>
+        <v>55</v>
+      </c>
+      <c r="T297" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="298" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A298" s="13"/>
-      <c r="B298" s="9"/>
-      <c r="C298" s="9"/>
-      <c r="D298" s="9"/>
-      <c r="E298" s="9"/>
-      <c r="F298" s="9"/>
-      <c r="G298" s="9"/>
-      <c r="H298" s="9"/>
-      <c r="I298" s="9"/>
-      <c r="J298" s="9"/>
-      <c r="K298" s="9"/>
-      <c r="L298" s="9"/>
-      <c r="M298" s="9"/>
-      <c r="N298" s="9"/>
-      <c r="O298" s="9"/>
-      <c r="P298" s="16"/>
-      <c r="Q298" s="9"/>
-      <c r="R298" s="9"/>
-      <c r="S298" s="17"/>
-      <c r="T298" s="9"/>
+      <c r="A298" s="16" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B298" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C298" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D298" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E298" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F298" s="17">
+        <v>218</v>
+      </c>
+      <c r="G298" s="9" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H298" s="9">
+        <f t="shared" ref="H298" si="92">YEAR(G298)</f>
+        <v>2024</v>
+      </c>
+      <c r="I298" s="9">
+        <f t="shared" ref="I298" si="93">MONTH(G298)</f>
+        <v>7</v>
+      </c>
+      <c r="J298" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K298" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L298" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M298" s="17">
+        <v>1</v>
+      </c>
+      <c r="N298" s="17">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="O298" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P298" s="16" t="s">
+        <v>1017</v>
+      </c>
+      <c r="Q298" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R298" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S298" s="17">
+        <f t="shared" si="81"/>
+        <v>247</v>
+      </c>
+      <c r="T298" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="299" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A299" s="13"/>
-      <c r="B299" s="9"/>
-      <c r="C299" s="9"/>
-      <c r="D299" s="9"/>
-      <c r="E299" s="9"/>
-      <c r="F299" s="9"/>
-      <c r="G299" s="9"/>
-      <c r="H299" s="9"/>
-      <c r="I299" s="9"/>
-      <c r="J299" s="9"/>
-      <c r="K299" s="9"/>
-      <c r="L299" s="9"/>
-      <c r="M299" s="9"/>
-      <c r="N299" s="9"/>
-      <c r="O299" s="9"/>
-      <c r="P299" s="16"/>
-      <c r="Q299" s="9"/>
-      <c r="R299" s="9"/>
-      <c r="S299" s="17"/>
-      <c r="T299" s="9"/>
+      <c r="A299" s="13" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B299" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C299" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D299" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E299" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F299" s="17">
+        <v>464</v>
+      </c>
+      <c r="G299" s="9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H299" s="9">
+        <f t="shared" ref="H299" si="94">YEAR(G299)</f>
+        <v>2024</v>
+      </c>
+      <c r="I299" s="9">
+        <f t="shared" ref="I299" si="95">MONTH(G299)</f>
+        <v>7</v>
+      </c>
+      <c r="J299" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K299" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L299" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="M299" s="17">
+        <v>3</v>
+      </c>
+      <c r="N299" s="17">
+        <v>24.95</v>
+      </c>
+      <c r="O299" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P299" s="16" t="s">
+        <v>1020</v>
+      </c>
+      <c r="Q299" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R299" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S299" s="17">
+        <f t="shared" si="81"/>
+        <v>229</v>
+      </c>
+      <c r="T299" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="300" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A300" s="13"/>
-      <c r="B300" s="9"/>
-      <c r="C300" s="9"/>
-      <c r="D300" s="9"/>
-      <c r="E300" s="9"/>
-      <c r="F300" s="9"/>
-      <c r="G300" s="9"/>
-      <c r="H300" s="9"/>
-      <c r="I300" s="9"/>
-      <c r="J300" s="9"/>
-      <c r="K300" s="9"/>
-      <c r="L300" s="9"/>
-      <c r="M300" s="9"/>
-      <c r="N300" s="9"/>
-      <c r="O300" s="9"/>
-      <c r="P300" s="16"/>
-      <c r="Q300" s="9"/>
-      <c r="R300" s="9"/>
-      <c r="S300" s="17"/>
-      <c r="T300" s="9"/>
+      <c r="A300" s="13" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B300" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C300" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D300" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E300" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F300" s="17">
+        <v>58</v>
+      </c>
+      <c r="G300" s="9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H300" s="9">
+        <f t="shared" ref="H300" si="96">YEAR(G300)</f>
+        <v>2024</v>
+      </c>
+      <c r="I300" s="9">
+        <f t="shared" ref="I300" si="97">MONTH(G300)</f>
+        <v>7</v>
+      </c>
+      <c r="J300" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K300" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L300" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M300" s="17">
+        <v>2</v>
+      </c>
+      <c r="N300" s="17">
+        <v>14.95</v>
+      </c>
+      <c r="O300" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P300" s="28" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Q300" s="9" t="s">
+        <v>959</v>
+      </c>
+      <c r="R300" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S300" s="17">
+        <f t="shared" si="81"/>
+        <v>45</v>
+      </c>
+      <c r="T300" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="301" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A301" s="9"/>
-      <c r="B301" s="9"/>
-      <c r="C301" s="9"/>
-      <c r="D301" s="9"/>
-      <c r="E301" s="9"/>
-      <c r="F301" s="9"/>
-      <c r="G301" s="9"/>
-      <c r="H301" s="9"/>
-      <c r="I301" s="9"/>
-      <c r="J301" s="9"/>
-      <c r="K301" s="9"/>
-      <c r="L301" s="9"/>
-      <c r="M301" s="9"/>
-      <c r="N301" s="9"/>
-      <c r="O301" s="9"/>
-      <c r="P301" s="9"/>
-      <c r="Q301" s="9"/>
-      <c r="R301" s="9"/>
-      <c r="S301" s="17"/>
-      <c r="T301" s="9"/>
+      <c r="A301" s="13" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B301" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C301" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D301" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E301" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F301" s="17">
+        <v>161</v>
+      </c>
+      <c r="G301" s="9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H301" s="9">
+        <f t="shared" ref="H301" si="98">YEAR(G301)</f>
+        <v>2024</v>
+      </c>
+      <c r="I301" s="9">
+        <f t="shared" ref="I301" si="99">MONTH(G301)</f>
+        <v>7</v>
+      </c>
+      <c r="J301" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K301" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L301" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="M301" s="17">
+        <v>2</v>
+      </c>
+      <c r="N301" s="43">
+        <v>35</v>
+      </c>
+      <c r="O301" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P301" s="13" t="s">
+        <v>1024</v>
+      </c>
+      <c r="Q301" s="9" t="s">
+        <v>904</v>
+      </c>
+      <c r="R301" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S301" s="17">
+        <f t="shared" si="81"/>
+        <v>103</v>
+      </c>
+      <c r="T301" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="302" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A302" s="9"/>
-      <c r="B302" s="9"/>
-      <c r="C302" s="9"/>
-      <c r="D302" s="9"/>
-      <c r="E302" s="9"/>
-      <c r="F302" s="9"/>
-      <c r="G302" s="9"/>
-      <c r="H302" s="9"/>
-      <c r="I302" s="9"/>
-      <c r="J302" s="9"/>
-      <c r="K302" s="9"/>
-      <c r="L302" s="9"/>
-      <c r="M302" s="9"/>
-      <c r="N302" s="9"/>
-      <c r="O302" s="9"/>
-      <c r="P302" s="9"/>
-      <c r="Q302" s="9"/>
-      <c r="R302" s="9"/>
-      <c r="S302" s="17"/>
-      <c r="T302" s="9"/>
+      <c r="A302" s="13" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B302" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C302" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D302" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E302" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F302" s="17">
+        <v>331</v>
+      </c>
+      <c r="G302" s="9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H302" s="9">
+        <f t="shared" ref="H302" si="100">YEAR(G302)</f>
+        <v>2024</v>
+      </c>
+      <c r="I302" s="9">
+        <f t="shared" ref="I302" si="101">MONTH(G302)</f>
+        <v>7</v>
+      </c>
+      <c r="J302" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K302" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L302" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M302" s="17">
+        <v>2</v>
+      </c>
+      <c r="N302" s="43">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="O302" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P302" s="16" t="s">
+        <v>1026</v>
+      </c>
+      <c r="Q302" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R302" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S302" s="17">
+        <f t="shared" si="81"/>
+        <v>176</v>
+      </c>
+      <c r="T302" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="303" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A303" s="9"/>
+      <c r="A303" s="13"/>
       <c r="B303" s="9"/>
       <c r="C303" s="9"/>
       <c r="D303" s="9"/>
@@ -30340,14 +30637,14 @@
       <c r="M303" s="9"/>
       <c r="N303" s="9"/>
       <c r="O303" s="9"/>
-      <c r="P303" s="9"/>
+      <c r="P303" s="13"/>
       <c r="Q303" s="9"/>
       <c r="R303" s="9"/>
       <c r="S303" s="17"/>
       <c r="T303" s="9"/>
     </row>
     <row r="304" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A304" s="9"/>
+      <c r="A304" s="13"/>
       <c r="B304" s="9"/>
       <c r="C304" s="9"/>
       <c r="D304" s="9"/>
@@ -30362,14 +30659,14 @@
       <c r="M304" s="9"/>
       <c r="N304" s="9"/>
       <c r="O304" s="9"/>
-      <c r="P304" s="9"/>
+      <c r="P304" s="13"/>
       <c r="Q304" s="9"/>
       <c r="R304" s="9"/>
       <c r="S304" s="17"/>
       <c r="T304" s="9"/>
     </row>
     <row r="305" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A305" s="9"/>
+      <c r="A305" s="13"/>
       <c r="B305" s="9"/>
       <c r="C305" s="9"/>
       <c r="D305" s="9"/>
@@ -30384,14 +30681,14 @@
       <c r="M305" s="9"/>
       <c r="N305" s="9"/>
       <c r="O305" s="9"/>
-      <c r="P305" s="9"/>
+      <c r="P305" s="13"/>
       <c r="Q305" s="9"/>
       <c r="R305" s="9"/>
       <c r="S305" s="17"/>
       <c r="T305" s="9"/>
     </row>
     <row r="306" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A306" s="9"/>
+      <c r="A306" s="13"/>
       <c r="B306" s="9"/>
       <c r="C306" s="9"/>
       <c r="D306" s="9"/>
@@ -30406,14 +30703,14 @@
       <c r="M306" s="9"/>
       <c r="N306" s="9"/>
       <c r="O306" s="9"/>
-      <c r="P306" s="9"/>
+      <c r="P306" s="13"/>
       <c r="Q306" s="9"/>
       <c r="R306" s="9"/>
       <c r="S306" s="17"/>
       <c r="T306" s="9"/>
     </row>
     <row r="307" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A307" s="9"/>
+      <c r="A307" s="13"/>
       <c r="B307" s="9"/>
       <c r="C307" s="9"/>
       <c r="D307" s="9"/>
@@ -30428,11 +30725,165 @@
       <c r="M307" s="9"/>
       <c r="N307" s="9"/>
       <c r="O307" s="9"/>
-      <c r="P307" s="9"/>
+      <c r="P307" s="13"/>
       <c r="Q307" s="9"/>
       <c r="R307" s="9"/>
       <c r="S307" s="17"/>
       <c r="T307" s="9"/>
+    </row>
+    <row r="308" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A308" s="13"/>
+      <c r="B308" s="9"/>
+      <c r="C308" s="9"/>
+      <c r="D308" s="9"/>
+      <c r="E308" s="9"/>
+      <c r="F308" s="9"/>
+      <c r="G308" s="9"/>
+      <c r="H308" s="9"/>
+      <c r="I308" s="9"/>
+      <c r="J308" s="9"/>
+      <c r="K308" s="9"/>
+      <c r="L308" s="9"/>
+      <c r="M308" s="9"/>
+      <c r="N308" s="9"/>
+      <c r="O308" s="9"/>
+      <c r="P308" s="13"/>
+      <c r="Q308" s="9"/>
+      <c r="R308" s="9"/>
+      <c r="S308" s="17"/>
+      <c r="T308" s="9"/>
+    </row>
+    <row r="309" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A309" s="13"/>
+      <c r="B309" s="9"/>
+      <c r="C309" s="9"/>
+      <c r="D309" s="9"/>
+      <c r="E309" s="9"/>
+      <c r="F309" s="9"/>
+      <c r="G309" s="9"/>
+      <c r="H309" s="9"/>
+      <c r="I309" s="9"/>
+      <c r="J309" s="9"/>
+      <c r="K309" s="9"/>
+      <c r="L309" s="9"/>
+      <c r="M309" s="9"/>
+      <c r="N309" s="9"/>
+      <c r="O309" s="9"/>
+      <c r="P309" s="13"/>
+      <c r="Q309" s="9"/>
+      <c r="R309" s="9"/>
+      <c r="S309" s="17"/>
+      <c r="T309" s="9"/>
+    </row>
+    <row r="310" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A310" s="13"/>
+      <c r="B310" s="9"/>
+      <c r="C310" s="9"/>
+      <c r="D310" s="9"/>
+      <c r="E310" s="9"/>
+      <c r="F310" s="9"/>
+      <c r="G310" s="9"/>
+      <c r="H310" s="9"/>
+      <c r="I310" s="9"/>
+      <c r="J310" s="9"/>
+      <c r="K310" s="9"/>
+      <c r="L310" s="9"/>
+      <c r="M310" s="9"/>
+      <c r="N310" s="9"/>
+      <c r="O310" s="9"/>
+      <c r="P310" s="13"/>
+      <c r="Q310" s="9"/>
+      <c r="R310" s="9"/>
+      <c r="S310" s="17"/>
+      <c r="T310" s="9"/>
+    </row>
+    <row r="311" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A311" s="13"/>
+      <c r="B311" s="9"/>
+      <c r="C311" s="9"/>
+      <c r="D311" s="9"/>
+      <c r="E311" s="9"/>
+      <c r="F311" s="9"/>
+      <c r="G311" s="9"/>
+      <c r="H311" s="9"/>
+      <c r="I311" s="9"/>
+      <c r="J311" s="9"/>
+      <c r="K311" s="9"/>
+      <c r="L311" s="9"/>
+      <c r="M311" s="9"/>
+      <c r="N311" s="9"/>
+      <c r="O311" s="9"/>
+      <c r="P311" s="13"/>
+      <c r="Q311" s="9"/>
+      <c r="R311" s="9"/>
+      <c r="S311" s="17"/>
+      <c r="T311" s="9"/>
+    </row>
+    <row r="312" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A312" s="13"/>
+      <c r="B312" s="9"/>
+      <c r="C312" s="9"/>
+      <c r="D312" s="9"/>
+      <c r="E312" s="9"/>
+      <c r="F312" s="9"/>
+      <c r="G312" s="9"/>
+      <c r="H312" s="9"/>
+      <c r="I312" s="9"/>
+      <c r="J312" s="9"/>
+      <c r="K312" s="9"/>
+      <c r="L312" s="9"/>
+      <c r="M312" s="9"/>
+      <c r="N312" s="9"/>
+      <c r="O312" s="9"/>
+      <c r="P312" s="13"/>
+      <c r="Q312" s="9"/>
+      <c r="R312" s="9"/>
+      <c r="S312" s="17"/>
+      <c r="T312" s="9"/>
+    </row>
+    <row r="313" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A313" s="13"/>
+      <c r="B313" s="9"/>
+      <c r="C313" s="9"/>
+      <c r="D313" s="9"/>
+      <c r="E313" s="9"/>
+      <c r="F313" s="9"/>
+      <c r="G313" s="9"/>
+      <c r="H313" s="9"/>
+      <c r="I313" s="9"/>
+      <c r="J313" s="9"/>
+      <c r="K313" s="9"/>
+      <c r="L313" s="9"/>
+      <c r="M313" s="9"/>
+      <c r="N313" s="9"/>
+      <c r="O313" s="9"/>
+      <c r="P313" s="13"/>
+      <c r="Q313" s="9"/>
+      <c r="R313" s="9"/>
+      <c r="S313" s="17"/>
+      <c r="T313" s="9"/>
+    </row>
+    <row r="314" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A314" s="13"/>
+      <c r="B314" s="9"/>
+      <c r="C314" s="9"/>
+      <c r="D314" s="9"/>
+      <c r="E314" s="9"/>
+      <c r="F314" s="9"/>
+      <c r="G314" s="9"/>
+      <c r="H314" s="9"/>
+      <c r="I314" s="9"/>
+      <c r="J314" s="9"/>
+      <c r="K314" s="9"/>
+      <c r="L314" s="9"/>
+      <c r="M314" s="9"/>
+      <c r="N314" s="9"/>
+      <c r="O314" s="9"/>
+      <c r="P314" s="13"/>
+      <c r="Q314" s="9"/>
+      <c r="R314" s="9"/>
+      <c r="S314" s="17"/>
+      <c r="T314" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated up to 2024-08-03.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4830" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4854" uniqueCount="1033">
   <si>
     <t>Format</t>
   </si>
@@ -3122,6 +3122,24 @@
   </si>
   <si>
     <t>Useless. Well written, but the author didn't write any original content, but just listed theories and concepts written by others. This book is below the Manning's average rate.</t>
+  </si>
+  <si>
+    <t>NixOS &amp; Flakes Book v0.4.3</t>
+  </si>
+  <si>
+    <t>Useful. It's an amateur book, but it's the first one available about NixOS, therefore we apprecciate the author's effort. The book contains some useful hints, but it's also a bit repetitive and in need of some editing.</t>
+  </si>
+  <si>
+    <t>NixOS in Production</t>
+  </si>
+  <si>
+    <t>2024-07-26</t>
+  </si>
+  <si>
+    <t>2024-08-01</t>
+  </si>
+  <si>
+    <t>Useless. It focalizes on the internals of Nix modules and on how to deploy NixOS to AWS.</t>
   </si>
 </sst>
 </file>
@@ -10967,9 +10985,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T314"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A303" sqref="A303"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P307" sqref="P307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -29834,7 +29852,7 @@
         <v>159</v>
       </c>
       <c r="S290" s="17">
-        <f t="shared" ref="S290:S302" si="81">LEN(P290)</f>
+        <f t="shared" ref="S290:S303" si="81">LEN(P290)</f>
         <v>152</v>
       </c>
       <c r="T290" s="14">
@@ -30622,48 +30640,134 @@
       </c>
     </row>
     <row r="303" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A303" s="13"/>
-      <c r="B303" s="9"/>
-      <c r="C303" s="9"/>
-      <c r="D303" s="9"/>
-      <c r="E303" s="9"/>
-      <c r="F303" s="9"/>
-      <c r="G303" s="9"/>
-      <c r="H303" s="9"/>
-      <c r="I303" s="9"/>
-      <c r="J303" s="9"/>
-      <c r="K303" s="9"/>
-      <c r="L303" s="9"/>
-      <c r="M303" s="9"/>
-      <c r="N303" s="9"/>
-      <c r="O303" s="9"/>
-      <c r="P303" s="13"/>
-      <c r="Q303" s="9"/>
-      <c r="R303" s="9"/>
-      <c r="S303" s="17"/>
-      <c r="T303" s="9"/>
+      <c r="A303" s="13" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B303" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C303" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D303" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E303" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F303" s="17">
+        <v>179</v>
+      </c>
+      <c r="G303" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H303" s="9">
+        <f t="shared" ref="H303" si="102">YEAR(G303)</f>
+        <v>2024</v>
+      </c>
+      <c r="I303" s="9">
+        <f t="shared" ref="I303" si="103">MONTH(G303)</f>
+        <v>7</v>
+      </c>
+      <c r="J303" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K303" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L303" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M303" s="17">
+        <v>3</v>
+      </c>
+      <c r="N303" s="43">
+        <v>0</v>
+      </c>
+      <c r="O303" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P303" s="13" t="s">
+        <v>1028</v>
+      </c>
+      <c r="Q303" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="R303" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S303" s="17">
+        <f t="shared" si="81"/>
+        <v>218</v>
+      </c>
+      <c r="T303" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="304" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A304" s="13"/>
-      <c r="B304" s="9"/>
-      <c r="C304" s="9"/>
-      <c r="D304" s="9"/>
-      <c r="E304" s="9"/>
-      <c r="F304" s="9"/>
-      <c r="G304" s="9"/>
-      <c r="H304" s="9"/>
-      <c r="I304" s="9"/>
-      <c r="J304" s="9"/>
-      <c r="K304" s="9"/>
-      <c r="L304" s="9"/>
-      <c r="M304" s="9"/>
-      <c r="N304" s="9"/>
-      <c r="O304" s="9"/>
-      <c r="P304" s="13"/>
-      <c r="Q304" s="9"/>
-      <c r="R304" s="9"/>
-      <c r="S304" s="17"/>
-      <c r="T304" s="9"/>
+      <c r="A304" s="13" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B304" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C304" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D304" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E304" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F304" s="17">
+        <v>123</v>
+      </c>
+      <c r="G304" s="9" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H304" s="9">
+        <f t="shared" ref="H304" si="104">YEAR(G304)</f>
+        <v>2024</v>
+      </c>
+      <c r="I304" s="9">
+        <f t="shared" ref="I304" si="105">MONTH(G304)</f>
+        <v>8</v>
+      </c>
+      <c r="J304" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K304" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L304" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M304" s="17">
+        <v>1</v>
+      </c>
+      <c r="N304" s="43">
+        <v>40</v>
+      </c>
+      <c r="O304" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P304" s="13" t="s">
+        <v>1032</v>
+      </c>
+      <c r="Q304" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="R304" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S304" s="17">
+        <f t="shared" ref="S304" si="106">LEN(P304)</f>
+        <v>88</v>
+      </c>
+      <c r="T304" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="305" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A305" s="13"/>

</xml_diff>

<commit_message>
#25 Reading List.xslx: updated up to 2024-08-11.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4854" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4866" uniqueCount="1036">
   <si>
     <t>Format</t>
   </si>
@@ -3140,6 +3140,15 @@
   </si>
   <si>
     <t>Useless. It focalizes on the internals of Nix modules and on how to deploy NixOS to AWS.</t>
+  </si>
+  <si>
+    <t>Building Data-Driven Applications with LLamaIndex</t>
+  </si>
+  <si>
+    <t>2024-08-11</t>
+  </si>
+  <si>
+    <t>Useful. It's definitely the most comprehensive book about RAG I read so far and it covers everything you need in depth. As every Packt book would require some editing and restructuring, because it tends to be repetitive and caotic.</t>
   </si>
 </sst>
 </file>
@@ -10985,9 +10994,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P307" sqref="P307"/>
+      <selection pane="bottomLeft" activeCell="A293" sqref="A293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -30762,7 +30771,7 @@
         <v>159</v>
       </c>
       <c r="S304" s="17">
-        <f t="shared" ref="S304" si="106">LEN(P304)</f>
+        <f t="shared" ref="S304:S305" si="106">LEN(P304)</f>
         <v>88</v>
       </c>
       <c r="T304" s="14">
@@ -30770,26 +30779,69 @@
       </c>
     </row>
     <row r="305" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A305" s="13"/>
-      <c r="B305" s="9"/>
-      <c r="C305" s="9"/>
-      <c r="D305" s="9"/>
-      <c r="E305" s="9"/>
-      <c r="F305" s="9"/>
-      <c r="G305" s="9"/>
-      <c r="H305" s="9"/>
-      <c r="I305" s="9"/>
-      <c r="J305" s="9"/>
-      <c r="K305" s="9"/>
-      <c r="L305" s="9"/>
-      <c r="M305" s="9"/>
-      <c r="N305" s="9"/>
-      <c r="O305" s="9"/>
-      <c r="P305" s="13"/>
-      <c r="Q305" s="9"/>
-      <c r="R305" s="9"/>
-      <c r="S305" s="17"/>
-      <c r="T305" s="9"/>
+      <c r="A305" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B305" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C305" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D305" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E305" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F305" s="17">
+        <v>368</v>
+      </c>
+      <c r="G305" s="9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H305" s="9">
+        <f t="shared" ref="H305" si="107">YEAR(G305)</f>
+        <v>2024</v>
+      </c>
+      <c r="I305" s="9">
+        <f t="shared" ref="I305" si="108">MONTH(G305)</f>
+        <v>8</v>
+      </c>
+      <c r="J305" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K305" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L305" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M305" s="17">
+        <v>4</v>
+      </c>
+      <c r="N305" s="17">
+        <v>43.13</v>
+      </c>
+      <c r="O305" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P305" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="Q305" s="9" t="s">
+        <v>959</v>
+      </c>
+      <c r="R305" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S305" s="17">
+        <f t="shared" si="106"/>
+        <v>231</v>
+      </c>
+      <c r="T305" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="306" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A306" s="13"/>

</xml_diff>

<commit_message>
#34 Reading List: updated to 27/10/2024.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4866" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4878" uniqueCount="1038">
   <si>
     <t>Format</t>
   </si>
@@ -3149,6 +3149,12 @@
   </si>
   <si>
     <t>Useful. It's definitely the most comprehensive book about RAG I read so far and it covers everything you need in depth. As every Packt book would require some editing and restructuring, because it tends to be repetitive and caotic.</t>
+  </si>
+  <si>
+    <t>The Well-Grounded Python Developer</t>
+  </si>
+  <si>
+    <t>Useful. It contains some useful bits of information, but the use of a bigger font instead of bold face to make important words to "pop" is massively annoying and it makes the reading experience a pain.</t>
   </si>
 </sst>
 </file>
@@ -3288,7 +3294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3424,6 +3430,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10992,11 +11001,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T314"/>
+  <dimension ref="A1:T315"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A293" sqref="A293"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U281" sqref="U281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -26026,7 +26035,7 @@
         <v>158</v>
       </c>
       <c r="S231" s="17">
-        <f t="shared" ref="S231:S286" si="32">LEN(P231)</f>
+        <f t="shared" ref="S231:S287" si="32">LEN(P231)</f>
         <v>54</v>
       </c>
       <c r="T231" s="14">
@@ -28045,7 +28054,7 @@
         <v>52</v>
       </c>
       <c r="T262" s="14">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="263" spans="1:20" x14ac:dyDescent="0.2">
@@ -28110,7 +28119,7 @@
         <v>128</v>
       </c>
       <c r="T263" s="14">
-        <v>0</v>
+        <v>509</v>
       </c>
     </row>
     <row r="264" spans="1:20" x14ac:dyDescent="0.2">
@@ -28136,11 +28145,11 @@
         <v>929</v>
       </c>
       <c r="H264" s="9">
-        <f t="shared" ref="H264" si="39">YEAR(G264)</f>
+        <f t="shared" ref="H264:H265" si="39">YEAR(G264)</f>
         <v>2024</v>
       </c>
       <c r="I264" s="9">
-        <f t="shared" ref="I264" si="40">MONTH(G264)</f>
+        <f t="shared" ref="I264:I265" si="40">MONTH(G264)</f>
         <v>2</v>
       </c>
       <c r="J264" s="9" t="s">
@@ -28161,8 +28170,8 @@
       <c r="O264" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P264" s="16" t="s">
-        <v>930</v>
+      <c r="P264" s="50" t="s">
+        <v>1037</v>
       </c>
       <c r="Q264" s="9" t="s">
         <v>569</v>
@@ -28172,18 +28181,18 @@
       </c>
       <c r="S264" s="17">
         <f t="shared" si="32"/>
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="T264" s="14">
-        <v>0</v>
+        <v>374</v>
       </c>
     </row>
     <row r="265" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A265" s="13" t="s">
-        <v>931</v>
+        <v>1036</v>
       </c>
       <c r="B265" s="17">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>21</v>
@@ -28195,17 +28204,17 @@
         <v>666</v>
       </c>
       <c r="F265" s="17">
-        <v>205</v>
+        <v>268</v>
       </c>
       <c r="G265" s="9" t="s">
         <v>929</v>
       </c>
       <c r="H265" s="9">
-        <f t="shared" ref="H265" si="41">YEAR(G265)</f>
+        <f t="shared" si="39"/>
         <v>2024</v>
       </c>
       <c r="I265" s="9">
-        <f t="shared" ref="I265" si="42">MONTH(G265)</f>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="J265" s="9" t="s">
@@ -28215,19 +28224,19 @@
         <v>159</v>
       </c>
       <c r="L265" s="9" t="s">
-        <v>602</v>
+        <v>369</v>
       </c>
       <c r="M265" s="17">
         <v>1</v>
       </c>
       <c r="N265" s="17">
-        <v>22.49</v>
+        <v>59.99</v>
       </c>
       <c r="O265" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P265" s="16" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="Q265" s="9" t="s">
         <v>569</v>
@@ -28237,15 +28246,15 @@
       </c>
       <c r="S265" s="17">
         <f t="shared" si="32"/>
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="T265" s="14">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="266" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A266" s="13" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B266" s="17">
         <v>2022</v>
@@ -28260,17 +28269,17 @@
         <v>666</v>
       </c>
       <c r="F266" s="17">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="G266" s="9" t="s">
         <v>929</v>
       </c>
       <c r="H266" s="9">
-        <f t="shared" ref="H266" si="43">YEAR(G266)</f>
+        <f t="shared" ref="H266" si="41">YEAR(G266)</f>
         <v>2024</v>
       </c>
       <c r="I266" s="9">
-        <f t="shared" ref="I266" si="44">MONTH(G266)</f>
+        <f t="shared" ref="I266" si="42">MONTH(G266)</f>
         <v>2</v>
       </c>
       <c r="J266" s="9" t="s">
@@ -28280,19 +28289,19 @@
         <v>159</v>
       </c>
       <c r="L266" s="9" t="s">
-        <v>372</v>
+        <v>602</v>
       </c>
       <c r="M266" s="17">
         <v>1</v>
       </c>
       <c r="N266" s="17">
-        <v>38.880000000000003</v>
+        <v>22.49</v>
       </c>
       <c r="O266" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P266" s="13" t="s">
-        <v>934</v>
+      <c r="P266" s="16" t="s">
+        <v>932</v>
       </c>
       <c r="Q266" s="9" t="s">
         <v>569</v>
@@ -28302,7 +28311,7 @@
       </c>
       <c r="S266" s="17">
         <f t="shared" si="32"/>
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="T266" s="14">
         <v>0</v>
@@ -28310,10 +28319,10 @@
     </row>
     <row r="267" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A267" s="13" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B267" s="17">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>21</v>
@@ -28325,17 +28334,17 @@
         <v>666</v>
       </c>
       <c r="F267" s="17">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="G267" s="9" t="s">
         <v>929</v>
       </c>
       <c r="H267" s="9">
-        <f t="shared" ref="H267:H268" si="45">YEAR(G267)</f>
+        <f t="shared" ref="H267" si="43">YEAR(G267)</f>
         <v>2024</v>
       </c>
       <c r="I267" s="9">
-        <f t="shared" ref="I267:I268" si="46">MONTH(G267)</f>
+        <f t="shared" ref="I267" si="44">MONTH(G267)</f>
         <v>2</v>
       </c>
       <c r="J267" s="9" t="s">
@@ -28345,19 +28354,19 @@
         <v>159</v>
       </c>
       <c r="L267" s="9" t="s">
-        <v>602</v>
+        <v>372</v>
       </c>
       <c r="M267" s="17">
         <v>1</v>
       </c>
       <c r="N267" s="17">
-        <v>49.99</v>
+        <v>38.880000000000003</v>
       </c>
       <c r="O267" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P267" s="13" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="Q267" s="9" t="s">
         <v>569</v>
@@ -28367,18 +28376,18 @@
       </c>
       <c r="S267" s="17">
         <f t="shared" si="32"/>
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="T267" s="14">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="268" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A268" s="13" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B268" s="17">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>21</v>
@@ -28390,577 +28399,577 @@
         <v>666</v>
       </c>
       <c r="F268" s="17">
+        <v>132</v>
+      </c>
+      <c r="G268" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="H268" s="9">
+        <f t="shared" ref="H268:H269" si="45">YEAR(G268)</f>
+        <v>2024</v>
+      </c>
+      <c r="I268" s="9">
+        <f t="shared" ref="I268:I269" si="46">MONTH(G268)</f>
+        <v>2</v>
+      </c>
+      <c r="J268" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K268" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L268" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M268" s="17">
+        <v>1</v>
+      </c>
+      <c r="N268" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O268" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P268" s="13" t="s">
+        <v>936</v>
+      </c>
+      <c r="Q268" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R268" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S268" s="17">
+        <f t="shared" si="32"/>
+        <v>121</v>
+      </c>
+      <c r="T268" s="14">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="269" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A269" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="B269" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C269" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D269" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E269" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F269" s="17">
         <v>715</v>
       </c>
-      <c r="G268" s="9" t="s">
+      <c r="G269" s="9" t="s">
         <v>937</v>
       </c>
-      <c r="H268" s="9">
+      <c r="H269" s="9">
         <f t="shared" si="45"/>
         <v>2024</v>
       </c>
-      <c r="I268" s="9">
+      <c r="I269" s="9">
         <f t="shared" si="46"/>
         <v>2</v>
       </c>
-      <c r="J268" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K268" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L268" s="9" t="s">
+      <c r="J269" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K269" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L269" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="M268" s="17">
+      <c r="M269" s="17">
         <v>2</v>
       </c>
-      <c r="N268" s="17">
+      <c r="N269" s="17">
         <v>38.24</v>
       </c>
-      <c r="O268" s="9" t="s">
+      <c r="O269" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P268" s="13" t="s">
+      <c r="P269" s="13" t="s">
         <v>939</v>
       </c>
-      <c r="Q268" s="9" t="s">
+      <c r="Q269" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R268" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S268" s="17">
+      <c r="R269" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S269" s="17">
         <f t="shared" si="32"/>
         <v>105</v>
       </c>
-      <c r="T268" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A269" s="13" t="s">
+      <c r="T269" s="14">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="270" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A270" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="B269" s="17">
+      <c r="B270" s="17">
         <v>2023</v>
       </c>
-      <c r="C269" s="9" t="s">
+      <c r="C270" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D269" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E269" s="9" t="s">
+      <c r="D270" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E270" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F269" s="17">
+      <c r="F270" s="17">
         <v>192</v>
       </c>
-      <c r="G269" s="9" t="s">
+      <c r="G270" s="9" t="s">
         <v>937</v>
       </c>
-      <c r="H269" s="9">
-        <f t="shared" ref="H269" si="47">YEAR(G269)</f>
+      <c r="H270" s="9">
+        <f t="shared" ref="H270" si="47">YEAR(G270)</f>
         <v>2024</v>
       </c>
-      <c r="I269" s="9">
-        <f t="shared" ref="I269" si="48">MONTH(G269)</f>
+      <c r="I270" s="9">
+        <f t="shared" ref="I270" si="48">MONTH(G270)</f>
         <v>2</v>
       </c>
-      <c r="J269" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K269" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L269" s="9" t="s">
+      <c r="J270" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K270" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L270" s="9" t="s">
         <v>941</v>
       </c>
-      <c r="M269" s="17">
+      <c r="M270" s="17">
         <v>1</v>
       </c>
-      <c r="N269" s="17">
+      <c r="N270" s="17">
         <v>54.99</v>
       </c>
-      <c r="O269" s="9" t="s">
+      <c r="O270" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P269" s="13" t="s">
+      <c r="P270" s="13" t="s">
         <v>942</v>
       </c>
-      <c r="Q269" s="9" t="s">
+      <c r="Q270" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R269" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S269" s="17">
+      <c r="R270" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S270" s="17">
         <f t="shared" si="32"/>
         <v>142</v>
       </c>
-      <c r="T269" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A270" s="13" t="s">
+      <c r="T270" s="14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="271" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A271" s="13" t="s">
         <v>943</v>
       </c>
-      <c r="B270" s="17">
+      <c r="B271" s="17">
         <v>2024</v>
       </c>
-      <c r="C270" s="9" t="s">
+      <c r="C271" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D270" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E270" s="9" t="s">
+      <c r="D271" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E271" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F270" s="17">
+      <c r="F271" s="17">
         <v>139</v>
       </c>
-      <c r="G270" s="9" t="s">
+      <c r="G271" s="9" t="s">
         <v>937</v>
       </c>
-      <c r="H270" s="9">
-        <f t="shared" ref="H270" si="49">YEAR(G270)</f>
+      <c r="H271" s="9">
+        <f t="shared" ref="H271" si="49">YEAR(G271)</f>
         <v>2024</v>
       </c>
-      <c r="I270" s="9">
-        <f t="shared" ref="I270" si="50">MONTH(G270)</f>
+      <c r="I271" s="9">
+        <f t="shared" ref="I271" si="50">MONTH(G271)</f>
         <v>2</v>
       </c>
-      <c r="J270" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K270" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L270" s="9" t="s">
+      <c r="J271" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K271" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L271" s="9" t="s">
         <v>944</v>
       </c>
-      <c r="M270" s="17">
+      <c r="M271" s="17">
         <v>1</v>
       </c>
-      <c r="N270" s="17">
+      <c r="N271" s="17">
         <v>59.95</v>
       </c>
-      <c r="O270" s="9" t="s">
+      <c r="O271" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P270" s="13" t="s">
+      <c r="P271" s="13" t="s">
         <v>945</v>
       </c>
-      <c r="Q270" s="9" t="s">
+      <c r="Q271" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R270" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S270" s="17">
+      <c r="R271" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S271" s="17">
         <f t="shared" si="32"/>
         <v>138</v>
       </c>
-      <c r="T270" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A271" s="13" t="s">
+      <c r="T271" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="272" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A272" s="13" t="s">
         <v>946</v>
       </c>
-      <c r="B271" s="17">
+      <c r="B272" s="17">
         <v>2023</v>
       </c>
-      <c r="C271" s="9" t="s">
+      <c r="C272" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D271" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E271" s="9" t="s">
+      <c r="D272" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E272" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F271" s="17">
+      <c r="F272" s="17">
         <v>963</v>
       </c>
-      <c r="G271" s="9" t="s">
+      <c r="G272" s="9" t="s">
         <v>937</v>
       </c>
-      <c r="H271" s="9">
-        <f t="shared" ref="H271" si="51">YEAR(G271)</f>
+      <c r="H272" s="9">
+        <f t="shared" ref="H272" si="51">YEAR(G272)</f>
         <v>2024</v>
       </c>
-      <c r="I271" s="9">
-        <f t="shared" ref="I271" si="52">MONTH(G271)</f>
+      <c r="I272" s="9">
+        <f t="shared" ref="I272" si="52">MONTH(G272)</f>
         <v>2</v>
       </c>
-      <c r="J271" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K271" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L271" s="9" t="s">
+      <c r="J272" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K272" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L272" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="M271" s="17">
+      <c r="M272" s="17">
         <v>3</v>
       </c>
-      <c r="N271" s="17">
+      <c r="N272" s="17">
         <v>65.23</v>
       </c>
-      <c r="O271" s="9" t="s">
+      <c r="O272" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P271" s="13" t="s">
+      <c r="P272" s="13" t="s">
         <v>947</v>
       </c>
-      <c r="Q271" s="9" t="s">
+      <c r="Q272" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R271" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S271" s="17">
+      <c r="R272" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S272" s="17">
         <f t="shared" si="32"/>
         <v>90</v>
       </c>
-      <c r="T271" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A272" s="13" t="s">
+      <c r="T272" s="14">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="273" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A273" s="13" t="s">
         <v>948</v>
       </c>
-      <c r="B272" s="17">
+      <c r="B273" s="17">
         <v>2024</v>
       </c>
-      <c r="C272" s="9" t="s">
+      <c r="C273" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D272" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E272" s="9" t="s">
+      <c r="D273" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E273" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F272" s="17">
+      <c r="F273" s="17">
         <v>229</v>
       </c>
-      <c r="G272" s="9" t="s">
+      <c r="G273" s="9" t="s">
         <v>937</v>
       </c>
-      <c r="H272" s="9">
-        <f t="shared" ref="H272:H273" si="53">YEAR(G272)</f>
+      <c r="H273" s="9">
+        <f t="shared" ref="H273:H274" si="53">YEAR(G273)</f>
         <v>2024</v>
       </c>
-      <c r="I272" s="9">
-        <f t="shared" ref="I272:I273" si="54">MONTH(G272)</f>
+      <c r="I273" s="9">
+        <f t="shared" ref="I273:I274" si="54">MONTH(G273)</f>
         <v>2</v>
       </c>
-      <c r="J272" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K272" s="9" t="s">
+      <c r="J273" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K273" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="L272" s="9" t="s">
+      <c r="L273" s="9" t="s">
         <v>941</v>
       </c>
-      <c r="M272" s="17">
+      <c r="M273" s="17">
         <v>2</v>
       </c>
-      <c r="N272" s="17">
+      <c r="N273" s="17">
         <v>54.99</v>
       </c>
-      <c r="O272" s="9" t="s">
+      <c r="O273" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P272" s="13" t="s">
+      <c r="P273" s="13" t="s">
         <v>949</v>
       </c>
-      <c r="Q272" s="9" t="s">
+      <c r="Q273" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R272" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S272" s="17">
+      <c r="R273" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S273" s="17">
         <f t="shared" si="32"/>
         <v>75</v>
       </c>
-      <c r="T272" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A273" s="13" t="s">
+      <c r="T273" s="14">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="274" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A274" s="13" t="s">
         <v>950</v>
       </c>
-      <c r="B273" s="17">
+      <c r="B274" s="17">
         <v>2018</v>
       </c>
-      <c r="C273" s="9" t="s">
+      <c r="C274" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D273" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E273" s="9" t="s">
+      <c r="D274" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E274" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F273" s="17">
+      <c r="F274" s="17">
         <v>978</v>
       </c>
-      <c r="G273" s="9" t="s">
+      <c r="G274" s="9" t="s">
         <v>951</v>
       </c>
-      <c r="H273" s="9">
+      <c r="H274" s="9">
         <f t="shared" si="53"/>
         <v>2024</v>
       </c>
-      <c r="I273" s="9">
+      <c r="I274" s="9">
         <f t="shared" si="54"/>
         <v>2</v>
       </c>
-      <c r="J273" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K273" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L273" s="9" t="s">
+      <c r="J274" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K274" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L274" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="M273" s="17">
+      <c r="M274" s="17">
         <v>2</v>
       </c>
-      <c r="N273" s="17">
+      <c r="N274" s="17">
         <v>33.99</v>
       </c>
-      <c r="O273" s="9" t="s">
+      <c r="O274" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P273" s="13" t="s">
+      <c r="P274" s="13" t="s">
         <v>952</v>
       </c>
-      <c r="Q273" s="9" t="s">
+      <c r="Q274" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R273" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S273" s="17">
+      <c r="R274" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S274" s="17">
         <f t="shared" si="32"/>
         <v>125</v>
       </c>
-      <c r="T273" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A274" s="13" t="s">
+      <c r="T274" s="14">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="275" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A275" s="13" t="s">
         <v>953</v>
       </c>
-      <c r="B274" s="17">
+      <c r="B275" s="17">
         <v>2022</v>
       </c>
-      <c r="C274" s="9" t="s">
+      <c r="C275" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D274" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E274" s="9" t="s">
+      <c r="D275" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E275" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F274" s="17">
+      <c r="F275" s="17">
         <v>264</v>
       </c>
-      <c r="G274" s="9" t="s">
+      <c r="G275" s="9" t="s">
         <v>951</v>
       </c>
-      <c r="H274" s="9">
-        <f t="shared" ref="H274" si="55">YEAR(G274)</f>
+      <c r="H275" s="9">
+        <f t="shared" ref="H275" si="55">YEAR(G275)</f>
         <v>2024</v>
       </c>
-      <c r="I274" s="9">
-        <f t="shared" ref="I274" si="56">MONTH(G274)</f>
+      <c r="I275" s="9">
+        <f t="shared" ref="I275" si="56">MONTH(G275)</f>
         <v>2</v>
       </c>
-      <c r="J274" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K274" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L274" s="9" t="s">
+      <c r="J275" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K275" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L275" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="M274" s="17">
+      <c r="M275" s="17">
         <v>3</v>
       </c>
-      <c r="N274" s="17">
+      <c r="N275" s="17">
         <v>39.49</v>
       </c>
-      <c r="O274" s="9" t="s">
+      <c r="O275" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P274" s="13" t="s">
+      <c r="P275" s="13" t="s">
         <v>954</v>
       </c>
-      <c r="Q274" s="9" t="s">
+      <c r="Q275" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R274" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S274" s="17">
+      <c r="R275" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S275" s="17">
         <f t="shared" si="32"/>
         <v>59</v>
       </c>
-      <c r="T274" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A275" s="13" t="s">
+      <c r="T275" s="14">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="276" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A276" s="13" t="s">
         <v>955</v>
       </c>
-      <c r="B275" s="17">
+      <c r="B276" s="17">
         <v>2022</v>
       </c>
-      <c r="C275" s="9" t="s">
+      <c r="C276" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D275" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E275" s="9" t="s">
+      <c r="D276" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E276" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F275" s="17">
+      <c r="F276" s="17">
         <v>243</v>
       </c>
-      <c r="G275" s="9" t="s">
+      <c r="G276" s="9" t="s">
         <v>951</v>
       </c>
-      <c r="H275" s="9">
-        <f t="shared" ref="H275:H278" si="57">YEAR(G275)</f>
+      <c r="H276" s="9">
+        <f t="shared" ref="H276:H279" si="57">YEAR(G276)</f>
         <v>2024</v>
       </c>
-      <c r="I275" s="9">
-        <f t="shared" ref="I275" si="58">MONTH(G275)</f>
+      <c r="I276" s="9">
+        <f t="shared" ref="I276" si="58">MONTH(G276)</f>
         <v>2</v>
       </c>
-      <c r="J275" s="9" t="s">
+      <c r="J276" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="K275" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L275" s="9" t="s">
+      <c r="K276" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L276" s="9" t="s">
         <v>944</v>
       </c>
-      <c r="M275" s="17">
-        <v>4</v>
-      </c>
-      <c r="N275" s="17">
+      <c r="M276" s="17">
+        <v>4</v>
+      </c>
+      <c r="N276" s="17">
         <v>48.95</v>
       </c>
-      <c r="O275" s="9" t="s">
+      <c r="O276" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P275" s="13" t="s">
+      <c r="P276" s="13" t="s">
         <v>956</v>
       </c>
-      <c r="Q275" s="9" t="s">
+      <c r="Q276" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="R275" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S275" s="17">
+      <c r="R276" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S276" s="17">
         <f t="shared" si="32"/>
         <v>140</v>
       </c>
-      <c r="T275" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A276" s="13" t="s">
-        <v>957</v>
-      </c>
-      <c r="B276" s="17">
-        <v>2024</v>
-      </c>
-      <c r="C276" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D276" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E276" s="9" t="s">
-        <v>666</v>
-      </c>
-      <c r="F276" s="17">
-        <v>337</v>
-      </c>
-      <c r="G276" s="9" t="s">
-        <v>958</v>
-      </c>
-      <c r="H276" s="9">
-        <f t="shared" si="57"/>
-        <v>2024</v>
-      </c>
-      <c r="I276" s="9">
-        <f t="shared" ref="I276:I282" si="59">MONTH(G276)</f>
-        <v>5</v>
-      </c>
-      <c r="J276" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K276" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L276" s="9" t="s">
-        <v>376</v>
-      </c>
-      <c r="M276" s="17">
-        <v>1</v>
-      </c>
-      <c r="N276" s="17">
-        <v>24.99</v>
-      </c>
-      <c r="O276" s="9" t="s">
-        <v>664</v>
-      </c>
-      <c r="P276" s="13" t="s">
-        <v>960</v>
-      </c>
-      <c r="Q276" s="9" t="s">
-        <v>959</v>
-      </c>
-      <c r="R276" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S276" s="17">
-        <f t="shared" si="32"/>
-        <v>168</v>
-      </c>
       <c r="T276" s="14">
-        <v>0</v>
+        <v>354</v>
       </c>
     </row>
     <row r="277" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A277" s="13" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="B277" s="17">
         <v>2024</v>
@@ -28975,7 +28984,7 @@
         <v>666</v>
       </c>
       <c r="F277" s="17">
-        <v>253</v>
+        <v>337</v>
       </c>
       <c r="G277" s="9" t="s">
         <v>958</v>
@@ -28985,7 +28994,7 @@
         <v>2024</v>
       </c>
       <c r="I277" s="9">
-        <f t="shared" si="59"/>
+        <f t="shared" ref="I277:I283" si="59">MONTH(G277)</f>
         <v>5</v>
       </c>
       <c r="J277" s="9" t="s">
@@ -29007,7 +29016,7 @@
         <v>664</v>
       </c>
       <c r="P277" s="13" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="Q277" s="9" t="s">
         <v>959</v>
@@ -29017,15 +29026,15 @@
       </c>
       <c r="S277" s="17">
         <f t="shared" si="32"/>
-        <v>99</v>
+        <v>168</v>
       </c>
       <c r="T277" s="14">
-        <v>0</v>
+        <v>317</v>
       </c>
     </row>
     <row r="278" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A278" s="13" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="B278" s="17">
         <v>2024</v>
@@ -29040,10 +29049,10 @@
         <v>666</v>
       </c>
       <c r="F278" s="17">
-        <v>316</v>
+        <v>253</v>
       </c>
       <c r="G278" s="9" t="s">
-        <v>965</v>
+        <v>958</v>
       </c>
       <c r="H278" s="9">
         <f t="shared" si="57"/>
@@ -29051,7 +29060,7 @@
       </c>
       <c r="I278" s="9">
         <f t="shared" si="59"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J278" s="9" t="s">
         <v>159</v>
@@ -29060,19 +29069,19 @@
         <v>159</v>
       </c>
       <c r="L278" s="9" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="M278" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N278" s="17">
-        <v>44.99</v>
+        <v>24.99</v>
       </c>
       <c r="O278" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P278" s="13" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="Q278" s="9" t="s">
         <v>959</v>
@@ -29082,15 +29091,15 @@
       </c>
       <c r="S278" s="17">
         <f t="shared" si="32"/>
-        <v>280</v>
+        <v>99</v>
       </c>
       <c r="T278" s="14">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="279" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A279" s="13" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B279" s="17">
         <v>2024</v>
@@ -29105,13 +29114,13 @@
         <v>666</v>
       </c>
       <c r="F279" s="17">
-        <v>112</v>
+        <v>316</v>
       </c>
       <c r="G279" s="9" t="s">
         <v>965</v>
       </c>
       <c r="H279" s="9">
-        <f t="shared" ref="H279" si="60">YEAR(G279)</f>
+        <f t="shared" si="57"/>
         <v>2024</v>
       </c>
       <c r="I279" s="9">
@@ -29125,37 +29134,37 @@
         <v>159</v>
       </c>
       <c r="L279" s="9" t="s">
-        <v>993</v>
+        <v>365</v>
       </c>
       <c r="M279" s="17">
         <v>3</v>
       </c>
-      <c r="N279" s="43">
-        <v>0</v>
+      <c r="N279" s="17">
+        <v>44.99</v>
       </c>
       <c r="O279" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P279" s="13" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="Q279" s="9" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="R279" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S279" s="17">
         <f t="shared" si="32"/>
-        <v>84</v>
+        <v>280</v>
       </c>
       <c r="T279" s="14">
-        <v>0</v>
+        <v>236</v>
       </c>
     </row>
     <row r="280" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A280" s="13" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B280" s="17">
         <v>2024</v>
@@ -29170,13 +29179,13 @@
         <v>666</v>
       </c>
       <c r="F280" s="17">
-        <v>1779</v>
+        <v>112</v>
       </c>
       <c r="G280" s="9" t="s">
         <v>965</v>
       </c>
       <c r="H280" s="9">
-        <f t="shared" ref="H280:H282" si="61">YEAR(G280)</f>
+        <f t="shared" ref="H280" si="60">YEAR(G280)</f>
         <v>2024</v>
       </c>
       <c r="I280" s="9">
@@ -29190,19 +29199,19 @@
         <v>159</v>
       </c>
       <c r="L280" s="9" t="s">
-        <v>365</v>
+        <v>993</v>
       </c>
       <c r="M280" s="17">
         <v>3</v>
       </c>
-      <c r="N280" s="17">
-        <v>40.549999999999997</v>
+      <c r="N280" s="43">
+        <v>0</v>
       </c>
       <c r="O280" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P280" s="13" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="Q280" s="9" t="s">
         <v>963</v>
@@ -29212,18 +29221,18 @@
       </c>
       <c r="S280" s="17">
         <f t="shared" si="32"/>
-        <v>152</v>
+        <v>84</v>
       </c>
       <c r="T280" s="14">
-        <v>0</v>
+        <v>286</v>
       </c>
     </row>
     <row r="281" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A281" s="13" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B281" s="17">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C281" s="9" t="s">
         <v>21</v>
@@ -29235,13 +29244,13 @@
         <v>666</v>
       </c>
       <c r="F281" s="17">
-        <v>365</v>
+        <v>1779</v>
       </c>
       <c r="G281" s="9" t="s">
-        <v>972</v>
+        <v>965</v>
       </c>
       <c r="H281" s="9">
-        <f t="shared" si="61"/>
+        <f t="shared" ref="H281:H283" si="61">YEAR(G281)</f>
         <v>2024</v>
       </c>
       <c r="I281" s="9">
@@ -29258,37 +29267,37 @@
         <v>365</v>
       </c>
       <c r="M281" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N281" s="17">
-        <v>49.15</v>
+        <v>40.549999999999997</v>
       </c>
       <c r="O281" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P281" s="16" t="s">
-        <v>973</v>
+      <c r="P281" s="13" t="s">
+        <v>970</v>
       </c>
       <c r="Q281" s="9" t="s">
-        <v>904</v>
+        <v>963</v>
       </c>
       <c r="R281" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S281" s="17">
         <f t="shared" si="32"/>
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="T281" s="14">
-        <v>0</v>
+        <v>259</v>
       </c>
     </row>
     <row r="282" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A282" s="13" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="B282" s="17">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C282" s="9" t="s">
         <v>21</v>
@@ -29300,10 +29309,10 @@
         <v>666</v>
       </c>
       <c r="F282" s="17">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="G282" s="9" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="H282" s="9">
         <f t="shared" si="61"/>
@@ -29311,7 +29320,7 @@
       </c>
       <c r="I282" s="9">
         <f t="shared" si="59"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J282" s="9" t="s">
         <v>159</v>
@@ -29320,29 +29329,29 @@
         <v>159</v>
       </c>
       <c r="L282" s="9" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="M282" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N282" s="17">
-        <v>50.21</v>
+        <v>49.15</v>
       </c>
       <c r="O282" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P282" s="13" t="s">
-        <v>976</v>
+      <c r="P282" s="16" t="s">
+        <v>973</v>
       </c>
       <c r="Q282" s="9" t="s">
-        <v>469</v>
+        <v>904</v>
       </c>
       <c r="R282" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S282" s="17">
         <f t="shared" si="32"/>
-        <v>64</v>
+        <v>160</v>
       </c>
       <c r="T282" s="14">
         <v>0</v>
@@ -29350,7 +29359,7 @@
     </row>
     <row r="283" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A283" s="13" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B283" s="17">
         <v>2023</v>
@@ -29365,17 +29374,17 @@
         <v>666</v>
       </c>
       <c r="F283" s="17">
-        <v>600</v>
+        <v>340</v>
       </c>
       <c r="G283" s="9" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="H283" s="9">
-        <f t="shared" ref="H283" si="62">YEAR(G283)</f>
+        <f t="shared" si="61"/>
         <v>2024</v>
       </c>
       <c r="I283" s="9">
-        <f t="shared" ref="I283" si="63">MONTH(G283)</f>
+        <f t="shared" si="59"/>
         <v>7</v>
       </c>
       <c r="J283" s="9" t="s">
@@ -29385,19 +29394,19 @@
         <v>159</v>
       </c>
       <c r="L283" s="9" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="M283" s="17">
         <v>2</v>
       </c>
       <c r="N283" s="17">
-        <v>43.13</v>
+        <v>50.21</v>
       </c>
       <c r="O283" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P283" s="13" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="Q283" s="9" t="s">
         <v>469</v>
@@ -29407,7 +29416,7 @@
       </c>
       <c r="S283" s="17">
         <f t="shared" si="32"/>
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="T283" s="14">
         <v>0</v>
@@ -29415,10 +29424,10 @@
     </row>
     <row r="284" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A284" s="13" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="B284" s="17">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C284" s="9" t="s">
         <v>21</v>
@@ -29430,17 +29439,17 @@
         <v>666</v>
       </c>
       <c r="F284" s="17">
-        <v>289</v>
+        <v>600</v>
       </c>
       <c r="G284" s="9" t="s">
         <v>978</v>
       </c>
       <c r="H284" s="9">
-        <f t="shared" ref="H284" si="64">YEAR(G284)</f>
+        <f t="shared" ref="H284" si="62">YEAR(G284)</f>
         <v>2024</v>
       </c>
       <c r="I284" s="9">
-        <f t="shared" ref="I284" si="65">MONTH(G284)</f>
+        <f t="shared" ref="I284" si="63">MONTH(G284)</f>
         <v>7</v>
       </c>
       <c r="J284" s="9" t="s">
@@ -29450,29 +29459,29 @@
         <v>159</v>
       </c>
       <c r="L284" s="9" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="M284" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N284" s="17">
-        <v>49.71</v>
+        <v>43.13</v>
       </c>
       <c r="O284" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P284" s="13" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="Q284" s="9" t="s">
-        <v>569</v>
+        <v>469</v>
       </c>
       <c r="R284" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S284" s="17">
         <f t="shared" si="32"/>
-        <v>224</v>
+        <v>106</v>
       </c>
       <c r="T284" s="14">
         <v>0</v>
@@ -29480,7 +29489,7 @@
     </row>
     <row r="285" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A285" s="13" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B285" s="17">
         <v>2024</v>
@@ -29495,17 +29504,17 @@
         <v>666</v>
       </c>
       <c r="F285" s="17">
-        <v>198</v>
+        <v>289</v>
       </c>
       <c r="G285" s="9" t="s">
         <v>978</v>
       </c>
       <c r="H285" s="9">
-        <f t="shared" ref="H285" si="66">YEAR(G285)</f>
+        <f t="shared" ref="H285" si="64">YEAR(G285)</f>
         <v>2024</v>
       </c>
       <c r="I285" s="9">
-        <f t="shared" ref="I285" si="67">MONTH(G285)</f>
+        <f t="shared" ref="I285" si="65">MONTH(G285)</f>
         <v>7</v>
       </c>
       <c r="J285" s="9" t="s">
@@ -29515,29 +29524,29 @@
         <v>159</v>
       </c>
       <c r="L285" s="9" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="M285" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N285" s="17">
-        <v>22.94</v>
+        <v>49.71</v>
       </c>
       <c r="O285" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P285" s="16" t="s">
-        <v>983</v>
+      <c r="P285" s="13" t="s">
+        <v>981</v>
       </c>
       <c r="Q285" s="9" t="s">
-        <v>963</v>
+        <v>569</v>
       </c>
       <c r="R285" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S285" s="17">
         <f t="shared" si="32"/>
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="T285" s="14">
         <v>0</v>
@@ -29545,7 +29554,7 @@
     </row>
     <row r="286" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A286" s="13" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B286" s="17">
         <v>2024</v>
@@ -29560,17 +29569,17 @@
         <v>666</v>
       </c>
       <c r="F286" s="17">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="G286" s="9" t="s">
         <v>978</v>
       </c>
       <c r="H286" s="9">
-        <f t="shared" ref="H286" si="68">YEAR(G286)</f>
+        <f t="shared" ref="H286" si="66">YEAR(G286)</f>
         <v>2024</v>
       </c>
       <c r="I286" s="9">
-        <f t="shared" ref="I286" si="69">MONTH(G286)</f>
+        <f t="shared" ref="I286" si="67">MONTH(G286)</f>
         <v>7</v>
       </c>
       <c r="J286" s="9" t="s">
@@ -29580,19 +29589,19 @@
         <v>159</v>
       </c>
       <c r="L286" s="9" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="M286" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N286" s="17">
-        <v>16.690000000000001</v>
+        <v>22.94</v>
       </c>
       <c r="O286" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P286" s="16" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="Q286" s="9" t="s">
         <v>963</v>
@@ -29602,7 +29611,7 @@
       </c>
       <c r="S286" s="17">
         <f t="shared" si="32"/>
-        <v>186</v>
+        <v>233</v>
       </c>
       <c r="T286" s="14">
         <v>0</v>
@@ -29610,10 +29619,10 @@
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A287" s="13" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B287" s="17">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C287" s="9" t="s">
         <v>21</v>
@@ -29625,17 +29634,17 @@
         <v>666</v>
       </c>
       <c r="F287" s="17">
-        <v>296</v>
+        <v>224</v>
       </c>
       <c r="G287" s="9" t="s">
-        <v>987</v>
+        <v>978</v>
       </c>
       <c r="H287" s="9">
-        <f t="shared" ref="H287" si="70">YEAR(G287)</f>
+        <f t="shared" ref="H287" si="68">YEAR(G287)</f>
         <v>2024</v>
       </c>
       <c r="I287" s="9">
-        <f t="shared" ref="I287" si="71">MONTH(G287)</f>
+        <f t="shared" ref="I287" si="69">MONTH(G287)</f>
         <v>7</v>
       </c>
       <c r="J287" s="9" t="s">
@@ -29645,19 +29654,19 @@
         <v>159</v>
       </c>
       <c r="L287" s="9" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="M287" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N287" s="17">
-        <v>31.99</v>
+        <v>16.690000000000001</v>
       </c>
       <c r="O287" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P287" s="16" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="Q287" s="9" t="s">
         <v>963</v>
@@ -29666,8 +29675,8 @@
         <v>159</v>
       </c>
       <c r="S287" s="17">
-        <f t="shared" ref="S287" si="72">LEN(P287)</f>
-        <v>98</v>
+        <f t="shared" si="32"/>
+        <v>186</v>
       </c>
       <c r="T287" s="14">
         <v>0</v>
@@ -29675,10 +29684,10 @@
     </row>
     <row r="288" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A288" s="13" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="B288" s="17">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C288" s="9" t="s">
         <v>21</v>
@@ -29690,17 +29699,17 @@
         <v>666</v>
       </c>
       <c r="F288" s="17">
-        <v>200</v>
+        <v>296</v>
       </c>
       <c r="G288" s="9" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="H288" s="9">
-        <f t="shared" ref="H288" si="73">YEAR(G288)</f>
+        <f t="shared" ref="H288" si="70">YEAR(G288)</f>
         <v>2024</v>
       </c>
       <c r="I288" s="9">
-        <f t="shared" ref="I288" si="74">MONTH(G288)</f>
+        <f t="shared" ref="I288" si="71">MONTH(G288)</f>
         <v>7</v>
       </c>
       <c r="J288" s="9" t="s">
@@ -29710,19 +29719,19 @@
         <v>159</v>
       </c>
       <c r="L288" s="9" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="M288" s="17">
         <v>3</v>
       </c>
       <c r="N288" s="17">
-        <v>27.99</v>
+        <v>31.99</v>
       </c>
       <c r="O288" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P288" s="16" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="Q288" s="9" t="s">
         <v>963</v>
@@ -29731,8 +29740,8 @@
         <v>159</v>
       </c>
       <c r="S288" s="17">
-        <f t="shared" ref="S288" si="75">LEN(P288)</f>
-        <v>57</v>
+        <f t="shared" ref="S288" si="72">LEN(P288)</f>
+        <v>98</v>
       </c>
       <c r="T288" s="14">
         <v>0</v>
@@ -29740,7 +29749,7 @@
     </row>
     <row r="289" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A289" s="13" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B289" s="17">
         <v>2023</v>
@@ -29755,17 +29764,17 @@
         <v>666</v>
       </c>
       <c r="F289" s="17">
-        <v>255</v>
+        <v>200</v>
       </c>
       <c r="G289" s="9" t="s">
         <v>990</v>
       </c>
       <c r="H289" s="9">
-        <f t="shared" ref="H289" si="76">YEAR(G289)</f>
+        <f t="shared" ref="H289" si="73">YEAR(G289)</f>
         <v>2024</v>
       </c>
       <c r="I289" s="9">
-        <f t="shared" ref="I289" si="77">MONTH(G289)</f>
+        <f t="shared" ref="I289" si="74">MONTH(G289)</f>
         <v>7</v>
       </c>
       <c r="J289" s="9" t="s">
@@ -29775,29 +29784,29 @@
         <v>159</v>
       </c>
       <c r="L289" s="9" t="s">
-        <v>602</v>
+        <v>370</v>
       </c>
       <c r="M289" s="17">
         <v>3</v>
       </c>
-      <c r="N289" s="43">
-        <v>49</v>
+      <c r="N289" s="17">
+        <v>27.99</v>
       </c>
       <c r="O289" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P289" s="16" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="Q289" s="9" t="s">
-        <v>469</v>
+        <v>963</v>
       </c>
       <c r="R289" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S289" s="17">
-        <f t="shared" ref="S289" si="78">LEN(P289)</f>
-        <v>84</v>
+        <f t="shared" ref="S289" si="75">LEN(P289)</f>
+        <v>57</v>
       </c>
       <c r="T289" s="14">
         <v>0</v>
@@ -29805,7 +29814,7 @@
     </row>
     <row r="290" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A290" s="13" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="B290" s="17">
         <v>2023</v>
@@ -29820,17 +29829,17 @@
         <v>666</v>
       </c>
       <c r="F290" s="17">
-        <v>192</v>
+        <v>255</v>
       </c>
       <c r="G290" s="9" t="s">
         <v>990</v>
       </c>
       <c r="H290" s="9">
-        <f t="shared" ref="H290" si="79">YEAR(G290)</f>
+        <f t="shared" ref="H290" si="76">YEAR(G290)</f>
         <v>2024</v>
       </c>
       <c r="I290" s="9">
-        <f t="shared" ref="I290" si="80">MONTH(G290)</f>
+        <f t="shared" ref="I290" si="77">MONTH(G290)</f>
         <v>7</v>
       </c>
       <c r="J290" s="9" t="s">
@@ -29840,29 +29849,29 @@
         <v>159</v>
       </c>
       <c r="L290" s="9" t="s">
-        <v>365</v>
+        <v>602</v>
       </c>
       <c r="M290" s="17">
-        <v>2</v>
-      </c>
-      <c r="N290" s="17">
-        <v>26.01</v>
+        <v>3</v>
+      </c>
+      <c r="N290" s="43">
+        <v>49</v>
       </c>
       <c r="O290" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P290" s="16" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="Q290" s="9" t="s">
-        <v>963</v>
+        <v>469</v>
       </c>
       <c r="R290" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S290" s="17">
-        <f t="shared" ref="S290:S303" si="81">LEN(P290)</f>
-        <v>152</v>
+        <f t="shared" ref="S290" si="78">LEN(P290)</f>
+        <v>84</v>
       </c>
       <c r="T290" s="14">
         <v>0</v>
@@ -29870,10 +29879,10 @@
     </row>
     <row r="291" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A291" s="13" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B291" s="17">
-        <v>2015</v>
+        <v>2023</v>
       </c>
       <c r="C291" s="9" t="s">
         <v>21</v>
@@ -29885,17 +29894,17 @@
         <v>666</v>
       </c>
       <c r="F291" s="17">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="G291" s="9" t="s">
         <v>990</v>
       </c>
       <c r="H291" s="9">
-        <f t="shared" ref="H291" si="82">YEAR(G291)</f>
+        <f t="shared" ref="H291" si="79">YEAR(G291)</f>
         <v>2024</v>
       </c>
       <c r="I291" s="9">
-        <f t="shared" ref="I291" si="83">MONTH(G291)</f>
+        <f t="shared" ref="I291" si="80">MONTH(G291)</f>
         <v>7</v>
       </c>
       <c r="J291" s="9" t="s">
@@ -29905,19 +29914,19 @@
         <v>159</v>
       </c>
       <c r="L291" s="9" t="s">
-        <v>993</v>
+        <v>365</v>
       </c>
       <c r="M291" s="17">
-        <v>3</v>
-      </c>
-      <c r="N291" s="43">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="N291" s="17">
+        <v>26.01</v>
       </c>
       <c r="O291" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P291" s="28" t="s">
-        <v>707</v>
+      <c r="P291" s="16" t="s">
+        <v>996</v>
       </c>
       <c r="Q291" s="9" t="s">
         <v>963</v>
@@ -29926,214 +29935,214 @@
         <v>159</v>
       </c>
       <c r="S291" s="17">
+        <f t="shared" ref="S291:S304" si="81">LEN(P291)</f>
+        <v>152</v>
+      </c>
+      <c r="T291" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A292" s="13" t="s">
+        <v>997</v>
+      </c>
+      <c r="B292" s="17">
+        <v>2015</v>
+      </c>
+      <c r="C292" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D292" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E292" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F292" s="17">
+        <v>96</v>
+      </c>
+      <c r="G292" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="H292" s="9">
+        <f t="shared" ref="H292" si="82">YEAR(G292)</f>
+        <v>2024</v>
+      </c>
+      <c r="I292" s="9">
+        <f t="shared" ref="I292" si="83">MONTH(G292)</f>
+        <v>7</v>
+      </c>
+      <c r="J292" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K292" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L292" s="9" t="s">
+        <v>993</v>
+      </c>
+      <c r="M292" s="17">
+        <v>3</v>
+      </c>
+      <c r="N292" s="43">
+        <v>0</v>
+      </c>
+      <c r="O292" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P292" s="28" t="s">
+        <v>707</v>
+      </c>
+      <c r="Q292" s="9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R292" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S292" s="17">
         <f t="shared" si="81"/>
         <v>26</v>
       </c>
-      <c r="T291" s="14">
+      <c r="T292" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A292" s="13" t="s">
+    <row r="293" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A293" s="13" t="s">
         <v>998</v>
       </c>
-      <c r="B292" s="17">
+      <c r="B293" s="17">
         <v>2022</v>
       </c>
-      <c r="C292" s="9" t="s">
+      <c r="C293" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D292" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E292" s="9" t="s">
+      <c r="D293" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E293" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F292" s="17">
+      <c r="F293" s="17">
         <v>194</v>
       </c>
-      <c r="G292" s="9" t="s">
+      <c r="G293" s="9" t="s">
         <v>999</v>
       </c>
-      <c r="H292" s="9">
-        <f t="shared" ref="H292" si="84">YEAR(G292)</f>
+      <c r="H293" s="9">
+        <f t="shared" ref="H293" si="84">YEAR(G293)</f>
         <v>2024</v>
       </c>
-      <c r="I292" s="9">
-        <f t="shared" ref="I292" si="85">MONTH(G292)</f>
+      <c r="I293" s="9">
+        <f t="shared" ref="I293" si="85">MONTH(G293)</f>
         <v>7</v>
       </c>
-      <c r="J292" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K292" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L292" s="9" t="s">
+      <c r="J293" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K293" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L293" s="9" t="s">
         <v>993</v>
       </c>
-      <c r="M292" s="17">
+      <c r="M293" s="17">
         <v>3</v>
       </c>
-      <c r="N292" s="43">
+      <c r="N293" s="43">
         <v>0</v>
       </c>
-      <c r="O292" s="9" t="s">
+      <c r="O293" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P292" s="28" t="s">
+      <c r="P293" s="28" t="s">
         <v>1000</v>
       </c>
-      <c r="Q292" s="9" t="s">
+      <c r="Q293" s="9" t="s">
         <v>963</v>
       </c>
-      <c r="R292" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S292" s="17">
+      <c r="R293" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S293" s="17">
         <f t="shared" si="81"/>
         <v>38</v>
       </c>
-      <c r="T292" s="14">
+      <c r="T293" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A293" s="13" t="s">
+    <row r="294" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A294" s="13" t="s">
         <v>1001</v>
       </c>
-      <c r="B293" s="17">
+      <c r="B294" s="17">
         <v>2018</v>
       </c>
-      <c r="C293" s="9" t="s">
+      <c r="C294" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D293" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E293" s="9" t="s">
+      <c r="D294" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E294" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="F293" s="17">
+      <c r="F294" s="17">
         <v>188</v>
       </c>
-      <c r="G293" s="9" t="s">
+      <c r="G294" s="9" t="s">
         <v>1002</v>
       </c>
-      <c r="H293" s="9">
-        <f t="shared" ref="H293:H295" si="86">YEAR(G293)</f>
+      <c r="H294" s="9">
+        <f t="shared" ref="H294:H296" si="86">YEAR(G294)</f>
         <v>2024</v>
       </c>
-      <c r="I293" s="9">
-        <f t="shared" ref="I293:I295" si="87">MONTH(G293)</f>
+      <c r="I294" s="9">
+        <f t="shared" ref="I294:I296" si="87">MONTH(G294)</f>
         <v>7</v>
       </c>
-      <c r="J293" s="9" t="s">
+      <c r="J294" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="K293" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L293" s="9" t="s">
+      <c r="K294" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L294" s="9" t="s">
         <v>1003</v>
       </c>
-      <c r="M293" s="17">
-        <v>4</v>
-      </c>
-      <c r="N293" s="43">
+      <c r="M294" s="17">
+        <v>4</v>
+      </c>
+      <c r="N294" s="43">
         <v>48</v>
       </c>
-      <c r="O293" s="9" t="s">
+      <c r="O294" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P293" s="16" t="s">
+      <c r="P294" s="16" t="s">
         <v>1004</v>
       </c>
-      <c r="Q293" s="9" t="s">
+      <c r="Q294" s="9" t="s">
         <v>469</v>
       </c>
-      <c r="R293" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S293" s="17">
+      <c r="R294" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S294" s="17">
         <f t="shared" si="81"/>
         <v>268</v>
       </c>
-      <c r="T293" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A294" s="13" t="s">
-        <v>1005</v>
-      </c>
-      <c r="B294" s="17">
-        <v>2021</v>
-      </c>
-      <c r="C294" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D294" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E294" s="9" t="s">
-        <v>666</v>
-      </c>
-      <c r="F294" s="17">
-        <v>631</v>
-      </c>
-      <c r="G294" s="9" t="s">
-        <v>1006</v>
-      </c>
-      <c r="H294" s="9">
-        <f t="shared" si="86"/>
-        <v>2024</v>
-      </c>
-      <c r="I294" s="9">
-        <f t="shared" si="87"/>
-        <v>7</v>
-      </c>
-      <c r="J294" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="K294" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L294" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="M294" s="17">
-        <v>3</v>
-      </c>
-      <c r="N294" s="17">
-        <v>49.99</v>
-      </c>
-      <c r="O294" s="9" t="s">
-        <v>664</v>
-      </c>
-      <c r="P294" s="16" t="s">
-        <v>1007</v>
-      </c>
-      <c r="Q294" s="9" t="s">
-        <v>569</v>
-      </c>
-      <c r="R294" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S294" s="17">
-        <f t="shared" si="81"/>
-        <v>131</v>
-      </c>
       <c r="T294" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A295" s="13" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="B295" s="17">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C295" s="9" t="s">
         <v>21</v>
@@ -30145,10 +30154,10 @@
         <v>666</v>
       </c>
       <c r="F295" s="17">
-        <v>318</v>
+        <v>631</v>
       </c>
       <c r="G295" s="9" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="H295" s="9">
         <f t="shared" si="86"/>
@@ -30168,7 +30177,7 @@
         <v>365</v>
       </c>
       <c r="M295" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N295" s="17">
         <v>49.99</v>
@@ -30177,17 +30186,17 @@
         <v>664</v>
       </c>
       <c r="P295" s="16" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="Q295" s="9" t="s">
-        <v>874</v>
+        <v>569</v>
       </c>
       <c r="R295" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S295" s="17">
         <f t="shared" si="81"/>
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="T295" s="14">
         <v>0</v>
@@ -30195,7 +30204,7 @@
     </row>
     <row r="296" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A296" s="13" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="B296" s="17">
         <v>2023</v>
@@ -30210,17 +30219,17 @@
         <v>666</v>
       </c>
       <c r="F296" s="17">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="G296" s="9" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="H296" s="9">
-        <f t="shared" ref="H296" si="88">YEAR(G296)</f>
+        <f t="shared" si="86"/>
         <v>2024</v>
       </c>
       <c r="I296" s="9">
-        <f t="shared" ref="I296" si="89">MONTH(G296)</f>
+        <f t="shared" si="87"/>
         <v>7</v>
       </c>
       <c r="J296" s="9" t="s">
@@ -30230,19 +30239,19 @@
         <v>159</v>
       </c>
       <c r="L296" s="9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="M296" s="17">
         <v>1</v>
       </c>
       <c r="N296" s="17">
-        <v>65.989999999999995</v>
+        <v>49.99</v>
       </c>
       <c r="O296" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P296" s="16" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="Q296" s="9" t="s">
         <v>874</v>
@@ -30252,7 +30261,7 @@
       </c>
       <c r="S296" s="17">
         <f t="shared" si="81"/>
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="T296" s="14">
         <v>0</v>
@@ -30260,7 +30269,7 @@
     </row>
     <row r="297" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A297" s="13" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B297" s="17">
         <v>2023</v>
@@ -30275,17 +30284,17 @@
         <v>666</v>
       </c>
       <c r="F297" s="17">
-        <v>636</v>
+        <v>298</v>
       </c>
       <c r="G297" s="9" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="H297" s="9">
-        <f t="shared" ref="H297" si="90">YEAR(G297)</f>
+        <f t="shared" ref="H297" si="88">YEAR(G297)</f>
         <v>2024</v>
       </c>
       <c r="I297" s="9">
-        <f t="shared" ref="I297" si="91">MONTH(G297)</f>
+        <f t="shared" ref="I297" si="89">MONTH(G297)</f>
         <v>7</v>
       </c>
       <c r="J297" s="9" t="s">
@@ -30295,13 +30304,13 @@
         <v>159</v>
       </c>
       <c r="L297" s="9" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="M297" s="17">
         <v>1</v>
       </c>
       <c r="N297" s="17">
-        <v>39.99</v>
+        <v>65.989999999999995</v>
       </c>
       <c r="O297" s="9" t="s">
         <v>664</v>
@@ -30310,7 +30319,7 @@
         <v>1013</v>
       </c>
       <c r="Q297" s="9" t="s">
-        <v>569</v>
+        <v>874</v>
       </c>
       <c r="R297" s="9" t="s">
         <v>159</v>
@@ -30324,8 +30333,8 @@
       </c>
     </row>
     <row r="298" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A298" s="16" t="s">
-        <v>1016</v>
+      <c r="A298" s="13" t="s">
+        <v>1014</v>
       </c>
       <c r="B298" s="17">
         <v>2023</v>
@@ -30340,17 +30349,17 @@
         <v>666</v>
       </c>
       <c r="F298" s="17">
-        <v>218</v>
+        <v>636</v>
       </c>
       <c r="G298" s="9" t="s">
         <v>1015</v>
       </c>
       <c r="H298" s="9">
-        <f t="shared" ref="H298" si="92">YEAR(G298)</f>
+        <f t="shared" ref="H298" si="90">YEAR(G298)</f>
         <v>2024</v>
       </c>
       <c r="I298" s="9">
-        <f t="shared" ref="I298" si="93">MONTH(G298)</f>
+        <f t="shared" ref="I298" si="91">MONTH(G298)</f>
         <v>7</v>
       </c>
       <c r="J298" s="9" t="s">
@@ -30360,19 +30369,19 @@
         <v>159</v>
       </c>
       <c r="L298" s="9" t="s">
-        <v>602</v>
+        <v>370</v>
       </c>
       <c r="M298" s="17">
         <v>1</v>
       </c>
       <c r="N298" s="17">
-        <v>19.989999999999998</v>
+        <v>39.99</v>
       </c>
       <c r="O298" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P298" s="16" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="Q298" s="9" t="s">
         <v>569</v>
@@ -30382,18 +30391,18 @@
       </c>
       <c r="S298" s="17">
         <f t="shared" si="81"/>
-        <v>247</v>
+        <v>55</v>
       </c>
       <c r="T298" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A299" s="13" t="s">
-        <v>1018</v>
+      <c r="A299" s="16" t="s">
+        <v>1016</v>
       </c>
       <c r="B299" s="17">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C299" s="9" t="s">
         <v>21</v>
@@ -30405,39 +30414,39 @@
         <v>666</v>
       </c>
       <c r="F299" s="17">
-        <v>464</v>
+        <v>218</v>
       </c>
       <c r="G299" s="9" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="H299" s="9">
-        <f t="shared" ref="H299" si="94">YEAR(G299)</f>
+        <f t="shared" ref="H299" si="92">YEAR(G299)</f>
         <v>2024</v>
       </c>
       <c r="I299" s="9">
-        <f t="shared" ref="I299" si="95">MONTH(G299)</f>
+        <f t="shared" ref="I299" si="93">MONTH(G299)</f>
         <v>7</v>
       </c>
       <c r="J299" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K299" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L299" s="9" t="s">
-        <v>880</v>
+        <v>602</v>
       </c>
       <c r="M299" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N299" s="17">
-        <v>24.95</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="O299" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P299" s="16" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q299" s="9" t="s">
         <v>569</v>
@@ -30447,7 +30456,7 @@
       </c>
       <c r="S299" s="17">
         <f t="shared" si="81"/>
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="T299" s="14">
         <v>0</v>
@@ -30455,10 +30464,10 @@
     </row>
     <row r="300" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A300" s="13" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="B300" s="17">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C300" s="9" t="s">
         <v>21</v>
@@ -30470,49 +30479,49 @@
         <v>666</v>
       </c>
       <c r="F300" s="17">
-        <v>58</v>
+        <v>464</v>
       </c>
       <c r="G300" s="9" t="s">
         <v>1019</v>
       </c>
       <c r="H300" s="9">
-        <f t="shared" ref="H300" si="96">YEAR(G300)</f>
+        <f t="shared" ref="H300" si="94">YEAR(G300)</f>
         <v>2024</v>
       </c>
       <c r="I300" s="9">
-        <f t="shared" ref="I300" si="97">MONTH(G300)</f>
+        <f t="shared" ref="I300" si="95">MONTH(G300)</f>
         <v>7</v>
       </c>
       <c r="J300" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K300" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L300" s="9" t="s">
-        <v>602</v>
+        <v>880</v>
       </c>
       <c r="M300" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N300" s="17">
-        <v>14.95</v>
+        <v>24.95</v>
       </c>
       <c r="O300" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P300" s="28" t="s">
-        <v>1022</v>
+      <c r="P300" s="16" t="s">
+        <v>1020</v>
       </c>
       <c r="Q300" s="9" t="s">
-        <v>959</v>
+        <v>569</v>
       </c>
       <c r="R300" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S300" s="17">
         <f t="shared" si="81"/>
-        <v>45</v>
+        <v>229</v>
       </c>
       <c r="T300" s="14">
         <v>0</v>
@@ -30520,7 +30529,7 @@
     </row>
     <row r="301" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A301" s="13" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B301" s="17">
         <v>2023</v>
@@ -30535,17 +30544,17 @@
         <v>666</v>
       </c>
       <c r="F301" s="17">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="G301" s="9" t="s">
         <v>1019</v>
       </c>
       <c r="H301" s="9">
-        <f t="shared" ref="H301" si="98">YEAR(G301)</f>
+        <f t="shared" ref="H301" si="96">YEAR(G301)</f>
         <v>2024</v>
       </c>
       <c r="I301" s="9">
-        <f t="shared" ref="I301" si="99">MONTH(G301)</f>
+        <f t="shared" ref="I301" si="97">MONTH(G301)</f>
         <v>7</v>
       </c>
       <c r="J301" s="9" t="s">
@@ -30555,29 +30564,29 @@
         <v>159</v>
       </c>
       <c r="L301" s="9" t="s">
-        <v>377</v>
+        <v>602</v>
       </c>
       <c r="M301" s="17">
         <v>2</v>
       </c>
-      <c r="N301" s="43">
-        <v>35</v>
+      <c r="N301" s="17">
+        <v>14.95</v>
       </c>
       <c r="O301" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P301" s="13" t="s">
-        <v>1024</v>
+      <c r="P301" s="28" t="s">
+        <v>1022</v>
       </c>
       <c r="Q301" s="9" t="s">
-        <v>904</v>
+        <v>959</v>
       </c>
       <c r="R301" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S301" s="17">
         <f t="shared" si="81"/>
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="T301" s="14">
         <v>0</v>
@@ -30585,7 +30594,7 @@
     </row>
     <row r="302" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A302" s="13" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B302" s="17">
         <v>2023</v>
@@ -30600,17 +30609,17 @@
         <v>666</v>
       </c>
       <c r="F302" s="17">
-        <v>331</v>
+        <v>161</v>
       </c>
       <c r="G302" s="9" t="s">
         <v>1019</v>
       </c>
       <c r="H302" s="9">
-        <f t="shared" ref="H302" si="100">YEAR(G302)</f>
+        <f t="shared" ref="H302" si="98">YEAR(G302)</f>
         <v>2024</v>
       </c>
       <c r="I302" s="9">
-        <f t="shared" ref="I302" si="101">MONTH(G302)</f>
+        <f t="shared" ref="I302" si="99">MONTH(G302)</f>
         <v>7</v>
       </c>
       <c r="J302" s="9" t="s">
@@ -30620,29 +30629,29 @@
         <v>159</v>
       </c>
       <c r="L302" s="9" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="M302" s="17">
         <v>2</v>
       </c>
       <c r="N302" s="43">
-        <v>35.700000000000003</v>
+        <v>35</v>
       </c>
       <c r="O302" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P302" s="16" t="s">
-        <v>1026</v>
+      <c r="P302" s="13" t="s">
+        <v>1024</v>
       </c>
       <c r="Q302" s="9" t="s">
-        <v>469</v>
+        <v>904</v>
       </c>
       <c r="R302" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S302" s="17">
         <f t="shared" si="81"/>
-        <v>176</v>
+        <v>103</v>
       </c>
       <c r="T302" s="14">
         <v>0</v>
@@ -30650,10 +30659,10 @@
     </row>
     <row r="303" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A303" s="13" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B303" s="17">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C303" s="9" t="s">
         <v>21</v>
@@ -30665,17 +30674,17 @@
         <v>666</v>
       </c>
       <c r="F303" s="17">
-        <v>179</v>
+        <v>331</v>
       </c>
       <c r="G303" s="9" t="s">
-        <v>1030</v>
+        <v>1019</v>
       </c>
       <c r="H303" s="9">
-        <f t="shared" ref="H303" si="102">YEAR(G303)</f>
+        <f t="shared" ref="H303" si="100">YEAR(G303)</f>
         <v>2024</v>
       </c>
       <c r="I303" s="9">
-        <f t="shared" ref="I303" si="103">MONTH(G303)</f>
+        <f t="shared" ref="I303" si="101">MONTH(G303)</f>
         <v>7</v>
       </c>
       <c r="J303" s="9" t="s">
@@ -30685,29 +30694,29 @@
         <v>159</v>
       </c>
       <c r="L303" s="9" t="s">
-        <v>602</v>
+        <v>369</v>
       </c>
       <c r="M303" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N303" s="43">
-        <v>0</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="O303" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P303" s="13" t="s">
-        <v>1028</v>
+      <c r="P303" s="16" t="s">
+        <v>1026</v>
       </c>
       <c r="Q303" s="9" t="s">
-        <v>501</v>
+        <v>469</v>
       </c>
       <c r="R303" s="9" t="s">
         <v>159</v>
       </c>
       <c r="S303" s="17">
         <f t="shared" si="81"/>
-        <v>218</v>
+        <v>176</v>
       </c>
       <c r="T303" s="14">
         <v>0</v>
@@ -30715,7 +30724,7 @@
     </row>
     <row r="304" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A304" s="13" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B304" s="17">
         <v>2024</v>
@@ -30730,18 +30739,18 @@
         <v>666</v>
       </c>
       <c r="F304" s="17">
-        <v>123</v>
+        <v>179</v>
       </c>
       <c r="G304" s="9" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="H304" s="9">
-        <f t="shared" ref="H304" si="104">YEAR(G304)</f>
+        <f t="shared" ref="H304" si="102">YEAR(G304)</f>
         <v>2024</v>
       </c>
       <c r="I304" s="9">
-        <f t="shared" ref="I304" si="105">MONTH(G304)</f>
-        <v>8</v>
+        <f t="shared" ref="I304" si="103">MONTH(G304)</f>
+        <v>7</v>
       </c>
       <c r="J304" s="9" t="s">
         <v>159</v>
@@ -30753,16 +30762,16 @@
         <v>602</v>
       </c>
       <c r="M304" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N304" s="43">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="O304" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P304" s="13" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="Q304" s="9" t="s">
         <v>501</v>
@@ -30771,8 +30780,8 @@
         <v>159</v>
       </c>
       <c r="S304" s="17">
-        <f t="shared" ref="S304:S305" si="106">LEN(P304)</f>
-        <v>88</v>
+        <f t="shared" si="81"/>
+        <v>218</v>
       </c>
       <c r="T304" s="14">
         <v>0</v>
@@ -30780,7 +30789,7 @@
     </row>
     <row r="305" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A305" s="13" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="B305" s="17">
         <v>2024</v>
@@ -30795,75 +30804,118 @@
         <v>666</v>
       </c>
       <c r="F305" s="17">
-        <v>368</v>
+        <v>123</v>
       </c>
       <c r="G305" s="9" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="H305" s="9">
-        <f t="shared" ref="H305" si="107">YEAR(G305)</f>
+        <f t="shared" ref="H305" si="104">YEAR(G305)</f>
         <v>2024</v>
       </c>
       <c r="I305" s="9">
-        <f t="shared" ref="I305" si="108">MONTH(G305)</f>
+        <f t="shared" ref="I305" si="105">MONTH(G305)</f>
         <v>8</v>
       </c>
       <c r="J305" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K305" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L305" s="9" t="s">
-        <v>365</v>
+        <v>602</v>
       </c>
       <c r="M305" s="17">
-        <v>4</v>
-      </c>
-      <c r="N305" s="17">
-        <v>43.13</v>
+        <v>1</v>
+      </c>
+      <c r="N305" s="43">
+        <v>40</v>
       </c>
       <c r="O305" s="9" t="s">
         <v>664</v>
       </c>
       <c r="P305" s="13" t="s">
+        <v>1032</v>
+      </c>
+      <c r="Q305" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="R305" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S305" s="17">
+        <f t="shared" ref="S305:S306" si="106">LEN(P305)</f>
+        <v>88</v>
+      </c>
+      <c r="T305" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A306" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B306" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C306" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D306" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E306" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F306" s="17">
+        <v>368</v>
+      </c>
+      <c r="G306" s="9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H306" s="9">
+        <f t="shared" ref="H306" si="107">YEAR(G306)</f>
+        <v>2024</v>
+      </c>
+      <c r="I306" s="9">
+        <f t="shared" ref="I306" si="108">MONTH(G306)</f>
+        <v>8</v>
+      </c>
+      <c r="J306" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K306" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L306" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M306" s="17">
+        <v>4</v>
+      </c>
+      <c r="N306" s="17">
+        <v>43.13</v>
+      </c>
+      <c r="O306" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P306" s="13" t="s">
         <v>1035</v>
       </c>
-      <c r="Q305" s="9" t="s">
+      <c r="Q306" s="9" t="s">
         <v>959</v>
       </c>
-      <c r="R305" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S305" s="17">
+      <c r="R306" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S306" s="17">
         <f t="shared" si="106"/>
         <v>231</v>
       </c>
-      <c r="T305" s="14">
+      <c r="T306" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="306" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A306" s="13"/>
-      <c r="B306" s="9"/>
-      <c r="C306" s="9"/>
-      <c r="D306" s="9"/>
-      <c r="E306" s="9"/>
-      <c r="F306" s="9"/>
-      <c r="G306" s="9"/>
-      <c r="H306" s="9"/>
-      <c r="I306" s="9"/>
-      <c r="J306" s="9"/>
-      <c r="K306" s="9"/>
-      <c r="L306" s="9"/>
-      <c r="M306" s="9"/>
-      <c r="N306" s="9"/>
-      <c r="O306" s="9"/>
-      <c r="P306" s="13"/>
-      <c r="Q306" s="9"/>
-      <c r="R306" s="9"/>
-      <c r="S306" s="17"/>
-      <c r="T306" s="9"/>
     </row>
     <row r="307" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A307" s="13"/>
@@ -31040,6 +31092,28 @@
       <c r="R314" s="9"/>
       <c r="S314" s="17"/>
       <c r="T314" s="9"/>
+    </row>
+    <row r="315" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A315" s="13"/>
+      <c r="B315" s="9"/>
+      <c r="C315" s="9"/>
+      <c r="D315" s="9"/>
+      <c r="E315" s="9"/>
+      <c r="F315" s="9"/>
+      <c r="G315" s="9"/>
+      <c r="H315" s="9"/>
+      <c r="I315" s="9"/>
+      <c r="J315" s="9"/>
+      <c r="K315" s="9"/>
+      <c r="L315" s="9"/>
+      <c r="M315" s="9"/>
+      <c r="N315" s="9"/>
+      <c r="O315" s="9"/>
+      <c r="P315" s="13"/>
+      <c r="Q315" s="9"/>
+      <c r="R315" s="9"/>
+      <c r="S315" s="17"/>
+      <c r="T315" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#34 Reading List: updated to 28/10/2024.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -3425,14 +3425,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3751,16 +3751,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48">
+      <c r="A1" s="49">
         <v>2016</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -5277,16 +5277,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48">
+      <c r="A1" s="49">
         <v>2017</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -6233,16 +6233,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48">
+      <c r="A1" s="49">
         <v>2018</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -7189,16 +7189,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48">
+      <c r="A1" s="49">
         <v>2019</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -8145,16 +8145,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48">
+      <c r="A1" s="49">
         <v>2020</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -9101,16 +9101,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48">
+      <c r="A1" s="49">
         <v>2021</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -10057,16 +10057,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48">
+      <c r="A1" s="49">
         <v>2022</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -11004,8 +11004,8 @@
   <dimension ref="A1:T315"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U281" sqref="U281"/>
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U294" sqref="U294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -28170,7 +28170,7 @@
       <c r="O264" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="P264" s="50" t="s">
+      <c r="P264" s="48" t="s">
         <v>1037</v>
       </c>
       <c r="Q264" s="9" t="s">
@@ -29354,7 +29354,7 @@
         <v>160</v>
       </c>
       <c r="T282" s="14">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="283" spans="1:20" x14ac:dyDescent="0.2">
@@ -29419,7 +29419,7 @@
         <v>64</v>
       </c>
       <c r="T283" s="14">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="284" spans="1:20" x14ac:dyDescent="0.2">
@@ -29484,7 +29484,7 @@
         <v>106</v>
       </c>
       <c r="T284" s="14">
-        <v>0</v>
+        <v>456</v>
       </c>
     </row>
     <row r="285" spans="1:20" x14ac:dyDescent="0.2">
@@ -29549,7 +29549,7 @@
         <v>224</v>
       </c>
       <c r="T285" s="14">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="286" spans="1:20" x14ac:dyDescent="0.2">
@@ -29614,7 +29614,7 @@
         <v>233</v>
       </c>
       <c r="T286" s="14">
-        <v>0</v>
+        <v>134</v>
       </c>
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.2">
@@ -29679,7 +29679,7 @@
         <v>186</v>
       </c>
       <c r="T287" s="14">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="288" spans="1:20" x14ac:dyDescent="0.2">
@@ -29744,7 +29744,7 @@
         <v>98</v>
       </c>
       <c r="T288" s="14">
-        <v>0</v>
+        <v>185</v>
       </c>
     </row>
     <row r="289" spans="1:20" x14ac:dyDescent="0.2">
@@ -29809,7 +29809,7 @@
         <v>57</v>
       </c>
       <c r="T289" s="14">
-        <v>0</v>
+        <v>479</v>
       </c>
     </row>
     <row r="290" spans="1:20" x14ac:dyDescent="0.2">
@@ -29874,7 +29874,7 @@
         <v>84</v>
       </c>
       <c r="T290" s="14">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="291" spans="1:20" x14ac:dyDescent="0.2">
@@ -29939,7 +29939,7 @@
         <v>152</v>
       </c>
       <c r="T291" s="14">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="292" spans="1:20" x14ac:dyDescent="0.2">
@@ -30004,7 +30004,7 @@
         <v>26</v>
       </c>
       <c r="T292" s="14">
-        <v>0</v>
+        <v>237</v>
       </c>
     </row>
     <row r="293" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#36 Reading List: updated to 05/11/2024.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Repositories\jupnb-nwreadinglist\nwreadinglist\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Repositories\py-nwreadinglist\nwreadinglist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4878" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4902" uniqueCount="1043">
   <si>
     <t>Format</t>
   </si>
@@ -3155,6 +3155,21 @@
   </si>
   <si>
     <t>Useful. It contains some useful bits of information, but the use of a bigger font instead of bold face to make important words to "pop" is massively annoying and it makes the reading experience a pain.</t>
+  </si>
+  <si>
+    <t>Crafting Test-Driven Software with Python</t>
+  </si>
+  <si>
+    <t>2024-11-05</t>
+  </si>
+  <si>
+    <t>Useful. To be a Packt book, it's quite well written and edited.</t>
+  </si>
+  <si>
+    <t>Data-Oriented Programming</t>
+  </si>
+  <si>
+    <t>Useful. This book is very hard to read due of the author abusing of diagrams and dialogues among fictional characters in every page. Without all this cumbersome and useless cognitive overhead, the book could have been reduced from 436 pages to around 80 without loss of knowledge. The good thing instead is that we finally have a book that collects all the relevant information about DOP in a single place.</t>
   </si>
 </sst>
 </file>
@@ -11003,9 +11018,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U294" sqref="U294"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H309" sqref="H309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -30845,7 +30860,7 @@
         <v>159</v>
       </c>
       <c r="S305" s="17">
-        <f t="shared" ref="S305:S306" si="106">LEN(P305)</f>
+        <f t="shared" ref="S305:S308" si="106">LEN(P305)</f>
         <v>88</v>
       </c>
       <c r="T305" s="14">
@@ -30918,48 +30933,134 @@
       </c>
     </row>
     <row r="307" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A307" s="13"/>
-      <c r="B307" s="9"/>
-      <c r="C307" s="9"/>
-      <c r="D307" s="9"/>
-      <c r="E307" s="9"/>
-      <c r="F307" s="9"/>
-      <c r="G307" s="9"/>
-      <c r="H307" s="9"/>
-      <c r="I307" s="9"/>
-      <c r="J307" s="9"/>
-      <c r="K307" s="9"/>
-      <c r="L307" s="9"/>
-      <c r="M307" s="9"/>
-      <c r="N307" s="9"/>
-      <c r="O307" s="9"/>
-      <c r="P307" s="13"/>
-      <c r="Q307" s="9"/>
-      <c r="R307" s="9"/>
-      <c r="S307" s="17"/>
-      <c r="T307" s="9"/>
+      <c r="A307" s="13" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B307" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C307" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D307" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E307" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F307" s="17">
+        <v>323</v>
+      </c>
+      <c r="G307" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H307" s="9">
+        <f t="shared" ref="H307" si="109">YEAR(G307)</f>
+        <v>2024</v>
+      </c>
+      <c r="I307" s="9">
+        <f t="shared" ref="I307" si="110">MONTH(G307)</f>
+        <v>11</v>
+      </c>
+      <c r="J307" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K307" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L307" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M307" s="17">
+        <v>3</v>
+      </c>
+      <c r="N307" s="17">
+        <v>48.99</v>
+      </c>
+      <c r="O307" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P307" s="13" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Q307" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R307" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S307" s="17">
+        <f t="shared" si="106"/>
+        <v>63</v>
+      </c>
+      <c r="T307" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="308" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A308" s="13"/>
-      <c r="B308" s="9"/>
-      <c r="C308" s="9"/>
-      <c r="D308" s="9"/>
-      <c r="E308" s="9"/>
-      <c r="F308" s="9"/>
-      <c r="G308" s="9"/>
-      <c r="H308" s="9"/>
-      <c r="I308" s="9"/>
-      <c r="J308" s="9"/>
-      <c r="K308" s="9"/>
-      <c r="L308" s="9"/>
-      <c r="M308" s="9"/>
-      <c r="N308" s="9"/>
-      <c r="O308" s="9"/>
-      <c r="P308" s="13"/>
-      <c r="Q308" s="9"/>
-      <c r="R308" s="9"/>
-      <c r="S308" s="17"/>
-      <c r="T308" s="9"/>
+      <c r="A308" s="13" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B308" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C308" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D308" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E308" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F308" s="17">
+        <v>426</v>
+      </c>
+      <c r="G308" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H308" s="9">
+        <f t="shared" ref="H308" si="111">YEAR(G308)</f>
+        <v>2024</v>
+      </c>
+      <c r="I308" s="9">
+        <f t="shared" ref="I308" si="112">MONTH(G308)</f>
+        <v>11</v>
+      </c>
+      <c r="J308" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K308" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L308" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M308" s="17">
+        <v>3</v>
+      </c>
+      <c r="N308" s="17">
+        <v>59.99</v>
+      </c>
+      <c r="O308" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P308" s="13" t="s">
+        <v>1042</v>
+      </c>
+      <c r="Q308" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R308" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S308" s="17">
+        <f t="shared" si="106"/>
+        <v>406</v>
+      </c>
+      <c r="T308" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="309" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A309" s="13"/>

</xml_diff>

<commit_message>
#38 Reading List: updated to 2024-11-19.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4902" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4998" uniqueCount="1065">
   <si>
     <t>Format</t>
   </si>
@@ -2704,9 +2704,6 @@
     <t>2023-09-08</t>
   </si>
   <si>
-    <t>Useful. Good overview for whom knows nothing about the topic and quite language-agnostic as well. But it advocates too much for the TDD methodology, which makes the book less objective.</t>
-  </si>
-  <si>
     <t>Machine Learning Yearning (Draft)</t>
   </si>
   <si>
@@ -3170,6 +3167,75 @@
   </si>
   <si>
     <t>Useful. This book is very hard to read due of the author abusing of diagrams and dialogues among fictional characters in every page. Without all this cumbersome and useless cognitive overhead, the book could have been reduced from 436 pages to around 80 without loss of knowledge. The good thing instead is that we finally have a book that collects all the relevant information about DOP in a single place.</t>
+  </si>
+  <si>
+    <t>Useless. It couples the (brief) insights in the principles of the clean architecture with a lot of TDD boilerplate code that unnecessarely increases the cognitive load of the book. This writing approach is indeed personal and original, but not practical, because it requires the reader to surf thru a lot of noise to get to the melody.</t>
+  </si>
+  <si>
+    <t>Mastering Python Design Patterns (3rd Edition)</t>
+  </si>
+  <si>
+    <t>2024-11-12</t>
+  </si>
+  <si>
+    <t>Useless. In theory it's good to have a book about design patterns in Python for reference, but inpractice most of them applied to Python look quite cumbersome compared to other languages (C#, Java). Design patterns are intended for more OOP-friendly languages.</t>
+  </si>
+  <si>
+    <t>Hacking APIs</t>
+  </si>
+  <si>
+    <t>2024-11-17</t>
+  </si>
+  <si>
+    <t>Useful. Well written and good overview, but nothing revolutionary.</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
+  <si>
+    <t>API Management (2nd Edition)</t>
+  </si>
+  <si>
+    <t>Useless. Yet another totally impersonal book, a copy'n'paste list of theories and strategies, with some degree of redundancy. On the positive side, the layout relies upon a fair amount of bold face, which makes skimming useless content easier.</t>
+  </si>
+  <si>
+    <t>Architecture Modernization</t>
+  </si>
+  <si>
+    <t>Useful. The author collected many fragments of useful knowledge and created an organic and very personal path thru all of them. The book is very comprehensive and original, but it could feel too much dense of information for a beginner. It lacks of bold face, therefore it's difficult to skim redundant information. Good to read after "Building Great Software Engineering Teams".</t>
+  </si>
+  <si>
+    <t>DevOps: A Journey From Microservices to Cloud-based Containerization</t>
+  </si>
+  <si>
+    <t>River Publishers</t>
+  </si>
+  <si>
+    <t>Useless. Ok book for beginners.</t>
+  </si>
+  <si>
+    <t>Docker Deep Dive (2024 Edition)</t>
+  </si>
+  <si>
+    <t>Useless. Ok overview for beginners.</t>
+  </si>
+  <si>
+    <t>The Self-Taught Cloud Computing Engineer (1st Edition)</t>
+  </si>
+  <si>
+    <t>Useless. Just a list of services offered by cloud providers.</t>
+  </si>
+  <si>
+    <t>2024-11-18</t>
+  </si>
+  <si>
+    <t>Product Roadmaps</t>
+  </si>
+  <si>
+    <t>2024-11-19</t>
+  </si>
+  <si>
+    <t>Useful. The most concise but comprehensive book about Product Management. In only 68 pages it equips the reader with a big baggage of actionable knowledge.</t>
   </si>
 </sst>
 </file>
@@ -11016,11 +11082,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T315"/>
+  <dimension ref="A1:T329"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H309" sqref="H309"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A317" sqref="A317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -11105,7 +11171,7 @@
         <v>860</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -12200,7 +12266,7 @@
         <v>60</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R18" s="9" t="s">
         <v>159</v>
@@ -12395,7 +12461,7 @@
         <v>695</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R21" s="9" t="s">
         <v>159</v>
@@ -12785,7 +12851,7 @@
         <v>698</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R27" s="9" t="s">
         <v>159</v>
@@ -12850,7 +12916,7 @@
         <v>699</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R28" s="9" t="s">
         <v>159</v>
@@ -12915,7 +12981,7 @@
         <v>668</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R29" s="9" t="s">
         <v>159</v>
@@ -13875,7 +13941,7 @@
         <v>159</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="M44" s="14">
         <v>4</v>
@@ -14330,7 +14396,7 @@
         <v>159</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="M51" s="14">
         <v>1</v>
@@ -14865,7 +14931,7 @@
         <v>60</v>
       </c>
       <c r="Q59" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R59" s="9" t="s">
         <v>159</v>
@@ -16880,7 +16946,7 @@
         <v>733</v>
       </c>
       <c r="Q90" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R90" s="9" t="s">
         <v>159</v>
@@ -17725,7 +17791,7 @@
         <v>742</v>
       </c>
       <c r="Q103" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R103" s="9" t="s">
         <v>159</v>
@@ -17790,7 +17856,7 @@
         <v>743</v>
       </c>
       <c r="Q104" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R104" s="9" t="s">
         <v>159</v>
@@ -17920,7 +17986,7 @@
         <v>745</v>
       </c>
       <c r="Q106" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R106" s="9" t="s">
         <v>159</v>
@@ -18894,7 +18960,7 @@
         <v>757</v>
       </c>
       <c r="Q121" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R121" s="9" t="s">
         <v>159</v>
@@ -19219,7 +19285,7 @@
         <v>762</v>
       </c>
       <c r="Q126" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R126" s="9" t="s">
         <v>159</v>
@@ -19284,7 +19350,7 @@
         <v>763</v>
       </c>
       <c r="Q127" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R127" s="9" t="s">
         <v>159</v>
@@ -19544,7 +19610,7 @@
         <v>767</v>
       </c>
       <c r="Q131" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R131" s="9" t="s">
         <v>159</v>
@@ -19999,7 +20065,7 @@
         <v>774</v>
       </c>
       <c r="Q138" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R138" s="9" t="s">
         <v>159</v>
@@ -20064,7 +20130,7 @@
         <v>775</v>
       </c>
       <c r="Q139" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R139" s="9" t="s">
         <v>159</v>
@@ -20454,7 +20520,7 @@
         <v>779</v>
       </c>
       <c r="Q145" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R145" s="9" t="s">
         <v>159</v>
@@ -20519,7 +20585,7 @@
         <v>674</v>
       </c>
       <c r="Q146" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R146" s="9" t="s">
         <v>159</v>
@@ -21104,7 +21170,7 @@
         <v>786</v>
       </c>
       <c r="Q155" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R155" s="9" t="s">
         <v>158</v>
@@ -22144,7 +22210,7 @@
         <v>799</v>
       </c>
       <c r="Q171" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R171" s="9" t="s">
         <v>158</v>
@@ -23054,7 +23120,7 @@
         <v>806</v>
       </c>
       <c r="Q185" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R185" s="9" t="s">
         <v>158</v>
@@ -23119,7 +23185,7 @@
         <v>807</v>
       </c>
       <c r="Q186" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R186" s="9" t="s">
         <v>158</v>
@@ -23249,7 +23315,7 @@
         <v>674</v>
       </c>
       <c r="Q188" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R188" s="9" t="s">
         <v>159</v>
@@ -24679,7 +24745,7 @@
         <v>821</v>
       </c>
       <c r="Q210" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R210" s="9" t="s">
         <v>159</v>
@@ -24744,7 +24810,7 @@
         <v>822</v>
       </c>
       <c r="Q211" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R211" s="9" t="s">
         <v>159</v>
@@ -24939,7 +25005,7 @@
         <v>825</v>
       </c>
       <c r="Q214" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R214" s="9" t="s">
         <v>159</v>
@@ -26174,7 +26240,7 @@
         <v>837</v>
       </c>
       <c r="Q233" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R233" s="9" t="s">
         <v>159</v>
@@ -26304,7 +26370,7 @@
         <v>859</v>
       </c>
       <c r="Q235" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R235" s="9" t="s">
         <v>159</v>
@@ -26434,7 +26500,7 @@
         <v>847</v>
       </c>
       <c r="Q237" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R237" s="9" t="s">
         <v>159</v>
@@ -26564,7 +26630,7 @@
         <v>58</v>
       </c>
       <c r="Q239" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R239" s="9" t="s">
         <v>159</v>
@@ -26954,7 +27020,7 @@
         <v>869</v>
       </c>
       <c r="Q245" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R245" s="9" t="s">
         <v>159</v>
@@ -27211,7 +27277,7 @@
         <v>664</v>
       </c>
       <c r="P249" s="16" t="s">
-        <v>887</v>
+        <v>1042</v>
       </c>
       <c r="Q249" s="9" t="s">
         <v>569</v>
@@ -27221,7 +27287,7 @@
       </c>
       <c r="S249" s="17">
         <f t="shared" si="32"/>
-        <v>185</v>
+        <v>335</v>
       </c>
       <c r="T249" s="14">
         <v>280</v>
@@ -27229,7 +27295,7 @@
     </row>
     <row r="250" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B250" s="17">
         <v>2018</v>
@@ -27247,7 +27313,7 @@
         <v>105</v>
       </c>
       <c r="G250" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H250" s="17">
         <f t="shared" si="30"/>
@@ -27276,10 +27342,10 @@
         <v>664</v>
       </c>
       <c r="P250" s="47" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="Q250" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R250" s="9" t="s">
         <v>159</v>
@@ -27294,7 +27360,7 @@
     </row>
     <row r="251" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B251" s="17">
         <v>2023</v>
@@ -27312,7 +27378,7 @@
         <v>240</v>
       </c>
       <c r="G251" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H251" s="17">
         <f t="shared" si="30"/>
@@ -27341,7 +27407,7 @@
         <v>664</v>
       </c>
       <c r="P251" s="13" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="Q251" s="9" t="s">
         <v>469</v>
@@ -27359,7 +27425,7 @@
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B252" s="17">
         <v>2023</v>
@@ -27377,7 +27443,7 @@
         <v>51</v>
       </c>
       <c r="G252" s="9" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H252" s="17">
         <f t="shared" si="30"/>
@@ -27394,7 +27460,7 @@
         <v>159</v>
       </c>
       <c r="L252" s="9" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="M252" s="14">
         <v>2</v>
@@ -27406,7 +27472,7 @@
         <v>664</v>
       </c>
       <c r="P252" s="13" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="Q252" s="9" t="s">
         <v>569</v>
@@ -27424,7 +27490,7 @@
     </row>
     <row r="253" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A253" s="13" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B253" s="17">
         <v>2023</v>
@@ -27442,7 +27508,7 @@
         <v>184</v>
       </c>
       <c r="G253" s="9" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H253" s="17">
         <f t="shared" si="30"/>
@@ -27471,10 +27537,10 @@
         <v>664</v>
       </c>
       <c r="P253" s="16" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="Q253" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R253" s="9" t="s">
         <v>159</v>
@@ -27489,7 +27555,7 @@
     </row>
     <row r="254" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A254" s="13" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B254" s="17">
         <v>2023</v>
@@ -27507,7 +27573,7 @@
         <v>203</v>
       </c>
       <c r="G254" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H254" s="17">
         <f t="shared" si="30"/>
@@ -27536,7 +27602,7 @@
         <v>664</v>
       </c>
       <c r="P254" s="9" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Q254" s="9" t="s">
         <v>469</v>
@@ -27554,7 +27620,7 @@
     </row>
     <row r="255" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A255" s="13" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B255" s="17">
         <v>2021</v>
@@ -27572,7 +27638,7 @@
         <v>338</v>
       </c>
       <c r="G255" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H255" s="17">
         <f t="shared" si="30"/>
@@ -27601,7 +27667,7 @@
         <v>664</v>
       </c>
       <c r="P255" s="13" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Q255" s="9" t="s">
         <v>569</v>
@@ -27619,7 +27685,7 @@
     </row>
     <row r="256" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A256" s="13" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B256" s="17">
         <v>2018</v>
@@ -27637,7 +27703,7 @@
         <v>229</v>
       </c>
       <c r="G256" s="9" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H256" s="17">
         <f t="shared" si="30"/>
@@ -27666,7 +27732,7 @@
         <v>664</v>
       </c>
       <c r="P256" s="13" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="Q256" s="9" t="s">
         <v>873</v>
@@ -27684,7 +27750,7 @@
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A257" s="13" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B257" s="17">
         <v>2022</v>
@@ -27702,7 +27768,7 @@
         <v>94</v>
       </c>
       <c r="G257" s="9" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H257" s="17">
         <f t="shared" ref="H257:H259" si="33">YEAR(G257)</f>
@@ -27731,7 +27797,7 @@
         <v>664</v>
       </c>
       <c r="P257" s="13" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="Q257" s="9" t="s">
         <v>569</v>
@@ -27749,7 +27815,7 @@
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A258" s="13" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B258" s="17">
         <v>2022</v>
@@ -27767,7 +27833,7 @@
         <v>265</v>
       </c>
       <c r="G258" s="9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H258" s="17">
         <f t="shared" si="33"/>
@@ -27796,7 +27862,7 @@
         <v>664</v>
       </c>
       <c r="P258" s="16" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="Q258" s="9" t="s">
         <v>569</v>
@@ -27814,7 +27880,7 @@
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A259" s="13" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B259" s="17">
         <v>2023</v>
@@ -27832,7 +27898,7 @@
         <v>288</v>
       </c>
       <c r="G259" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H259" s="9">
         <f t="shared" si="33"/>
@@ -27861,7 +27927,7 @@
         <v>664</v>
       </c>
       <c r="P259" s="16" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q259" s="9" t="s">
         <v>569</v>
@@ -27879,7 +27945,7 @@
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A260" s="13" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B260" s="17">
         <v>2023</v>
@@ -27897,7 +27963,7 @@
         <v>151</v>
       </c>
       <c r="G260" s="9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H260" s="9">
         <f t="shared" ref="H260" si="35">YEAR(G260)</f>
@@ -27926,7 +27992,7 @@
         <v>664</v>
       </c>
       <c r="P260" s="13" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="Q260" s="9" t="s">
         <v>469</v>
@@ -27944,7 +28010,7 @@
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A261" s="13" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B261" s="17">
         <v>2022</v>
@@ -27962,7 +28028,7 @@
         <v>416</v>
       </c>
       <c r="G261" s="9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H261" s="9">
         <f t="shared" ref="H261:H263" si="37">YEAR(G261)</f>
@@ -27991,7 +28057,7 @@
         <v>664</v>
       </c>
       <c r="P261" s="13" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="Q261" s="9" t="s">
         <v>469</v>
@@ -28009,7 +28075,7 @@
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A262" s="13" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B262" s="17">
         <v>2022</v>
@@ -28027,7 +28093,7 @@
         <v>535</v>
       </c>
       <c r="G262" s="9" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="H262" s="9">
         <f t="shared" si="37"/>
@@ -28056,7 +28122,7 @@
         <v>664</v>
       </c>
       <c r="P262" s="13" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="Q262" s="9" t="s">
         <v>875</v>
@@ -28074,7 +28140,7 @@
     </row>
     <row r="263" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A263" s="13" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B263" s="17">
         <v>2018</v>
@@ -28092,7 +28158,7 @@
         <v>429</v>
       </c>
       <c r="G263" s="9" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="H263" s="9">
         <f t="shared" si="37"/>
@@ -28121,7 +28187,7 @@
         <v>664</v>
       </c>
       <c r="P263" s="16" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="Q263" s="9" t="s">
         <v>469</v>
@@ -28139,7 +28205,7 @@
     </row>
     <row r="264" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A264" s="13" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B264" s="17">
         <v>2023</v>
@@ -28157,7 +28223,7 @@
         <v>455</v>
       </c>
       <c r="G264" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H264" s="9">
         <f t="shared" ref="H264:H265" si="39">YEAR(G264)</f>
@@ -28186,7 +28252,7 @@
         <v>664</v>
       </c>
       <c r="P264" s="48" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="Q264" s="9" t="s">
         <v>569</v>
@@ -28204,7 +28270,7 @@
     </row>
     <row r="265" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A265" s="13" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B265" s="17">
         <v>2023</v>
@@ -28222,7 +28288,7 @@
         <v>268</v>
       </c>
       <c r="G265" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H265" s="9">
         <f t="shared" si="39"/>
@@ -28251,7 +28317,7 @@
         <v>664</v>
       </c>
       <c r="P265" s="16" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="Q265" s="9" t="s">
         <v>569</v>
@@ -28269,7 +28335,7 @@
     </row>
     <row r="266" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A266" s="13" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B266" s="17">
         <v>2022</v>
@@ -28287,7 +28353,7 @@
         <v>205</v>
       </c>
       <c r="G266" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H266" s="9">
         <f t="shared" ref="H266" si="41">YEAR(G266)</f>
@@ -28316,7 +28382,7 @@
         <v>664</v>
       </c>
       <c r="P266" s="16" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="Q266" s="9" t="s">
         <v>569</v>
@@ -28334,7 +28400,7 @@
     </row>
     <row r="267" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A267" s="13" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B267" s="17">
         <v>2022</v>
@@ -28352,7 +28418,7 @@
         <v>94</v>
       </c>
       <c r="G267" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H267" s="9">
         <f t="shared" ref="H267" si="43">YEAR(G267)</f>
@@ -28381,7 +28447,7 @@
         <v>664</v>
       </c>
       <c r="P267" s="13" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="Q267" s="9" t="s">
         <v>569</v>
@@ -28399,7 +28465,7 @@
     </row>
     <row r="268" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A268" s="13" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B268" s="17">
         <v>2020</v>
@@ -28417,7 +28483,7 @@
         <v>132</v>
       </c>
       <c r="G268" s="9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H268" s="9">
         <f t="shared" ref="H268:H269" si="45">YEAR(G268)</f>
@@ -28446,7 +28512,7 @@
         <v>664</v>
       </c>
       <c r="P268" s="13" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="Q268" s="9" t="s">
         <v>569</v>
@@ -28464,7 +28530,7 @@
     </row>
     <row r="269" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A269" s="13" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B269" s="17">
         <v>2021</v>
@@ -28482,7 +28548,7 @@
         <v>715</v>
       </c>
       <c r="G269" s="9" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H269" s="9">
         <f t="shared" si="45"/>
@@ -28511,7 +28577,7 @@
         <v>664</v>
       </c>
       <c r="P269" s="13" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="Q269" s="9" t="s">
         <v>569</v>
@@ -28529,7 +28595,7 @@
     </row>
     <row r="270" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A270" s="13" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B270" s="17">
         <v>2023</v>
@@ -28547,7 +28613,7 @@
         <v>192</v>
       </c>
       <c r="G270" s="9" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H270" s="9">
         <f t="shared" ref="H270" si="47">YEAR(G270)</f>
@@ -28564,7 +28630,7 @@
         <v>159</v>
       </c>
       <c r="L270" s="9" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="M270" s="17">
         <v>1</v>
@@ -28576,7 +28642,7 @@
         <v>664</v>
       </c>
       <c r="P270" s="13" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="Q270" s="9" t="s">
         <v>569</v>
@@ -28594,7 +28660,7 @@
     </row>
     <row r="271" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A271" s="13" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B271" s="17">
         <v>2024</v>
@@ -28612,7 +28678,7 @@
         <v>139</v>
       </c>
       <c r="G271" s="9" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H271" s="9">
         <f t="shared" ref="H271" si="49">YEAR(G271)</f>
@@ -28629,7 +28695,7 @@
         <v>159</v>
       </c>
       <c r="L271" s="9" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="M271" s="17">
         <v>1</v>
@@ -28641,7 +28707,7 @@
         <v>664</v>
       </c>
       <c r="P271" s="13" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Q271" s="9" t="s">
         <v>569</v>
@@ -28659,7 +28725,7 @@
     </row>
     <row r="272" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A272" s="13" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B272" s="17">
         <v>2023</v>
@@ -28677,7 +28743,7 @@
         <v>963</v>
       </c>
       <c r="G272" s="9" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H272" s="9">
         <f t="shared" ref="H272" si="51">YEAR(G272)</f>
@@ -28706,7 +28772,7 @@
         <v>664</v>
       </c>
       <c r="P272" s="13" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Q272" s="9" t="s">
         <v>569</v>
@@ -28724,7 +28790,7 @@
     </row>
     <row r="273" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A273" s="13" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B273" s="17">
         <v>2024</v>
@@ -28742,7 +28808,7 @@
         <v>229</v>
       </c>
       <c r="G273" s="9" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H273" s="9">
         <f t="shared" ref="H273:H274" si="53">YEAR(G273)</f>
@@ -28759,7 +28825,7 @@
         <v>158</v>
       </c>
       <c r="L273" s="9" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="M273" s="17">
         <v>2</v>
@@ -28771,7 +28837,7 @@
         <v>664</v>
       </c>
       <c r="P273" s="13" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Q273" s="9" t="s">
         <v>569</v>
@@ -28789,7 +28855,7 @@
     </row>
     <row r="274" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A274" s="13" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B274" s="17">
         <v>2018</v>
@@ -28807,7 +28873,7 @@
         <v>978</v>
       </c>
       <c r="G274" s="9" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H274" s="9">
         <f t="shared" si="53"/>
@@ -28836,7 +28902,7 @@
         <v>664</v>
       </c>
       <c r="P274" s="13" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Q274" s="9" t="s">
         <v>569</v>
@@ -28854,7 +28920,7 @@
     </row>
     <row r="275" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A275" s="13" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B275" s="17">
         <v>2022</v>
@@ -28872,7 +28938,7 @@
         <v>264</v>
       </c>
       <c r="G275" s="9" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H275" s="9">
         <f t="shared" ref="H275" si="55">YEAR(G275)</f>
@@ -28901,7 +28967,7 @@
         <v>664</v>
       </c>
       <c r="P275" s="13" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Q275" s="9" t="s">
         <v>569</v>
@@ -28919,7 +28985,7 @@
     </row>
     <row r="276" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A276" s="13" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B276" s="17">
         <v>2022</v>
@@ -28937,7 +29003,7 @@
         <v>243</v>
       </c>
       <c r="G276" s="9" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H276" s="9">
         <f t="shared" ref="H276:H279" si="57">YEAR(G276)</f>
@@ -28954,7 +29020,7 @@
         <v>159</v>
       </c>
       <c r="L276" s="9" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="M276" s="17">
         <v>4</v>
@@ -28966,7 +29032,7 @@
         <v>664</v>
       </c>
       <c r="P276" s="13" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="Q276" s="9" t="s">
         <v>569</v>
@@ -28984,7 +29050,7 @@
     </row>
     <row r="277" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A277" s="13" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B277" s="17">
         <v>2024</v>
@@ -29002,7 +29068,7 @@
         <v>337</v>
       </c>
       <c r="G277" s="9" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H277" s="9">
         <f t="shared" si="57"/>
@@ -29031,10 +29097,10 @@
         <v>664</v>
       </c>
       <c r="P277" s="13" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="Q277" s="9" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="R277" s="9" t="s">
         <v>159</v>
@@ -29049,7 +29115,7 @@
     </row>
     <row r="278" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A278" s="13" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B278" s="17">
         <v>2024</v>
@@ -29067,7 +29133,7 @@
         <v>253</v>
       </c>
       <c r="G278" s="9" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H278" s="9">
         <f t="shared" si="57"/>
@@ -29096,10 +29162,10 @@
         <v>664</v>
       </c>
       <c r="P278" s="13" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="Q278" s="9" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="R278" s="9" t="s">
         <v>159</v>
@@ -29114,7 +29180,7 @@
     </row>
     <row r="279" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A279" s="13" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B279" s="17">
         <v>2024</v>
@@ -29132,7 +29198,7 @@
         <v>316</v>
       </c>
       <c r="G279" s="9" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H279" s="9">
         <f t="shared" si="57"/>
@@ -29161,10 +29227,10 @@
         <v>664</v>
       </c>
       <c r="P279" s="13" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="Q279" s="9" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="R279" s="9" t="s">
         <v>159</v>
@@ -29179,7 +29245,7 @@
     </row>
     <row r="280" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A280" s="13" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B280" s="17">
         <v>2024</v>
@@ -29197,7 +29263,7 @@
         <v>112</v>
       </c>
       <c r="G280" s="9" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H280" s="9">
         <f t="shared" ref="H280" si="60">YEAR(G280)</f>
@@ -29214,7 +29280,7 @@
         <v>159</v>
       </c>
       <c r="L280" s="9" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="M280" s="17">
         <v>3</v>
@@ -29226,10 +29292,10 @@
         <v>664</v>
       </c>
       <c r="P280" s="13" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="Q280" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R280" s="9" t="s">
         <v>159</v>
@@ -29244,7 +29310,7 @@
     </row>
     <row r="281" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A281" s="13" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B281" s="17">
         <v>2024</v>
@@ -29262,7 +29328,7 @@
         <v>1779</v>
       </c>
       <c r="G281" s="9" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H281" s="9">
         <f t="shared" ref="H281:H283" si="61">YEAR(G281)</f>
@@ -29291,10 +29357,10 @@
         <v>664</v>
       </c>
       <c r="P281" s="13" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="Q281" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R281" s="9" t="s">
         <v>159</v>
@@ -29309,7 +29375,7 @@
     </row>
     <row r="282" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A282" s="13" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B282" s="17">
         <v>2022</v>
@@ -29327,7 +29393,7 @@
         <v>365</v>
       </c>
       <c r="G282" s="9" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="H282" s="9">
         <f t="shared" si="61"/>
@@ -29356,10 +29422,10 @@
         <v>664</v>
       </c>
       <c r="P282" s="16" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="Q282" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R282" s="9" t="s">
         <v>159</v>
@@ -29374,7 +29440,7 @@
     </row>
     <row r="283" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A283" s="13" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B283" s="17">
         <v>2023</v>
@@ -29392,7 +29458,7 @@
         <v>340</v>
       </c>
       <c r="G283" s="9" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H283" s="9">
         <f t="shared" si="61"/>
@@ -29421,7 +29487,7 @@
         <v>664</v>
       </c>
       <c r="P283" s="13" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="Q283" s="9" t="s">
         <v>469</v>
@@ -29439,7 +29505,7 @@
     </row>
     <row r="284" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A284" s="13" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B284" s="17">
         <v>2023</v>
@@ -29457,7 +29523,7 @@
         <v>600</v>
       </c>
       <c r="G284" s="9" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="H284" s="9">
         <f t="shared" ref="H284" si="62">YEAR(G284)</f>
@@ -29486,7 +29552,7 @@
         <v>664</v>
       </c>
       <c r="P284" s="13" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="Q284" s="9" t="s">
         <v>469</v>
@@ -29504,7 +29570,7 @@
     </row>
     <row r="285" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A285" s="13" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B285" s="17">
         <v>2024</v>
@@ -29522,7 +29588,7 @@
         <v>289</v>
       </c>
       <c r="G285" s="9" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="H285" s="9">
         <f t="shared" ref="H285" si="64">YEAR(G285)</f>
@@ -29551,7 +29617,7 @@
         <v>664</v>
       </c>
       <c r="P285" s="13" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="Q285" s="9" t="s">
         <v>569</v>
@@ -29569,7 +29635,7 @@
     </row>
     <row r="286" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A286" s="13" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B286" s="17">
         <v>2024</v>
@@ -29587,7 +29653,7 @@
         <v>198</v>
       </c>
       <c r="G286" s="9" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="H286" s="9">
         <f t="shared" ref="H286" si="66">YEAR(G286)</f>
@@ -29616,10 +29682,10 @@
         <v>664</v>
       </c>
       <c r="P286" s="16" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="Q286" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R286" s="9" t="s">
         <v>159</v>
@@ -29634,7 +29700,7 @@
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A287" s="13" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B287" s="17">
         <v>2024</v>
@@ -29652,7 +29718,7 @@
         <v>224</v>
       </c>
       <c r="G287" s="9" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="H287" s="9">
         <f t="shared" ref="H287" si="68">YEAR(G287)</f>
@@ -29681,10 +29747,10 @@
         <v>664</v>
       </c>
       <c r="P287" s="16" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="Q287" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R287" s="9" t="s">
         <v>159</v>
@@ -29699,7 +29765,7 @@
     </row>
     <row r="288" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A288" s="13" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B288" s="17">
         <v>2022</v>
@@ -29717,7 +29783,7 @@
         <v>296</v>
       </c>
       <c r="G288" s="9" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="H288" s="9">
         <f t="shared" ref="H288" si="70">YEAR(G288)</f>
@@ -29746,10 +29812,10 @@
         <v>664</v>
       </c>
       <c r="P288" s="16" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="Q288" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R288" s="9" t="s">
         <v>159</v>
@@ -29764,7 +29830,7 @@
     </row>
     <row r="289" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A289" s="13" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B289" s="17">
         <v>2023</v>
@@ -29782,7 +29848,7 @@
         <v>200</v>
       </c>
       <c r="G289" s="9" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="H289" s="9">
         <f t="shared" ref="H289" si="73">YEAR(G289)</f>
@@ -29811,10 +29877,10 @@
         <v>664</v>
       </c>
       <c r="P289" s="16" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="Q289" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R289" s="9" t="s">
         <v>159</v>
@@ -29829,7 +29895,7 @@
     </row>
     <row r="290" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A290" s="13" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B290" s="17">
         <v>2023</v>
@@ -29847,7 +29913,7 @@
         <v>255</v>
       </c>
       <c r="G290" s="9" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="H290" s="9">
         <f t="shared" ref="H290" si="76">YEAR(G290)</f>
@@ -29876,7 +29942,7 @@
         <v>664</v>
       </c>
       <c r="P290" s="16" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="Q290" s="9" t="s">
         <v>469</v>
@@ -29894,7 +29960,7 @@
     </row>
     <row r="291" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A291" s="13" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B291" s="17">
         <v>2023</v>
@@ -29912,7 +29978,7 @@
         <v>192</v>
       </c>
       <c r="G291" s="9" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="H291" s="9">
         <f t="shared" ref="H291" si="79">YEAR(G291)</f>
@@ -29941,10 +30007,10 @@
         <v>664</v>
       </c>
       <c r="P291" s="16" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="Q291" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R291" s="9" t="s">
         <v>159</v>
@@ -29959,7 +30025,7 @@
     </row>
     <row r="292" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A292" s="13" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B292" s="17">
         <v>2015</v>
@@ -29977,7 +30043,7 @@
         <v>96</v>
       </c>
       <c r="G292" s="9" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="H292" s="9">
         <f t="shared" ref="H292" si="82">YEAR(G292)</f>
@@ -29994,7 +30060,7 @@
         <v>159</v>
       </c>
       <c r="L292" s="9" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="M292" s="17">
         <v>3</v>
@@ -30009,7 +30075,7 @@
         <v>707</v>
       </c>
       <c r="Q292" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R292" s="9" t="s">
         <v>159</v>
@@ -30024,7 +30090,7 @@
     </row>
     <row r="293" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A293" s="13" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B293" s="17">
         <v>2022</v>
@@ -30042,7 +30108,7 @@
         <v>194</v>
       </c>
       <c r="G293" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="H293" s="9">
         <f t="shared" ref="H293" si="84">YEAR(G293)</f>
@@ -30059,7 +30125,7 @@
         <v>159</v>
       </c>
       <c r="L293" s="9" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="M293" s="17">
         <v>3</v>
@@ -30071,10 +30137,10 @@
         <v>664</v>
       </c>
       <c r="P293" s="28" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="Q293" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="R293" s="9" t="s">
         <v>159</v>
@@ -30089,7 +30155,7 @@
     </row>
     <row r="294" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A294" s="13" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B294" s="17">
         <v>2018</v>
@@ -30107,7 +30173,7 @@
         <v>188</v>
       </c>
       <c r="G294" s="9" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="H294" s="9">
         <f t="shared" ref="H294:H296" si="86">YEAR(G294)</f>
@@ -30124,7 +30190,7 @@
         <v>159</v>
       </c>
       <c r="L294" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="M294" s="17">
         <v>4</v>
@@ -30136,7 +30202,7 @@
         <v>664</v>
       </c>
       <c r="P294" s="16" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="Q294" s="9" t="s">
         <v>469</v>
@@ -30154,7 +30220,7 @@
     </row>
     <row r="295" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A295" s="13" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B295" s="17">
         <v>2021</v>
@@ -30172,7 +30238,7 @@
         <v>631</v>
       </c>
       <c r="G295" s="9" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="H295" s="9">
         <f t="shared" si="86"/>
@@ -30201,7 +30267,7 @@
         <v>664</v>
       </c>
       <c r="P295" s="16" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="Q295" s="9" t="s">
         <v>569</v>
@@ -30219,7 +30285,7 @@
     </row>
     <row r="296" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A296" s="13" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B296" s="17">
         <v>2023</v>
@@ -30237,7 +30303,7 @@
         <v>318</v>
       </c>
       <c r="G296" s="9" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="H296" s="9">
         <f t="shared" si="86"/>
@@ -30266,7 +30332,7 @@
         <v>664</v>
       </c>
       <c r="P296" s="16" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="Q296" s="9" t="s">
         <v>874</v>
@@ -30284,7 +30350,7 @@
     </row>
     <row r="297" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A297" s="13" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B297" s="17">
         <v>2023</v>
@@ -30302,7 +30368,7 @@
         <v>298</v>
       </c>
       <c r="G297" s="9" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="H297" s="9">
         <f t="shared" ref="H297" si="88">YEAR(G297)</f>
@@ -30331,7 +30397,7 @@
         <v>664</v>
       </c>
       <c r="P297" s="16" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="Q297" s="9" t="s">
         <v>874</v>
@@ -30349,7 +30415,7 @@
     </row>
     <row r="298" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A298" s="13" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B298" s="17">
         <v>2023</v>
@@ -30367,7 +30433,7 @@
         <v>636</v>
       </c>
       <c r="G298" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="H298" s="9">
         <f t="shared" ref="H298" si="90">YEAR(G298)</f>
@@ -30396,7 +30462,7 @@
         <v>664</v>
       </c>
       <c r="P298" s="16" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="Q298" s="9" t="s">
         <v>569</v>
@@ -30414,7 +30480,7 @@
     </row>
     <row r="299" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A299" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B299" s="17">
         <v>2023</v>
@@ -30432,7 +30498,7 @@
         <v>218</v>
       </c>
       <c r="G299" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="H299" s="9">
         <f t="shared" ref="H299" si="92">YEAR(G299)</f>
@@ -30461,7 +30527,7 @@
         <v>664</v>
       </c>
       <c r="P299" s="16" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="Q299" s="9" t="s">
         <v>569</v>
@@ -30479,7 +30545,7 @@
     </row>
     <row r="300" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A300" s="13" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B300" s="17">
         <v>2022</v>
@@ -30497,7 +30563,7 @@
         <v>464</v>
       </c>
       <c r="G300" s="9" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H300" s="9">
         <f t="shared" ref="H300" si="94">YEAR(G300)</f>
@@ -30526,7 +30592,7 @@
         <v>664</v>
       </c>
       <c r="P300" s="16" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="Q300" s="9" t="s">
         <v>569</v>
@@ -30544,7 +30610,7 @@
     </row>
     <row r="301" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A301" s="13" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B301" s="17">
         <v>2023</v>
@@ -30562,7 +30628,7 @@
         <v>58</v>
       </c>
       <c r="G301" s="9" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H301" s="9">
         <f t="shared" ref="H301" si="96">YEAR(G301)</f>
@@ -30591,10 +30657,10 @@
         <v>664</v>
       </c>
       <c r="P301" s="28" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Q301" s="9" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="R301" s="9" t="s">
         <v>159</v>
@@ -30609,7 +30675,7 @@
     </row>
     <row r="302" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A302" s="13" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B302" s="17">
         <v>2023</v>
@@ -30627,7 +30693,7 @@
         <v>161</v>
       </c>
       <c r="G302" s="9" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H302" s="9">
         <f t="shared" ref="H302" si="98">YEAR(G302)</f>
@@ -30656,10 +30722,10 @@
         <v>664</v>
       </c>
       <c r="P302" s="13" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="Q302" s="9" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R302" s="9" t="s">
         <v>159</v>
@@ -30674,7 +30740,7 @@
     </row>
     <row r="303" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A303" s="13" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B303" s="17">
         <v>2023</v>
@@ -30692,7 +30758,7 @@
         <v>331</v>
       </c>
       <c r="G303" s="9" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H303" s="9">
         <f t="shared" ref="H303" si="100">YEAR(G303)</f>
@@ -30721,7 +30787,7 @@
         <v>664</v>
       </c>
       <c r="P303" s="16" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="Q303" s="9" t="s">
         <v>469</v>
@@ -30739,7 +30805,7 @@
     </row>
     <row r="304" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A304" s="13" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B304" s="17">
         <v>2024</v>
@@ -30757,7 +30823,7 @@
         <v>179</v>
       </c>
       <c r="G304" s="9" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="H304" s="9">
         <f t="shared" ref="H304" si="102">YEAR(G304)</f>
@@ -30786,7 +30852,7 @@
         <v>664</v>
       </c>
       <c r="P304" s="13" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="Q304" s="9" t="s">
         <v>501</v>
@@ -30804,7 +30870,7 @@
     </row>
     <row r="305" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A305" s="13" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B305" s="17">
         <v>2024</v>
@@ -30822,7 +30888,7 @@
         <v>123</v>
       </c>
       <c r="G305" s="9" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="H305" s="9">
         <f t="shared" ref="H305" si="104">YEAR(G305)</f>
@@ -30851,7 +30917,7 @@
         <v>664</v>
       </c>
       <c r="P305" s="13" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="Q305" s="9" t="s">
         <v>501</v>
@@ -30860,7 +30926,7 @@
         <v>159</v>
       </c>
       <c r="S305" s="17">
-        <f t="shared" ref="S305:S308" si="106">LEN(P305)</f>
+        <f t="shared" ref="S305:S313" si="106">LEN(P305)</f>
         <v>88</v>
       </c>
       <c r="T305" s="14">
@@ -30869,7 +30935,7 @@
     </row>
     <row r="306" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A306" s="13" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B306" s="17">
         <v>2024</v>
@@ -30887,7 +30953,7 @@
         <v>368</v>
       </c>
       <c r="G306" s="9" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="H306" s="9">
         <f t="shared" ref="H306" si="107">YEAR(G306)</f>
@@ -30916,10 +30982,10 @@
         <v>664</v>
       </c>
       <c r="P306" s="13" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="Q306" s="9" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="R306" s="9" t="s">
         <v>159</v>
@@ -30934,7 +31000,7 @@
     </row>
     <row r="307" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A307" s="13" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B307" s="17">
         <v>2021</v>
@@ -30952,7 +31018,7 @@
         <v>323</v>
       </c>
       <c r="G307" s="9" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="H307" s="9">
         <f t="shared" ref="H307" si="109">YEAR(G307)</f>
@@ -30981,7 +31047,7 @@
         <v>664</v>
       </c>
       <c r="P307" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="Q307" s="9" t="s">
         <v>569</v>
@@ -30999,7 +31065,7 @@
     </row>
     <row r="308" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A308" s="13" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B308" s="17">
         <v>2022</v>
@@ -31017,14 +31083,14 @@
         <v>426</v>
       </c>
       <c r="G308" s="9" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="H308" s="9">
-        <f t="shared" ref="H308" si="111">YEAR(G308)</f>
+        <f t="shared" ref="H308:H309" si="111">YEAR(G308)</f>
         <v>2024</v>
       </c>
       <c r="I308" s="9">
-        <f t="shared" ref="I308" si="112">MONTH(G308)</f>
+        <f t="shared" ref="I308:I309" si="112">MONTH(G308)</f>
         <v>11</v>
       </c>
       <c r="J308" s="9" t="s">
@@ -31046,7 +31112,7 @@
         <v>664</v>
       </c>
       <c r="P308" s="13" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="Q308" s="9" t="s">
         <v>469</v>
@@ -31063,158 +31129,810 @@
       </c>
     </row>
     <row r="309" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A309" s="13"/>
-      <c r="B309" s="9"/>
-      <c r="C309" s="9"/>
-      <c r="D309" s="9"/>
-      <c r="E309" s="9"/>
-      <c r="F309" s="9"/>
-      <c r="G309" s="9"/>
-      <c r="H309" s="9"/>
-      <c r="I309" s="9"/>
-      <c r="J309" s="9"/>
-      <c r="K309" s="9"/>
-      <c r="L309" s="9"/>
-      <c r="M309" s="9"/>
-      <c r="N309" s="9"/>
-      <c r="O309" s="9"/>
-      <c r="P309" s="13"/>
-      <c r="Q309" s="9"/>
-      <c r="R309" s="9"/>
-      <c r="S309" s="17"/>
-      <c r="T309" s="9"/>
+      <c r="A309" s="13" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B309" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C309" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D309" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E309" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F309" s="17">
+        <v>296</v>
+      </c>
+      <c r="G309" s="9" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H309" s="9">
+        <f t="shared" si="111"/>
+        <v>2024</v>
+      </c>
+      <c r="I309" s="9">
+        <f t="shared" si="112"/>
+        <v>11</v>
+      </c>
+      <c r="J309" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K309" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L309" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M309" s="17">
+        <v>2</v>
+      </c>
+      <c r="N309" s="17">
+        <v>39.909999999999997</v>
+      </c>
+      <c r="O309" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P309" s="16" t="s">
+        <v>1045</v>
+      </c>
+      <c r="Q309" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R309" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S309" s="17">
+        <f t="shared" si="106"/>
+        <v>260</v>
+      </c>
+      <c r="T309" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="310" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A310" s="13"/>
-      <c r="B310" s="9"/>
-      <c r="C310" s="9"/>
-      <c r="D310" s="9"/>
-      <c r="E310" s="9"/>
-      <c r="F310" s="9"/>
-      <c r="G310" s="9"/>
-      <c r="H310" s="9"/>
-      <c r="I310" s="9"/>
-      <c r="J310" s="9"/>
-      <c r="K310" s="9"/>
-      <c r="L310" s="9"/>
-      <c r="M310" s="9"/>
-      <c r="N310" s="9"/>
-      <c r="O310" s="9"/>
-      <c r="P310" s="13"/>
-      <c r="Q310" s="9"/>
-      <c r="R310" s="9"/>
-      <c r="S310" s="17"/>
-      <c r="T310" s="9"/>
+      <c r="A310" s="13" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B310" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C310" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D310" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E310" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F310" s="17">
+        <v>363</v>
+      </c>
+      <c r="G310" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H310" s="9">
+        <f t="shared" ref="H310" si="113">YEAR(G310)</f>
+        <v>2024</v>
+      </c>
+      <c r="I310" s="9">
+        <f t="shared" ref="I310" si="114">MONTH(G310)</f>
+        <v>11</v>
+      </c>
+      <c r="J310" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K310" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L310" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="M310" s="17">
+        <v>2</v>
+      </c>
+      <c r="N310" s="17">
+        <v>59.99</v>
+      </c>
+      <c r="O310" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P310" s="13" t="s">
+        <v>1048</v>
+      </c>
+      <c r="Q310" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="R310" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S310" s="17">
+        <f t="shared" si="106"/>
+        <v>66</v>
+      </c>
+      <c r="T310" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="311" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A311" s="13"/>
-      <c r="B311" s="9"/>
-      <c r="C311" s="9"/>
-      <c r="D311" s="9"/>
-      <c r="E311" s="9"/>
-      <c r="F311" s="9"/>
-      <c r="G311" s="9"/>
-      <c r="H311" s="9"/>
-      <c r="I311" s="9"/>
-      <c r="J311" s="9"/>
-      <c r="K311" s="9"/>
-      <c r="L311" s="9"/>
-      <c r="M311" s="9"/>
-      <c r="N311" s="9"/>
-      <c r="O311" s="9"/>
-      <c r="P311" s="13"/>
-      <c r="Q311" s="9"/>
-      <c r="R311" s="9"/>
-      <c r="S311" s="17"/>
-      <c r="T311" s="9"/>
+      <c r="A311" s="13" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B311" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C311" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D311" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E311" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F311" s="17">
+        <v>434</v>
+      </c>
+      <c r="G311" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H311" s="9">
+        <f t="shared" ref="H311" si="115">YEAR(G311)</f>
+        <v>2024</v>
+      </c>
+      <c r="I311" s="9">
+        <f t="shared" ref="I311" si="116">MONTH(G311)</f>
+        <v>11</v>
+      </c>
+      <c r="J311" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K311" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L311" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="M311" s="17">
+        <v>2</v>
+      </c>
+      <c r="N311" s="17">
+        <v>54.99</v>
+      </c>
+      <c r="O311" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P311" s="16" t="s">
+        <v>1051</v>
+      </c>
+      <c r="Q311" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R311" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S311" s="17">
+        <f t="shared" si="106"/>
+        <v>243</v>
+      </c>
+      <c r="T311" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="312" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A312" s="13"/>
-      <c r="B312" s="9"/>
-      <c r="C312" s="9"/>
-      <c r="D312" s="9"/>
-      <c r="E312" s="9"/>
-      <c r="F312" s="9"/>
-      <c r="G312" s="9"/>
-      <c r="H312" s="9"/>
-      <c r="I312" s="9"/>
-      <c r="J312" s="9"/>
-      <c r="K312" s="9"/>
-      <c r="L312" s="9"/>
-      <c r="M312" s="9"/>
-      <c r="N312" s="9"/>
-      <c r="O312" s="9"/>
-      <c r="P312" s="13"/>
-      <c r="Q312" s="9"/>
-      <c r="R312" s="9"/>
-      <c r="S312" s="17"/>
-      <c r="T312" s="9"/>
+      <c r="A312" s="13" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B312" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C312" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D312" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E312" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F312" s="17">
+        <v>490</v>
+      </c>
+      <c r="G312" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H312" s="9">
+        <f t="shared" ref="H312" si="117">YEAR(G312)</f>
+        <v>2024</v>
+      </c>
+      <c r="I312" s="9">
+        <f t="shared" ref="I312" si="118">MONTH(G312)</f>
+        <v>11</v>
+      </c>
+      <c r="J312" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K312" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L312" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M312" s="17">
+        <v>4</v>
+      </c>
+      <c r="N312" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O312" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P312" s="16" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Q312" s="9" t="s">
+        <v>962</v>
+      </c>
+      <c r="R312" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S312" s="17">
+        <f t="shared" si="106"/>
+        <v>379</v>
+      </c>
+      <c r="T312" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="313" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A313" s="13"/>
-      <c r="B313" s="9"/>
-      <c r="C313" s="9"/>
-      <c r="D313" s="9"/>
-      <c r="E313" s="9"/>
-      <c r="F313" s="9"/>
-      <c r="G313" s="9"/>
-      <c r="H313" s="9"/>
-      <c r="I313" s="9"/>
-      <c r="J313" s="9"/>
-      <c r="K313" s="9"/>
-      <c r="L313" s="9"/>
-      <c r="M313" s="9"/>
-      <c r="N313" s="9"/>
-      <c r="O313" s="9"/>
-      <c r="P313" s="13"/>
-      <c r="Q313" s="9"/>
-      <c r="R313" s="9"/>
-      <c r="S313" s="17"/>
-      <c r="T313" s="9"/>
+      <c r="A313" s="13" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B313" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C313" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D313" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E313" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F313" s="17">
+        <v>195</v>
+      </c>
+      <c r="G313" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H313" s="9">
+        <f t="shared" ref="H313" si="119">YEAR(G313)</f>
+        <v>2024</v>
+      </c>
+      <c r="I313" s="9">
+        <f t="shared" ref="I313" si="120">MONTH(G313)</f>
+        <v>11</v>
+      </c>
+      <c r="J313" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K313" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L313" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="M313" s="17">
+        <v>1</v>
+      </c>
+      <c r="N313" s="17">
+        <v>122.67</v>
+      </c>
+      <c r="O313" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P313" s="13" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Q313" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="R313" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S313" s="17">
+        <f t="shared" si="106"/>
+        <v>31</v>
+      </c>
+      <c r="T313" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="314" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A314" s="13"/>
-      <c r="B314" s="9"/>
-      <c r="C314" s="9"/>
-      <c r="D314" s="9"/>
-      <c r="E314" s="9"/>
-      <c r="F314" s="9"/>
-      <c r="G314" s="9"/>
-      <c r="H314" s="9"/>
-      <c r="I314" s="9"/>
-      <c r="J314" s="9"/>
-      <c r="K314" s="9"/>
-      <c r="L314" s="9"/>
-      <c r="M314" s="9"/>
-      <c r="N314" s="9"/>
-      <c r="O314" s="9"/>
-      <c r="P314" s="13"/>
-      <c r="Q314" s="9"/>
-      <c r="R314" s="9"/>
-      <c r="S314" s="17"/>
-      <c r="T314" s="9"/>
+      <c r="A314" s="13" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B314" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C314" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D314" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E314" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F314" s="17">
+        <v>280</v>
+      </c>
+      <c r="G314" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H314" s="9">
+        <f t="shared" ref="H314" si="121">YEAR(G314)</f>
+        <v>2024</v>
+      </c>
+      <c r="I314" s="9">
+        <f t="shared" ref="I314" si="122">MONTH(G314)</f>
+        <v>11</v>
+      </c>
+      <c r="J314" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K314" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L314" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M314" s="17">
+        <v>2</v>
+      </c>
+      <c r="N314" s="17">
+        <v>60.18</v>
+      </c>
+      <c r="O314" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P314" s="13" t="s">
+        <v>1058</v>
+      </c>
+      <c r="Q314" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="R314" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S314" s="17">
+        <f t="shared" ref="S314:S316" si="123">LEN(P314)</f>
+        <v>35</v>
+      </c>
+      <c r="T314" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="315" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A315" s="13"/>
-      <c r="B315" s="9"/>
-      <c r="C315" s="9"/>
-      <c r="D315" s="9"/>
-      <c r="E315" s="9"/>
-      <c r="F315" s="9"/>
-      <c r="G315" s="9"/>
-      <c r="H315" s="9"/>
-      <c r="I315" s="9"/>
-      <c r="J315" s="9"/>
-      <c r="K315" s="9"/>
-      <c r="L315" s="9"/>
-      <c r="M315" s="9"/>
-      <c r="N315" s="9"/>
-      <c r="O315" s="9"/>
-      <c r="P315" s="13"/>
-      <c r="Q315" s="9"/>
-      <c r="R315" s="9"/>
-      <c r="S315" s="17"/>
-      <c r="T315" s="9"/>
+      <c r="A315" s="13" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B315" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C315" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D315" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E315" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F315" s="17">
+        <v>472</v>
+      </c>
+      <c r="G315" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H315" s="9">
+        <f t="shared" ref="H315" si="124">YEAR(G315)</f>
+        <v>2024</v>
+      </c>
+      <c r="I315" s="9">
+        <f t="shared" ref="I315" si="125">MONTH(G315)</f>
+        <v>11</v>
+      </c>
+      <c r="J315" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K315" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L315" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M315" s="17">
+        <v>1</v>
+      </c>
+      <c r="N315" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O315" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P315" s="13" t="s">
+        <v>1060</v>
+      </c>
+      <c r="Q315" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="R315" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S315" s="17">
+        <f t="shared" si="123"/>
+        <v>60</v>
+      </c>
+      <c r="T315" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A316" s="13" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B316" s="17">
+        <v>2016</v>
+      </c>
+      <c r="C316" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D316" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E316" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F316" s="17">
+        <v>68</v>
+      </c>
+      <c r="G316" s="9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="H316" s="9">
+        <f t="shared" ref="H316" si="126">YEAR(G316)</f>
+        <v>2024</v>
+      </c>
+      <c r="I316" s="9">
+        <f t="shared" ref="I316" si="127">MONTH(G316)</f>
+        <v>11</v>
+      </c>
+      <c r="J316" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K316" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L316" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M316" s="17">
+        <v>5</v>
+      </c>
+      <c r="N316" s="43">
+        <v>0</v>
+      </c>
+      <c r="O316" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P316" s="16" t="s">
+        <v>1064</v>
+      </c>
+      <c r="Q316" s="9" t="s">
+        <v>962</v>
+      </c>
+      <c r="R316" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S316" s="17">
+        <f t="shared" si="123"/>
+        <v>155</v>
+      </c>
+      <c r="T316" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A317" s="9"/>
+      <c r="B317" s="9"/>
+      <c r="C317" s="9"/>
+      <c r="D317" s="9"/>
+      <c r="E317" s="9"/>
+      <c r="F317" s="9"/>
+      <c r="G317" s="9"/>
+      <c r="H317" s="9"/>
+      <c r="I317" s="9"/>
+      <c r="J317" s="9"/>
+      <c r="K317" s="9"/>
+      <c r="L317" s="9"/>
+      <c r="M317" s="9"/>
+      <c r="N317" s="9"/>
+      <c r="O317" s="9"/>
+      <c r="P317" s="9"/>
+      <c r="Q317" s="9"/>
+      <c r="R317" s="9"/>
+      <c r="S317" s="17"/>
+      <c r="T317" s="9"/>
+    </row>
+    <row r="318" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A318" s="9"/>
+      <c r="B318" s="9"/>
+      <c r="C318" s="9"/>
+      <c r="D318" s="9"/>
+      <c r="E318" s="9"/>
+      <c r="F318" s="9"/>
+      <c r="G318" s="9"/>
+      <c r="H318" s="9"/>
+      <c r="I318" s="9"/>
+      <c r="J318" s="9"/>
+      <c r="K318" s="9"/>
+      <c r="L318" s="9"/>
+      <c r="M318" s="9"/>
+      <c r="N318" s="9"/>
+      <c r="O318" s="9"/>
+      <c r="P318" s="9"/>
+      <c r="Q318" s="9"/>
+      <c r="R318" s="9"/>
+      <c r="S318" s="17"/>
+      <c r="T318" s="9"/>
+    </row>
+    <row r="319" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A319" s="9"/>
+      <c r="B319" s="9"/>
+      <c r="C319" s="9"/>
+      <c r="D319" s="9"/>
+      <c r="E319" s="9"/>
+      <c r="F319" s="9"/>
+      <c r="G319" s="9"/>
+      <c r="H319" s="9"/>
+      <c r="I319" s="9"/>
+      <c r="J319" s="9"/>
+      <c r="K319" s="9"/>
+      <c r="L319" s="9"/>
+      <c r="M319" s="9"/>
+      <c r="N319" s="9"/>
+      <c r="O319" s="9"/>
+      <c r="P319" s="9"/>
+      <c r="Q319" s="9"/>
+      <c r="R319" s="9"/>
+      <c r="S319" s="17"/>
+      <c r="T319" s="9"/>
+    </row>
+    <row r="320" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A320" s="9"/>
+      <c r="B320" s="9"/>
+      <c r="C320" s="9"/>
+      <c r="D320" s="9"/>
+      <c r="E320" s="9"/>
+      <c r="F320" s="9"/>
+      <c r="G320" s="9"/>
+      <c r="H320" s="9"/>
+      <c r="I320" s="9"/>
+      <c r="J320" s="9"/>
+      <c r="K320" s="9"/>
+      <c r="L320" s="9"/>
+      <c r="M320" s="9"/>
+      <c r="N320" s="9"/>
+      <c r="O320" s="9"/>
+      <c r="P320" s="9"/>
+      <c r="Q320" s="9"/>
+      <c r="R320" s="9"/>
+      <c r="S320" s="17"/>
+      <c r="T320" s="9"/>
+    </row>
+    <row r="321" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A321" s="9"/>
+      <c r="B321" s="9"/>
+      <c r="C321" s="9"/>
+      <c r="D321" s="9"/>
+      <c r="E321" s="9"/>
+      <c r="F321" s="9"/>
+      <c r="G321" s="9"/>
+      <c r="H321" s="9"/>
+      <c r="I321" s="9"/>
+      <c r="J321" s="9"/>
+      <c r="K321" s="9"/>
+      <c r="L321" s="9"/>
+      <c r="M321" s="9"/>
+      <c r="N321" s="9"/>
+      <c r="O321" s="9"/>
+      <c r="P321" s="9"/>
+      <c r="Q321" s="9"/>
+      <c r="R321" s="9"/>
+      <c r="S321" s="17"/>
+      <c r="T321" s="9"/>
+    </row>
+    <row r="322" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A322" s="9"/>
+      <c r="B322" s="9"/>
+      <c r="C322" s="9"/>
+      <c r="D322" s="9"/>
+      <c r="E322" s="9"/>
+      <c r="F322" s="9"/>
+      <c r="G322" s="9"/>
+      <c r="H322" s="9"/>
+      <c r="I322" s="9"/>
+      <c r="J322" s="9"/>
+      <c r="K322" s="9"/>
+      <c r="L322" s="9"/>
+      <c r="M322" s="9"/>
+      <c r="N322" s="9"/>
+      <c r="O322" s="9"/>
+      <c r="P322" s="9"/>
+      <c r="Q322" s="9"/>
+      <c r="R322" s="9"/>
+      <c r="S322" s="17"/>
+      <c r="T322" s="9"/>
+    </row>
+    <row r="323" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A323" s="9"/>
+      <c r="B323" s="9"/>
+      <c r="C323" s="9"/>
+      <c r="D323" s="9"/>
+      <c r="E323" s="9"/>
+      <c r="F323" s="9"/>
+      <c r="G323" s="9"/>
+      <c r="H323" s="9"/>
+      <c r="I323" s="9"/>
+      <c r="J323" s="9"/>
+      <c r="K323" s="9"/>
+      <c r="L323" s="9"/>
+      <c r="M323" s="9"/>
+      <c r="N323" s="9"/>
+      <c r="O323" s="9"/>
+      <c r="P323" s="9"/>
+      <c r="Q323" s="9"/>
+      <c r="R323" s="9"/>
+      <c r="S323" s="17"/>
+      <c r="T323" s="9"/>
+    </row>
+    <row r="324" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A324" s="9"/>
+      <c r="B324" s="9"/>
+      <c r="C324" s="9"/>
+      <c r="D324" s="9"/>
+      <c r="E324" s="9"/>
+      <c r="F324" s="9"/>
+      <c r="G324" s="9"/>
+      <c r="H324" s="9"/>
+      <c r="I324" s="9"/>
+      <c r="J324" s="9"/>
+      <c r="K324" s="9"/>
+      <c r="L324" s="9"/>
+      <c r="M324" s="9"/>
+      <c r="N324" s="9"/>
+      <c r="O324" s="9"/>
+      <c r="P324" s="9"/>
+      <c r="Q324" s="9"/>
+      <c r="R324" s="9"/>
+      <c r="S324" s="17"/>
+      <c r="T324" s="9"/>
+    </row>
+    <row r="325" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A325" s="9"/>
+      <c r="B325" s="9"/>
+      <c r="C325" s="9"/>
+      <c r="D325" s="9"/>
+      <c r="E325" s="9"/>
+      <c r="F325" s="9"/>
+      <c r="G325" s="9"/>
+      <c r="H325" s="9"/>
+      <c r="I325" s="9"/>
+      <c r="J325" s="9"/>
+      <c r="K325" s="9"/>
+      <c r="L325" s="9"/>
+      <c r="M325" s="9"/>
+      <c r="N325" s="9"/>
+      <c r="O325" s="9"/>
+      <c r="P325" s="9"/>
+      <c r="Q325" s="9"/>
+      <c r="R325" s="9"/>
+      <c r="S325" s="17"/>
+      <c r="T325" s="9"/>
+    </row>
+    <row r="326" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A326" s="9"/>
+      <c r="B326" s="9"/>
+      <c r="C326" s="9"/>
+      <c r="D326" s="9"/>
+      <c r="E326" s="9"/>
+      <c r="F326" s="9"/>
+      <c r="G326" s="9"/>
+      <c r="H326" s="9"/>
+      <c r="I326" s="9"/>
+      <c r="J326" s="9"/>
+      <c r="K326" s="9"/>
+      <c r="L326" s="9"/>
+      <c r="M326" s="9"/>
+      <c r="N326" s="9"/>
+      <c r="O326" s="9"/>
+      <c r="P326" s="9"/>
+      <c r="Q326" s="9"/>
+      <c r="R326" s="9"/>
+      <c r="S326" s="17"/>
+      <c r="T326" s="9"/>
+    </row>
+    <row r="327" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A327" s="9"/>
+      <c r="B327" s="9"/>
+      <c r="C327" s="9"/>
+      <c r="D327" s="9"/>
+      <c r="E327" s="9"/>
+      <c r="F327" s="9"/>
+      <c r="G327" s="9"/>
+      <c r="H327" s="9"/>
+      <c r="I327" s="9"/>
+      <c r="J327" s="9"/>
+      <c r="K327" s="9"/>
+      <c r="L327" s="9"/>
+      <c r="M327" s="9"/>
+      <c r="N327" s="9"/>
+      <c r="O327" s="9"/>
+      <c r="P327" s="9"/>
+      <c r="Q327" s="9"/>
+      <c r="R327" s="9"/>
+      <c r="S327" s="17"/>
+      <c r="T327" s="9"/>
+    </row>
+    <row r="328" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A328" s="9"/>
+      <c r="B328" s="9"/>
+      <c r="C328" s="9"/>
+      <c r="D328" s="9"/>
+      <c r="E328" s="9"/>
+      <c r="F328" s="9"/>
+      <c r="G328" s="9"/>
+      <c r="H328" s="9"/>
+      <c r="I328" s="9"/>
+      <c r="J328" s="9"/>
+      <c r="K328" s="9"/>
+      <c r="L328" s="9"/>
+      <c r="M328" s="9"/>
+      <c r="N328" s="9"/>
+      <c r="O328" s="9"/>
+      <c r="P328" s="9"/>
+      <c r="Q328" s="9"/>
+      <c r="R328" s="9"/>
+      <c r="S328" s="17"/>
+      <c r="T328" s="9"/>
+    </row>
+    <row r="329" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A329" s="9"/>
+      <c r="B329" s="9"/>
+      <c r="C329" s="9"/>
+      <c r="D329" s="9"/>
+      <c r="E329" s="9"/>
+      <c r="F329" s="9"/>
+      <c r="G329" s="9"/>
+      <c r="H329" s="9"/>
+      <c r="I329" s="9"/>
+      <c r="J329" s="9"/>
+      <c r="K329" s="9"/>
+      <c r="L329" s="9"/>
+      <c r="M329" s="9"/>
+      <c r="N329" s="9"/>
+      <c r="O329" s="9"/>
+      <c r="P329" s="9"/>
+      <c r="Q329" s="9"/>
+      <c r="R329" s="9"/>
+      <c r="S329" s="17"/>
+      <c r="T329" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#38 Reading List: updated to 2024-11-27.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4998" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5082" uniqueCount="1081">
   <si>
     <t>Format</t>
   </si>
@@ -3236,6 +3236,54 @@
   </si>
   <si>
     <t>Useful. The most concise but comprehensive book about Product Management. In only 68 pages it equips the reader with a big baggage of actionable knowledge.</t>
+  </si>
+  <si>
+    <t>Pandas for Everyone (2nd Edition)</t>
+  </si>
+  <si>
+    <t>2024-11-24</t>
+  </si>
+  <si>
+    <t>Useful. Well written and a fairly comprehensive book for beginners.</t>
+  </si>
+  <si>
+    <t>Pandas Workout</t>
+  </si>
+  <si>
+    <t>Useless. The cookbook-like approach is more convenient for the author than for the reader, because the constant context switching about the dataset used increases the cognitive load by a factor of 4x.</t>
+  </si>
+  <si>
+    <t>Powerful Python</t>
+  </si>
+  <si>
+    <t>Useless. A bag of basic knowledge and cumbersome of magic methods.</t>
+  </si>
+  <si>
+    <t>Practical Python Backend Programming</t>
+  </si>
+  <si>
+    <t>GitforGits</t>
+  </si>
+  <si>
+    <t>Useless. Usual impersonal list of copy'n'paste knowledge.</t>
+  </si>
+  <si>
+    <t>Hypermodern Python Tooling</t>
+  </si>
+  <si>
+    <t>Useless. A bag of basic knowledge, nothing "hypermodern" about it.</t>
+  </si>
+  <si>
+    <t>Testing in Python: Robust Automation for Professionals</t>
+  </si>
+  <si>
+    <t>Useful. Very personal book, also if a bit repetitive. I particularly apprecciated the authors focus on Makefiles, code linting and code metrics.</t>
+  </si>
+  <si>
+    <t>Modern Software Testing Techniques</t>
+  </si>
+  <si>
+    <t>Useful. The first part of the book is very interesting and it provides original theoretical knowledge about testing, while in the second part the author go a bit mental.</t>
   </si>
 </sst>
 </file>
@@ -11082,11 +11130,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T329"/>
+  <dimension ref="A1:T346"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A317" sqref="A317"/>
+      <pane ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A323" sqref="A323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -31511,7 +31559,7 @@
         <v>159</v>
       </c>
       <c r="S314" s="17">
-        <f t="shared" ref="S314:S316" si="123">LEN(P314)</f>
+        <f t="shared" ref="S314:S323" si="123">LEN(P314)</f>
         <v>35</v>
       </c>
       <c r="T314" s="14">
@@ -31606,11 +31654,11 @@
         <v>1063</v>
       </c>
       <c r="H316" s="9">
-        <f t="shared" ref="H316" si="126">YEAR(G316)</f>
+        <f t="shared" ref="H316:H317" si="126">YEAR(G316)</f>
         <v>2024</v>
       </c>
       <c r="I316" s="9">
-        <f t="shared" ref="I316" si="127">MONTH(G316)</f>
+        <f t="shared" ref="I316:I317" si="127">MONTH(G316)</f>
         <v>11</v>
       </c>
       <c r="J316" s="9" t="s">
@@ -31649,161 +31697,462 @@
       </c>
     </row>
     <row r="317" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A317" s="9"/>
-      <c r="B317" s="9"/>
-      <c r="C317" s="9"/>
-      <c r="D317" s="9"/>
-      <c r="E317" s="9"/>
-      <c r="F317" s="9"/>
-      <c r="G317" s="9"/>
-      <c r="H317" s="9"/>
-      <c r="I317" s="9"/>
-      <c r="J317" s="9"/>
-      <c r="K317" s="9"/>
-      <c r="L317" s="9"/>
-      <c r="M317" s="9"/>
-      <c r="N317" s="9"/>
-      <c r="O317" s="9"/>
-      <c r="P317" s="9"/>
-      <c r="Q317" s="9"/>
-      <c r="R317" s="9"/>
-      <c r="S317" s="17"/>
-      <c r="T317" s="9"/>
+      <c r="A317" s="13" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B317" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C317" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D317" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E317" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F317" s="17">
+        <v>512</v>
+      </c>
+      <c r="G317" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H317" s="9">
+        <f t="shared" si="126"/>
+        <v>2024</v>
+      </c>
+      <c r="I317" s="9">
+        <f t="shared" si="127"/>
+        <v>11</v>
+      </c>
+      <c r="J317" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K317" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L317" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="M317" s="17">
+        <v>3</v>
+      </c>
+      <c r="N317" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O317" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P317" s="13" t="s">
+        <v>1067</v>
+      </c>
+      <c r="Q317" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R317" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S317" s="17">
+        <f t="shared" si="123"/>
+        <v>67</v>
+      </c>
+      <c r="T317" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="318" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A318" s="9"/>
-      <c r="B318" s="9"/>
-      <c r="C318" s="9"/>
-      <c r="D318" s="9"/>
-      <c r="E318" s="9"/>
-      <c r="F318" s="9"/>
-      <c r="G318" s="9"/>
-      <c r="H318" s="9"/>
-      <c r="I318" s="9"/>
-      <c r="J318" s="9"/>
-      <c r="K318" s="9"/>
-      <c r="L318" s="9"/>
-      <c r="M318" s="9"/>
-      <c r="N318" s="9"/>
-      <c r="O318" s="9"/>
-      <c r="P318" s="9"/>
-      <c r="Q318" s="9"/>
-      <c r="R318" s="9"/>
-      <c r="S318" s="17"/>
-      <c r="T318" s="9"/>
+      <c r="A318" s="13" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B318" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C318" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D318" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E318" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F318" s="17">
+        <v>442</v>
+      </c>
+      <c r="G318" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H318" s="9">
+        <f t="shared" ref="H318" si="128">YEAR(G318)</f>
+        <v>2024</v>
+      </c>
+      <c r="I318" s="9">
+        <f t="shared" ref="I318" si="129">MONTH(G318)</f>
+        <v>11</v>
+      </c>
+      <c r="J318" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K318" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L318" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M318" s="17">
+        <v>1</v>
+      </c>
+      <c r="N318" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O318" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P318" s="13" t="s">
+        <v>1069</v>
+      </c>
+      <c r="Q318" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R318" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S318" s="17">
+        <f t="shared" si="123"/>
+        <v>200</v>
+      </c>
+      <c r="T318" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="319" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A319" s="9"/>
-      <c r="B319" s="9"/>
-      <c r="C319" s="9"/>
-      <c r="D319" s="9"/>
-      <c r="E319" s="9"/>
-      <c r="F319" s="9"/>
-      <c r="G319" s="9"/>
-      <c r="H319" s="9"/>
-      <c r="I319" s="9"/>
-      <c r="J319" s="9"/>
-      <c r="K319" s="9"/>
-      <c r="L319" s="9"/>
-      <c r="M319" s="9"/>
-      <c r="N319" s="9"/>
-      <c r="O319" s="9"/>
-      <c r="P319" s="9"/>
-      <c r="Q319" s="9"/>
-      <c r="R319" s="9"/>
-      <c r="S319" s="17"/>
-      <c r="T319" s="9"/>
+      <c r="A319" s="13" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B319" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C319" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D319" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E319" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F319" s="17">
+        <v>265</v>
+      </c>
+      <c r="G319" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H319" s="9">
+        <f t="shared" ref="H319" si="130">YEAR(G319)</f>
+        <v>2024</v>
+      </c>
+      <c r="I319" s="9">
+        <f t="shared" ref="I319" si="131">MONTH(G319)</f>
+        <v>11</v>
+      </c>
+      <c r="J319" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K319" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L319" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M319" s="17">
+        <v>1</v>
+      </c>
+      <c r="N319" s="17">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="O319" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P319" s="13" t="s">
+        <v>1071</v>
+      </c>
+      <c r="Q319" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R319" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S319" s="17">
+        <f t="shared" si="123"/>
+        <v>66</v>
+      </c>
+      <c r="T319" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="320" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A320" s="9"/>
-      <c r="B320" s="9"/>
-      <c r="C320" s="9"/>
-      <c r="D320" s="9"/>
-      <c r="E320" s="9"/>
-      <c r="F320" s="9"/>
-      <c r="G320" s="9"/>
-      <c r="H320" s="9"/>
-      <c r="I320" s="9"/>
-      <c r="J320" s="9"/>
-      <c r="K320" s="9"/>
-      <c r="L320" s="9"/>
-      <c r="M320" s="9"/>
-      <c r="N320" s="9"/>
-      <c r="O320" s="9"/>
-      <c r="P320" s="9"/>
-      <c r="Q320" s="9"/>
-      <c r="R320" s="9"/>
-      <c r="S320" s="17"/>
-      <c r="T320" s="9"/>
+      <c r="A320" s="13" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B320" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C320" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D320" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E320" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F320" s="17">
+        <v>333</v>
+      </c>
+      <c r="G320" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H320" s="9">
+        <f t="shared" ref="H320" si="132">YEAR(G320)</f>
+        <v>2024</v>
+      </c>
+      <c r="I320" s="9">
+        <f t="shared" ref="I320" si="133">MONTH(G320)</f>
+        <v>11</v>
+      </c>
+      <c r="J320" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K320" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L320" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="M320" s="17">
+        <v>1</v>
+      </c>
+      <c r="N320" s="17">
+        <v>37.99</v>
+      </c>
+      <c r="O320" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P320" s="13" t="s">
+        <v>1074</v>
+      </c>
+      <c r="Q320" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R320" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S320" s="17">
+        <f t="shared" si="123"/>
+        <v>57</v>
+      </c>
+      <c r="T320" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="321" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A321" s="9"/>
-      <c r="B321" s="9"/>
-      <c r="C321" s="9"/>
-      <c r="D321" s="9"/>
-      <c r="E321" s="9"/>
-      <c r="F321" s="9"/>
-      <c r="G321" s="9"/>
-      <c r="H321" s="9"/>
-      <c r="I321" s="9"/>
-      <c r="J321" s="9"/>
-      <c r="K321" s="9"/>
-      <c r="L321" s="9"/>
-      <c r="M321" s="9"/>
-      <c r="N321" s="9"/>
-      <c r="O321" s="9"/>
-      <c r="P321" s="9"/>
-      <c r="Q321" s="9"/>
-      <c r="R321" s="9"/>
-      <c r="S321" s="17"/>
-      <c r="T321" s="9"/>
+      <c r="A321" s="13" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B321" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C321" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D321" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E321" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F321" s="17">
+        <v>386</v>
+      </c>
+      <c r="G321" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H321" s="9">
+        <f t="shared" ref="H321" si="134">YEAR(G321)</f>
+        <v>2024</v>
+      </c>
+      <c r="I321" s="9">
+        <f t="shared" ref="I321" si="135">MONTH(G321)</f>
+        <v>11</v>
+      </c>
+      <c r="J321" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K321" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L321" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M321" s="17">
+        <v>1</v>
+      </c>
+      <c r="N321" s="17">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="O321" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P321" s="13" t="s">
+        <v>1076</v>
+      </c>
+      <c r="Q321" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R321" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S321" s="17">
+        <f t="shared" si="123"/>
+        <v>66</v>
+      </c>
+      <c r="T321" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="322" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A322" s="9"/>
-      <c r="B322" s="9"/>
-      <c r="C322" s="9"/>
-      <c r="D322" s="9"/>
-      <c r="E322" s="9"/>
-      <c r="F322" s="9"/>
-      <c r="G322" s="9"/>
-      <c r="H322" s="9"/>
-      <c r="I322" s="9"/>
-      <c r="J322" s="9"/>
-      <c r="K322" s="9"/>
-      <c r="L322" s="9"/>
-      <c r="M322" s="9"/>
-      <c r="N322" s="9"/>
-      <c r="O322" s="9"/>
-      <c r="P322" s="9"/>
-      <c r="Q322" s="9"/>
-      <c r="R322" s="9"/>
-      <c r="S322" s="17"/>
-      <c r="T322" s="9"/>
+      <c r="A322" s="13" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B322" s="17">
+        <v>2020</v>
+      </c>
+      <c r="C322" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D322" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E322" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F322" s="17">
+        <v>213</v>
+      </c>
+      <c r="G322" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H322" s="9">
+        <f t="shared" ref="H322" si="136">YEAR(G322)</f>
+        <v>2024</v>
+      </c>
+      <c r="I322" s="9">
+        <f t="shared" ref="I322" si="137">MONTH(G322)</f>
+        <v>11</v>
+      </c>
+      <c r="J322" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K322" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L322" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M322" s="17">
+        <v>4</v>
+      </c>
+      <c r="N322" s="17">
+        <v>39.99</v>
+      </c>
+      <c r="O322" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P322" s="16" t="s">
+        <v>1078</v>
+      </c>
+      <c r="Q322" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="R322" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S322" s="17">
+        <f t="shared" si="123"/>
+        <v>144</v>
+      </c>
+      <c r="T322" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="323" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A323" s="9"/>
-      <c r="B323" s="9"/>
-      <c r="C323" s="9"/>
-      <c r="D323" s="9"/>
-      <c r="E323" s="9"/>
-      <c r="F323" s="9"/>
-      <c r="G323" s="9"/>
-      <c r="H323" s="9"/>
-      <c r="I323" s="9"/>
-      <c r="J323" s="9"/>
-      <c r="K323" s="9"/>
-      <c r="L323" s="9"/>
-      <c r="M323" s="9"/>
-      <c r="N323" s="9"/>
-      <c r="O323" s="9"/>
-      <c r="P323" s="9"/>
-      <c r="Q323" s="9"/>
-      <c r="R323" s="9"/>
-      <c r="S323" s="17"/>
-      <c r="T323" s="9"/>
+      <c r="A323" s="13" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B323" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C323" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D323" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E323" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F323" s="17">
+        <v>277</v>
+      </c>
+      <c r="G323" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H323" s="9">
+        <f t="shared" ref="H323" si="138">YEAR(G323)</f>
+        <v>2024</v>
+      </c>
+      <c r="I323" s="9">
+        <f t="shared" ref="I323" si="139">MONTH(G323)</f>
+        <v>11</v>
+      </c>
+      <c r="J323" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K323" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L323" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="M323" s="17">
+        <v>3</v>
+      </c>
+      <c r="N323" s="43">
+        <v>43.9</v>
+      </c>
+      <c r="O323" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P323" s="13" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Q323" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R323" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S323" s="17">
+        <f t="shared" si="123"/>
+        <v>169</v>
+      </c>
+      <c r="T323" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="324" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A324" s="9"/>
+      <c r="A324" s="13"/>
       <c r="B324" s="9"/>
       <c r="C324" s="9"/>
       <c r="D324" s="9"/>
@@ -31818,14 +32167,14 @@
       <c r="M324" s="9"/>
       <c r="N324" s="9"/>
       <c r="O324" s="9"/>
-      <c r="P324" s="9"/>
+      <c r="P324" s="13"/>
       <c r="Q324" s="9"/>
       <c r="R324" s="9"/>
       <c r="S324" s="17"/>
       <c r="T324" s="9"/>
     </row>
     <row r="325" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A325" s="9"/>
+      <c r="A325" s="13"/>
       <c r="B325" s="9"/>
       <c r="C325" s="9"/>
       <c r="D325" s="9"/>
@@ -31840,14 +32189,14 @@
       <c r="M325" s="9"/>
       <c r="N325" s="9"/>
       <c r="O325" s="9"/>
-      <c r="P325" s="9"/>
+      <c r="P325" s="13"/>
       <c r="Q325" s="9"/>
       <c r="R325" s="9"/>
       <c r="S325" s="17"/>
       <c r="T325" s="9"/>
     </row>
     <row r="326" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A326" s="9"/>
+      <c r="A326" s="13"/>
       <c r="B326" s="9"/>
       <c r="C326" s="9"/>
       <c r="D326" s="9"/>
@@ -31862,14 +32211,14 @@
       <c r="M326" s="9"/>
       <c r="N326" s="9"/>
       <c r="O326" s="9"/>
-      <c r="P326" s="9"/>
+      <c r="P326" s="13"/>
       <c r="Q326" s="9"/>
       <c r="R326" s="9"/>
       <c r="S326" s="17"/>
       <c r="T326" s="9"/>
     </row>
     <row r="327" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A327" s="9"/>
+      <c r="A327" s="13"/>
       <c r="B327" s="9"/>
       <c r="C327" s="9"/>
       <c r="D327" s="9"/>
@@ -31884,14 +32233,14 @@
       <c r="M327" s="9"/>
       <c r="N327" s="9"/>
       <c r="O327" s="9"/>
-      <c r="P327" s="9"/>
+      <c r="P327" s="13"/>
       <c r="Q327" s="9"/>
       <c r="R327" s="9"/>
       <c r="S327" s="17"/>
       <c r="T327" s="9"/>
     </row>
     <row r="328" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A328" s="9"/>
+      <c r="A328" s="13"/>
       <c r="B328" s="9"/>
       <c r="C328" s="9"/>
       <c r="D328" s="9"/>
@@ -31906,14 +32255,14 @@
       <c r="M328" s="9"/>
       <c r="N328" s="9"/>
       <c r="O328" s="9"/>
-      <c r="P328" s="9"/>
+      <c r="P328" s="13"/>
       <c r="Q328" s="9"/>
       <c r="R328" s="9"/>
       <c r="S328" s="17"/>
       <c r="T328" s="9"/>
     </row>
     <row r="329" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A329" s="9"/>
+      <c r="A329" s="13"/>
       <c r="B329" s="9"/>
       <c r="C329" s="9"/>
       <c r="D329" s="9"/>
@@ -31928,11 +32277,385 @@
       <c r="M329" s="9"/>
       <c r="N329" s="9"/>
       <c r="O329" s="9"/>
-      <c r="P329" s="9"/>
+      <c r="P329" s="13"/>
       <c r="Q329" s="9"/>
       <c r="R329" s="9"/>
       <c r="S329" s="17"/>
       <c r="T329" s="9"/>
+    </row>
+    <row r="330" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A330" s="9"/>
+      <c r="B330" s="9"/>
+      <c r="C330" s="9"/>
+      <c r="D330" s="9"/>
+      <c r="E330" s="9"/>
+      <c r="F330" s="9"/>
+      <c r="G330" s="9"/>
+      <c r="H330" s="9"/>
+      <c r="I330" s="9"/>
+      <c r="J330" s="9"/>
+      <c r="K330" s="9"/>
+      <c r="L330" s="9"/>
+      <c r="M330" s="9"/>
+      <c r="N330" s="9"/>
+      <c r="O330" s="9"/>
+      <c r="P330" s="9"/>
+      <c r="Q330" s="9"/>
+      <c r="R330" s="9"/>
+      <c r="S330" s="17"/>
+      <c r="T330" s="9"/>
+    </row>
+    <row r="331" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A331" s="9"/>
+      <c r="B331" s="9"/>
+      <c r="C331" s="9"/>
+      <c r="D331" s="9"/>
+      <c r="E331" s="9"/>
+      <c r="F331" s="9"/>
+      <c r="G331" s="9"/>
+      <c r="H331" s="9"/>
+      <c r="I331" s="9"/>
+      <c r="J331" s="9"/>
+      <c r="K331" s="9"/>
+      <c r="L331" s="9"/>
+      <c r="M331" s="9"/>
+      <c r="N331" s="9"/>
+      <c r="O331" s="9"/>
+      <c r="P331" s="9"/>
+      <c r="Q331" s="9"/>
+      <c r="R331" s="9"/>
+      <c r="S331" s="17"/>
+      <c r="T331" s="9"/>
+    </row>
+    <row r="332" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A332" s="9"/>
+      <c r="B332" s="9"/>
+      <c r="C332" s="9"/>
+      <c r="D332" s="9"/>
+      <c r="E332" s="9"/>
+      <c r="F332" s="9"/>
+      <c r="G332" s="9"/>
+      <c r="H332" s="9"/>
+      <c r="I332" s="9"/>
+      <c r="J332" s="9"/>
+      <c r="K332" s="9"/>
+      <c r="L332" s="9"/>
+      <c r="M332" s="9"/>
+      <c r="N332" s="9"/>
+      <c r="O332" s="9"/>
+      <c r="P332" s="9"/>
+      <c r="Q332" s="9"/>
+      <c r="R332" s="9"/>
+      <c r="S332" s="17"/>
+      <c r="T332" s="9"/>
+    </row>
+    <row r="333" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A333" s="9"/>
+      <c r="B333" s="9"/>
+      <c r="C333" s="9"/>
+      <c r="D333" s="9"/>
+      <c r="E333" s="9"/>
+      <c r="F333" s="9"/>
+      <c r="G333" s="9"/>
+      <c r="H333" s="9"/>
+      <c r="I333" s="9"/>
+      <c r="J333" s="9"/>
+      <c r="K333" s="9"/>
+      <c r="L333" s="9"/>
+      <c r="M333" s="9"/>
+      <c r="N333" s="9"/>
+      <c r="O333" s="9"/>
+      <c r="P333" s="9"/>
+      <c r="Q333" s="9"/>
+      <c r="R333" s="9"/>
+      <c r="S333" s="17"/>
+      <c r="T333" s="9"/>
+    </row>
+    <row r="334" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A334" s="9"/>
+      <c r="B334" s="9"/>
+      <c r="C334" s="9"/>
+      <c r="D334" s="9"/>
+      <c r="E334" s="9"/>
+      <c r="F334" s="9"/>
+      <c r="G334" s="9"/>
+      <c r="H334" s="9"/>
+      <c r="I334" s="9"/>
+      <c r="J334" s="9"/>
+      <c r="K334" s="9"/>
+      <c r="L334" s="9"/>
+      <c r="M334" s="9"/>
+      <c r="N334" s="9"/>
+      <c r="O334" s="9"/>
+      <c r="P334" s="9"/>
+      <c r="Q334" s="9"/>
+      <c r="R334" s="9"/>
+      <c r="S334" s="17"/>
+      <c r="T334" s="9"/>
+    </row>
+    <row r="335" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A335" s="9"/>
+      <c r="B335" s="9"/>
+      <c r="C335" s="9"/>
+      <c r="D335" s="9"/>
+      <c r="E335" s="9"/>
+      <c r="F335" s="9"/>
+      <c r="G335" s="9"/>
+      <c r="H335" s="9"/>
+      <c r="I335" s="9"/>
+      <c r="J335" s="9"/>
+      <c r="K335" s="9"/>
+      <c r="L335" s="9"/>
+      <c r="M335" s="9"/>
+      <c r="N335" s="9"/>
+      <c r="O335" s="9"/>
+      <c r="P335" s="9"/>
+      <c r="Q335" s="9"/>
+      <c r="R335" s="9"/>
+      <c r="S335" s="17"/>
+      <c r="T335" s="9"/>
+    </row>
+    <row r="336" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A336" s="9"/>
+      <c r="B336" s="9"/>
+      <c r="C336" s="9"/>
+      <c r="D336" s="9"/>
+      <c r="E336" s="9"/>
+      <c r="F336" s="9"/>
+      <c r="G336" s="9"/>
+      <c r="H336" s="9"/>
+      <c r="I336" s="9"/>
+      <c r="J336" s="9"/>
+      <c r="K336" s="9"/>
+      <c r="L336" s="9"/>
+      <c r="M336" s="9"/>
+      <c r="N336" s="9"/>
+      <c r="O336" s="9"/>
+      <c r="P336" s="9"/>
+      <c r="Q336" s="9"/>
+      <c r="R336" s="9"/>
+      <c r="S336" s="17"/>
+      <c r="T336" s="9"/>
+    </row>
+    <row r="337" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A337" s="9"/>
+      <c r="B337" s="9"/>
+      <c r="C337" s="9"/>
+      <c r="D337" s="9"/>
+      <c r="E337" s="9"/>
+      <c r="F337" s="9"/>
+      <c r="G337" s="9"/>
+      <c r="H337" s="9"/>
+      <c r="I337" s="9"/>
+      <c r="J337" s="9"/>
+      <c r="K337" s="9"/>
+      <c r="L337" s="9"/>
+      <c r="M337" s="9"/>
+      <c r="N337" s="9"/>
+      <c r="O337" s="9"/>
+      <c r="P337" s="9"/>
+      <c r="Q337" s="9"/>
+      <c r="R337" s="9"/>
+      <c r="S337" s="17"/>
+      <c r="T337" s="9"/>
+    </row>
+    <row r="338" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A338" s="9"/>
+      <c r="B338" s="9"/>
+      <c r="C338" s="9"/>
+      <c r="D338" s="9"/>
+      <c r="E338" s="9"/>
+      <c r="F338" s="9"/>
+      <c r="G338" s="9"/>
+      <c r="H338" s="9"/>
+      <c r="I338" s="9"/>
+      <c r="J338" s="9"/>
+      <c r="K338" s="9"/>
+      <c r="L338" s="9"/>
+      <c r="M338" s="9"/>
+      <c r="N338" s="9"/>
+      <c r="O338" s="9"/>
+      <c r="P338" s="9"/>
+      <c r="Q338" s="9"/>
+      <c r="R338" s="9"/>
+      <c r="S338" s="17"/>
+      <c r="T338" s="9"/>
+    </row>
+    <row r="339" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A339" s="9"/>
+      <c r="B339" s="9"/>
+      <c r="C339" s="9"/>
+      <c r="D339" s="9"/>
+      <c r="E339" s="9"/>
+      <c r="F339" s="9"/>
+      <c r="G339" s="9"/>
+      <c r="H339" s="9"/>
+      <c r="I339" s="9"/>
+      <c r="J339" s="9"/>
+      <c r="K339" s="9"/>
+      <c r="L339" s="9"/>
+      <c r="M339" s="9"/>
+      <c r="N339" s="9"/>
+      <c r="O339" s="9"/>
+      <c r="P339" s="9"/>
+      <c r="Q339" s="9"/>
+      <c r="R339" s="9"/>
+      <c r="S339" s="17"/>
+      <c r="T339" s="9"/>
+    </row>
+    <row r="340" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A340" s="9"/>
+      <c r="B340" s="9"/>
+      <c r="C340" s="9"/>
+      <c r="D340" s="9"/>
+      <c r="E340" s="9"/>
+      <c r="F340" s="9"/>
+      <c r="G340" s="9"/>
+      <c r="H340" s="9"/>
+      <c r="I340" s="9"/>
+      <c r="J340" s="9"/>
+      <c r="K340" s="9"/>
+      <c r="L340" s="9"/>
+      <c r="M340" s="9"/>
+      <c r="N340" s="9"/>
+      <c r="O340" s="9"/>
+      <c r="P340" s="9"/>
+      <c r="Q340" s="9"/>
+      <c r="R340" s="9"/>
+      <c r="S340" s="17"/>
+      <c r="T340" s="9"/>
+    </row>
+    <row r="341" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A341" s="9"/>
+      <c r="B341" s="9"/>
+      <c r="C341" s="9"/>
+      <c r="D341" s="9"/>
+      <c r="E341" s="9"/>
+      <c r="F341" s="9"/>
+      <c r="G341" s="9"/>
+      <c r="H341" s="9"/>
+      <c r="I341" s="9"/>
+      <c r="J341" s="9"/>
+      <c r="K341" s="9"/>
+      <c r="L341" s="9"/>
+      <c r="M341" s="9"/>
+      <c r="N341" s="9"/>
+      <c r="O341" s="9"/>
+      <c r="P341" s="9"/>
+      <c r="Q341" s="9"/>
+      <c r="R341" s="9"/>
+      <c r="S341" s="17"/>
+      <c r="T341" s="9"/>
+    </row>
+    <row r="342" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A342" s="9"/>
+      <c r="B342" s="9"/>
+      <c r="C342" s="9"/>
+      <c r="D342" s="9"/>
+      <c r="E342" s="9"/>
+      <c r="F342" s="9"/>
+      <c r="G342" s="9"/>
+      <c r="H342" s="9"/>
+      <c r="I342" s="9"/>
+      <c r="J342" s="9"/>
+      <c r="K342" s="9"/>
+      <c r="L342" s="9"/>
+      <c r="M342" s="9"/>
+      <c r="N342" s="9"/>
+      <c r="O342" s="9"/>
+      <c r="P342" s="9"/>
+      <c r="Q342" s="9"/>
+      <c r="R342" s="9"/>
+      <c r="S342" s="17"/>
+      <c r="T342" s="9"/>
+    </row>
+    <row r="343" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A343" s="9"/>
+      <c r="B343" s="9"/>
+      <c r="C343" s="9"/>
+      <c r="D343" s="9"/>
+      <c r="E343" s="9"/>
+      <c r="F343" s="9"/>
+      <c r="G343" s="9"/>
+      <c r="H343" s="9"/>
+      <c r="I343" s="9"/>
+      <c r="J343" s="9"/>
+      <c r="K343" s="9"/>
+      <c r="L343" s="9"/>
+      <c r="M343" s="9"/>
+      <c r="N343" s="9"/>
+      <c r="O343" s="9"/>
+      <c r="P343" s="9"/>
+      <c r="Q343" s="9"/>
+      <c r="R343" s="9"/>
+      <c r="S343" s="17"/>
+      <c r="T343" s="9"/>
+    </row>
+    <row r="344" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A344" s="9"/>
+      <c r="B344" s="9"/>
+      <c r="C344" s="9"/>
+      <c r="D344" s="9"/>
+      <c r="E344" s="9"/>
+      <c r="F344" s="9"/>
+      <c r="G344" s="9"/>
+      <c r="H344" s="9"/>
+      <c r="I344" s="9"/>
+      <c r="J344" s="9"/>
+      <c r="K344" s="9"/>
+      <c r="L344" s="9"/>
+      <c r="M344" s="9"/>
+      <c r="N344" s="9"/>
+      <c r="O344" s="9"/>
+      <c r="P344" s="9"/>
+      <c r="Q344" s="9"/>
+      <c r="R344" s="9"/>
+      <c r="S344" s="17"/>
+      <c r="T344" s="9"/>
+    </row>
+    <row r="345" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A345" s="9"/>
+      <c r="B345" s="9"/>
+      <c r="C345" s="9"/>
+      <c r="D345" s="9"/>
+      <c r="E345" s="9"/>
+      <c r="F345" s="9"/>
+      <c r="G345" s="9"/>
+      <c r="H345" s="9"/>
+      <c r="I345" s="9"/>
+      <c r="J345" s="9"/>
+      <c r="K345" s="9"/>
+      <c r="L345" s="9"/>
+      <c r="M345" s="9"/>
+      <c r="N345" s="9"/>
+      <c r="O345" s="9"/>
+      <c r="P345" s="9"/>
+      <c r="Q345" s="9"/>
+      <c r="R345" s="9"/>
+      <c r="S345" s="17"/>
+      <c r="T345" s="9"/>
+    </row>
+    <row r="346" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A346" s="9"/>
+      <c r="B346" s="9"/>
+      <c r="C346" s="9"/>
+      <c r="D346" s="9"/>
+      <c r="E346" s="9"/>
+      <c r="F346" s="9"/>
+      <c r="G346" s="9"/>
+      <c r="H346" s="9"/>
+      <c r="I346" s="9"/>
+      <c r="J346" s="9"/>
+      <c r="K346" s="9"/>
+      <c r="L346" s="9"/>
+      <c r="M346" s="9"/>
+      <c r="N346" s="9"/>
+      <c r="O346" s="9"/>
+      <c r="P346" s="9"/>
+      <c r="Q346" s="9"/>
+      <c r="R346" s="9"/>
+      <c r="S346" s="17"/>
+      <c r="T346" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#43 Reading List: updated to 2025-01-01.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5082" uniqueCount="1081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5142" uniqueCount="1092">
   <si>
     <t>Format</t>
   </si>
@@ -3284,6 +3284,39 @@
   </si>
   <si>
     <t>Useful. The first part of the book is very interesting and it provides original theoretical knowledge about testing, while in the second part the author go a bit mental.</t>
+  </si>
+  <si>
+    <t>Better APIs: Quality, Stability, Observability</t>
+  </si>
+  <si>
+    <t>2024-12-31</t>
+  </si>
+  <si>
+    <t>Useless. It's personal, but it contains no original content. It's just the usual walkthrough thru well-known programming best practices.</t>
+  </si>
+  <si>
+    <t>Mastering API Architecture</t>
+  </si>
+  <si>
+    <t>Useless. Well written, but no original content.</t>
+  </si>
+  <si>
+    <t>GitHub Actions in Action</t>
+  </si>
+  <si>
+    <t>Useful. A good getting started book.</t>
+  </si>
+  <si>
+    <t>Learning GitHub Actions</t>
+  </si>
+  <si>
+    <t>2025-01-01</t>
+  </si>
+  <si>
+    <t>Useless. Just an unemotional showcase of Github features.</t>
+  </si>
+  <si>
+    <t>Gray Hat Python</t>
   </si>
 </sst>
 </file>
@@ -11134,7 +11167,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A323" sqref="A323"/>
+      <selection pane="bottomLeft" activeCell="A332" sqref="A332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -31559,7 +31592,7 @@
         <v>159</v>
       </c>
       <c r="S314" s="17">
-        <f t="shared" ref="S314:S323" si="123">LEN(P314)</f>
+        <f t="shared" ref="S314:S328" si="123">LEN(P314)</f>
         <v>35</v>
       </c>
       <c r="T314" s="14">
@@ -32152,114 +32185,329 @@
       </c>
     </row>
     <row r="324" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A324" s="13"/>
-      <c r="B324" s="9"/>
-      <c r="C324" s="9"/>
-      <c r="D324" s="9"/>
-      <c r="E324" s="9"/>
-      <c r="F324" s="9"/>
-      <c r="G324" s="9"/>
-      <c r="H324" s="9"/>
-      <c r="I324" s="9"/>
-      <c r="J324" s="9"/>
-      <c r="K324" s="9"/>
-      <c r="L324" s="9"/>
-      <c r="M324" s="9"/>
-      <c r="N324" s="9"/>
-      <c r="O324" s="9"/>
-      <c r="P324" s="13"/>
-      <c r="Q324" s="9"/>
-      <c r="R324" s="9"/>
-      <c r="S324" s="17"/>
-      <c r="T324" s="9"/>
+      <c r="A324" s="13" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B324" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C324" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D324" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E324" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F324" s="17">
+        <v>132</v>
+      </c>
+      <c r="G324" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H324" s="9">
+        <f t="shared" ref="H324" si="140">YEAR(G324)</f>
+        <v>2024</v>
+      </c>
+      <c r="I324" s="9">
+        <f t="shared" ref="I324" si="141">MONTH(G324)</f>
+        <v>12</v>
+      </c>
+      <c r="J324" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K324" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L324" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M324" s="17">
+        <v>2</v>
+      </c>
+      <c r="N324" s="43">
+        <v>10</v>
+      </c>
+      <c r="O324" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P324" s="16" t="s">
+        <v>1083</v>
+      </c>
+      <c r="Q324" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R324" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S324" s="17">
+        <f t="shared" si="123"/>
+        <v>136</v>
+      </c>
+      <c r="T324" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="325" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A325" s="13"/>
-      <c r="B325" s="9"/>
-      <c r="C325" s="9"/>
-      <c r="D325" s="9"/>
-      <c r="E325" s="9"/>
-      <c r="F325" s="9"/>
-      <c r="G325" s="9"/>
-      <c r="H325" s="9"/>
-      <c r="I325" s="9"/>
-      <c r="J325" s="9"/>
-      <c r="K325" s="9"/>
-      <c r="L325" s="9"/>
-      <c r="M325" s="9"/>
-      <c r="N325" s="9"/>
-      <c r="O325" s="9"/>
-      <c r="P325" s="13"/>
-      <c r="Q325" s="9"/>
-      <c r="R325" s="9"/>
-      <c r="S325" s="17"/>
-      <c r="T325" s="9"/>
+      <c r="A325" s="13" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B325" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C325" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D325" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E325" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F325" s="17">
+        <v>289</v>
+      </c>
+      <c r="G325" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H325" s="9">
+        <f t="shared" ref="H325" si="142">YEAR(G325)</f>
+        <v>2024</v>
+      </c>
+      <c r="I325" s="9">
+        <f t="shared" ref="I325" si="143">MONTH(G325)</f>
+        <v>12</v>
+      </c>
+      <c r="J325" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K325" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L325" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M325" s="17">
+        <v>2</v>
+      </c>
+      <c r="N325" s="17">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="O325" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P325" s="13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="Q325" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R325" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S325" s="17">
+        <f t="shared" si="123"/>
+        <v>47</v>
+      </c>
+      <c r="T325" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="326" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A326" s="13"/>
-      <c r="B326" s="9"/>
-      <c r="C326" s="9"/>
-      <c r="D326" s="9"/>
-      <c r="E326" s="9"/>
-      <c r="F326" s="9"/>
-      <c r="G326" s="9"/>
-      <c r="H326" s="9"/>
-      <c r="I326" s="9"/>
-      <c r="J326" s="9"/>
-      <c r="K326" s="9"/>
-      <c r="L326" s="9"/>
-      <c r="M326" s="9"/>
-      <c r="N326" s="9"/>
-      <c r="O326" s="9"/>
-      <c r="P326" s="13"/>
-      <c r="Q326" s="9"/>
-      <c r="R326" s="9"/>
-      <c r="S326" s="17"/>
-      <c r="T326" s="9"/>
+      <c r="A326" s="13" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B326" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C326" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D326" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E326" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F326" s="17">
+        <v>257</v>
+      </c>
+      <c r="G326" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H326" s="9">
+        <f t="shared" ref="H326" si="144">YEAR(G326)</f>
+        <v>2024</v>
+      </c>
+      <c r="I326" s="9">
+        <f t="shared" ref="I326" si="145">MONTH(G326)</f>
+        <v>12</v>
+      </c>
+      <c r="J326" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K326" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L326" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M326" s="17">
+        <v>3</v>
+      </c>
+      <c r="N326" s="17">
+        <v>49.99</v>
+      </c>
+      <c r="O326" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P326" s="13" t="s">
+        <v>1087</v>
+      </c>
+      <c r="Q326" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="R326" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S326" s="17">
+        <f t="shared" si="123"/>
+        <v>36</v>
+      </c>
+      <c r="T326" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="327" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A327" s="13"/>
-      <c r="B327" s="9"/>
-      <c r="C327" s="9"/>
-      <c r="D327" s="9"/>
-      <c r="E327" s="9"/>
-      <c r="F327" s="9"/>
-      <c r="G327" s="9"/>
-      <c r="H327" s="9"/>
-      <c r="I327" s="9"/>
-      <c r="J327" s="9"/>
-      <c r="K327" s="9"/>
-      <c r="L327" s="9"/>
-      <c r="M327" s="9"/>
-      <c r="N327" s="9"/>
-      <c r="O327" s="9"/>
-      <c r="P327" s="13"/>
-      <c r="Q327" s="9"/>
-      <c r="R327" s="9"/>
-      <c r="S327" s="17"/>
-      <c r="T327" s="9"/>
+      <c r="A327" s="13" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B327" s="17">
+        <v>2023</v>
+      </c>
+      <c r="C327" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D327" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E327" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F327" s="17">
+        <v>573</v>
+      </c>
+      <c r="G327" s="9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="H327" s="9">
+        <f t="shared" ref="H327" si="146">YEAR(G327)</f>
+        <v>2025</v>
+      </c>
+      <c r="I327" s="9">
+        <f t="shared" ref="I327" si="147">MONTH(G327)</f>
+        <v>1</v>
+      </c>
+      <c r="J327" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K327" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L327" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M327" s="17">
+        <v>1</v>
+      </c>
+      <c r="N327" s="17">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="O327" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P327" s="13" t="s">
+        <v>1090</v>
+      </c>
+      <c r="Q327" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="R327" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S327" s="17">
+        <f t="shared" si="123"/>
+        <v>57</v>
+      </c>
+      <c r="T327" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="328" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A328" s="13"/>
-      <c r="B328" s="9"/>
-      <c r="C328" s="9"/>
-      <c r="D328" s="9"/>
-      <c r="E328" s="9"/>
-      <c r="F328" s="9"/>
-      <c r="G328" s="9"/>
-      <c r="H328" s="9"/>
-      <c r="I328" s="9"/>
-      <c r="J328" s="9"/>
-      <c r="K328" s="9"/>
-      <c r="L328" s="9"/>
-      <c r="M328" s="9"/>
-      <c r="N328" s="9"/>
-      <c r="O328" s="9"/>
-      <c r="P328" s="13"/>
-      <c r="Q328" s="9"/>
-      <c r="R328" s="9"/>
-      <c r="S328" s="17"/>
-      <c r="T328" s="9"/>
+      <c r="A328" s="13" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B328" s="17">
+        <v>2009</v>
+      </c>
+      <c r="C328" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D328" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E328" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F328" s="17">
+        <v>220</v>
+      </c>
+      <c r="G328" s="9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="H328" s="9">
+        <f t="shared" ref="H328" si="148">YEAR(G328)</f>
+        <v>2025</v>
+      </c>
+      <c r="I328" s="9">
+        <f t="shared" ref="I328" si="149">MONTH(G328)</f>
+        <v>1</v>
+      </c>
+      <c r="J328" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K328" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="L328" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="M328" s="17">
+        <v>3</v>
+      </c>
+      <c r="N328" s="17">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="O328" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P328" s="13" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q328" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="R328" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S328" s="17">
+        <f t="shared" si="123"/>
+        <v>16</v>
+      </c>
+      <c r="T328" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="329" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A329" s="13"/>

</xml_diff>

<commit_message>
#43 Reading List: added latest KBSizes.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -11226,8 +11226,8 @@
   <dimension ref="A1:T346"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A317" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A334" sqref="A334"/>
+      <pane ySplit="1" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q341" sqref="Q341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -30290,8 +30290,8 @@
         <f t="shared" si="81"/>
         <v>38</v>
       </c>
-      <c r="T293" s="14">
-        <v>0</v>
+      <c r="T293" s="49">
+        <v>256</v>
       </c>
     </row>
     <row r="294" spans="1:20" x14ac:dyDescent="0.2">
@@ -30355,8 +30355,8 @@
         <f t="shared" si="81"/>
         <v>268</v>
       </c>
-      <c r="T294" s="14">
-        <v>0</v>
+      <c r="T294" s="49">
+        <v>576</v>
       </c>
     </row>
     <row r="295" spans="1:20" x14ac:dyDescent="0.2">
@@ -30420,8 +30420,8 @@
         <f t="shared" si="81"/>
         <v>131</v>
       </c>
-      <c r="T295" s="14">
-        <v>0</v>
+      <c r="T295" s="49">
+        <v>708</v>
       </c>
     </row>
     <row r="296" spans="1:20" x14ac:dyDescent="0.2">
@@ -30485,8 +30485,8 @@
         <f t="shared" si="81"/>
         <v>77</v>
       </c>
-      <c r="T296" s="14">
-        <v>0</v>
+      <c r="T296" s="49">
+        <v>143</v>
       </c>
     </row>
     <row r="297" spans="1:20" x14ac:dyDescent="0.2">
@@ -30550,8 +30550,8 @@
         <f t="shared" si="81"/>
         <v>55</v>
       </c>
-      <c r="T297" s="14">
-        <v>0</v>
+      <c r="T297" s="49">
+        <v>105</v>
       </c>
     </row>
     <row r="298" spans="1:20" x14ac:dyDescent="0.2">
@@ -30615,8 +30615,8 @@
         <f t="shared" si="81"/>
         <v>55</v>
       </c>
-      <c r="T298" s="14">
-        <v>0</v>
+      <c r="T298" s="49">
+        <v>15</v>
       </c>
     </row>
     <row r="299" spans="1:20" x14ac:dyDescent="0.2">
@@ -30680,8 +30680,8 @@
         <f t="shared" si="81"/>
         <v>247</v>
       </c>
-      <c r="T299" s="14">
-        <v>0</v>
+      <c r="T299" s="49">
+        <v>50</v>
       </c>
     </row>
     <row r="300" spans="1:20" x14ac:dyDescent="0.2">
@@ -30745,8 +30745,8 @@
         <f t="shared" si="81"/>
         <v>229</v>
       </c>
-      <c r="T300" s="14">
-        <v>0</v>
+      <c r="T300" s="49">
+        <v>248</v>
       </c>
     </row>
     <row r="301" spans="1:20" x14ac:dyDescent="0.2">
@@ -30810,8 +30810,8 @@
         <f t="shared" si="81"/>
         <v>45</v>
       </c>
-      <c r="T301" s="14">
-        <v>0</v>
+      <c r="T301" s="49">
+        <v>56</v>
       </c>
     </row>
     <row r="302" spans="1:20" x14ac:dyDescent="0.2">
@@ -30875,8 +30875,8 @@
         <f t="shared" si="81"/>
         <v>103</v>
       </c>
-      <c r="T302" s="14">
-        <v>0</v>
+      <c r="T302" s="49">
+        <v>135</v>
       </c>
     </row>
     <row r="303" spans="1:20" x14ac:dyDescent="0.2">
@@ -30940,8 +30940,8 @@
         <f t="shared" si="81"/>
         <v>176</v>
       </c>
-      <c r="T303" s="14">
-        <v>0</v>
+      <c r="T303" s="49">
+        <v>67</v>
       </c>
     </row>
     <row r="304" spans="1:20" x14ac:dyDescent="0.2">
@@ -31005,8 +31005,8 @@
         <f t="shared" si="81"/>
         <v>218</v>
       </c>
-      <c r="T304" s="14">
-        <v>0</v>
+      <c r="T304" s="49">
+        <v>499</v>
       </c>
     </row>
     <row r="305" spans="1:20" x14ac:dyDescent="0.2">
@@ -31070,8 +31070,8 @@
         <f t="shared" ref="S305:S313" si="106">LEN(P305)</f>
         <v>88</v>
       </c>
-      <c r="T305" s="14">
-        <v>0</v>
+      <c r="T305" s="49">
+        <v>42</v>
       </c>
     </row>
     <row r="306" spans="1:20" x14ac:dyDescent="0.2">
@@ -31135,8 +31135,8 @@
         <f t="shared" si="106"/>
         <v>231</v>
       </c>
-      <c r="T306" s="14">
-        <v>0</v>
+      <c r="T306" s="49">
+        <v>1376</v>
       </c>
     </row>
     <row r="307" spans="1:20" x14ac:dyDescent="0.2">
@@ -31200,8 +31200,8 @@
         <f t="shared" si="106"/>
         <v>63</v>
       </c>
-      <c r="T307" s="14">
-        <v>0</v>
+      <c r="T307" s="49">
+        <v>337</v>
       </c>
     </row>
     <row r="308" spans="1:20" x14ac:dyDescent="0.2">
@@ -31265,8 +31265,8 @@
         <f t="shared" si="106"/>
         <v>406</v>
       </c>
-      <c r="T308" s="14">
-        <v>0</v>
+      <c r="T308" s="49">
+        <v>272</v>
       </c>
     </row>
     <row r="309" spans="1:20" x14ac:dyDescent="0.2">
@@ -31330,8 +31330,8 @@
         <f t="shared" si="106"/>
         <v>260</v>
       </c>
-      <c r="T309" s="14">
-        <v>0</v>
+      <c r="T309" s="49">
+        <v>336</v>
       </c>
     </row>
     <row r="310" spans="1:20" x14ac:dyDescent="0.2">
@@ -31395,8 +31395,8 @@
         <f t="shared" si="106"/>
         <v>66</v>
       </c>
-      <c r="T310" s="14">
-        <v>0</v>
+      <c r="T310" s="49">
+        <v>868</v>
       </c>
     </row>
     <row r="311" spans="1:20" x14ac:dyDescent="0.2">
@@ -31460,8 +31460,8 @@
         <f t="shared" si="106"/>
         <v>243</v>
       </c>
-      <c r="T311" s="14">
-        <v>0</v>
+      <c r="T311" s="49">
+        <v>366</v>
       </c>
     </row>
     <row r="312" spans="1:20" x14ac:dyDescent="0.2">
@@ -31525,8 +31525,8 @@
         <f t="shared" si="106"/>
         <v>379</v>
       </c>
-      <c r="T312" s="14">
-        <v>0</v>
+      <c r="T312" s="49">
+        <v>844</v>
       </c>
     </row>
     <row r="313" spans="1:20" x14ac:dyDescent="0.2">
@@ -31590,8 +31590,8 @@
         <f t="shared" si="106"/>
         <v>31</v>
       </c>
-      <c r="T313" s="14">
-        <v>0</v>
+      <c r="T313" s="49">
+        <v>78</v>
       </c>
     </row>
     <row r="314" spans="1:20" x14ac:dyDescent="0.2">
@@ -31655,8 +31655,8 @@
         <f t="shared" ref="S314:S334" si="123">LEN(P314)</f>
         <v>35</v>
       </c>
-      <c r="T314" s="14">
-        <v>0</v>
+      <c r="T314" s="49">
+        <v>139</v>
       </c>
     </row>
     <row r="315" spans="1:20" x14ac:dyDescent="0.2">
@@ -31720,8 +31720,8 @@
         <f t="shared" si="123"/>
         <v>60</v>
       </c>
-      <c r="T315" s="14">
-        <v>0</v>
+      <c r="T315" s="49">
+        <v>59</v>
       </c>
     </row>
     <row r="316" spans="1:20" x14ac:dyDescent="0.2">
@@ -31785,8 +31785,8 @@
         <f t="shared" si="123"/>
         <v>155</v>
       </c>
-      <c r="T316" s="14">
-        <v>0</v>
+      <c r="T316" s="49">
+        <v>523</v>
       </c>
     </row>
     <row r="317" spans="1:20" x14ac:dyDescent="0.2">
@@ -31850,8 +31850,8 @@
         <f t="shared" si="123"/>
         <v>67</v>
       </c>
-      <c r="T317" s="14">
-        <v>0</v>
+      <c r="T317" s="49">
+        <v>224</v>
       </c>
     </row>
     <row r="318" spans="1:20" x14ac:dyDescent="0.2">
@@ -31915,8 +31915,8 @@
         <f t="shared" si="123"/>
         <v>200</v>
       </c>
-      <c r="T318" s="14">
-        <v>0</v>
+      <c r="T318" s="49">
+        <v>133</v>
       </c>
     </row>
     <row r="319" spans="1:20" x14ac:dyDescent="0.2">
@@ -31980,8 +31980,8 @@
         <f t="shared" si="123"/>
         <v>66</v>
       </c>
-      <c r="T319" s="14">
-        <v>0</v>
+      <c r="T319" s="49">
+        <v>32</v>
       </c>
     </row>
     <row r="320" spans="1:20" x14ac:dyDescent="0.2">
@@ -32045,7 +32045,7 @@
         <f t="shared" si="123"/>
         <v>57</v>
       </c>
-      <c r="T320" s="14">
+      <c r="T320" s="49">
         <v>0</v>
       </c>
     </row>
@@ -32110,8 +32110,8 @@
         <f t="shared" si="123"/>
         <v>66</v>
       </c>
-      <c r="T321" s="14">
-        <v>0</v>
+      <c r="T321" s="49">
+        <v>37</v>
       </c>
     </row>
     <row r="322" spans="1:20" x14ac:dyDescent="0.2">
@@ -32175,8 +32175,8 @@
         <f t="shared" si="123"/>
         <v>144</v>
       </c>
-      <c r="T322" s="14">
-        <v>0</v>
+      <c r="T322" s="49">
+        <v>162</v>
       </c>
     </row>
     <row r="323" spans="1:20" x14ac:dyDescent="0.2">
@@ -32240,8 +32240,8 @@
         <f t="shared" si="123"/>
         <v>169</v>
       </c>
-      <c r="T323" s="14">
-        <v>0</v>
+      <c r="T323" s="49">
+        <v>218</v>
       </c>
     </row>
     <row r="324" spans="1:20" x14ac:dyDescent="0.2">
@@ -32305,8 +32305,8 @@
         <f t="shared" si="123"/>
         <v>136</v>
       </c>
-      <c r="T324" s="14">
-        <v>0</v>
+      <c r="T324" s="49">
+        <v>160</v>
       </c>
     </row>
     <row r="325" spans="1:20" x14ac:dyDescent="0.2">
@@ -32370,8 +32370,8 @@
         <f t="shared" si="123"/>
         <v>47</v>
       </c>
-      <c r="T325" s="14">
-        <v>0</v>
+      <c r="T325" s="49">
+        <v>358</v>
       </c>
     </row>
     <row r="326" spans="1:20" x14ac:dyDescent="0.2">
@@ -32435,8 +32435,8 @@
         <f t="shared" si="123"/>
         <v>36</v>
       </c>
-      <c r="T326" s="14">
-        <v>0</v>
+      <c r="T326" s="49">
+        <v>355</v>
       </c>
     </row>
     <row r="327" spans="1:20" x14ac:dyDescent="0.2">
@@ -32500,8 +32500,8 @@
         <f t="shared" si="123"/>
         <v>57</v>
       </c>
-      <c r="T327" s="14">
-        <v>0</v>
+      <c r="T327" s="49">
+        <v>97</v>
       </c>
     </row>
     <row r="328" spans="1:20" x14ac:dyDescent="0.2">
@@ -32565,8 +32565,8 @@
         <f t="shared" si="123"/>
         <v>16</v>
       </c>
-      <c r="T328" s="14">
-        <v>0</v>
+      <c r="T328" s="49">
+        <v>259</v>
       </c>
     </row>
     <row r="329" spans="1:20" x14ac:dyDescent="0.2">
@@ -32630,8 +32630,8 @@
         <f t="shared" si="123"/>
         <v>40</v>
       </c>
-      <c r="T329" s="14">
-        <v>0</v>
+      <c r="T329" s="49">
+        <v>630</v>
       </c>
     </row>
     <row r="330" spans="1:20" x14ac:dyDescent="0.2">
@@ -32695,8 +32695,8 @@
         <f t="shared" si="123"/>
         <v>38</v>
       </c>
-      <c r="T330" s="14">
-        <v>0</v>
+      <c r="T330" s="49">
+        <v>80</v>
       </c>
     </row>
     <row r="331" spans="1:20" x14ac:dyDescent="0.2">
@@ -32760,8 +32760,8 @@
         <f t="shared" si="123"/>
         <v>197</v>
       </c>
-      <c r="T331" s="14">
-        <v>0</v>
+      <c r="T331" s="49">
+        <v>253</v>
       </c>
     </row>
     <row r="332" spans="1:20" x14ac:dyDescent="0.2">
@@ -32825,8 +32825,8 @@
         <f t="shared" si="123"/>
         <v>107</v>
       </c>
-      <c r="T332" s="14">
-        <v>0</v>
+      <c r="T332" s="49">
+        <v>95</v>
       </c>
     </row>
     <row r="333" spans="1:20" x14ac:dyDescent="0.2">
@@ -32890,8 +32890,8 @@
         <f t="shared" si="123"/>
         <v>61</v>
       </c>
-      <c r="T333" s="14">
-        <v>0</v>
+      <c r="T333" s="49">
+        <v>369</v>
       </c>
     </row>
     <row r="334" spans="1:20" x14ac:dyDescent="0.2">
@@ -32955,8 +32955,8 @@
         <f t="shared" si="123"/>
         <v>174</v>
       </c>
-      <c r="T334" s="14">
-        <v>0</v>
+      <c r="T334" s="49">
+        <v>509</v>
       </c>
     </row>
     <row r="335" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
#43 Added latest four books.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5214" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5262" uniqueCount="1118">
   <si>
     <t>Format</t>
   </si>
@@ -3368,6 +3368,33 @@
   </si>
   <si>
     <t>Useful. This book could be even better by removing repetitions. A concept should be mentioned and explained only once, and not anticipated or spread around multiple sections.</t>
+  </si>
+  <si>
+    <t>Software Architecture and Decision-Making</t>
+  </si>
+  <si>
+    <t>2025-05-05</t>
+  </si>
+  <si>
+    <t>Useless. Well written but no original knowledge.</t>
+  </si>
+  <si>
+    <t>Kickstart Software Design Architecture</t>
+  </si>
+  <si>
+    <t>Orange Education</t>
+  </si>
+  <si>
+    <t>Principles of Software Architecture Modernization</t>
+  </si>
+  <si>
+    <t>Useless. Very repetitive and it doesn't contain original knowledge.</t>
+  </si>
+  <si>
+    <t>Product Management 101 Playbook</t>
+  </si>
+  <si>
+    <t>Useless. Very basic, no original knowledge.</t>
   </si>
 </sst>
 </file>
@@ -11227,7 +11254,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q341" sqref="Q341"/>
+      <selection pane="bottomLeft" activeCell="A342" sqref="A342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -31652,7 +31679,7 @@
         <v>159</v>
       </c>
       <c r="S314" s="17">
-        <f t="shared" ref="S314:S334" si="123">LEN(P314)</f>
+        <f t="shared" ref="S314:S338" si="123">LEN(P314)</f>
         <v>35</v>
       </c>
       <c r="T314" s="49">
@@ -32917,11 +32944,11 @@
         <v>1104</v>
       </c>
       <c r="H334" s="9">
-        <f t="shared" ref="H334" si="156">YEAR(G334)</f>
+        <f t="shared" ref="H334:H335" si="156">YEAR(G334)</f>
         <v>2025</v>
       </c>
       <c r="I334" s="9">
-        <f t="shared" ref="I334" si="157">MONTH(G334)</f>
+        <f>MONTH(G334)</f>
         <v>3</v>
       </c>
       <c r="J334" s="9" t="s">
@@ -32960,92 +32987,264 @@
       </c>
     </row>
     <row r="335" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A335" s="13"/>
-      <c r="B335" s="9"/>
-      <c r="C335" s="9"/>
-      <c r="D335" s="9"/>
-      <c r="E335" s="9"/>
-      <c r="F335" s="9"/>
-      <c r="G335" s="9"/>
-      <c r="H335" s="9"/>
-      <c r="I335" s="9"/>
-      <c r="J335" s="9"/>
-      <c r="K335" s="9"/>
-      <c r="L335" s="9"/>
-      <c r="M335" s="9"/>
-      <c r="N335" s="9"/>
-      <c r="O335" s="9"/>
-      <c r="P335" s="13"/>
-      <c r="Q335" s="9"/>
-      <c r="R335" s="9"/>
-      <c r="S335" s="17"/>
-      <c r="T335" s="9"/>
+      <c r="A335" s="13" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B335" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C335" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D335" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E335" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F335" s="17">
+        <v>286</v>
+      </c>
+      <c r="G335" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="H335" s="9">
+        <f t="shared" si="156"/>
+        <v>2025</v>
+      </c>
+      <c r="I335" s="9">
+        <f>MONTH(G335)</f>
+        <v>5</v>
+      </c>
+      <c r="J335" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K335" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L335" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="M335" s="17">
+        <v>2</v>
+      </c>
+      <c r="N335" s="17">
+        <v>39.99</v>
+      </c>
+      <c r="O335" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P335" s="13" t="s">
+        <v>1111</v>
+      </c>
+      <c r="Q335" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R335" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S335" s="17">
+        <f t="shared" si="123"/>
+        <v>48</v>
+      </c>
+      <c r="T335" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="336" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A336" s="13"/>
-      <c r="B336" s="9"/>
-      <c r="C336" s="9"/>
-      <c r="D336" s="9"/>
-      <c r="E336" s="9"/>
-      <c r="F336" s="9"/>
-      <c r="G336" s="9"/>
-      <c r="H336" s="9"/>
-      <c r="I336" s="9"/>
-      <c r="J336" s="9"/>
-      <c r="K336" s="9"/>
-      <c r="L336" s="9"/>
-      <c r="M336" s="9"/>
-      <c r="N336" s="9"/>
-      <c r="O336" s="9"/>
-      <c r="P336" s="13"/>
-      <c r="Q336" s="9"/>
-      <c r="R336" s="9"/>
-      <c r="S336" s="17"/>
-      <c r="T336" s="9"/>
+      <c r="A336" s="13" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B336" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C336" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D336" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E336" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F336" s="17">
+        <v>418</v>
+      </c>
+      <c r="G336" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="H336" s="9">
+        <f t="shared" ref="H336" si="157">YEAR(G336)</f>
+        <v>2025</v>
+      </c>
+      <c r="I336" s="9">
+        <f>MONTH(G336)</f>
+        <v>5</v>
+      </c>
+      <c r="J336" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K336" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L336" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="M336" s="17">
+        <v>2</v>
+      </c>
+      <c r="N336" s="17">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="O336" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P336" s="13" t="s">
+        <v>1111</v>
+      </c>
+      <c r="Q336" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R336" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S336" s="17">
+        <f t="shared" si="123"/>
+        <v>48</v>
+      </c>
+      <c r="T336" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="337" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A337" s="13"/>
-      <c r="B337" s="9"/>
-      <c r="C337" s="9"/>
-      <c r="D337" s="9"/>
-      <c r="E337" s="9"/>
-      <c r="F337" s="9"/>
-      <c r="G337" s="9"/>
-      <c r="H337" s="9"/>
-      <c r="I337" s="9"/>
-      <c r="J337" s="9"/>
-      <c r="K337" s="9"/>
-      <c r="L337" s="9"/>
-      <c r="M337" s="9"/>
-      <c r="N337" s="9"/>
-      <c r="O337" s="9"/>
-      <c r="P337" s="13"/>
-      <c r="Q337" s="9"/>
-      <c r="R337" s="9"/>
-      <c r="S337" s="17"/>
-      <c r="T337" s="9"/>
+      <c r="A337" s="13" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B337" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C337" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D337" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E337" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F337" s="17">
+        <v>611</v>
+      </c>
+      <c r="G337" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="H337" s="9">
+        <f t="shared" ref="H337" si="158">YEAR(G337)</f>
+        <v>2025</v>
+      </c>
+      <c r="I337" s="9">
+        <f>MONTH(G337)</f>
+        <v>5</v>
+      </c>
+      <c r="J337" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K337" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L337" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="M337" s="17">
+        <v>2</v>
+      </c>
+      <c r="N337" s="17">
+        <v>37.950000000000003</v>
+      </c>
+      <c r="O337" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P337" s="13" t="s">
+        <v>1115</v>
+      </c>
+      <c r="Q337" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R337" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S337" s="17">
+        <f t="shared" si="123"/>
+        <v>67</v>
+      </c>
+      <c r="T337" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="338" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A338" s="13"/>
-      <c r="B338" s="9"/>
-      <c r="C338" s="9"/>
-      <c r="D338" s="9"/>
-      <c r="E338" s="9"/>
-      <c r="F338" s="9"/>
-      <c r="G338" s="9"/>
-      <c r="H338" s="9"/>
-      <c r="I338" s="9"/>
-      <c r="J338" s="9"/>
-      <c r="K338" s="9"/>
-      <c r="L338" s="9"/>
-      <c r="M338" s="9"/>
-      <c r="N338" s="9"/>
-      <c r="O338" s="9"/>
-      <c r="P338" s="13"/>
-      <c r="Q338" s="9"/>
-      <c r="R338" s="9"/>
-      <c r="S338" s="17"/>
-      <c r="T338" s="9"/>
+      <c r="A338" s="13" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B338" s="17">
+        <v>2024</v>
+      </c>
+      <c r="C338" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D338" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E338" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F338" s="17">
+        <v>55</v>
+      </c>
+      <c r="G338" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="H338" s="9">
+        <f t="shared" ref="H338" si="159">YEAR(G338)</f>
+        <v>2025</v>
+      </c>
+      <c r="I338" s="9">
+        <f>MONTH(G338)</f>
+        <v>5</v>
+      </c>
+      <c r="J338" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K338" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L338" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M338" s="17">
+        <v>2</v>
+      </c>
+      <c r="N338" s="43">
+        <v>0</v>
+      </c>
+      <c r="O338" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P338" s="13" t="s">
+        <v>1117</v>
+      </c>
+      <c r="Q338" s="9" t="s">
+        <v>962</v>
+      </c>
+      <c r="R338" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S338" s="17">
+        <f t="shared" si="123"/>
+        <v>43</v>
+      </c>
+      <c r="T338" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="339" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A339" s="13"/>

</xml_diff>

<commit_message>
#43 Reading List: updated to 2025-05-06.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5262" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5286" uniqueCount="1123">
   <si>
     <t>Format</t>
   </si>
@@ -3395,6 +3395,21 @@
   </si>
   <si>
     <t>Useless. Very basic, no original knowledge.</t>
+  </si>
+  <si>
+    <t>Software Engineering At Google</t>
+  </si>
+  <si>
+    <t>2025-05-06</t>
+  </si>
+  <si>
+    <t>Useless. This book wasted 602 pages to state the obvious and the layout totally lacks of bold fonts, which makes skimming impossible.</t>
+  </si>
+  <si>
+    <t>Why Programs Fail (2nd Edition)</t>
+  </si>
+  <si>
+    <t>Useless. This book is a mix between a debugging guide for super-beginners and a hundreds page long mind masturbation about the topic.</t>
   </si>
 </sst>
 </file>
@@ -3677,13 +3692,13 @@
     <xf numFmtId="1" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4003,16 +4018,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50">
+      <c r="A1" s="51">
         <v>2016</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -5529,16 +5544,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50">
+      <c r="A1" s="51">
         <v>2017</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -6485,16 +6500,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50">
+      <c r="A1" s="51">
         <v>2018</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -7441,16 +7456,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50">
+      <c r="A1" s="51">
         <v>2019</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -8397,16 +8412,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50">
+      <c r="A1" s="51">
         <v>2020</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -9353,16 +9368,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50">
+      <c r="A1" s="51">
         <v>2021</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -10309,16 +10324,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50">
+      <c r="A1" s="51">
         <v>2022</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -11253,11 +11268,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:T346"/>
+  <dimension ref="A1:T356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R342" sqref="R342"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A325" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A341" sqref="A341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -31682,7 +31697,7 @@
         <v>159</v>
       </c>
       <c r="S314" s="17">
-        <f t="shared" ref="S314:S338" si="123">LEN(P314)</f>
+        <f t="shared" ref="S314:S340" si="123">LEN(P314)</f>
         <v>35</v>
       </c>
       <c r="T314" s="49">
@@ -33050,7 +33065,7 @@
         <f t="shared" si="123"/>
         <v>48</v>
       </c>
-      <c r="T335" s="52">
+      <c r="T335" s="50">
         <v>352</v>
       </c>
     </row>
@@ -33115,7 +33130,7 @@
         <f t="shared" si="123"/>
         <v>48</v>
       </c>
-      <c r="T336" s="52">
+      <c r="T336" s="50">
         <v>137</v>
       </c>
     </row>
@@ -33180,7 +33195,7 @@
         <f t="shared" si="123"/>
         <v>67</v>
       </c>
-      <c r="T337" s="52">
+      <c r="T337" s="50">
         <v>205</v>
       </c>
     </row>
@@ -33245,53 +33260,139 @@
         <f t="shared" si="123"/>
         <v>43</v>
       </c>
-      <c r="T338" s="52">
+      <c r="T338" s="50">
         <v>59</v>
       </c>
     </row>
     <row r="339" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A339" s="13"/>
-      <c r="B339" s="9"/>
-      <c r="C339" s="9"/>
-      <c r="D339" s="9"/>
-      <c r="E339" s="9"/>
-      <c r="F339" s="9"/>
-      <c r="G339" s="9"/>
-      <c r="H339" s="9"/>
-      <c r="I339" s="9"/>
-      <c r="J339" s="9"/>
-      <c r="K339" s="9"/>
-      <c r="L339" s="9"/>
-      <c r="M339" s="9"/>
-      <c r="N339" s="9"/>
-      <c r="O339" s="9"/>
-      <c r="P339" s="13"/>
-      <c r="Q339" s="9"/>
-      <c r="R339" s="9"/>
-      <c r="S339" s="17"/>
-      <c r="T339" s="9"/>
+      <c r="A339" s="13" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B339" s="17">
+        <v>2020</v>
+      </c>
+      <c r="C339" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D339" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E339" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F339" s="17">
+        <v>602</v>
+      </c>
+      <c r="G339" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="H339" s="9">
+        <f t="shared" ref="H339" si="160">YEAR(G339)</f>
+        <v>2025</v>
+      </c>
+      <c r="I339" s="9">
+        <f>MONTH(G339)</f>
+        <v>5</v>
+      </c>
+      <c r="J339" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K339" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L339" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="M339" s="17">
+        <v>1</v>
+      </c>
+      <c r="N339" s="17">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="O339" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P339" s="13" t="s">
+        <v>1120</v>
+      </c>
+      <c r="Q339" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R339" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S339" s="17">
+        <f t="shared" si="123"/>
+        <v>133</v>
+      </c>
+      <c r="T339" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="340" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A340" s="13"/>
-      <c r="B340" s="9"/>
-      <c r="C340" s="9"/>
-      <c r="D340" s="9"/>
-      <c r="E340" s="9"/>
-      <c r="F340" s="9"/>
-      <c r="G340" s="9"/>
-      <c r="H340" s="9"/>
-      <c r="I340" s="9"/>
-      <c r="J340" s="9"/>
-      <c r="K340" s="9"/>
-      <c r="L340" s="9"/>
-      <c r="M340" s="9"/>
-      <c r="N340" s="9"/>
-      <c r="O340" s="9"/>
-      <c r="P340" s="13"/>
-      <c r="Q340" s="9"/>
-      <c r="R340" s="9"/>
-      <c r="S340" s="17"/>
-      <c r="T340" s="9"/>
+      <c r="A340" s="13" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B340" s="17">
+        <v>2009</v>
+      </c>
+      <c r="C340" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D340" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E340" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F340" s="17">
+        <v>388</v>
+      </c>
+      <c r="G340" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="H340" s="9">
+        <f t="shared" ref="H340" si="161">YEAR(G340)</f>
+        <v>2025</v>
+      </c>
+      <c r="I340" s="9">
+        <f>MONTH(G340)</f>
+        <v>5</v>
+      </c>
+      <c r="J340" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K340" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L340" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="M340" s="17">
+        <v>1</v>
+      </c>
+      <c r="N340" s="17">
+        <v>69.95</v>
+      </c>
+      <c r="O340" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="P340" s="13" t="s">
+        <v>1122</v>
+      </c>
+      <c r="Q340" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="R340" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="S340" s="17">
+        <f t="shared" si="123"/>
+        <v>133</v>
+      </c>
+      <c r="T340" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="341" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A341" s="13"/>
@@ -33424,6 +33525,226 @@
       <c r="R346" s="9"/>
       <c r="S346" s="17"/>
       <c r="T346" s="9"/>
+    </row>
+    <row r="347" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A347" s="9"/>
+      <c r="B347" s="9"/>
+      <c r="C347" s="9"/>
+      <c r="D347" s="9"/>
+      <c r="E347" s="9"/>
+      <c r="F347" s="9"/>
+      <c r="G347" s="9"/>
+      <c r="H347" s="9"/>
+      <c r="I347" s="9"/>
+      <c r="J347" s="9"/>
+      <c r="K347" s="9"/>
+      <c r="L347" s="9"/>
+      <c r="M347" s="9"/>
+      <c r="N347" s="9"/>
+      <c r="O347" s="9"/>
+      <c r="P347" s="9"/>
+      <c r="Q347" s="9"/>
+      <c r="R347" s="9"/>
+      <c r="S347" s="17"/>
+      <c r="T347" s="9"/>
+    </row>
+    <row r="348" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A348" s="9"/>
+      <c r="B348" s="9"/>
+      <c r="C348" s="9"/>
+      <c r="D348" s="9"/>
+      <c r="E348" s="9"/>
+      <c r="F348" s="9"/>
+      <c r="G348" s="9"/>
+      <c r="H348" s="9"/>
+      <c r="I348" s="9"/>
+      <c r="J348" s="9"/>
+      <c r="K348" s="9"/>
+      <c r="L348" s="9"/>
+      <c r="M348" s="9"/>
+      <c r="N348" s="9"/>
+      <c r="O348" s="9"/>
+      <c r="P348" s="9"/>
+      <c r="Q348" s="9"/>
+      <c r="R348" s="9"/>
+      <c r="S348" s="17"/>
+      <c r="T348" s="9"/>
+    </row>
+    <row r="349" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A349" s="9"/>
+      <c r="B349" s="9"/>
+      <c r="C349" s="9"/>
+      <c r="D349" s="9"/>
+      <c r="E349" s="9"/>
+      <c r="F349" s="9"/>
+      <c r="G349" s="9"/>
+      <c r="H349" s="9"/>
+      <c r="I349" s="9"/>
+      <c r="J349" s="9"/>
+      <c r="K349" s="9"/>
+      <c r="L349" s="9"/>
+      <c r="M349" s="9"/>
+      <c r="N349" s="9"/>
+      <c r="O349" s="9"/>
+      <c r="P349" s="9"/>
+      <c r="Q349" s="9"/>
+      <c r="R349" s="9"/>
+      <c r="S349" s="17"/>
+      <c r="T349" s="9"/>
+    </row>
+    <row r="350" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A350" s="9"/>
+      <c r="B350" s="9"/>
+      <c r="C350" s="9"/>
+      <c r="D350" s="9"/>
+      <c r="E350" s="9"/>
+      <c r="F350" s="9"/>
+      <c r="G350" s="9"/>
+      <c r="H350" s="9"/>
+      <c r="I350" s="9"/>
+      <c r="J350" s="9"/>
+      <c r="K350" s="9"/>
+      <c r="L350" s="9"/>
+      <c r="M350" s="9"/>
+      <c r="N350" s="9"/>
+      <c r="O350" s="9"/>
+      <c r="P350" s="9"/>
+      <c r="Q350" s="9"/>
+      <c r="R350" s="9"/>
+      <c r="S350" s="17"/>
+      <c r="T350" s="9"/>
+    </row>
+    <row r="351" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A351" s="9"/>
+      <c r="B351" s="9"/>
+      <c r="C351" s="9"/>
+      <c r="D351" s="9"/>
+      <c r="E351" s="9"/>
+      <c r="F351" s="9"/>
+      <c r="G351" s="9"/>
+      <c r="H351" s="9"/>
+      <c r="I351" s="9"/>
+      <c r="J351" s="9"/>
+      <c r="K351" s="9"/>
+      <c r="L351" s="9"/>
+      <c r="M351" s="9"/>
+      <c r="N351" s="9"/>
+      <c r="O351" s="9"/>
+      <c r="P351" s="9"/>
+      <c r="Q351" s="9"/>
+      <c r="R351" s="9"/>
+      <c r="S351" s="17"/>
+      <c r="T351" s="9"/>
+    </row>
+    <row r="352" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A352" s="9"/>
+      <c r="B352" s="9"/>
+      <c r="C352" s="9"/>
+      <c r="D352" s="9"/>
+      <c r="E352" s="9"/>
+      <c r="F352" s="9"/>
+      <c r="G352" s="9"/>
+      <c r="H352" s="9"/>
+      <c r="I352" s="9"/>
+      <c r="J352" s="9"/>
+      <c r="K352" s="9"/>
+      <c r="L352" s="9"/>
+      <c r="M352" s="9"/>
+      <c r="N352" s="9"/>
+      <c r="O352" s="9"/>
+      <c r="P352" s="9"/>
+      <c r="Q352" s="9"/>
+      <c r="R352" s="9"/>
+      <c r="S352" s="17"/>
+      <c r="T352" s="9"/>
+    </row>
+    <row r="353" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A353" s="9"/>
+      <c r="B353" s="9"/>
+      <c r="C353" s="9"/>
+      <c r="D353" s="9"/>
+      <c r="E353" s="9"/>
+      <c r="F353" s="9"/>
+      <c r="G353" s="9"/>
+      <c r="H353" s="9"/>
+      <c r="I353" s="9"/>
+      <c r="J353" s="9"/>
+      <c r="K353" s="9"/>
+      <c r="L353" s="9"/>
+      <c r="M353" s="9"/>
+      <c r="N353" s="9"/>
+      <c r="O353" s="9"/>
+      <c r="P353" s="9"/>
+      <c r="Q353" s="9"/>
+      <c r="R353" s="9"/>
+      <c r="S353" s="17"/>
+      <c r="T353" s="9"/>
+    </row>
+    <row r="354" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A354" s="9"/>
+      <c r="B354" s="9"/>
+      <c r="C354" s="9"/>
+      <c r="D354" s="9"/>
+      <c r="E354" s="9"/>
+      <c r="F354" s="9"/>
+      <c r="G354" s="9"/>
+      <c r="H354" s="9"/>
+      <c r="I354" s="9"/>
+      <c r="J354" s="9"/>
+      <c r="K354" s="9"/>
+      <c r="L354" s="9"/>
+      <c r="M354" s="9"/>
+      <c r="N354" s="9"/>
+      <c r="O354" s="9"/>
+      <c r="P354" s="9"/>
+      <c r="Q354" s="9"/>
+      <c r="R354" s="9"/>
+      <c r="S354" s="17"/>
+      <c r="T354" s="9"/>
+    </row>
+    <row r="355" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A355" s="9"/>
+      <c r="B355" s="9"/>
+      <c r="C355" s="9"/>
+      <c r="D355" s="9"/>
+      <c r="E355" s="9"/>
+      <c r="F355" s="9"/>
+      <c r="G355" s="9"/>
+      <c r="H355" s="9"/>
+      <c r="I355" s="9"/>
+      <c r="J355" s="9"/>
+      <c r="K355" s="9"/>
+      <c r="L355" s="9"/>
+      <c r="M355" s="9"/>
+      <c r="N355" s="9"/>
+      <c r="O355" s="9"/>
+      <c r="P355" s="9"/>
+      <c r="Q355" s="9"/>
+      <c r="R355" s="9"/>
+      <c r="S355" s="17"/>
+      <c r="T355" s="9"/>
+    </row>
+    <row r="356" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A356" s="9"/>
+      <c r="B356" s="9"/>
+      <c r="C356" s="9"/>
+      <c r="D356" s="9"/>
+      <c r="E356" s="9"/>
+      <c r="F356" s="9"/>
+      <c r="G356" s="9"/>
+      <c r="H356" s="9"/>
+      <c r="I356" s="9"/>
+      <c r="J356" s="9"/>
+      <c r="K356" s="9"/>
+      <c r="L356" s="9"/>
+      <c r="M356" s="9"/>
+      <c r="N356" s="9"/>
+      <c r="O356" s="9"/>
+      <c r="P356" s="9"/>
+      <c r="Q356" s="9"/>
+      <c r="R356" s="9"/>
+      <c r="S356" s="17"/>
+      <c r="T356" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#43 Reading List: updated to 2025-05-11.
</commit_message>
<xml_diff>
--- a/data/Reading List.xlsx
+++ b/data/Reading List.xlsx
@@ -11272,7 +11272,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A325" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A341" sqref="A341"/>
+      <selection pane="bottomLeft" activeCell="J342" sqref="J342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -32966,7 +32966,7 @@
         <v>2025</v>
       </c>
       <c r="I334" s="9">
-        <f>MONTH(G334)</f>
+        <f t="shared" ref="I334:I340" si="157">MONTH(G334)</f>
         <v>3</v>
       </c>
       <c r="J334" s="9" t="s">
@@ -33031,7 +33031,7 @@
         <v>2025</v>
       </c>
       <c r="I335" s="9">
-        <f>MONTH(G335)</f>
+        <f t="shared" si="157"/>
         <v>5</v>
       </c>
       <c r="J335" s="9" t="s">
@@ -33092,11 +33092,11 @@
         <v>1110</v>
       </c>
       <c r="H336" s="9">
-        <f t="shared" ref="H336" si="157">YEAR(G336)</f>
+        <f t="shared" ref="H336" si="158">YEAR(G336)</f>
         <v>2025</v>
       </c>
       <c r="I336" s="9">
-        <f>MONTH(G336)</f>
+        <f t="shared" si="157"/>
         <v>5</v>
       </c>
       <c r="J336" s="9" t="s">
@@ -33157,11 +33157,11 @@
         <v>1110</v>
       </c>
       <c r="H337" s="9">
-        <f t="shared" ref="H337" si="158">YEAR(G337)</f>
+        <f t="shared" ref="H337" si="159">YEAR(G337)</f>
         <v>2025</v>
       </c>
       <c r="I337" s="9">
-        <f>MONTH(G337)</f>
+        <f t="shared" si="157"/>
         <v>5</v>
       </c>
       <c r="J337" s="9" t="s">
@@ -33222,11 +33222,11 @@
         <v>1110</v>
       </c>
       <c r="H338" s="9">
-        <f t="shared" ref="H338" si="159">YEAR(G338)</f>
+        <f t="shared" ref="H338" si="160">YEAR(G338)</f>
         <v>2025</v>
       </c>
       <c r="I338" s="9">
-        <f>MONTH(G338)</f>
+        <f t="shared" si="157"/>
         <v>5</v>
       </c>
       <c r="J338" s="9" t="s">
@@ -33287,11 +33287,11 @@
         <v>1119</v>
       </c>
       <c r="H339" s="9">
-        <f t="shared" ref="H339" si="160">YEAR(G339)</f>
+        <f t="shared" ref="H339" si="161">YEAR(G339)</f>
         <v>2025</v>
       </c>
       <c r="I339" s="9">
-        <f>MONTH(G339)</f>
+        <f t="shared" si="157"/>
         <v>5</v>
       </c>
       <c r="J339" s="9" t="s">
@@ -33325,8 +33325,8 @@
         <f t="shared" si="123"/>
         <v>133</v>
       </c>
-      <c r="T339" s="17">
-        <v>0</v>
+      <c r="T339" s="50">
+        <v>177</v>
       </c>
     </row>
     <row r="340" spans="1:20" x14ac:dyDescent="0.2">
@@ -33352,11 +33352,11 @@
         <v>1119</v>
       </c>
       <c r="H340" s="9">
-        <f t="shared" ref="H340" si="161">YEAR(G340)</f>
+        <f t="shared" ref="H340" si="162">YEAR(G340)</f>
         <v>2025</v>
       </c>
       <c r="I340" s="9">
-        <f>MONTH(G340)</f>
+        <f t="shared" si="157"/>
         <v>5</v>
       </c>
       <c r="J340" s="9" t="s">
@@ -33390,8 +33390,8 @@
         <f t="shared" si="123"/>
         <v>133</v>
       </c>
-      <c r="T340" s="17">
-        <v>0</v>
+      <c r="T340" s="50">
+        <v>96</v>
       </c>
     </row>
     <row r="341" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>